<commit_message>
Reorg and small fixes
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\ATDD Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44657F3C-8F03-4ED8-B4B5-001FFE120606}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEA522B-04E4-40D2-A09C-C9731B64ACBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -713,6 +713,54 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -775,54 +823,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -837,28 +837,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M168" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M168" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:M168" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:M169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A165" sqref="A165:M165"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:XFD146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5049,341 +5049,341 @@
       </c>
       <c r="M118"/>
     </row>
-    <row r="119" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="s">
         <v>81</v>
       </c>
       <c r="B119" s="20" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="C119" s="20"/>
       <c r="D119" s="21"/>
       <c r="E119" s="21"/>
       <c r="F119" s="22" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="G119" s="20"/>
       <c r="H119" s="23"/>
       <c r="I119" s="24">
+        <v>26</v>
+      </c>
+      <c r="J119" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
+      </c>
+      <c r="K119" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
+      </c>
+      <c r="L119" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0026 'Check that lookup value is inherited from customer template to customer when creating customer from contact' {</v>
+      </c>
+      <c r="M119" s="20"/>
+    </row>
+    <row r="120" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" t="s">
+        <v>158</v>
+      </c>
+      <c r="G120" t="s">
+        <v>15</v>
+      </c>
+      <c r="H120" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="I120" s="14">
+        <v>26</v>
+      </c>
+      <c r="J120" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] A customer template with lookup value</v>
+      </c>
+      <c r="K120" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] A customer template with lookup value</v>
+      </c>
+      <c r="L120" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A customer template with lookup value' } }</v>
+      </c>
+      <c r="M120"/>
+    </row>
+    <row r="121" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>81</v>
+      </c>
+      <c r="B121" t="s">
+        <v>158</v>
+      </c>
+      <c r="G121" t="s">
+        <v>15</v>
+      </c>
+      <c r="H121" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="I121" s="14">
+        <v>26</v>
+      </c>
+      <c r="J121" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] A contact</v>
+      </c>
+      <c r="K121" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] A contact</v>
+      </c>
+      <c r="L121" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A contact' } }</v>
+      </c>
+      <c r="M121"/>
+    </row>
+    <row r="122" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" t="s">
+        <v>158</v>
+      </c>
+      <c r="G122" t="s">
+        <v>18</v>
+      </c>
+      <c r="H122" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I122" s="14">
+        <v>26</v>
+      </c>
+      <c r="J122" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Customer is created from contact</v>
+      </c>
+      <c r="K122" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Customer is created from contact</v>
+      </c>
+      <c r="L122" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Customer is created from contact' } }</v>
+      </c>
+      <c r="M122"/>
+    </row>
+    <row r="123" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>81</v>
+      </c>
+      <c r="B123" t="s">
+        <v>158</v>
+      </c>
+      <c r="G123" t="s">
+        <v>20</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="I123" s="14">
+        <v>26</v>
+      </c>
+      <c r="J123" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
+      </c>
+      <c r="K123" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
+      </c>
+      <c r="L123" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer has lookup value code field populated with lookup value from customer template'</v>
+      </c>
+      <c r="M123"/>
+    </row>
+    <row r="124" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B124" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124" s="20"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G124" s="20"/>
+      <c r="H124" s="23"/>
+      <c r="I124" s="24">
         <v>28</v>
       </c>
-      <c r="J119" s="20" t="str">
+      <c r="J124" s="20" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0028] Create customer from configuration template with lookup value</v>
       </c>
-      <c r="K119" s="26" t="str">
+      <c r="K124" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0028] Create customer from configuration template with lookup value</v>
       </c>
-      <c r="L119" s="33" t="str">
+      <c r="L124" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0028 'Create customer from configuration template with lookup value' {</v>
       </c>
-      <c r="M119" s="20"/>
-    </row>
-    <row r="120" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>81</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="M124" s="20"/>
+    </row>
+    <row r="125" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>81</v>
+      </c>
+      <c r="B125" t="s">
         <v>125</v>
       </c>
-      <c r="G120" t="s">
-        <v>15</v>
-      </c>
-      <c r="H120" s="13" t="s">
+      <c r="G125" t="s">
+        <v>15</v>
+      </c>
+      <c r="H125" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I120" s="14">
+      <c r="I125" s="14">
         <v>28</v>
       </c>
-      <c r="J120" t="str">
+      <c r="J125" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] A configuration template (customer) with lookup value</v>
       </c>
-      <c r="K120" s="17" t="str">
+      <c r="K125" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] A configuration template (customer) with lookup value</v>
       </c>
-      <c r="L120" s="31" t="str">
+      <c r="L125" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'A configuration template (customer) with lookup value' } }</v>
       </c>
-      <c r="M120"/>
-    </row>
-    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>81</v>
-      </c>
-      <c r="B121" t="s">
+      <c r="M125"/>
+    </row>
+    <row r="126" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>81</v>
+      </c>
+      <c r="B126" t="s">
         <v>125</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G126" t="s">
         <v>18</v>
       </c>
-      <c r="H121" s="13" t="s">
+      <c r="H126" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I121" s="14">
+      <c r="I126" s="14">
         <v>28</v>
       </c>
-      <c r="J121" t="str">
+      <c r="J126" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Create customer from configuration template</v>
       </c>
-      <c r="K121" s="17" t="str">
+      <c r="K126" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Create customer from configuration template</v>
       </c>
-      <c r="L121" s="31" t="str">
+      <c r="L126" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'Create customer from configuration template' } }</v>
       </c>
-      <c r="M121"/>
-    </row>
-    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>81</v>
-      </c>
-      <c r="B122" t="s">
+      <c r="M126"/>
+    </row>
+    <row r="127" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>81</v>
+      </c>
+      <c r="B127" t="s">
         <v>125</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G127" t="s">
         <v>20</v>
       </c>
-      <c r="H122" s="13" t="s">
+      <c r="H127" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I122" s="14">
+      <c r="I127" s="14">
         <v>28</v>
       </c>
-      <c r="J122" t="str">
+      <c r="J127" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
       </c>
-      <c r="K122" s="17" t="str">
+      <c r="K127" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
       </c>
-      <c r="L122" s="31" t="str">
+      <c r="L127" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value on customer is populated with lookup value of configuration template'</v>
       </c>
-      <c r="M122"/>
-    </row>
-    <row r="123" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B123" s="20" t="s">
+      <c r="M127"/>
+    </row>
+    <row r="128" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B128" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C123" s="20"/>
-      <c r="D123" s="21"/>
-      <c r="E123" s="21"/>
-      <c r="F123" s="22" t="s">
+      <c r="C128" s="20"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G123" s="20"/>
-      <c r="H123" s="23"/>
-      <c r="I123" s="24">
+      <c r="G128" s="20"/>
+      <c r="H128" s="23"/>
+      <c r="I128" s="24">
         <v>30</v>
       </c>
-      <c r="J123" s="20" t="str">
+      <c r="J128" s="20" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
       </c>
-      <c r="K123" s="26" t="str">
+      <c r="K128" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
       </c>
-      <c r="L123" s="33" t="str">
+      <c r="L128" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0030 'Create warehouse shipment from sales order with lookup value' {</v>
       </c>
-      <c r="M123" s="20"/>
-    </row>
-    <row r="124" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>81</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="M128" s="20"/>
+    </row>
+    <row r="129" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>81</v>
+      </c>
+      <c r="B129" t="s">
         <v>157</v>
       </c>
-      <c r="G124" t="s">
-        <v>15</v>
-      </c>
-      <c r="H124" s="13" t="s">
+      <c r="G129" t="s">
+        <v>15</v>
+      </c>
+      <c r="H129" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I124" s="14">
+      <c r="I129" s="14">
         <v>30</v>
       </c>
-      <c r="J124" t="str">
+      <c r="J129" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] A lookup value</v>
       </c>
-      <c r="K124" s="17" t="str">
+      <c r="K129" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] A lookup value</v>
       </c>
-      <c r="L124" s="31" t="str">
+      <c r="L129" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'A lookup value' } }</v>
       </c>
-      <c r="M124"/>
-    </row>
-    <row r="125" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>81</v>
-      </c>
-      <c r="B125" t="s">
-        <v>157</v>
-      </c>
-      <c r="G125" t="s">
-        <v>15</v>
-      </c>
-      <c r="H125" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I125" s="14">
-        <v>30</v>
-      </c>
-      <c r="J125" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A location with require shipment</v>
-      </c>
-      <c r="K125" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A location with require shipment</v>
-      </c>
-      <c r="L125" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A location with require shipment' } }</v>
-      </c>
-      <c r="M125"/>
-    </row>
-    <row r="126" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>81</v>
-      </c>
-      <c r="B126" t="s">
-        <v>157</v>
-      </c>
-      <c r="G126" t="s">
-        <v>15</v>
-      </c>
-      <c r="H126" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I126" s="14">
-        <v>30</v>
-      </c>
-      <c r="J126" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A warehouse employee for current user</v>
-      </c>
-      <c r="K126" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A warehouse employee for current user</v>
-      </c>
-      <c r="L126" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A warehouse employee for current user' } }</v>
-      </c>
-      <c r="M126"/>
-    </row>
-    <row r="127" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>81</v>
-      </c>
-      <c r="B127" t="s">
-        <v>157</v>
-      </c>
-      <c r="G127" t="s">
-        <v>18</v>
-      </c>
-      <c r="H127" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I127" s="14">
-        <v>30</v>
-      </c>
-      <c r="J127" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="K127" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="L127" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location' } }</v>
-      </c>
-      <c r="M127"/>
-    </row>
-    <row r="128" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>81</v>
-      </c>
-      <c r="B128" t="s">
-        <v>157</v>
-      </c>
-      <c r="G128" t="s">
-        <v>20</v>
-      </c>
-      <c r="H128" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I128" s="14">
-        <v>30</v>
-      </c>
-      <c r="J128" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
-      </c>
-      <c r="K128" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
-      </c>
-      <c r="L128" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
-      </c>
-      <c r="M128"/>
-    </row>
-    <row r="129" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B129" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C129" s="20"/>
-      <c r="D129" s="21"/>
-      <c r="E129" s="21"/>
-      <c r="F129" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G129" s="20"/>
-      <c r="H129" s="23"/>
-      <c r="I129" s="24">
-        <v>31</v>
-      </c>
-      <c r="J129" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
-      </c>
-      <c r="K129" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
-      </c>
-      <c r="L129" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0031 'Get sales order with lookup value on warehouse shipment' {</v>
-      </c>
-      <c r="M129" s="20"/>
+      <c r="M129"/>
     </row>
     <row r="130" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
@@ -5396,26 +5396,26 @@
         <v>15</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="I130" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J130" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A lookup value</v>
+        <v>[GIVEN] A location with require shipment</v>
       </c>
       <c r="K130" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A lookup value</v>
+        <v>//[GIVEN] A location with require shipment</v>
       </c>
       <c r="L130" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A lookup value' } }</v>
+        <v>Given 'A location with require shipment' } }</v>
       </c>
       <c r="M130"/>
     </row>
-    <row r="131" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>81</v>
       </c>
@@ -5426,26 +5426,26 @@
         <v>15</v>
       </c>
       <c r="H131" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I131" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J131" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A location with require shipment</v>
+        <v>[GIVEN] A warehouse employee for current user</v>
       </c>
       <c r="K131" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A location with require shipment</v>
+        <v>//[GIVEN] A warehouse employee for current user</v>
       </c>
       <c r="L131" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A location with require shipment' } }</v>
+        <v>Given 'A warehouse employee for current user' } }</v>
       </c>
       <c r="M131"/>
     </row>
-    <row r="132" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>81</v>
       </c>
@@ -5453,29 +5453,29 @@
         <v>157</v>
       </c>
       <c r="G132" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="I132" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J132" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A warehouse employee for current user</v>
+        <v>[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="K132" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A warehouse employee for current user</v>
+        <v>//[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="L132" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A warehouse employee for current user' } }</v>
+        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location' } }</v>
       </c>
       <c r="M132"/>
     </row>
-    <row r="133" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>81</v>
       </c>
@@ -5483,59 +5483,61 @@
         <v>157</v>
       </c>
       <c r="G133" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I133" s="14">
+        <v>30</v>
+      </c>
+      <c r="J133" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="K133" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="L133" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+      </c>
+      <c r="M133"/>
+    </row>
+    <row r="134" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B134" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C134" s="20"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="21"/>
+      <c r="F134" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G134" s="20"/>
+      <c r="H134" s="23"/>
+      <c r="I134" s="24">
         <v>31</v>
       </c>
-      <c r="J133" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="K133" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="L133" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A released sales order with lookup value and with line with require shipment location' } }</v>
-      </c>
-      <c r="M133"/>
-    </row>
-    <row r="134" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>81</v>
-      </c>
-      <c r="B134" t="s">
-        <v>157</v>
-      </c>
-      <c r="G134" t="s">
-        <v>15</v>
-      </c>
-      <c r="H134" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I134" s="14">
-        <v>31</v>
-      </c>
-      <c r="J134" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A warehouse shipment without lines</v>
-      </c>
-      <c r="K134" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A warehouse shipment without lines</v>
-      </c>
-      <c r="L134" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A warehouse shipment without lines' } }</v>
-      </c>
-      <c r="M134"/>
-    </row>
-    <row r="135" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="J134" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="K134" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="L134" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0031 'Get sales order with lookup value on warehouse shipment' {</v>
+      </c>
+      <c r="M134" s="20"/>
+    </row>
+    <row r="135" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>81</v>
       </c>
@@ -5543,29 +5545,29 @@
         <v>157</v>
       </c>
       <c r="G135" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H135" s="13" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="I135" s="14">
         <v>31</v>
       </c>
       <c r="J135" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Get sales order with lookup value on warehouse shipment</v>
+        <v>[GIVEN] A lookup value</v>
       </c>
       <c r="K135" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Get sales order with lookup value on warehouse shipment</v>
+        <v>//[GIVEN] A lookup value</v>
       </c>
       <c r="L135" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Get sales order with lookup value on warehouse shipment' } }</v>
+        <v>Given 'A lookup value' } }</v>
       </c>
       <c r="M135"/>
     </row>
-    <row r="136" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>81</v>
       </c>
@@ -5573,87 +5575,85 @@
         <v>157</v>
       </c>
       <c r="G136" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I136" s="14">
         <v>31</v>
       </c>
       <c r="J136" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
+        <v>[GIVEN] A location with require shipment</v>
       </c>
       <c r="K136" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
+        <v>//[GIVEN] A location with require shipment</v>
       </c>
       <c r="L136" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+        <v>Given 'A location with require shipment' } }</v>
       </c>
       <c r="M136"/>
     </row>
-    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B137" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C137" s="20"/>
-      <c r="D137" s="21"/>
-      <c r="E137" s="21"/>
-      <c r="F137" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G137" s="20"/>
-      <c r="H137" s="23"/>
-      <c r="I137" s="24">
-        <v>26</v>
-      </c>
-      <c r="J137" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
-      </c>
-      <c r="K137" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
-      </c>
-      <c r="L137" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0026 'Check that lookup value is inherited from customer template to customer when creating customer from contact' {</v>
-      </c>
-      <c r="M137" s="20"/>
-    </row>
-    <row r="138" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>81</v>
+      </c>
+      <c r="B137" t="s">
+        <v>157</v>
+      </c>
+      <c r="G137" t="s">
+        <v>15</v>
+      </c>
+      <c r="H137" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I137" s="14">
+        <v>31</v>
+      </c>
+      <c r="J137" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] A warehouse employee for current user</v>
+      </c>
+      <c r="K137" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] A warehouse employee for current user</v>
+      </c>
+      <c r="L137" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A warehouse employee for current user' } }</v>
+      </c>
+      <c r="M137"/>
+    </row>
+    <row r="138" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>81</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G138" t="s">
         <v>15</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="I138" s="14">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J138" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A customer template with lookup value</v>
+        <v>[GIVEN] A released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="K138" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A customer template with lookup value</v>
+        <v>//[GIVEN] A released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="L138" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A customer template with lookup value' } }</v>
+        <v>Given 'A released sales order with lookup value and with line with require shipment location' } }</v>
       </c>
       <c r="M138"/>
     </row>
@@ -5662,88 +5662,88 @@
         <v>81</v>
       </c>
       <c r="B139" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="I139" s="14">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J139" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A contact</v>
+        <v>[GIVEN] A warehouse shipment without lines</v>
       </c>
       <c r="K139" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A contact</v>
+        <v>//[GIVEN] A warehouse shipment without lines</v>
       </c>
       <c r="L139" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A contact' } }</v>
+        <v>Given 'A warehouse shipment without lines' } }</v>
       </c>
       <c r="M139"/>
     </row>
-    <row r="140" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>81</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G140" t="s">
         <v>18</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="I140" s="14">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J140" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Customer is created from contact</v>
+        <v>[WHEN] Get sales order with lookup value on warehouse shipment</v>
       </c>
       <c r="K140" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Customer is created from contact</v>
+        <v>//[WHEN] Get sales order with lookup value on warehouse shipment</v>
       </c>
       <c r="L140" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Customer is created from contact' } }</v>
+        <v>When 'Get sales order with lookup value on warehouse shipment' } }</v>
       </c>
       <c r="M140"/>
     </row>
-    <row r="141" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>81</v>
       </c>
       <c r="B141" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G141" t="s">
         <v>20</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="I141" s="14">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J141" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
+        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="K141" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
+        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="L141" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer has lookup value code field populated with lookup value from customer template' } }</v>
+        <v>Then 'Warehouse shipment line has lookup value code field populated' } }</v>
       </c>
       <c r="M141"/>
     </row>
@@ -6649,28 +6649,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cleaned up [FEATURE] references and ATDD sheets
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD9853-EFE5-4CB5-8F8C-293CA91A754B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F309E-88C3-467D-B8C0-0365A8E508BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -315,9 +315,6 @@
     <t>Inheritance</t>
   </si>
   <si>
-    <t>Inheritance / Sales Document / Customer</t>
-  </si>
-  <si>
     <t>Assign customer lookup value to sales document</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>Lookup value on sales document is populated with lookup value of customer</t>
   </si>
   <si>
-    <t>Inheritance / Customer / Configuration Templates</t>
-  </si>
-  <si>
     <t>Create customer from configuration template with lookup value</t>
   </si>
   <si>
@@ -405,12 +399,6 @@
     <t>FEATURE</t>
   </si>
   <si>
-    <t>Inheritance / Warehouse Shipment</t>
-  </si>
-  <si>
-    <t>Inheritance / Contact</t>
-  </si>
-  <si>
     <t>Lookup value</t>
   </si>
   <si>
@@ -508,6 +496,18 @@
   </si>
   <si>
     <t>Released sales order with lookup value and with line with require shipment location</t>
+  </si>
+  <si>
+    <t>Inheritance - Sales Document / Customer</t>
+  </si>
+  <si>
+    <t>Inheritance - Contact</t>
+  </si>
+  <si>
+    <t>Inheritance - Customer / Configuration Templates</t>
+  </si>
+  <si>
+    <t>Inheritance - Warehouse Shipment</t>
   </si>
 </sst>
 </file>
@@ -710,6 +710,54 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -772,54 +820,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -834,28 +834,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M168" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M168" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:M168" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:M169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1215,7 +1215,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -1234,7 +1234,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="8" t="str">
@@ -1296,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I4" s="14">
         <v>1</v>
@@ -1449,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I9" s="14">
         <v>2</v>
@@ -1481,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I10" s="14">
         <v>2</v>
@@ -1611,7 +1611,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I14" s="14">
         <v>3</v>
@@ -1643,7 +1643,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I15" s="14">
         <v>3</v>
@@ -1738,7 +1738,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
       <c r="H18" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="18" t="str">
@@ -1798,7 +1798,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I20" s="14">
         <v>4</v>
@@ -1827,7 +1827,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I21" s="14">
         <v>4</v>
@@ -1951,7 +1951,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I25" s="14">
         <v>5</v>
@@ -1983,7 +1983,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I26" s="14">
         <v>5</v>
@@ -2118,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I30" s="14">
         <v>6</v>
@@ -2153,7 +2153,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I31" s="14">
         <v>6</v>
@@ -2294,7 +2294,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I35" s="14">
         <v>7</v>
@@ -2329,7 +2329,7 @@
         <v>15</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I36" s="14">
         <v>7</v>
@@ -2470,7 +2470,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I40" s="14">
         <v>8</v>
@@ -2505,7 +2505,7 @@
         <v>15</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I41" s="14">
         <v>8</v>
@@ -2646,7 +2646,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I45" s="14">
         <v>9</v>
@@ -2681,7 +2681,7 @@
         <v>15</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I46" s="14">
         <v>9</v>
@@ -2822,7 +2822,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I50" s="14">
         <v>10</v>
@@ -2857,7 +2857,7 @@
         <v>15</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I51" s="14">
         <v>10</v>
@@ -2998,7 +2998,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I55" s="14">
         <v>11</v>
@@ -3033,7 +3033,7 @@
         <v>15</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I56" s="14">
         <v>11</v>
@@ -3134,7 +3134,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="5"/>
       <c r="H59" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="18" t="str">
@@ -3196,7 +3196,7 @@
         <v>15</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I61" s="14">
         <v>12</v>
@@ -3225,7 +3225,7 @@
         <v>15</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I62" s="14">
         <v>12</v>
@@ -3349,7 +3349,7 @@
         <v>15</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I66" s="14">
         <v>13</v>
@@ -3381,7 +3381,7 @@
         <v>15</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I67" s="14">
         <v>13</v>
@@ -3511,7 +3511,7 @@
         <v>15</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I71" s="14">
         <v>14</v>
@@ -3543,7 +3543,7 @@
         <v>15</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I72" s="14">
         <v>14</v>
@@ -3638,7 +3638,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="5"/>
       <c r="H75" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="18" t="str">
@@ -3698,7 +3698,7 @@
         <v>15</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I77" s="14">
         <v>15</v>
@@ -3727,7 +3727,7 @@
         <v>15</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I78" s="14">
         <v>15</v>
@@ -3756,7 +3756,7 @@
         <v>15</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I79" s="14">
         <v>15</v>
@@ -3785,7 +3785,7 @@
         <v>15</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I80" s="14">
         <v>15</v>
@@ -3909,7 +3909,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I84" s="14">
         <v>16</v>
@@ -3927,7 +3927,7 @@
         <v>Given 'Non-existing lookup value' }</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>15</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I85" s="14">
         <v>16</v>
@@ -4071,7 +4071,7 @@
         <v>15</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I89" s="14">
         <v>17</v>
@@ -4103,7 +4103,7 @@
         <v>15</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I90" s="14">
         <v>17</v>
@@ -4135,7 +4135,7 @@
         <v>15</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I91" s="14">
         <v>17</v>
@@ -4167,7 +4167,7 @@
         <v>15</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I92" s="14">
         <v>17</v>
@@ -4217,7 +4217,7 @@
         <v>When 'Set lookup value on warehouse shipment line on warehouse shipment document page' } }</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>65</v>
       </c>
@@ -4246,367 +4246,340 @@
       </c>
       <c r="L94" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated' } }</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="I95" s="9"/>
-      <c r="J95" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue Sales Archive</v>
-      </c>
-      <c r="K95" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue Sales Archive</v>
-      </c>
-      <c r="L95" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue Sales Archive' {</v>
-      </c>
-      <c r="M95" s="8"/>
-    </row>
-    <row r="96" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B96" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C96" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D96" s="21"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G96" s="20"/>
-      <c r="H96" s="23"/>
-      <c r="I96" s="24">
-        <v>18</v>
-      </c>
-      <c r="J96" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0018] Archive sales order with lookup value</v>
-      </c>
-      <c r="K96" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0018] Archive sales order with lookup value</v>
-      </c>
-      <c r="L96" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0018 'Archive sales order with lookup value' {</v>
-      </c>
-      <c r="M96" s="23"/>
+        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C95" s="20"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G95" s="20"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="24">
+        <v>30</v>
+      </c>
+      <c r="J95" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
+      </c>
+      <c r="K95" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
+      </c>
+      <c r="L95" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0030 'Create warehouse shipment from sales order with lookup value' {</v>
+      </c>
+      <c r="M95" s="20"/>
+    </row>
+    <row r="96" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" t="s">
+        <v>157</v>
+      </c>
+      <c r="G96" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I96" s="14">
+        <v>30</v>
+      </c>
+      <c r="J96" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value</v>
+      </c>
+      <c r="K96" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup value</v>
+      </c>
+      <c r="L96" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value' } }</v>
+      </c>
+      <c r="M96"/>
     </row>
     <row r="97" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>77</v>
-      </c>
-      <c r="C97" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I97" s="14">
+        <v>30</v>
+      </c>
+      <c r="J97" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Location with require shipment</v>
+      </c>
+      <c r="K97" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Location with require shipment</v>
+      </c>
+      <c r="L97" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment' } }</v>
+      </c>
+      <c r="M97"/>
+    </row>
+    <row r="98" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98" t="s">
+        <v>157</v>
+      </c>
+      <c r="G98" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I98" s="14">
+        <v>30</v>
+      </c>
+      <c r="J98" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse employee for current user</v>
+      </c>
+      <c r="K98" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse employee for current user</v>
+      </c>
+      <c r="L98" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user' } }</v>
+      </c>
+      <c r="M98"/>
+    </row>
+    <row r="99" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>65</v>
+      </c>
+      <c r="B99" t="s">
+        <v>157</v>
+      </c>
+      <c r="G99" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I99" s="14">
+        <v>30</v>
+      </c>
+      <c r="J99" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
+      </c>
+      <c r="K99" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
+      </c>
+      <c r="L99" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location' } }</v>
+      </c>
+      <c r="M99"/>
+    </row>
+    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" t="s">
+        <v>157</v>
+      </c>
+      <c r="G100" t="s">
         <v>18</v>
       </c>
-      <c r="J97" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales order with Lookup value</v>
-      </c>
-      <c r="K97" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales order with Lookup value</v>
-      </c>
-      <c r="L97" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order with Lookup value' } }</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>65</v>
-      </c>
-      <c r="B98" t="s">
-        <v>77</v>
-      </c>
-      <c r="C98" t="s">
-        <v>37</v>
-      </c>
-      <c r="G98" t="s">
-        <v>16</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="I98" s="14">
-        <v>18</v>
-      </c>
-      <c r="J98" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales order is archived</v>
-      </c>
-      <c r="K98" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales order is archived</v>
-      </c>
-      <c r="L98" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is archived' } }</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>65</v>
-      </c>
-      <c r="B99" t="s">
-        <v>77</v>
-      </c>
-      <c r="C99" t="s">
-        <v>37</v>
-      </c>
-      <c r="G99" t="s">
-        <v>18</v>
-      </c>
-      <c r="H99" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I99" s="14">
-        <v>18</v>
-      </c>
-      <c r="J99" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Archived sales order has lookup value from sales order</v>
-      </c>
-      <c r="K99" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Archived sales order has lookup value from sales order</v>
-      </c>
-      <c r="L99" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales order has lookup value from sales order'</v>
-      </c>
-      <c r="M99"/>
-    </row>
-    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C100" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="21"/>
-      <c r="E100" s="21"/>
-      <c r="F100" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="G100" s="20"/>
-      <c r="H100" s="23"/>
-      <c r="I100" s="24">
-        <v>19</v>
-      </c>
-      <c r="J100" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0019] Archive sales quote with lookup value</v>
-      </c>
-      <c r="K100" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0019] Archive sales quote with lookup value</v>
-      </c>
-      <c r="L100" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0019 'Archive sales quote with lookup value' {</v>
-      </c>
-      <c r="M100" s="20"/>
-    </row>
-    <row r="101" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>65</v>
-      </c>
-      <c r="B101" t="s">
-        <v>77</v>
-      </c>
-      <c r="C101" t="s">
-        <v>33</v>
-      </c>
-      <c r="G101" t="s">
-        <v>15</v>
-      </c>
-      <c r="H101" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I101" s="14">
-        <v>19</v>
-      </c>
-      <c r="J101" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales quote with Lookup value</v>
-      </c>
-      <c r="K101" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales quote with Lookup value</v>
-      </c>
-      <c r="L101" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales quote with Lookup value' } }</v>
-      </c>
-      <c r="M101"/>
+      <c r="H100" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I100" s="14">
+        <v>30</v>
+      </c>
+      <c r="J100" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="K100" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="L100" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+      </c>
+      <c r="M100"/>
+    </row>
+    <row r="101" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" s="20"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G101" s="20"/>
+      <c r="H101" s="23"/>
+      <c r="I101" s="24">
+        <v>31</v>
+      </c>
+      <c r="J101" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="K101" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="L101" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0031 'Get sales order with lookup value on warehouse shipment' {</v>
+      </c>
+      <c r="M101" s="20"/>
     </row>
     <row r="102" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>65</v>
       </c>
       <c r="B102" t="s">
-        <v>77</v>
-      </c>
-      <c r="C102" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="G102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="I102" s="14">
-        <v>19</v>
-      </c>
-      <c r="J102" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales quote is archived</v>
+        <v>31</v>
+      </c>
+      <c r="J102" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value</v>
       </c>
       <c r="K102" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales quote is archived</v>
+        <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L102" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales quote is archived' } }</v>
+        <v>Given 'Lookup value' } }</v>
       </c>
       <c r="M102"/>
     </row>
-    <row r="103" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
-      </c>
-      <c r="C103" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="G103" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="I103" s="14">
-        <v>19</v>
-      </c>
-      <c r="J103" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Archived sales quote has lookup value from sales quote</v>
+        <v>31</v>
+      </c>
+      <c r="J103" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="K103" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Archived sales quote has lookup value from sales quote</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L103" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales quote has lookup value from sales quote'</v>
+        <v>Given 'Location with require shipment' } }</v>
       </c>
       <c r="M103"/>
     </row>
-    <row r="104" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B104" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C104" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D104" s="21"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G104" s="20"/>
-      <c r="H104" s="23"/>
-      <c r="I104" s="24">
-        <v>20</v>
-      </c>
-      <c r="J104" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0020] Archive sales return order with lookup value</v>
-      </c>
-      <c r="K104" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0020] Archive sales return order with lookup value</v>
-      </c>
-      <c r="L104" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0020 'Archive sales return order with lookup value' {</v>
-      </c>
-      <c r="M104" s="20"/>
-    </row>
-    <row r="105" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>65</v>
+      </c>
+      <c r="B104" t="s">
+        <v>157</v>
+      </c>
+      <c r="G104" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I104" s="14">
+        <v>31</v>
+      </c>
+      <c r="J104" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse employee for current user</v>
+      </c>
+      <c r="K104" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse employee for current user</v>
+      </c>
+      <c r="L104" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user' } }</v>
+      </c>
+      <c r="M104"/>
+    </row>
+    <row r="105" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>77</v>
-      </c>
-      <c r="C105" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="G105" t="s">
         <v>15</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="I105" s="14">
-        <v>20</v>
-      </c>
-      <c r="J105" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales return order with Lookup value</v>
+        <v>31</v>
+      </c>
+      <c r="J105" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="K105" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales return order with Lookup value</v>
+        <v>//[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="L105" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales return order with Lookup value' } }</v>
+        <v>Given 'Released sales order with lookup value and with line with require shipment location' } }</v>
       </c>
       <c r="M105"/>
     </row>
@@ -4615,31 +4588,28 @@
         <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>77</v>
-      </c>
-      <c r="C106" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="G106" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="I106" s="14">
-        <v>20</v>
-      </c>
-      <c r="J106" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales return order is archived</v>
+        <v>31</v>
+      </c>
+      <c r="J106" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse shipment without lines</v>
       </c>
       <c r="K106" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales return order is archived</v>
+        <v>//[GIVEN] Warehouse shipment without lines</v>
       </c>
       <c r="L106" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales return order is archived' } }</v>
+        <v>Given 'Warehouse shipment without lines' } }</v>
       </c>
       <c r="M106"/>
     </row>
@@ -4648,141 +4618,126 @@
         <v>65</v>
       </c>
       <c r="B107" t="s">
+        <v>157</v>
+      </c>
+      <c r="G107" t="s">
+        <v>16</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I107" s="14">
+        <v>31</v>
+      </c>
+      <c r="J107" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="K107" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Get sales order with lookup value on warehouse shipment</v>
+      </c>
+      <c r="L107" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Get sales order with lookup value on warehouse shipment' } }</v>
+      </c>
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" t="s">
+        <v>157</v>
+      </c>
+      <c r="G108" t="s">
+        <v>18</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I108" s="14">
+        <v>31</v>
+      </c>
+      <c r="J108" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="K108" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
+      </c>
+      <c r="L108" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated' } }</v>
+      </c>
+      <c r="M108"/>
+    </row>
+    <row r="109" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C107" t="s">
-        <v>49</v>
-      </c>
-      <c r="G107" t="s">
+      <c r="C109" s="5"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I109" s="9"/>
+      <c r="J109" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue Sales Archive</v>
+      </c>
+      <c r="K109" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue Sales Archive</v>
+      </c>
+      <c r="L109" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue Sales Archive' {</v>
+      </c>
+      <c r="M109" s="8"/>
+    </row>
+    <row r="110" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D110" s="21"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G110" s="20"/>
+      <c r="H110" s="23"/>
+      <c r="I110" s="24">
         <v>18</v>
       </c>
-      <c r="H107" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="I107" s="14">
-        <v>20</v>
-      </c>
-      <c r="J107" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Archived sales return order has lookup value from sales return order</v>
-      </c>
-      <c r="K107" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Archived sales return order has lookup value from sales return order</v>
-      </c>
-      <c r="L107" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales return order has lookup value from sales return order'</v>
-      </c>
-      <c r="M107"/>
-    </row>
-    <row r="108" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C108" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D108" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E108" s="21"/>
-      <c r="F108" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G108" s="20"/>
-      <c r="H108" s="23"/>
-      <c r="I108" s="24">
-        <v>21</v>
-      </c>
-      <c r="J108" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0021] Check that lookup value is shown right on Sales List Archive</v>
-      </c>
-      <c r="K108" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0021] Check that lookup value is shown right on Sales List Archive</v>
-      </c>
-      <c r="L108" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0021 'Check that lookup value is shown right on Sales List Archive' {</v>
-      </c>
-      <c r="M108" s="23"/>
-    </row>
-    <row r="109" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>65</v>
-      </c>
-      <c r="B109" t="s">
-        <v>77</v>
-      </c>
-      <c r="C109" t="s">
-        <v>87</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G109" t="s">
-        <v>15</v>
-      </c>
-      <c r="H109" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="I109" s="14">
-        <v>21</v>
-      </c>
-      <c r="J109" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales document with Lookup value</v>
-      </c>
-      <c r="K109" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales document with Lookup value</v>
-      </c>
-      <c r="L109" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales document with Lookup value' } }</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>65</v>
-      </c>
-      <c r="B110" t="s">
-        <v>77</v>
-      </c>
-      <c r="C110" t="s">
-        <v>87</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G110" t="s">
-        <v>16</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="I110" s="14">
-        <v>21</v>
-      </c>
-      <c r="J110" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales document is archived</v>
-      </c>
-      <c r="K110" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales document is archived</v>
-      </c>
-      <c r="L110" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales document is archived' } }</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="J110" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0018] Archive sales order with lookup value</v>
+      </c>
+      <c r="K110" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0018] Archive sales order with lookup value</v>
+      </c>
+      <c r="L110" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0018 'Archive sales order with lookup value' {</v>
+      </c>
+      <c r="M110" s="23"/>
+    </row>
+    <row r="111" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>65</v>
       </c>
@@ -4790,34 +4745,31 @@
         <v>77</v>
       </c>
       <c r="C111" t="s">
-        <v>87</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G111" t="s">
+        <v>15</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I111" s="14">
         <v>18</v>
       </c>
-      <c r="H111" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I111" s="14">
-        <v>21</v>
-      </c>
       <c r="J111" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Archived sales document has lookup value from sales document</v>
+        <v>[GIVEN] Sales order with Lookup value</v>
       </c>
       <c r="K111" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Archived sales document has lookup value from sales document</v>
+        <v>//[GIVEN] Sales order with Lookup value</v>
       </c>
       <c r="L111" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales document has lookup value from sales document' } }</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>Given 'Sales order with Lookup value' } }</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>65</v>
       </c>
@@ -4825,92 +4777,94 @@
         <v>77</v>
       </c>
       <c r="C112" t="s">
-        <v>87</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G112" t="s">
+        <v>16</v>
+      </c>
+      <c r="H112" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I112" s="14">
         <v>18</v>
       </c>
-      <c r="H112" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="I112" s="14">
-        <v>21</v>
-      </c>
       <c r="J112" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] lookup value is shown right on Sales List Archive</v>
+        <v>[WHEN] Sales order is archived</v>
       </c>
       <c r="K112" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] lookup value is shown right on Sales List Archive</v>
+        <v>//[WHEN] Sales order is archived</v>
       </c>
       <c r="L112" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'lookup value is shown right on Sales List Archive' } }</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" ht="15" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="7"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="I113" s="9"/>
-      <c r="J113" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue Inheritance</v>
-      </c>
-      <c r="K113" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue Inheritance</v>
-      </c>
-      <c r="L113" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue Inheritance' {</v>
-      </c>
-      <c r="M113" s="8"/>
-    </row>
-    <row r="114" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>When 'Sales order is archived' } }</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>65</v>
+      </c>
+      <c r="B113" t="s">
+        <v>77</v>
+      </c>
+      <c r="C113" t="s">
+        <v>37</v>
+      </c>
+      <c r="G113" t="s">
+        <v>18</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I113" s="14">
+        <v>18</v>
+      </c>
+      <c r="J113" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Archived sales order has lookup value from sales order</v>
+      </c>
+      <c r="K113" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Archived sales order has lookup value from sales order</v>
+      </c>
+      <c r="L113" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales order has lookup value from sales order'</v>
+      </c>
+      <c r="M113"/>
+    </row>
+    <row r="114" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B114" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C114" s="20"/>
-      <c r="D114" s="20"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20" t="s">
-        <v>94</v>
+        <v>77</v>
+      </c>
+      <c r="C114" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="G114" s="20"/>
-      <c r="H114" s="20"/>
+      <c r="H114" s="23"/>
       <c r="I114" s="24">
-        <v>24</v>
-      </c>
-      <c r="J114" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0024] Assign customer lookup value to sales document</v>
+        <v>19</v>
+      </c>
+      <c r="J114" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0019] Archive sales quote with lookup value</v>
       </c>
       <c r="K114" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0024] Assign customer lookup value to sales document</v>
+        <v>//[SCENARIO #0019] Archive sales quote with lookup value</v>
       </c>
       <c r="L114" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0024 'Assign customer lookup value to sales document' {</v>
+        <v>Scenario 0019 'Archive sales quote with lookup value' {</v>
       </c>
       <c r="M114" s="20"/>
     </row>
@@ -4919,436 +4873,468 @@
         <v>65</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
-      </c>
-      <c r="D115"/>
-      <c r="E115"/>
-      <c r="F115"/>
+        <v>77</v>
+      </c>
+      <c r="C115" t="s">
+        <v>33</v>
+      </c>
       <c r="G115" t="s">
         <v>15</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="I115" s="28">
-        <v>24</v>
-      </c>
-      <c r="J115" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with Lookup value</v>
+        <v>138</v>
+      </c>
+      <c r="I115" s="14">
+        <v>19</v>
+      </c>
+      <c r="J115" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales quote with Lookup value</v>
       </c>
       <c r="K115" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with Lookup value</v>
+        <v>//[GIVEN] Sales quote with Lookup value</v>
       </c>
       <c r="L115" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with Lookup value' } }</v>
+        <v>Given 'Sales quote with Lookup value' } }</v>
       </c>
       <c r="M115"/>
     </row>
-    <row r="116" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>65</v>
       </c>
       <c r="B116" t="s">
-        <v>93</v>
-      </c>
-      <c r="D116"/>
-      <c r="E116"/>
-      <c r="F116"/>
+        <v>77</v>
+      </c>
+      <c r="C116" t="s">
+        <v>33</v>
+      </c>
       <c r="G116" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="I116" s="28">
-        <v>24</v>
-      </c>
-      <c r="J116" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales document (invoice) without Lookup value</v>
+        <v>82</v>
+      </c>
+      <c r="I116" s="14">
+        <v>19</v>
+      </c>
+      <c r="J116" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Sales quote is archived</v>
       </c>
       <c r="K116" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales document (invoice) without Lookup value</v>
+        <v>//[WHEN] Sales quote is archived</v>
       </c>
       <c r="L116" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales document (invoice) without Lookup value' } }</v>
+        <v>When 'Sales quote is archived' } }</v>
       </c>
       <c r="M116"/>
     </row>
-    <row r="117" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>65</v>
       </c>
       <c r="B117" t="s">
-        <v>93</v>
-      </c>
-      <c r="D117"/>
-      <c r="E117"/>
-      <c r="F117"/>
+        <v>77</v>
+      </c>
+      <c r="C117" t="s">
+        <v>33</v>
+      </c>
       <c r="G117" t="s">
+        <v>18</v>
+      </c>
+      <c r="H117" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I117" s="14">
+        <v>19</v>
+      </c>
+      <c r="J117" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Archived sales quote has lookup value from sales quote</v>
+      </c>
+      <c r="K117" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Archived sales quote has lookup value from sales quote</v>
+      </c>
+      <c r="L117" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales quote has lookup value from sales quote'</v>
+      </c>
+      <c r="M117"/>
+    </row>
+    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C118" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D118" s="21"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G118" s="20"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="24">
+        <v>20</v>
+      </c>
+      <c r="J118" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0020] Archive sales return order with lookup value</v>
+      </c>
+      <c r="K118" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0020] Archive sales return order with lookup value</v>
+      </c>
+      <c r="L118" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0020 'Archive sales return order with lookup value' {</v>
+      </c>
+      <c r="M118" s="20"/>
+    </row>
+    <row r="119" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>65</v>
+      </c>
+      <c r="B119" t="s">
+        <v>77</v>
+      </c>
+      <c r="C119" t="s">
+        <v>49</v>
+      </c>
+      <c r="G119" t="s">
+        <v>15</v>
+      </c>
+      <c r="H119" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I119" s="14">
+        <v>20</v>
+      </c>
+      <c r="J119" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales return order with Lookup value</v>
+      </c>
+      <c r="K119" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales return order with Lookup value</v>
+      </c>
+      <c r="L119" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales return order with Lookup value' } }</v>
+      </c>
+      <c r="M119"/>
+    </row>
+    <row r="120" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>65</v>
+      </c>
+      <c r="B120" t="s">
+        <v>77</v>
+      </c>
+      <c r="C120" t="s">
+        <v>49</v>
+      </c>
+      <c r="G120" t="s">
         <v>16</v>
       </c>
-      <c r="H117" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I117" s="28">
-        <v>24</v>
-      </c>
-      <c r="J117" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Set customer on sales header</v>
-      </c>
-      <c r="K117" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Set customer on sales header</v>
-      </c>
-      <c r="L117" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set customer on sales header' } }</v>
-      </c>
-      <c r="M117"/>
-    </row>
-    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>65</v>
-      </c>
-      <c r="B118" t="s">
-        <v>93</v>
-      </c>
-      <c r="D118"/>
-      <c r="E118"/>
-      <c r="F118"/>
-      <c r="G118" t="s">
+      <c r="H120" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I120" s="14">
+        <v>20</v>
+      </c>
+      <c r="J120" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Sales return order is archived</v>
+      </c>
+      <c r="K120" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Sales return order is archived</v>
+      </c>
+      <c r="L120" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales return order is archived' } }</v>
+      </c>
+      <c r="M120"/>
+    </row>
+    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>65</v>
+      </c>
+      <c r="B121" t="s">
+        <v>77</v>
+      </c>
+      <c r="C121" t="s">
+        <v>49</v>
+      </c>
+      <c r="G121" t="s">
         <v>18</v>
       </c>
-      <c r="H118" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="I118" s="28">
-        <v>24</v>
-      </c>
-      <c r="J118" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on sales document is populated with lookup value of customer</v>
-      </c>
-      <c r="K118" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on sales document is populated with lookup value of customer</v>
-      </c>
-      <c r="L118" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on sales document is populated with lookup value of customer'</v>
-      </c>
-      <c r="M118"/>
-    </row>
-    <row r="119" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B119" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C119" s="20"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="G119" s="20"/>
-      <c r="H119" s="23"/>
-      <c r="I119" s="24">
-        <v>26</v>
-      </c>
-      <c r="J119" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
-      </c>
-      <c r="K119" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
-      </c>
-      <c r="L119" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0026 'Check that lookup value is inherited from customer template to customer when creating customer from contact' {</v>
-      </c>
-      <c r="M119" s="20"/>
-    </row>
-    <row r="120" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>65</v>
-      </c>
-      <c r="B120" t="s">
-        <v>124</v>
-      </c>
-      <c r="G120" t="s">
-        <v>15</v>
-      </c>
-      <c r="H120" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="I120" s="14">
-        <v>26</v>
-      </c>
-      <c r="J120" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="K120" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="L120" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value' } }</v>
-      </c>
-      <c r="M120"/>
-    </row>
-    <row r="121" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>65</v>
-      </c>
-      <c r="B121" t="s">
-        <v>124</v>
-      </c>
-      <c r="G121" t="s">
-        <v>15</v>
-      </c>
       <c r="H121" s="13" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="I121" s="14">
-        <v>26</v>
-      </c>
-      <c r="J121" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Contact</v>
+        <v>20</v>
+      </c>
+      <c r="J121" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Archived sales return order has lookup value from sales return order</v>
       </c>
       <c r="K121" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Contact</v>
+        <v>//[THEN] Archived sales return order has lookup value from sales return order</v>
       </c>
       <c r="L121" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Contact' } }</v>
+        <v>Then 'Archived sales return order has lookup value from sales return order'</v>
       </c>
       <c r="M121"/>
     </row>
-    <row r="122" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>65</v>
-      </c>
-      <c r="B122" t="s">
-        <v>124</v>
-      </c>
-      <c r="G122" t="s">
+    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C122" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D122" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E122" s="21"/>
+      <c r="F122" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G122" s="20"/>
+      <c r="H122" s="23"/>
+      <c r="I122" s="24">
+        <v>21</v>
+      </c>
+      <c r="J122" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0021] Check that lookup value is shown right on Sales List Archive</v>
+      </c>
+      <c r="K122" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0021] Check that lookup value is shown right on Sales List Archive</v>
+      </c>
+      <c r="L122" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0021 'Check that lookup value is shown right on Sales List Archive' {</v>
+      </c>
+      <c r="M122" s="23"/>
+    </row>
+    <row r="123" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>65</v>
+      </c>
+      <c r="B123" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" t="s">
+        <v>87</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G123" t="s">
+        <v>15</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I123" s="14">
+        <v>21</v>
+      </c>
+      <c r="J123" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales document with Lookup value</v>
+      </c>
+      <c r="K123" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales document with Lookup value</v>
+      </c>
+      <c r="L123" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales document with Lookup value' } }</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>65</v>
+      </c>
+      <c r="B124" t="s">
+        <v>77</v>
+      </c>
+      <c r="C124" t="s">
+        <v>87</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G124" t="s">
         <v>16</v>
       </c>
-      <c r="H122" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="I122" s="14">
-        <v>26</v>
-      </c>
-      <c r="J122" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Customer is created from contact</v>
-      </c>
-      <c r="K122" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Customer is created from contact</v>
-      </c>
-      <c r="L122" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Customer is created from contact' } }</v>
-      </c>
-      <c r="M122"/>
-    </row>
-    <row r="123" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>65</v>
-      </c>
-      <c r="B123" t="s">
-        <v>124</v>
-      </c>
-      <c r="G123" t="s">
-        <v>18</v>
-      </c>
-      <c r="H123" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I123" s="14">
-        <v>26</v>
-      </c>
-      <c r="J123" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
-      </c>
-      <c r="K123" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
-      </c>
-      <c r="L123" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer has lookup value code field populated with lookup value from customer template'</v>
-      </c>
-      <c r="M123"/>
-    </row>
-    <row r="124" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B124" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C124" s="20"/>
-      <c r="D124" s="21"/>
-      <c r="E124" s="21"/>
-      <c r="F124" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="G124" s="20"/>
-      <c r="H124" s="23"/>
-      <c r="I124" s="24">
-        <v>28</v>
-      </c>
-      <c r="J124" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0028] Create customer from configuration template with lookup value</v>
-      </c>
-      <c r="K124" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0028] Create customer from configuration template with lookup value</v>
-      </c>
-      <c r="L124" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0028 'Create customer from configuration template with lookup value' {</v>
-      </c>
-      <c r="M124" s="20"/>
+      <c r="H124" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I124" s="14">
+        <v>21</v>
+      </c>
+      <c r="J124" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Sales document is archived</v>
+      </c>
+      <c r="K124" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Sales document is archived</v>
+      </c>
+      <c r="L124" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales document is archived' } }</v>
+      </c>
     </row>
     <row r="125" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>65</v>
       </c>
       <c r="B125" t="s">
-        <v>97</v>
+        <v>77</v>
+      </c>
+      <c r="C125" t="s">
+        <v>87</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="G125" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="I125" s="14">
-        <v>28</v>
-      </c>
-      <c r="J125" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>21</v>
+      </c>
+      <c r="J125" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Archived sales document has lookup value from sales document</v>
       </c>
       <c r="K125" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>//[THEN] Archived sales document has lookup value from sales document</v>
       </c>
       <c r="L125" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Configuration template (customer) with lookup value' } }</v>
-      </c>
-      <c r="M125"/>
-    </row>
-    <row r="126" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Archived sales document has lookup value from sales document' } }</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>65</v>
       </c>
       <c r="B126" t="s">
-        <v>97</v>
+        <v>77</v>
+      </c>
+      <c r="C126" t="s">
+        <v>87</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="G126" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H126" s="13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I126" s="14">
-        <v>28</v>
-      </c>
-      <c r="J126" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create customer from configuration template</v>
+        <v>21</v>
+      </c>
+      <c r="J126" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] lookup value is shown right on Sales List Archive</v>
       </c>
       <c r="K126" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create customer from configuration template</v>
+        <v>//[THEN] lookup value is shown right on Sales List Archive</v>
       </c>
       <c r="L126" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create customer from configuration template' } }</v>
-      </c>
-      <c r="M126"/>
-    </row>
-    <row r="127" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>65</v>
-      </c>
-      <c r="B127" t="s">
-        <v>97</v>
-      </c>
-      <c r="G127" t="s">
-        <v>18</v>
-      </c>
-      <c r="H127" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I127" s="14">
-        <v>28</v>
-      </c>
-      <c r="J127" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
-      </c>
-      <c r="K127" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
-      </c>
-      <c r="L127" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of configuration template'</v>
-      </c>
-      <c r="M127"/>
-    </row>
-    <row r="128" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'lookup value is shown right on Sales List Archive' } }</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="15" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="7"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I127" s="9"/>
+      <c r="J127" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue Inheritance</v>
+      </c>
+      <c r="K127" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue Inheritance</v>
+      </c>
+      <c r="L127" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue Inheritance' {</v>
+      </c>
+      <c r="M127" s="8"/>
+    </row>
+    <row r="128" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="C128" s="20"/>
-      <c r="D128" s="21"/>
-      <c r="E128" s="21"/>
-      <c r="F128" s="22" t="s">
-        <v>74</v>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="G128" s="20"/>
-      <c r="H128" s="23"/>
+      <c r="H128" s="20"/>
       <c r="I128" s="24">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J128" s="20" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
+        <v>[SCENARIO #0024] Assign customer lookup value to sales document</v>
       </c>
       <c r="K128" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
+        <v>//[SCENARIO #0024] Assign customer lookup value to sales document</v>
       </c>
       <c r="L128" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0030 'Create warehouse shipment from sales order with lookup value' {</v>
+        <v>Scenario 0024 'Assign customer lookup value to sales document' {</v>
       </c>
       <c r="M128" s="20"/>
     </row>
@@ -5357,210 +5343,222 @@
         <v>65</v>
       </c>
       <c r="B129" t="s">
-        <v>123</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129"/>
       <c r="G129" t="s">
         <v>15</v>
       </c>
       <c r="H129" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I129" s="14">
-        <v>30</v>
+        <v>127</v>
+      </c>
+      <c r="I129" s="28">
+        <v>24</v>
       </c>
       <c r="J129" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup value</v>
+        <v>[GIVEN] Customer with Lookup value</v>
       </c>
       <c r="K129" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup value</v>
+        <v>//[GIVEN] Customer with Lookup value</v>
       </c>
       <c r="L129" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <v>Given 'Customer with Lookup value' } }</v>
       </c>
       <c r="M129"/>
     </row>
-    <row r="130" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>65</v>
       </c>
       <c r="B130" t="s">
-        <v>123</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130"/>
       <c r="G130" t="s">
         <v>15</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="I130" s="14">
-        <v>30</v>
+        <v>141</v>
+      </c>
+      <c r="I130" s="28">
+        <v>24</v>
       </c>
       <c r="J130" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Sales document (invoice) without Lookup value</v>
       </c>
       <c r="K130" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Sales document (invoice) without Lookup value</v>
       </c>
       <c r="L130" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <v>Given 'Sales document (invoice) without Lookup value' } }</v>
       </c>
       <c r="M130"/>
     </row>
-    <row r="131" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>65</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131"/>
       <c r="G131" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H131" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="I131" s="14">
-        <v>30</v>
+        <v>94</v>
+      </c>
+      <c r="I131" s="28">
+        <v>24</v>
       </c>
       <c r="J131" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user</v>
+        <v>[WHEN] Set customer on sales header</v>
       </c>
       <c r="K131" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user</v>
+        <v>//[WHEN] Set customer on sales header</v>
       </c>
       <c r="L131" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <v>When 'Set customer on sales header' } }</v>
       </c>
       <c r="M131"/>
     </row>
-    <row r="132" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>65</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D132"/>
+      <c r="E132"/>
+      <c r="F132"/>
       <c r="G132" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I132" s="14">
-        <v>30</v>
+        <v>95</v>
+      </c>
+      <c r="I132" s="28">
+        <v>24</v>
       </c>
       <c r="J132" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
+        <v>[THEN] Lookup value on sales document is populated with lookup value of customer</v>
       </c>
       <c r="K132" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
+        <v>//[THEN] Lookup value on sales document is populated with lookup value of customer</v>
       </c>
       <c r="L132" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location' } }</v>
+        <v>Then 'Lookup value on sales document is populated with lookup value of customer'</v>
       </c>
       <c r="M132"/>
     </row>
-    <row r="133" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>65</v>
-      </c>
-      <c r="B133" t="s">
-        <v>123</v>
-      </c>
-      <c r="G133" t="s">
-        <v>18</v>
-      </c>
-      <c r="H133" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I133" s="14">
-        <v>30</v>
-      </c>
-      <c r="J133" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
-      </c>
-      <c r="K133" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
-      </c>
-      <c r="L133" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
-      </c>
-      <c r="M133"/>
-    </row>
-    <row r="134" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B134" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C134" s="20"/>
-      <c r="D134" s="21"/>
-      <c r="E134" s="21"/>
-      <c r="F134" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G134" s="20"/>
-      <c r="H134" s="23"/>
-      <c r="I134" s="24">
-        <v>31</v>
-      </c>
-      <c r="J134" s="20" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
-      </c>
-      <c r="K134" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
-      </c>
-      <c r="L134" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0031 'Get sales order with lookup value on warehouse shipment' {</v>
-      </c>
-      <c r="M134" s="20"/>
+    <row r="133" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C133" s="20"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
+      <c r="F133" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G133" s="20"/>
+      <c r="H133" s="23"/>
+      <c r="I133" s="24">
+        <v>26</v>
+      </c>
+      <c r="J133" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
+      </c>
+      <c r="K133" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
+      </c>
+      <c r="L133" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0026 'Check that lookup value is inherited from customer template to customer when creating customer from contact' {</v>
+      </c>
+      <c r="M133" s="20"/>
+    </row>
+    <row r="134" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>65</v>
+      </c>
+      <c r="B134" t="s">
+        <v>155</v>
+      </c>
+      <c r="G134" t="s">
+        <v>15</v>
+      </c>
+      <c r="H134" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I134" s="14">
+        <v>26</v>
+      </c>
+      <c r="J134" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="K134" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="L134" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template with lookup value' } }</v>
+      </c>
+      <c r="M134"/>
     </row>
     <row r="135" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>65</v>
       </c>
       <c r="B135" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="G135" t="s">
         <v>15</v>
       </c>
       <c r="H135" s="13" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="I135" s="14">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J135" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup value</v>
+        <v>[GIVEN] Contact</v>
       </c>
       <c r="K135" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup value</v>
+        <v>//[GIVEN] Contact</v>
       </c>
       <c r="L135" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <v>Given 'Contact' } }</v>
       </c>
       <c r="M135"/>
     </row>
@@ -5569,118 +5567,120 @@
         <v>65</v>
       </c>
       <c r="B136" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="G136" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="I136" s="14">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J136" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[WHEN] Customer is created from contact</v>
       </c>
       <c r="K136" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[WHEN] Customer is created from contact</v>
       </c>
       <c r="L136" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <v>When 'Customer is created from contact' } }</v>
       </c>
       <c r="M136"/>
     </row>
-    <row r="137" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>65</v>
       </c>
       <c r="B137" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="G137" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="I137" s="14">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J137" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user</v>
+        <v>[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
       </c>
       <c r="K137" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user</v>
+        <v>//[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
       </c>
       <c r="L137" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <v>Then 'Customer has lookup value code field populated with lookup value from customer template'</v>
       </c>
       <c r="M137"/>
     </row>
-    <row r="138" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>65</v>
-      </c>
-      <c r="B138" t="s">
-        <v>123</v>
-      </c>
-      <c r="G138" t="s">
-        <v>15</v>
-      </c>
-      <c r="H138" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="I138" s="14">
-        <v>31</v>
-      </c>
-      <c r="J138" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="K138" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
-      </c>
-      <c r="L138" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Released sales order with lookup value and with line with require shipment location' } }</v>
-      </c>
-      <c r="M138"/>
-    </row>
-    <row r="139" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B138" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C138" s="20"/>
+      <c r="D138" s="21"/>
+      <c r="E138" s="21"/>
+      <c r="F138" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G138" s="20"/>
+      <c r="H138" s="23"/>
+      <c r="I138" s="24">
+        <v>28</v>
+      </c>
+      <c r="J138" s="20" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+      </c>
+      <c r="K138" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+      </c>
+      <c r="L138" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0028 'Create customer from configuration template with lookup value' {</v>
+      </c>
+      <c r="M138" s="20"/>
+    </row>
+    <row r="139" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>65</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I139" s="14">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J139" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment without lines</v>
+        <v>[GIVEN] Configuration template (customer) with lookup value</v>
       </c>
       <c r="K139" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment without lines</v>
+        <v>//[GIVEN] Configuration template (customer) with lookup value</v>
       </c>
       <c r="L139" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment without lines' } }</v>
+        <v>Given 'Configuration template (customer) with lookup value' } }</v>
       </c>
       <c r="M139"/>
     </row>
@@ -5689,58 +5689,58 @@
         <v>65</v>
       </c>
       <c r="B140" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="G140" t="s">
         <v>16</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="I140" s="14">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J140" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Get sales order with lookup value on warehouse shipment</v>
+        <v>[WHEN] Create customer from configuration template</v>
       </c>
       <c r="K140" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Get sales order with lookup value on warehouse shipment</v>
+        <v>//[WHEN] Create customer from configuration template</v>
       </c>
       <c r="L140" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Get sales order with lookup value on warehouse shipment' } }</v>
+        <v>When 'Create customer from configuration template' } }</v>
       </c>
       <c r="M140"/>
     </row>
-    <row r="141" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="39.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>65</v>
       </c>
       <c r="B141" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="G141" t="s">
         <v>18</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="I141" s="14">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J141" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
+        <v>[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
       </c>
       <c r="K141" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
+        <v>//[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
       </c>
       <c r="L141" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated' } }</v>
+        <v>Then 'Lookup value on customer is populated with lookup value of configuration template' } }</v>
       </c>
       <c r="M141"/>
     </row>
@@ -5749,7 +5749,7 @@
         <v>65</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="6"/>
@@ -5757,7 +5757,7 @@
       <c r="F142" s="7"/>
       <c r="G142" s="5"/>
       <c r="H142" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I142" s="9"/>
       <c r="J142" s="18" t="str">
@@ -5779,7 +5779,7 @@
         <v>65</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C143" s="20" t="s">
         <v>37</v>
@@ -5787,7 +5787,7 @@
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G143" s="20"/>
       <c r="H143" s="23"/>
@@ -5813,7 +5813,7 @@
         <v>65</v>
       </c>
       <c r="B144" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C144" t="s">
         <v>37</v>
@@ -5822,7 +5822,7 @@
         <v>15</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I144" s="14">
         <v>22</v>
@@ -5845,7 +5845,7 @@
         <v>65</v>
       </c>
       <c r="B145" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C145" t="s">
         <v>37</v>
@@ -5854,7 +5854,7 @@
         <v>16</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I145" s="14">
         <v>22</v>
@@ -5877,7 +5877,7 @@
         <v>65</v>
       </c>
       <c r="B146" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C146" t="s">
         <v>37</v>
@@ -5886,7 +5886,7 @@
         <v>18</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I146" s="14">
         <v>22</v>
@@ -5909,7 +5909,7 @@
         <v>65</v>
       </c>
       <c r="B147" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C147" t="s">
         <v>37</v>
@@ -5918,7 +5918,7 @@
         <v>18</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I147" s="14">
         <v>22</v>
@@ -5941,7 +5941,7 @@
         <v>65</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C148" s="20" t="s">
         <v>37</v>
@@ -5951,7 +5951,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G148" s="20"/>
       <c r="H148" s="23"/>
@@ -5977,7 +5977,7 @@
         <v>65</v>
       </c>
       <c r="B149" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C149" t="s">
         <v>37</v>
@@ -5989,7 +5989,7 @@
         <v>15</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I149" s="14">
         <v>27</v>
@@ -6012,7 +6012,7 @@
         <v>65</v>
       </c>
       <c r="B150" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C150" t="s">
         <v>37</v>
@@ -6024,7 +6024,7 @@
         <v>16</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I150" s="14">
         <v>27</v>
@@ -6047,7 +6047,7 @@
         <v>65</v>
       </c>
       <c r="B151" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C151" t="s">
         <v>37</v>
@@ -6059,7 +6059,7 @@
         <v>18</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I151" s="14">
         <v>27</v>
@@ -6082,7 +6082,7 @@
         <v>65</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C152" s="20" t="s">
         <v>66</v>
@@ -6090,7 +6090,7 @@
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G152" s="20"/>
       <c r="H152" s="23"/>
@@ -6113,10 +6113,10 @@
     </row>
     <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B153" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C153" t="s">
         <v>66</v>
@@ -6125,7 +6125,7 @@
         <v>15</v>
       </c>
       <c r="H153" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I153" s="14">
         <v>23</v>
@@ -6145,10 +6145,10 @@
     </row>
     <row r="154" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B154" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C154" t="s">
         <v>66</v>
@@ -6157,7 +6157,7 @@
         <v>15</v>
       </c>
       <c r="H154" s="27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I154" s="14">
         <v>23</v>
@@ -6177,10 +6177,10 @@
     </row>
     <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B155" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C155" t="s">
         <v>66</v>
@@ -6189,7 +6189,7 @@
         <v>15</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I155" s="14">
         <v>23</v>
@@ -6212,7 +6212,7 @@
         <v>65</v>
       </c>
       <c r="B156" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C156" t="s">
         <v>66</v>
@@ -6221,7 +6221,7 @@
         <v>16</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I156" s="14">
         <v>23</v>
@@ -6244,7 +6244,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C157" t="s">
         <v>66</v>
@@ -6253,7 +6253,7 @@
         <v>18</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I157" s="14">
         <v>23</v>
@@ -6276,7 +6276,7 @@
         <v>65</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C158" s="20" t="s">
         <v>66</v>
@@ -6286,7 +6286,7 @@
         <v>23</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G158" s="20"/>
       <c r="H158" s="23"/>
@@ -6309,10 +6309,10 @@
     </row>
     <row r="159" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B159" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C159" t="s">
         <v>66</v>
@@ -6324,7 +6324,7 @@
         <v>15</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I159" s="14">
         <v>25</v>
@@ -6344,10 +6344,10 @@
     </row>
     <row r="160" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B160" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C160" t="s">
         <v>66</v>
@@ -6359,7 +6359,7 @@
         <v>15</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I160" s="14">
         <v>25</v>
@@ -6379,10 +6379,10 @@
     </row>
     <row r="161" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B161" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C161" t="s">
         <v>66</v>
@@ -6394,7 +6394,7 @@
         <v>15</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I161" s="14">
         <v>25</v>
@@ -6417,7 +6417,7 @@
         <v>65</v>
       </c>
       <c r="B162" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C162" t="s">
         <v>66</v>
@@ -6429,7 +6429,7 @@
         <v>16</v>
       </c>
       <c r="H162" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I162" s="14">
         <v>25</v>
@@ -6452,7 +6452,7 @@
         <v>65</v>
       </c>
       <c r="B163" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C163" t="s">
         <v>66</v>
@@ -6464,7 +6464,7 @@
         <v>18</v>
       </c>
       <c r="H163" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I163" s="14">
         <v>25</v>
@@ -6487,7 +6487,7 @@
         <v>65</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
@@ -6495,7 +6495,7 @@
       <c r="F164" s="7"/>
       <c r="G164" s="5"/>
       <c r="H164" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I164" s="9"/>
       <c r="J164" s="18" t="str">
@@ -6517,13 +6517,13 @@
         <v>65</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C165" s="20"/>
       <c r="D165" s="21"/>
       <c r="E165" s="21"/>
       <c r="F165" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G165" s="20"/>
       <c r="H165" s="23"/>
@@ -6549,13 +6549,13 @@
         <v>65</v>
       </c>
       <c r="B166" t="s">
+        <v>113</v>
+      </c>
+      <c r="G166" t="s">
+        <v>15</v>
+      </c>
+      <c r="H166" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="G166" t="s">
-        <v>15</v>
-      </c>
-      <c r="H166" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="I166" s="14">
         <v>29</v>
@@ -6578,13 +6578,13 @@
         <v>65</v>
       </c>
       <c r="B167" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G167" t="s">
         <v>16</v>
       </c>
       <c r="H167" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I167" s="14">
         <v>29</v>
@@ -6607,13 +6607,13 @@
         <v>65</v>
       </c>
       <c r="B168" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G168" t="s">
         <v>18</v>
       </c>
       <c r="H168" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I168" s="14">
         <v>29</v>
@@ -6646,28 +6646,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added scenarios #0041 through #0048 (test example 8)
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F309E-88C3-467D-B8C0-0365A8E508BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96655830-F68C-48C3-84F3-F22D75A44B4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="183">
   <si>
     <t>Feature</t>
   </si>
@@ -508,6 +508,104 @@
   </si>
   <si>
     <t>Inheritance - Warehouse Shipment</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Create lookup value without permissions</t>
+  </si>
+  <si>
+    <t>Create lookup value with permissions</t>
+  </si>
+  <si>
+    <t>Open Lookup Values Page without permissions</t>
+  </si>
+  <si>
+    <t>Open Lookup Values Page with permissions</t>
+  </si>
+  <si>
+    <t>Check lookup value on customer card without permissions</t>
+  </si>
+  <si>
+    <t>Check lookup value on customer card with permissions</t>
+  </si>
+  <si>
+    <t>Starting restricted base permissions</t>
+  </si>
+  <si>
+    <t>Starting restricted base permissions extended with Lookup Value permissions</t>
+  </si>
+  <si>
+    <t>Starting unrestricted permissions</t>
+  </si>
+  <si>
+    <t>Create lookup value</t>
+  </si>
+  <si>
+    <t>Insert permissions error thrown</t>
+  </si>
+  <si>
+    <t>Lookup value exists</t>
+  </si>
+  <si>
+    <t>Restricted base permissions</t>
+  </si>
+  <si>
+    <t>Open Lookup Values page</t>
+  </si>
+  <si>
+    <t>Read permissions error thrown</t>
+  </si>
+  <si>
+    <t>No error thrown</t>
+  </si>
+  <si>
+    <t>Open customer card</t>
+  </si>
+  <si>
+    <t>Lookup value field not shown</t>
+  </si>
+  <si>
+    <t>Lookup value field shown</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lookup value field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> shown</t>
+    </r>
+  </si>
+  <si>
+    <t>Check lookup value on customer list without permissions</t>
+  </si>
+  <si>
+    <t>Open customer list</t>
+  </si>
+  <si>
+    <t>Check lookup value on customer list with permissions</t>
+  </si>
+  <si>
+    <t>Clear last error</t>
   </si>
 </sst>
 </file>
@@ -517,7 +615,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +640,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -834,8 +940,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M168" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:M168" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M204" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:M204" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
@@ -1158,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M169"/>
+  <dimension ref="A1:M205"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1282,7 @@
     <col min="8" max="8" width="75.5703125" style="13" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="14" customWidth="1"/>
     <col min="10" max="11" width="48.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="48.42578125" style="29" customWidth="1"/>
+    <col min="12" max="12" width="77.42578125" style="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3016,7 +3122,7 @@
         <v>Given 'Lookup value' } }</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -5136,7 +5242,7 @@
       </c>
       <c r="M122" s="23"/>
     </row>
-    <row r="123" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>65</v>
       </c>
@@ -6342,7 +6448,7 @@
         <v>Given 'Location with require shipment' }</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>107</v>
       </c>
@@ -6602,7 +6708,7 @@
         <v>When 'Run report CustomerList' } }</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>65</v>
       </c>
@@ -6631,7 +6737,1233 @@
         <v>Then 'Report dataset contains both customers with lookup value' } }</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C169" s="5"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="7"/>
+      <c r="G169" s="5"/>
+      <c r="H169" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I169" s="9"/>
+      <c r="J169" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue Permissions</v>
+      </c>
+      <c r="K169" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue Permissions</v>
+      </c>
+      <c r="L169" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue Permissions' {</v>
+      </c>
+      <c r="M169" s="8"/>
+    </row>
+    <row r="170" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B170" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C170" s="20"/>
+      <c r="D170" s="21"/>
+      <c r="E170" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F170" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="G170" s="20"/>
+      <c r="H170" s="23"/>
+      <c r="I170" s="24">
+        <v>41</v>
+      </c>
+      <c r="J170" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0041] Create lookup value without permissions</v>
+      </c>
+      <c r="K170" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0041] Create lookup value without permissions</v>
+      </c>
+      <c r="L170" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0041 'Create lookup value without permissions' {</v>
+      </c>
+      <c r="M170" s="23"/>
+    </row>
+    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>65</v>
+      </c>
+      <c r="B171" t="s">
+        <v>158</v>
+      </c>
+      <c r="E171" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G171" t="s">
+        <v>15</v>
+      </c>
+      <c r="H171" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I171" s="14">
+        <v>41</v>
+      </c>
+      <c r="J171" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K171" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L171" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>65</v>
+      </c>
+      <c r="B172" t="s">
+        <v>158</v>
+      </c>
+      <c r="E172" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G172" t="s">
+        <v>16</v>
+      </c>
+      <c r="H172" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I172" s="14">
+        <v>41</v>
+      </c>
+      <c r="J172" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Create lookup value</v>
+      </c>
+      <c r="K172" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Create lookup value</v>
+      </c>
+      <c r="L172" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create lookup value' }</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>65</v>
+      </c>
+      <c r="B173" t="s">
+        <v>158</v>
+      </c>
+      <c r="E173" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G173" t="s">
+        <v>18</v>
+      </c>
+      <c r="H173" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="I173" s="14">
+        <v>41</v>
+      </c>
+      <c r="J173" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Insert permissions error thrown</v>
+      </c>
+      <c r="K173" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Insert permissions error thrown</v>
+      </c>
+      <c r="L173" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Insert permissions error thrown'</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B174" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C174" s="20"/>
+      <c r="D174" s="21"/>
+      <c r="E174" s="21"/>
+      <c r="F174" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G174" s="20"/>
+      <c r="H174" s="23"/>
+      <c r="I174" s="24">
+        <v>42</v>
+      </c>
+      <c r="J174" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0042] Create lookup value with permissions</v>
+      </c>
+      <c r="K174" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0042] Create lookup value with permissions</v>
+      </c>
+      <c r="L174" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0042 'Create lookup value with permissions' {</v>
+      </c>
+      <c r="M174" s="23"/>
+    </row>
+    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>65</v>
+      </c>
+      <c r="B175" t="s">
+        <v>158</v>
+      </c>
+      <c r="G175" t="s">
+        <v>15</v>
+      </c>
+      <c r="H175" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I175" s="14">
+        <v>42</v>
+      </c>
+      <c r="J175" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="K175" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="L175" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>65</v>
+      </c>
+      <c r="B176" t="s">
+        <v>158</v>
+      </c>
+      <c r="G176" t="s">
+        <v>16</v>
+      </c>
+      <c r="H176" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I176" s="14">
+        <v>42</v>
+      </c>
+      <c r="J176" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Create lookup value</v>
+      </c>
+      <c r="K176" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Create lookup value</v>
+      </c>
+      <c r="L176" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create lookup value' } }</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>65</v>
+      </c>
+      <c r="B177" t="s">
+        <v>158</v>
+      </c>
+      <c r="G177" t="s">
+        <v>18</v>
+      </c>
+      <c r="H177" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I177" s="14">
+        <v>42</v>
+      </c>
+      <c r="J177" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value exists</v>
+      </c>
+      <c r="K177" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value exists</v>
+      </c>
+      <c r="L177" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists'</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B178" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C178" s="20"/>
+      <c r="D178" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E178" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F178" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="G178" s="20"/>
+      <c r="H178" s="23"/>
+      <c r="I178" s="24">
+        <v>43</v>
+      </c>
+      <c r="J178" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0043] Open Lookup Values Page without permissions</v>
+      </c>
+      <c r="K178" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0043] Open Lookup Values Page without permissions</v>
+      </c>
+      <c r="L178" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0043 'Open Lookup Values Page without permissions' {</v>
+      </c>
+      <c r="M178" s="23"/>
+    </row>
+    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" t="s">
+        <v>158</v>
+      </c>
+      <c r="D179" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E179" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G179" t="s">
+        <v>15</v>
+      </c>
+      <c r="H179" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I179" s="14">
+        <v>43</v>
+      </c>
+      <c r="J179" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="K179" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="L179" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>65</v>
+      </c>
+      <c r="B180" t="s">
+        <v>158</v>
+      </c>
+      <c r="G180" t="s">
+        <v>15</v>
+      </c>
+      <c r="H180" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I180" s="14">
+        <v>43</v>
+      </c>
+      <c r="J180" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value</v>
+      </c>
+      <c r="K180" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup value</v>
+      </c>
+      <c r="L180" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value' } }</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>65</v>
+      </c>
+      <c r="B181" t="s">
+        <v>158</v>
+      </c>
+      <c r="G181" t="s">
+        <v>15</v>
+      </c>
+      <c r="H181" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I181" s="14">
+        <v>43</v>
+      </c>
+      <c r="J181" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="K181" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="L181" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>65</v>
+      </c>
+      <c r="B182" t="s">
+        <v>158</v>
+      </c>
+      <c r="D182" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E182" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G182" t="s">
+        <v>16</v>
+      </c>
+      <c r="H182" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I182" s="14">
+        <v>43</v>
+      </c>
+      <c r="J182" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="K182" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="L182" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page' }</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>65</v>
+      </c>
+      <c r="B183" t="s">
+        <v>158</v>
+      </c>
+      <c r="D183" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E183" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G183" t="s">
+        <v>18</v>
+      </c>
+      <c r="H183" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I183" s="14">
+        <v>43</v>
+      </c>
+      <c r="J183" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="K183" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="L183" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Read permissions error thrown'</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B184" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C184" s="20"/>
+      <c r="D184" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E184" s="21"/>
+      <c r="F184" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G184" s="20"/>
+      <c r="H184" s="23"/>
+      <c r="I184" s="24">
+        <v>44</v>
+      </c>
+      <c r="J184" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0044] Open Lookup Values Page with permissions</v>
+      </c>
+      <c r="K184" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0044] Open Lookup Values Page with permissions</v>
+      </c>
+      <c r="L184" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0044 'Open Lookup Values Page with permissions' {</v>
+      </c>
+      <c r="M184" s="23"/>
+    </row>
+    <row r="185" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>65</v>
+      </c>
+      <c r="B185" t="s">
+        <v>158</v>
+      </c>
+      <c r="D185" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G185" t="s">
+        <v>15</v>
+      </c>
+      <c r="H185" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I185" s="14">
+        <v>44</v>
+      </c>
+      <c r="J185" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="K185" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="L185" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>65</v>
+      </c>
+      <c r="B186" t="s">
+        <v>158</v>
+      </c>
+      <c r="D186" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G186" t="s">
+        <v>15</v>
+      </c>
+      <c r="H186" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="I186" s="14">
+        <v>44</v>
+      </c>
+      <c r="J186" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Clear last error</v>
+      </c>
+      <c r="K186" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Clear last error</v>
+      </c>
+      <c r="L186" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Clear last error' } }</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>65</v>
+      </c>
+      <c r="B187" t="s">
+        <v>158</v>
+      </c>
+      <c r="D187" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G187" t="s">
+        <v>16</v>
+      </c>
+      <c r="H187" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I187" s="14">
+        <v>44</v>
+      </c>
+      <c r="J187" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="K187" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="L187" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page' } }</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>65</v>
+      </c>
+      <c r="B188" t="s">
+        <v>158</v>
+      </c>
+      <c r="D188" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G188" t="s">
+        <v>18</v>
+      </c>
+      <c r="H188" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="I188" s="14">
+        <v>44</v>
+      </c>
+      <c r="J188" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] No error thrown</v>
+      </c>
+      <c r="K188" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] No error thrown</v>
+      </c>
+      <c r="L188" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No error thrown'</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B189" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C189" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E189" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F189" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="G189" s="20"/>
+      <c r="H189" s="23"/>
+      <c r="I189" s="24">
+        <v>45</v>
+      </c>
+      <c r="J189" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0045] Check lookup value on customer card without permissions</v>
+      </c>
+      <c r="K189" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0045] Check lookup value on customer card without permissions</v>
+      </c>
+      <c r="L189" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0045 'Check lookup value on customer card without permissions' {</v>
+      </c>
+      <c r="M189" s="23"/>
+    </row>
+    <row r="190" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>65</v>
+      </c>
+      <c r="B190" t="s">
+        <v>158</v>
+      </c>
+      <c r="C190" t="s">
+        <v>12</v>
+      </c>
+      <c r="D190" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E190" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G190" t="s">
+        <v>15</v>
+      </c>
+      <c r="H190" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I190" s="14">
+        <v>45</v>
+      </c>
+      <c r="J190" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K190" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L190" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>65</v>
+      </c>
+      <c r="B191" t="s">
+        <v>158</v>
+      </c>
+      <c r="C191" t="s">
+        <v>12</v>
+      </c>
+      <c r="D191" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E191" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G191" t="s">
+        <v>16</v>
+      </c>
+      <c r="H191" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I191" s="14">
+        <v>45</v>
+      </c>
+      <c r="J191" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer card</v>
+      </c>
+      <c r="K191" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer card</v>
+      </c>
+      <c r="L191" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card' }</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>65</v>
+      </c>
+      <c r="B192" t="s">
+        <v>158</v>
+      </c>
+      <c r="C192" t="s">
+        <v>12</v>
+      </c>
+      <c r="D192" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E192" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G192" t="s">
+        <v>18</v>
+      </c>
+      <c r="H192" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I192" s="14">
+        <v>45</v>
+      </c>
+      <c r="J192" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="K192" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="L192" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown'</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B193" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C193" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D193" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E193" s="21"/>
+      <c r="F193" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="G193" s="20"/>
+      <c r="H193" s="23"/>
+      <c r="I193" s="24">
+        <v>46</v>
+      </c>
+      <c r="J193" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0046] Check lookup value on customer card with permissions</v>
+      </c>
+      <c r="K193" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0046] Check lookup value on customer card with permissions</v>
+      </c>
+      <c r="L193" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0046 'Check lookup value on customer card with permissions' {</v>
+      </c>
+      <c r="M193" s="23"/>
+    </row>
+    <row r="194" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>65</v>
+      </c>
+      <c r="B194" t="s">
+        <v>158</v>
+      </c>
+      <c r="C194" t="s">
+        <v>12</v>
+      </c>
+      <c r="D194" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G194" t="s">
+        <v>15</v>
+      </c>
+      <c r="H194" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I194" s="14">
+        <v>46</v>
+      </c>
+      <c r="J194" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K194" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L194" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' } }</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>65</v>
+      </c>
+      <c r="B195" t="s">
+        <v>158</v>
+      </c>
+      <c r="C195" t="s">
+        <v>12</v>
+      </c>
+      <c r="D195" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G195" t="s">
+        <v>16</v>
+      </c>
+      <c r="H195" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I195" s="14">
+        <v>46</v>
+      </c>
+      <c r="J195" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer card</v>
+      </c>
+      <c r="K195" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer card</v>
+      </c>
+      <c r="L195" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card' } }</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>65</v>
+      </c>
+      <c r="B196" t="s">
+        <v>158</v>
+      </c>
+      <c r="C196" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G196" t="s">
+        <v>18</v>
+      </c>
+      <c r="H196" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="I196" s="14">
+        <v>46</v>
+      </c>
+      <c r="J196" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field shown</v>
+      </c>
+      <c r="K196" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field shown</v>
+      </c>
+      <c r="L196" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field shown'</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B197" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D197" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E197" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F197" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="G197" s="20"/>
+      <c r="H197" s="23"/>
+      <c r="I197" s="24">
+        <v>47</v>
+      </c>
+      <c r="J197" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0047] Check lookup value on customer list without permissions</v>
+      </c>
+      <c r="K197" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0047] Check lookup value on customer list without permissions</v>
+      </c>
+      <c r="L197" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0047 'Check lookup value on customer list without permissions' {</v>
+      </c>
+      <c r="M197" s="23"/>
+    </row>
+    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>65</v>
+      </c>
+      <c r="B198" t="s">
+        <v>158</v>
+      </c>
+      <c r="C198" t="s">
+        <v>12</v>
+      </c>
+      <c r="D198" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E198" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G198" t="s">
+        <v>15</v>
+      </c>
+      <c r="H198" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I198" s="14">
+        <v>47</v>
+      </c>
+      <c r="J198" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K198" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L198" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>65</v>
+      </c>
+      <c r="B199" t="s">
+        <v>158</v>
+      </c>
+      <c r="C199" t="s">
+        <v>12</v>
+      </c>
+      <c r="D199" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E199" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G199" t="s">
+        <v>16</v>
+      </c>
+      <c r="H199" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="I199" s="14">
+        <v>47</v>
+      </c>
+      <c r="J199" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer list</v>
+      </c>
+      <c r="K199" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer list</v>
+      </c>
+      <c r="L199" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list' }</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>65</v>
+      </c>
+      <c r="B200" t="s">
+        <v>158</v>
+      </c>
+      <c r="C200" t="s">
+        <v>12</v>
+      </c>
+      <c r="D200" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E200" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G200" t="s">
+        <v>18</v>
+      </c>
+      <c r="H200" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I200" s="14">
+        <v>47</v>
+      </c>
+      <c r="J200" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="K200" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="L200" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown'</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B201" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C201" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D201" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E201" s="21"/>
+      <c r="F201" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G201" s="20"/>
+      <c r="H201" s="23"/>
+      <c r="I201" s="24">
+        <v>48</v>
+      </c>
+      <c r="J201" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0048] Check lookup value on customer list with permissions</v>
+      </c>
+      <c r="K201" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0048] Check lookup value on customer list with permissions</v>
+      </c>
+      <c r="L201" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0048 'Check lookup value on customer list with permissions' {</v>
+      </c>
+      <c r="M201" s="23"/>
+    </row>
+    <row r="202" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>65</v>
+      </c>
+      <c r="B202" t="s">
+        <v>158</v>
+      </c>
+      <c r="C202" t="s">
+        <v>12</v>
+      </c>
+      <c r="D202" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G202" t="s">
+        <v>15</v>
+      </c>
+      <c r="H202" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I202" s="14">
+        <v>48</v>
+      </c>
+      <c r="J202" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K202" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L202" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' } }</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>65</v>
+      </c>
+      <c r="B203" t="s">
+        <v>158</v>
+      </c>
+      <c r="C203" t="s">
+        <v>12</v>
+      </c>
+      <c r="D203" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G203" t="s">
+        <v>16</v>
+      </c>
+      <c r="H203" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="I203" s="14">
+        <v>48</v>
+      </c>
+      <c r="J203" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer list</v>
+      </c>
+      <c r="K203" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer list</v>
+      </c>
+      <c r="L203" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list' } }</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>65</v>
+      </c>
+      <c r="B204" t="s">
+        <v>158</v>
+      </c>
+      <c r="C204" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G204" t="s">
+        <v>18</v>
+      </c>
+      <c r="H204" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="I204" s="14">
+        <v>48</v>
+      </c>
+      <c r="J204" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field shown</v>
+      </c>
+      <c r="K204" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field shown</v>
+      </c>
+      <c r="L204" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field shown' } }</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
Modified and added scenarios #41 through #54 (test example 8)
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96655830-F68C-48C3-84F3-F22D75A44B4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450412F6-A061-4D5A-8E65-03184124B941}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="196">
   <si>
     <t>Feature</t>
   </si>
@@ -606,6 +606,45 @@
   </si>
   <si>
     <t>Clear last error</t>
+  </si>
+  <si>
+    <t>Read lookup value without permissions</t>
+  </si>
+  <si>
+    <t>Read lookup value</t>
+  </si>
+  <si>
+    <t>Read lookup value with permissions</t>
+  </si>
+  <si>
+    <t>Restricted base permissions extended with Lookup Value permissions</t>
+  </si>
+  <si>
+    <t>Modify lookup value without permissions</t>
+  </si>
+  <si>
+    <t>Modify lookup value</t>
+  </si>
+  <si>
+    <t>Modify permissions error thrown</t>
+  </si>
+  <si>
+    <t>Modify lookup value with permissions</t>
+  </si>
+  <si>
+    <t>Delete lookup value without permissions</t>
+  </si>
+  <si>
+    <t>Delete lookup value</t>
+  </si>
+  <si>
+    <t>Delete permissions error thrown</t>
+  </si>
+  <si>
+    <t>Delete lookup value with permissions</t>
+  </si>
+  <si>
+    <t>Lookup value does not exist</t>
   </si>
 </sst>
 </file>
@@ -814,7 +853,175 @@
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -940,28 +1147,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M204" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:M204" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M240" totalsRowShown="0" headerRowDxfId="39">
+  <autoFilter ref="A1:M240" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="36"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="33">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="31">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M205"/>
+  <dimension ref="A1:M241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B169" sqref="B169"/>
+      <selection activeCell="I238" sqref="I238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7016,7 +7223,7 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
@@ -7024,14 +7231,12 @@
         <v>158</v>
       </c>
       <c r="C178" s="20"/>
-      <c r="D178" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="D178" s="21"/>
       <c r="E178" s="21" t="s">
         <v>23</v>
       </c>
       <c r="F178" s="22" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
@@ -7040,15 +7245,15 @@
       </c>
       <c r="J178" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0043] Open Lookup Values Page without permissions</v>
+        <v>[SCENARIO #0043] Read lookup value without permissions</v>
       </c>
       <c r="K178" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0043] Open Lookup Values Page without permissions</v>
+        <v>//[SCENARIO #0043] Read lookup value without permissions</v>
       </c>
       <c r="L178" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0043 'Open Lookup Values Page without permissions' {</v>
+        <v>Scenario 0043 'Read lookup value without permissions' {</v>
       </c>
       <c r="M178" s="23"/>
     </row>
@@ -7059,9 +7264,6 @@
       <c r="B179" t="s">
         <v>158</v>
       </c>
-      <c r="D179" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="E179" s="11" t="s">
         <v>23</v>
       </c>
@@ -7084,7 +7286,7 @@
       </c>
       <c r="L179" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' } }</v>
+        <v>Given 'Starting unrestricted permissions' }</v>
       </c>
     </row>
     <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7094,26 +7296,29 @@
       <c r="B180" t="s">
         <v>158</v>
       </c>
+      <c r="E180" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G180" t="s">
         <v>15</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="I180" s="14">
         <v>43</v>
       </c>
       <c r="J180" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup value</v>
+        <v>[GIVEN] Lookup Value</v>
       </c>
       <c r="K180" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup value</v>
+        <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L180" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <v>Given 'Lookup Value' }</v>
       </c>
     </row>
     <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7123,6 +7328,9 @@
       <c r="B181" t="s">
         <v>158</v>
       </c>
+      <c r="E181" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G181" t="s">
         <v>15</v>
       </c>
@@ -7152,9 +7360,6 @@
       <c r="B182" t="s">
         <v>158</v>
       </c>
-      <c r="D182" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="E182" s="11" t="s">
         <v>23</v>
       </c>
@@ -7162,22 +7367,22 @@
         <v>16</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="I182" s="14">
         <v>43</v>
       </c>
       <c r="J182" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open Lookup Values page</v>
+        <v>[WHEN] Read lookup value</v>
       </c>
       <c r="K182" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open Lookup Values page</v>
+        <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L182" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open Lookup Values page' }</v>
+        <v>When 'Read lookup value' }</v>
       </c>
     </row>
     <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7187,9 +7392,6 @@
       <c r="B183" t="s">
         <v>158</v>
       </c>
-      <c r="D183" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="E183" s="11" t="s">
         <v>23</v>
       </c>
@@ -7215,7 +7417,7 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
@@ -7223,12 +7425,10 @@
         <v>158</v>
       </c>
       <c r="C184" s="20"/>
-      <c r="D184" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="22" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="23"/>
@@ -7237,48 +7437,45 @@
       </c>
       <c r="J184" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0044] Open Lookup Values Page with permissions</v>
+        <v>[SCENARIO #0044] Read lookup value with permissions</v>
       </c>
       <c r="K184" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0044] Open Lookup Values Page with permissions</v>
+        <v>//[SCENARIO #0044] Read lookup value with permissions</v>
       </c>
       <c r="L184" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0044 'Open Lookup Values Page with permissions' {</v>
+        <v>Scenario 0044 'Read lookup value with permissions' {</v>
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
       <c r="B185" t="s">
         <v>158</v>
       </c>
-      <c r="D185" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
       </c>
       <c r="J185" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="K185" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="L185" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Starting unrestricted permissions' } }</v>
       </c>
     </row>
     <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7288,29 +7485,26 @@
       <c r="B186" t="s">
         <v>158</v>
       </c>
-      <c r="D186" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G186" t="s">
         <v>15</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="I186" s="14">
         <v>44</v>
       </c>
       <c r="J186" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Clear last error</v>
+        <v>[GIVEN] Lookup Value</v>
       </c>
       <c r="K186" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Clear last error</v>
+        <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L186" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Clear last error' } }</v>
+        <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
     <row r="187" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7320,29 +7514,26 @@
       <c r="B187" t="s">
         <v>158</v>
       </c>
-      <c r="D187" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G187" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
       </c>
       <c r="J187" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open Lookup Values page</v>
+        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K187" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open Lookup Values page</v>
+        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L187" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open Lookup Values page' } }</v>
+        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
     <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7352,106 +7543,90 @@
       <c r="B188" t="s">
         <v>158</v>
       </c>
-      <c r="D188" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G188" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="I188" s="14">
         <v>44</v>
       </c>
       <c r="J188" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] No error thrown</v>
+        <v>[WHEN] Read lookup value</v>
       </c>
       <c r="K188" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] No error thrown</v>
+        <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L188" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'No error thrown'</v>
-      </c>
-    </row>
-    <row r="189" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B189" s="20" t="s">
+        <v>When 'Read lookup value' } }</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>65</v>
+      </c>
+      <c r="B189" t="s">
         <v>158</v>
       </c>
-      <c r="C189" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D189" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E189" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F189" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="G189" s="20"/>
-      <c r="H189" s="23"/>
-      <c r="I189" s="24">
+      <c r="G189" t="s">
+        <v>18</v>
+      </c>
+      <c r="H189" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I189" s="14">
+        <v>44</v>
+      </c>
+      <c r="J189" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value exists</v>
+      </c>
+      <c r="K189" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value exists</v>
+      </c>
+      <c r="L189" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists'</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B190" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C190" s="20"/>
+      <c r="D190" s="21"/>
+      <c r="E190" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F190" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="G190" s="20"/>
+      <c r="H190" s="23"/>
+      <c r="I190" s="24">
         <v>45</v>
       </c>
-      <c r="J189" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0045] Check lookup value on customer card without permissions</v>
-      </c>
-      <c r="K189" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0045] Check lookup value on customer card without permissions</v>
-      </c>
-      <c r="L189" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0045 'Check lookup value on customer card without permissions' {</v>
-      </c>
-      <c r="M189" s="23"/>
-    </row>
-    <row r="190" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>65</v>
-      </c>
-      <c r="B190" t="s">
-        <v>158</v>
-      </c>
-      <c r="C190" t="s">
-        <v>12</v>
-      </c>
-      <c r="D190" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E190" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G190" t="s">
-        <v>15</v>
-      </c>
-      <c r="H190" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="I190" s="14">
-        <v>45</v>
-      </c>
-      <c r="J190" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
-      </c>
-      <c r="K190" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
-      </c>
-      <c r="L190" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' }</v>
-      </c>
+      <c r="J190" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0045] Modify lookup value without permissions</v>
+      </c>
+      <c r="K190" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0045] Modify lookup value without permissions</v>
+      </c>
+      <c r="L190" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0045 'Modify lookup value without permissions' {</v>
+      </c>
+      <c r="M190" s="23"/>
     </row>
     <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
@@ -7460,35 +7635,29 @@
       <c r="B191" t="s">
         <v>158</v>
       </c>
-      <c r="C191" t="s">
-        <v>12</v>
-      </c>
-      <c r="D191" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="E191" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G191" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
       </c>
       <c r="J191" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open customer card</v>
+        <v>[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="K191" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open customer card</v>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="L191" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer card' }</v>
+        <v>Given 'Starting unrestricted permissions' }</v>
       </c>
     </row>
     <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7498,106 +7667,93 @@
       <c r="B192" t="s">
         <v>158</v>
       </c>
-      <c r="C192" t="s">
-        <v>12</v>
-      </c>
-      <c r="D192" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="E192" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G192" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H192" s="13" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="I192" s="14">
         <v>45</v>
       </c>
       <c r="J192" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value field not shown</v>
+        <v>[GIVEN] Lookup Value</v>
       </c>
       <c r="K192" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value field not shown</v>
+        <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L192" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field not shown'</v>
-      </c>
-    </row>
-    <row r="193" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B193" s="20" t="s">
+        <v>Given 'Lookup Value' }</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>65</v>
+      </c>
+      <c r="B193" t="s">
         <v>158</v>
       </c>
-      <c r="C193" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D193" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E193" s="21"/>
-      <c r="F193" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="G193" s="20"/>
-      <c r="H193" s="23"/>
-      <c r="I193" s="24">
-        <v>46</v>
-      </c>
-      <c r="J193" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0046] Check lookup value on customer card with permissions</v>
-      </c>
-      <c r="K193" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0046] Check lookup value on customer card with permissions</v>
-      </c>
-      <c r="L193" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0046 'Check lookup value on customer card with permissions' {</v>
-      </c>
-      <c r="M193" s="23"/>
-    </row>
-    <row r="194" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="E193" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G193" t="s">
+        <v>15</v>
+      </c>
+      <c r="H193" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I193" s="14">
+        <v>45</v>
+      </c>
+      <c r="J193" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="K193" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="L193" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
       <c r="B194" t="s">
         <v>158</v>
       </c>
-      <c r="C194" t="s">
-        <v>12</v>
-      </c>
-      <c r="D194" s="11" t="s">
+      <c r="E194" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G194" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H194" s="13" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="I194" s="14">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J194" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[WHEN] Modify lookup value</v>
       </c>
       <c r="K194" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[WHEN] Modify lookup value</v>
       </c>
       <c r="L194" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' } }</v>
+        <v>When 'Modify lookup value' }</v>
       </c>
     </row>
     <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7607,106 +7763,91 @@
       <c r="B195" t="s">
         <v>158</v>
       </c>
-      <c r="C195" t="s">
-        <v>12</v>
-      </c>
-      <c r="D195" s="11" t="s">
+      <c r="E195" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G195" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H195" s="13" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="I195" s="14">
+        <v>45</v>
+      </c>
+      <c r="J195" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Modify permissions error thrown</v>
+      </c>
+      <c r="K195" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Modify permissions error thrown</v>
+      </c>
+      <c r="L195" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Modify permissions error thrown'</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B196" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C196" s="20"/>
+      <c r="D196" s="21"/>
+      <c r="E196" s="21"/>
+      <c r="F196" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="G196" s="20"/>
+      <c r="H196" s="23"/>
+      <c r="I196" s="24">
         <v>46</v>
       </c>
-      <c r="J195" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open customer card</v>
-      </c>
-      <c r="K195" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open customer card</v>
-      </c>
-      <c r="L195" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer card' } }</v>
-      </c>
-    </row>
-    <row r="196" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>65</v>
-      </c>
-      <c r="B196" t="s">
+      <c r="J196" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0046] Modify lookup value with permissions</v>
+      </c>
+      <c r="K196" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0046] Modify lookup value with permissions</v>
+      </c>
+      <c r="L196" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0046 'Modify lookup value with permissions' {</v>
+      </c>
+      <c r="M196" s="23"/>
+    </row>
+    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>65</v>
+      </c>
+      <c r="B197" t="s">
         <v>158</v>
       </c>
-      <c r="C196" t="s">
-        <v>12</v>
-      </c>
-      <c r="D196" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G196" t="s">
-        <v>18</v>
-      </c>
-      <c r="H196" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="I196" s="14">
+      <c r="G197" t="s">
+        <v>15</v>
+      </c>
+      <c r="H197" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I197" s="14">
         <v>46</v>
       </c>
-      <c r="J196" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value field shown</v>
-      </c>
-      <c r="K196" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value field shown</v>
-      </c>
-      <c r="L196" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field shown'</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B197" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C197" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D197" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E197" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F197" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="G197" s="20"/>
-      <c r="H197" s="23"/>
-      <c r="I197" s="24">
-        <v>47</v>
-      </c>
-      <c r="J197" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0047] Check lookup value on customer list without permissions</v>
-      </c>
-      <c r="K197" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0047] Check lookup value on customer list without permissions</v>
-      </c>
-      <c r="L197" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0047 'Check lookup value on customer list without permissions' {</v>
-      </c>
-      <c r="M197" s="23"/>
+      <c r="J197" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="K197" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="L197" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting unrestricted permissions' } }</v>
+      </c>
     </row>
     <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
@@ -7715,35 +7856,26 @@
       <c r="B198" t="s">
         <v>158</v>
       </c>
-      <c r="C198" t="s">
-        <v>12</v>
-      </c>
-      <c r="D198" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E198" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G198" t="s">
         <v>15</v>
       </c>
       <c r="H198" s="13" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="I198" s="14">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J198" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Lookup Value</v>
       </c>
       <c r="K198" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L198" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' }</v>
+        <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
     <row r="199" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7753,35 +7885,26 @@
       <c r="B199" t="s">
         <v>158</v>
       </c>
-      <c r="C199" t="s">
-        <v>12</v>
-      </c>
-      <c r="D199" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E199" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G199" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="I199" s="14">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J199" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open customer list</v>
+        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K199" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open customer list</v>
+        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L199" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer list' }</v>
+        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
     <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7791,107 +7914,90 @@
       <c r="B200" t="s">
         <v>158</v>
       </c>
-      <c r="C200" t="s">
-        <v>12</v>
-      </c>
-      <c r="D200" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E200" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G200" t="s">
+        <v>16</v>
+      </c>
+      <c r="H200" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="I200" s="14">
+        <v>46</v>
+      </c>
+      <c r="J200" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Modify lookup value</v>
+      </c>
+      <c r="K200" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Modify lookup value</v>
+      </c>
+      <c r="L200" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Modify lookup value' } }</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>65</v>
+      </c>
+      <c r="B201" t="s">
+        <v>158</v>
+      </c>
+      <c r="G201" t="s">
         <v>18</v>
       </c>
-      <c r="H200" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="I200" s="14">
+      <c r="H201" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I201" s="14">
+        <v>46</v>
+      </c>
+      <c r="J201" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value exists</v>
+      </c>
+      <c r="K201" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value exists</v>
+      </c>
+      <c r="L201" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists'</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B202" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C202" s="20"/>
+      <c r="D202" s="21"/>
+      <c r="E202" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F202" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="G202" s="20"/>
+      <c r="H202" s="23"/>
+      <c r="I202" s="24">
         <v>47</v>
       </c>
-      <c r="J200" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value field not shown</v>
-      </c>
-      <c r="K200" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value field not shown</v>
-      </c>
-      <c r="L200" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field not shown'</v>
-      </c>
-    </row>
-    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B201" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C201" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D201" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E201" s="21"/>
-      <c r="F201" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="G201" s="20"/>
-      <c r="H201" s="23"/>
-      <c r="I201" s="24">
-        <v>48</v>
-      </c>
-      <c r="J201" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0048] Check lookup value on customer list with permissions</v>
-      </c>
-      <c r="K201" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0048] Check lookup value on customer list with permissions</v>
-      </c>
-      <c r="L201" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0048 'Check lookup value on customer list with permissions' {</v>
-      </c>
-      <c r="M201" s="23"/>
-    </row>
-    <row r="202" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>65</v>
-      </c>
-      <c r="B202" t="s">
-        <v>158</v>
-      </c>
-      <c r="C202" t="s">
-        <v>12</v>
-      </c>
-      <c r="D202" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G202" t="s">
-        <v>15</v>
-      </c>
-      <c r="H202" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="I202" s="14">
-        <v>48</v>
-      </c>
-      <c r="J202" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
-      </c>
-      <c r="K202" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
-      </c>
-      <c r="L202" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' } }</v>
-      </c>
+      <c r="J202" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0047] Delete lookup value without permissions</v>
+      </c>
+      <c r="K202" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0047] Delete lookup value without permissions</v>
+      </c>
+      <c r="L202" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0047 'Delete lookup value without permissions' {</v>
+      </c>
+      <c r="M202" s="23"/>
     </row>
     <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
@@ -7900,32 +8006,29 @@
       <c r="B203" t="s">
         <v>158</v>
       </c>
-      <c r="C203" t="s">
-        <v>12</v>
-      </c>
-      <c r="D203" s="11" t="s">
+      <c r="E203" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G203" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="I203" s="14">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J203" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Open customer list</v>
+        <v>[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="K203" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Open customer list</v>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
       </c>
       <c r="L203" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer list' } }</v>
+        <v>Given 'Starting unrestricted permissions' }</v>
       </c>
     </row>
     <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7935,38 +8038,1255 @@
       <c r="B204" t="s">
         <v>158</v>
       </c>
-      <c r="C204" t="s">
+      <c r="E204" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G204" t="s">
+        <v>15</v>
+      </c>
+      <c r="H204" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I204" s="14">
+        <v>47</v>
+      </c>
+      <c r="J204" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup Value</v>
+      </c>
+      <c r="K204" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup Value</v>
+      </c>
+      <c r="L204" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value' }</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>65</v>
+      </c>
+      <c r="B205" t="s">
+        <v>158</v>
+      </c>
+      <c r="E205" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G205" t="s">
+        <v>15</v>
+      </c>
+      <c r="H205" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I205" s="14">
+        <v>47</v>
+      </c>
+      <c r="J205" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="K205" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="L205" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>65</v>
+      </c>
+      <c r="B206" t="s">
+        <v>158</v>
+      </c>
+      <c r="E206" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G206" t="s">
+        <v>16</v>
+      </c>
+      <c r="H206" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I206" s="14">
+        <v>47</v>
+      </c>
+      <c r="J206" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Delete lookup value</v>
+      </c>
+      <c r="K206" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Delete lookup value</v>
+      </c>
+      <c r="L206" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete lookup value' }</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>65</v>
+      </c>
+      <c r="B207" t="s">
+        <v>158</v>
+      </c>
+      <c r="E207" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G207" t="s">
+        <v>18</v>
+      </c>
+      <c r="H207" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I207" s="14">
+        <v>47</v>
+      </c>
+      <c r="J207" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Delete permissions error thrown</v>
+      </c>
+      <c r="K207" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Delete permissions error thrown</v>
+      </c>
+      <c r="L207" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Delete permissions error thrown'</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B208" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C208" s="20"/>
+      <c r="D208" s="21"/>
+      <c r="E208" s="21"/>
+      <c r="F208" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="G208" s="20"/>
+      <c r="H208" s="23"/>
+      <c r="I208" s="24">
+        <v>48</v>
+      </c>
+      <c r="J208" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0048] Delete lookup value with permissions</v>
+      </c>
+      <c r="K208" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0048] Delete lookup value with permissions</v>
+      </c>
+      <c r="L208" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0048 'Delete lookup value with permissions' {</v>
+      </c>
+      <c r="M208" s="23"/>
+    </row>
+    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>65</v>
+      </c>
+      <c r="B209" t="s">
+        <v>158</v>
+      </c>
+      <c r="G209" t="s">
+        <v>15</v>
+      </c>
+      <c r="H209" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I209" s="14">
+        <v>48</v>
+      </c>
+      <c r="J209" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="K209" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="L209" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>65</v>
+      </c>
+      <c r="B210" t="s">
+        <v>158</v>
+      </c>
+      <c r="G210" t="s">
+        <v>15</v>
+      </c>
+      <c r="H210" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I210" s="14">
+        <v>48</v>
+      </c>
+      <c r="J210" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup Value</v>
+      </c>
+      <c r="K210" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup Value</v>
+      </c>
+      <c r="L210" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value' } }</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>65</v>
+      </c>
+      <c r="B211" t="s">
+        <v>158</v>
+      </c>
+      <c r="G211" t="s">
+        <v>15</v>
+      </c>
+      <c r="H211" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="I211" s="14">
+        <v>48</v>
+      </c>
+      <c r="J211" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="K211" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="L211" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>65</v>
+      </c>
+      <c r="B212" t="s">
+        <v>158</v>
+      </c>
+      <c r="G212" t="s">
+        <v>16</v>
+      </c>
+      <c r="H212" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I212" s="14">
+        <v>48</v>
+      </c>
+      <c r="J212" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Delete lookup value</v>
+      </c>
+      <c r="K212" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Delete lookup value</v>
+      </c>
+      <c r="L212" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete lookup value' } }</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>65</v>
+      </c>
+      <c r="B213" t="s">
+        <v>158</v>
+      </c>
+      <c r="G213" t="s">
+        <v>18</v>
+      </c>
+      <c r="H213" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="I213" s="14">
+        <v>48</v>
+      </c>
+      <c r="J213" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value does not exist</v>
+      </c>
+      <c r="K213" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value does not exist</v>
+      </c>
+      <c r="L213" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value does not exist'</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B214" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C214" s="20"/>
+      <c r="D214" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E214" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F214" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="G214" s="20"/>
+      <c r="H214" s="23"/>
+      <c r="I214" s="24">
+        <v>49</v>
+      </c>
+      <c r="J214" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0049] Open Lookup Values Page without permissions</v>
+      </c>
+      <c r="K214" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0049] Open Lookup Values Page without permissions</v>
+      </c>
+      <c r="L214" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0049 'Open Lookup Values Page without permissions' {</v>
+      </c>
+      <c r="M214" s="23"/>
+    </row>
+    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>65</v>
+      </c>
+      <c r="B215" t="s">
+        <v>158</v>
+      </c>
+      <c r="D215" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E215" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G215" t="s">
+        <v>15</v>
+      </c>
+      <c r="H215" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I215" s="14">
+        <v>49</v>
+      </c>
+      <c r="J215" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="K215" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting unrestricted permissions</v>
+      </c>
+      <c r="L215" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>65</v>
+      </c>
+      <c r="B216" t="s">
+        <v>158</v>
+      </c>
+      <c r="G216" t="s">
+        <v>15</v>
+      </c>
+      <c r="H216" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I216" s="14">
+        <v>49</v>
+      </c>
+      <c r="J216" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value</v>
+      </c>
+      <c r="K216" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup value</v>
+      </c>
+      <c r="L216" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value' } }</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>65</v>
+      </c>
+      <c r="B217" t="s">
+        <v>158</v>
+      </c>
+      <c r="G217" t="s">
+        <v>15</v>
+      </c>
+      <c r="H217" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="I217" s="14">
+        <v>49</v>
+      </c>
+      <c r="J217" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="K217" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Restricted base permissions</v>
+      </c>
+      <c r="L217" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>65</v>
+      </c>
+      <c r="B218" t="s">
+        <v>158</v>
+      </c>
+      <c r="D218" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E218" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G218" t="s">
+        <v>16</v>
+      </c>
+      <c r="H218" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I218" s="14">
+        <v>49</v>
+      </c>
+      <c r="J218" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="K218" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="L218" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page' }</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>65</v>
+      </c>
+      <c r="B219" t="s">
+        <v>158</v>
+      </c>
+      <c r="D219" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E219" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G219" t="s">
+        <v>18</v>
+      </c>
+      <c r="H219" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I219" s="14">
+        <v>49</v>
+      </c>
+      <c r="J219" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="K219" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="L219" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Read permissions error thrown'</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B220" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C220" s="20"/>
+      <c r="D220" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E220" s="21"/>
+      <c r="F220" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G220" s="20"/>
+      <c r="H220" s="23"/>
+      <c r="I220" s="24">
+        <v>50</v>
+      </c>
+      <c r="J220" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0050] Open Lookup Values Page with permissions</v>
+      </c>
+      <c r="K220" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0050] Open Lookup Values Page with permissions</v>
+      </c>
+      <c r="L220" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0050 'Open Lookup Values Page with permissions' {</v>
+      </c>
+      <c r="M220" s="23"/>
+    </row>
+    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>65</v>
+      </c>
+      <c r="B221" t="s">
+        <v>158</v>
+      </c>
+      <c r="D221" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G221" t="s">
+        <v>15</v>
+      </c>
+      <c r="H221" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I221" s="14">
+        <v>50</v>
+      </c>
+      <c r="J221" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="K221" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+      </c>
+      <c r="L221" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>65</v>
+      </c>
+      <c r="B222" t="s">
+        <v>158</v>
+      </c>
+      <c r="D222" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G222" t="s">
+        <v>15</v>
+      </c>
+      <c r="H222" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="I222" s="14">
+        <v>50</v>
+      </c>
+      <c r="J222" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Clear last error</v>
+      </c>
+      <c r="K222" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Clear last error</v>
+      </c>
+      <c r="L222" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Clear last error' } }</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>65</v>
+      </c>
+      <c r="B223" t="s">
+        <v>158</v>
+      </c>
+      <c r="D223" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G223" t="s">
+        <v>16</v>
+      </c>
+      <c r="H223" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I223" s="14">
+        <v>50</v>
+      </c>
+      <c r="J223" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="K223" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open Lookup Values page</v>
+      </c>
+      <c r="L223" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page' } }</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>65</v>
+      </c>
+      <c r="B224" t="s">
+        <v>158</v>
+      </c>
+      <c r="D224" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G224" t="s">
+        <v>18</v>
+      </c>
+      <c r="H224" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="I224" s="14">
+        <v>50</v>
+      </c>
+      <c r="J224" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] No error thrown</v>
+      </c>
+      <c r="K224" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] No error thrown</v>
+      </c>
+      <c r="L224" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No error thrown'</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B225" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C225" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D204" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G204" t="s">
+      <c r="D225" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E225" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F225" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="G225" s="20"/>
+      <c r="H225" s="23"/>
+      <c r="I225" s="24">
+        <v>51</v>
+      </c>
+      <c r="J225" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0051] Check lookup value on customer card without permissions</v>
+      </c>
+      <c r="K225" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0051] Check lookup value on customer card without permissions</v>
+      </c>
+      <c r="L225" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0051 'Check lookup value on customer card without permissions' {</v>
+      </c>
+      <c r="M225" s="23"/>
+    </row>
+    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>65</v>
+      </c>
+      <c r="B226" t="s">
+        <v>158</v>
+      </c>
+      <c r="C226" t="s">
+        <v>12</v>
+      </c>
+      <c r="D226" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E226" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G226" t="s">
+        <v>15</v>
+      </c>
+      <c r="H226" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I226" s="14">
+        <v>51</v>
+      </c>
+      <c r="J226" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K226" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L226" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>65</v>
+      </c>
+      <c r="B227" t="s">
+        <v>158</v>
+      </c>
+      <c r="C227" t="s">
+        <v>12</v>
+      </c>
+      <c r="D227" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E227" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G227" t="s">
+        <v>16</v>
+      </c>
+      <c r="H227" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I227" s="14">
+        <v>51</v>
+      </c>
+      <c r="J227" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer card</v>
+      </c>
+      <c r="K227" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer card</v>
+      </c>
+      <c r="L227" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card' }</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>65</v>
+      </c>
+      <c r="B228" t="s">
+        <v>158</v>
+      </c>
+      <c r="C228" t="s">
+        <v>12</v>
+      </c>
+      <c r="D228" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E228" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G228" t="s">
         <v>18</v>
       </c>
-      <c r="H204" s="13" t="s">
+      <c r="H228" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I228" s="14">
+        <v>51</v>
+      </c>
+      <c r="J228" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="K228" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="L228" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown'</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B229" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C229" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D229" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E229" s="21"/>
+      <c r="F229" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="G229" s="20"/>
+      <c r="H229" s="23"/>
+      <c r="I229" s="24">
+        <v>52</v>
+      </c>
+      <c r="J229" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0052] Check lookup value on customer card with permissions</v>
+      </c>
+      <c r="K229" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0052] Check lookup value on customer card with permissions</v>
+      </c>
+      <c r="L229" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0052 'Check lookup value on customer card with permissions' {</v>
+      </c>
+      <c r="M229" s="23"/>
+    </row>
+    <row r="230" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>65</v>
+      </c>
+      <c r="B230" t="s">
+        <v>158</v>
+      </c>
+      <c r="C230" t="s">
+        <v>12</v>
+      </c>
+      <c r="D230" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G230" t="s">
+        <v>15</v>
+      </c>
+      <c r="H230" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I230" s="14">
+        <v>52</v>
+      </c>
+      <c r="J230" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K230" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L230" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' } }</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>65</v>
+      </c>
+      <c r="B231" t="s">
+        <v>158</v>
+      </c>
+      <c r="C231" t="s">
+        <v>12</v>
+      </c>
+      <c r="D231" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G231" t="s">
+        <v>16</v>
+      </c>
+      <c r="H231" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I231" s="14">
+        <v>52</v>
+      </c>
+      <c r="J231" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer card</v>
+      </c>
+      <c r="K231" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer card</v>
+      </c>
+      <c r="L231" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card' } }</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>65</v>
+      </c>
+      <c r="B232" t="s">
+        <v>158</v>
+      </c>
+      <c r="C232" t="s">
+        <v>12</v>
+      </c>
+      <c r="D232" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G232" t="s">
+        <v>18</v>
+      </c>
+      <c r="H232" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I204" s="14">
-        <v>48</v>
-      </c>
-      <c r="J204" s="16" t="str">
+      <c r="I232" s="14">
+        <v>52</v>
+      </c>
+      <c r="J232" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Lookup value field shown</v>
       </c>
-      <c r="K204" s="17" t="str">
+      <c r="K232" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Lookup value field shown</v>
       </c>
-      <c r="L204" s="31" t="str">
+      <c r="L232" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field shown'</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B233" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C233" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D233" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E233" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F233" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="G233" s="20"/>
+      <c r="H233" s="23"/>
+      <c r="I233" s="24">
+        <v>53</v>
+      </c>
+      <c r="J233" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0053] Check lookup value on customer list without permissions</v>
+      </c>
+      <c r="K233" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0053] Check lookup value on customer list without permissions</v>
+      </c>
+      <c r="L233" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0053 'Check lookup value on customer list without permissions' {</v>
+      </c>
+      <c r="M233" s="23"/>
+    </row>
+    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>65</v>
+      </c>
+      <c r="B234" t="s">
+        <v>158</v>
+      </c>
+      <c r="C234" t="s">
+        <v>12</v>
+      </c>
+      <c r="D234" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E234" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G234" t="s">
+        <v>15</v>
+      </c>
+      <c r="H234" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I234" s="14">
+        <v>53</v>
+      </c>
+      <c r="J234" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K234" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L234" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' }</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>65</v>
+      </c>
+      <c r="B235" t="s">
+        <v>158</v>
+      </c>
+      <c r="C235" t="s">
+        <v>12</v>
+      </c>
+      <c r="D235" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E235" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G235" t="s">
+        <v>16</v>
+      </c>
+      <c r="H235" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="I235" s="14">
+        <v>53</v>
+      </c>
+      <c r="J235" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer list</v>
+      </c>
+      <c r="K235" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer list</v>
+      </c>
+      <c r="L235" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list' }</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>65</v>
+      </c>
+      <c r="B236" t="s">
+        <v>158</v>
+      </c>
+      <c r="C236" t="s">
+        <v>12</v>
+      </c>
+      <c r="D236" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E236" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G236" t="s">
+        <v>18</v>
+      </c>
+      <c r="H236" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I236" s="14">
+        <v>53</v>
+      </c>
+      <c r="J236" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="K236" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field not shown</v>
+      </c>
+      <c r="L236" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown'</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B237" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C237" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D237" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E237" s="21"/>
+      <c r="F237" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G237" s="20"/>
+      <c r="H237" s="23"/>
+      <c r="I237" s="24">
+        <v>54</v>
+      </c>
+      <c r="J237" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0054] Check lookup value on customer list with permissions</v>
+      </c>
+      <c r="K237" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0054] Check lookup value on customer list with permissions</v>
+      </c>
+      <c r="L237" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0054 'Check lookup value on customer list with permissions' {</v>
+      </c>
+      <c r="M237" s="23"/>
+    </row>
+    <row r="238" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>65</v>
+      </c>
+      <c r="B238" t="s">
+        <v>158</v>
+      </c>
+      <c r="C238" t="s">
+        <v>12</v>
+      </c>
+      <c r="D238" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G238" t="s">
+        <v>15</v>
+      </c>
+      <c r="H238" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I238" s="14">
+        <v>54</v>
+      </c>
+      <c r="J238" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="K238" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Starting restricted base permissions</v>
+      </c>
+      <c r="L238" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Starting restricted base permissions' } }</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>65</v>
+      </c>
+      <c r="B239" t="s">
+        <v>158</v>
+      </c>
+      <c r="C239" t="s">
+        <v>12</v>
+      </c>
+      <c r="D239" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G239" t="s">
+        <v>16</v>
+      </c>
+      <c r="H239" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="I239" s="14">
+        <v>54</v>
+      </c>
+      <c r="J239" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Open customer list</v>
+      </c>
+      <c r="K239" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Open customer list</v>
+      </c>
+      <c r="L239" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list' } }</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>65</v>
+      </c>
+      <c r="B240" t="s">
+        <v>158</v>
+      </c>
+      <c r="C240" t="s">
+        <v>12</v>
+      </c>
+      <c r="D240" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G240" t="s">
+        <v>18</v>
+      </c>
+      <c r="H240" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="I240" s="14">
+        <v>54</v>
+      </c>
+      <c r="J240" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value field shown</v>
+      </c>
+      <c r="K240" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value field shown</v>
+      </c>
+      <c r="L240" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7978,29 +9298,117 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="G1:G184 G189:G190 G196 G213:G1048576">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G185:G188">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G191:G195">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G197:G199">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G200">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G201:G202 G206:G208">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G203:G205">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G209:G211">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G212">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"LookupValue Permissions" not refactored
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450412F6-A061-4D5A-8E65-03184124B941}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968C1E39-8E42-4DE9-9A53-1BCE87483A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="194">
   <si>
     <t>Feature</t>
   </si>
@@ -531,15 +531,6 @@
     <t>Check lookup value on customer card with permissions</t>
   </si>
   <si>
-    <t>Starting restricted base permissions</t>
-  </si>
-  <si>
-    <t>Starting restricted base permissions extended with Lookup Value permissions</t>
-  </si>
-  <si>
-    <t>Starting unrestricted permissions</t>
-  </si>
-  <si>
     <t>Create lookup value</t>
   </si>
   <si>
@@ -547,9 +538,6 @@
   </si>
   <si>
     <t>Lookup value exists</t>
-  </si>
-  <si>
-    <t>Restricted base permissions</t>
   </si>
   <si>
     <t>Open Lookup Values page</t>
@@ -617,9 +605,6 @@
     <t>Read lookup value with permissions</t>
   </si>
   <si>
-    <t>Restricted base permissions extended with Lookup Value permissions</t>
-  </si>
-  <si>
     <t>Modify lookup value without permissions</t>
   </si>
   <si>
@@ -645,6 +630,15 @@
   </si>
   <si>
     <t>Lookup value does not exist</t>
+  </si>
+  <si>
+    <t>Unrestricted permissions</t>
+  </si>
+  <si>
+    <t>Non-restrictive base permissions</t>
+  </si>
+  <si>
+    <t>Non-restrictive base permissions extended with Lookup Value permissions</t>
   </si>
 </sst>
 </file>
@@ -854,6 +848,69 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1070,69 +1127,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1147,28 +1141,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M240" totalsRowShown="0" headerRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M240" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:M240" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="31">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1471,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M241"/>
+  <dimension ref="A1:M240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I238" sqref="I238"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H221" sqref="H221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2654,7 @@
         <v>Given 'Sales order document page' } }</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -3556,7 +3550,7 @@
         <v>Given 'Customer template' } }</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -4058,7 +4052,7 @@
         <v>Given 'Location with require shipment' } }</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -4087,7 +4081,7 @@
         <v>Given 'Warehouse employee for current user' } }</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -4240,7 +4234,7 @@
         <v>Given 'Non-existing lookup value' }</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -4466,7 +4460,7 @@
         <v>Given 'Warehouse employee for current user' } }</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>65</v>
       </c>
@@ -4654,7 +4648,7 @@
       </c>
       <c r="M97"/>
     </row>
-    <row r="98" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -4836,7 +4830,7 @@
       </c>
       <c r="M103"/>
     </row>
-    <row r="104" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -4866,7 +4860,7 @@
       </c>
       <c r="M104"/>
     </row>
-    <row r="105" spans="1:13" ht="39" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>65</v>
       </c>
@@ -5314,7 +5308,7 @@
       </c>
       <c r="M118" s="20"/>
     </row>
-    <row r="119" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>65</v>
       </c>
@@ -5815,7 +5809,7 @@
       </c>
       <c r="M133" s="20"/>
     </row>
-    <row r="134" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>65</v>
       </c>
@@ -6027,7 +6021,7 @@
       </c>
       <c r="M140"/>
     </row>
-    <row r="141" spans="1:13" ht="39.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>65</v>
       </c>
@@ -6087,7 +6081,7 @@
       </c>
       <c r="M142" s="8"/>
     </row>
-    <row r="143" spans="1:13" ht="39.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A143" s="20" t="s">
         <v>65</v>
       </c>
@@ -6153,7 +6147,7 @@
         <v>Given 'Sales order with Lookup value' } }</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>65</v>
       </c>
@@ -6320,7 +6314,7 @@
         <v>Given 'Sales order without Lookup value' }</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>65</v>
       </c>
@@ -6456,7 +6450,7 @@
         <v>Given 'Location with require shipment' } }</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>107</v>
       </c>
@@ -6857,7 +6851,7 @@
       </c>
       <c r="M165" s="23"/>
     </row>
-    <row r="166" spans="1:13" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>65</v>
       </c>
@@ -6974,7 +6968,7 @@
       </c>
       <c r="M169" s="8"/>
     </row>
-    <row r="170" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="30.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="s">
         <v>65</v>
       </c>
@@ -7008,7 +7002,7 @@
       </c>
       <c r="M170" s="23"/>
     </row>
-    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
@@ -7022,25 +7016,25 @@
         <v>15</v>
       </c>
       <c r="H171" s="13" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="I171" s="14">
         <v>41</v>
       </c>
       <c r="J171" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K171" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L171" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>65</v>
       </c>
@@ -7054,7 +7048,7 @@
         <v>16</v>
       </c>
       <c r="H172" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I172" s="14">
         <v>41</v>
@@ -7072,7 +7066,7 @@
         <v>When 'Create lookup value' }</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
@@ -7086,7 +7080,7 @@
         <v>18</v>
       </c>
       <c r="H173" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I173" s="14">
         <v>41</v>
@@ -7104,7 +7098,7 @@
         <v>Then 'Insert permissions error thrown'</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
@@ -7136,7 +7130,7 @@
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
@@ -7147,25 +7141,25 @@
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="I175" s="14">
         <v>42</v>
       </c>
       <c r="J175" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K175" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L175" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>65</v>
       </c>
@@ -7176,7 +7170,7 @@
         <v>16</v>
       </c>
       <c r="H176" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I176" s="14">
         <v>42</v>
@@ -7194,7 +7188,7 @@
         <v>When 'Create lookup value' } }</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>65</v>
       </c>
@@ -7205,7 +7199,7 @@
         <v>18</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I177" s="14">
         <v>42</v>
@@ -7223,7 +7217,7 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
@@ -7236,7 +7230,7 @@
         <v>23</v>
       </c>
       <c r="F178" s="22" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
@@ -7257,7 +7251,7 @@
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
@@ -7271,25 +7265,25 @@
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I179" s="14">
         <v>43</v>
       </c>
       <c r="J179" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K179" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L179" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' }</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>65</v>
       </c>
@@ -7321,7 +7315,7 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>65</v>
       </c>
@@ -7335,25 +7329,25 @@
         <v>15</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="I181" s="14">
         <v>43</v>
       </c>
       <c r="J181" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K181" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L181" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>65</v>
       </c>
@@ -7367,7 +7361,7 @@
         <v>16</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I182" s="14">
         <v>43</v>
@@ -7385,7 +7379,7 @@
         <v>When 'Read lookup value' }</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>65</v>
       </c>
@@ -7399,7 +7393,7 @@
         <v>18</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I183" s="14">
         <v>43</v>
@@ -7417,7 +7411,7 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
@@ -7428,7 +7422,7 @@
       <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="22" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="23"/>
@@ -7449,7 +7443,7 @@
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
@@ -7460,25 +7454,25 @@
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
       </c>
       <c r="J185" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K185" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L185" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
@@ -7507,7 +7501,7 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
@@ -7518,25 +7512,25 @@
         <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
       </c>
       <c r="J187" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K187" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L187" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>65</v>
       </c>
@@ -7547,7 +7541,7 @@
         <v>16</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I188" s="14">
         <v>44</v>
@@ -7565,7 +7559,7 @@
         <v>When 'Read lookup value' } }</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>65</v>
       </c>
@@ -7576,7 +7570,7 @@
         <v>18</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I189" s="14">
         <v>44</v>
@@ -7594,7 +7588,7 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
         <v>65</v>
       </c>
@@ -7607,7 +7601,7 @@
         <v>23</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="23"/>
@@ -7628,7 +7622,7 @@
       </c>
       <c r="M190" s="23"/>
     </row>
-    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
@@ -7642,25 +7636,25 @@
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
       </c>
       <c r="J191" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K191" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L191" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' }</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>65</v>
       </c>
@@ -7692,7 +7686,7 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>65</v>
       </c>
@@ -7706,25 +7700,25 @@
         <v>15</v>
       </c>
       <c r="H193" s="13" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="I193" s="14">
         <v>45</v>
       </c>
       <c r="J193" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K193" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L193" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
@@ -7738,7 +7732,7 @@
         <v>16</v>
       </c>
       <c r="H194" s="13" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I194" s="14">
         <v>45</v>
@@ -7756,7 +7750,7 @@
         <v>When 'Modify lookup value' }</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>65</v>
       </c>
@@ -7770,7 +7764,7 @@
         <v>18</v>
       </c>
       <c r="H195" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I195" s="14">
         <v>45</v>
@@ -7788,7 +7782,7 @@
         <v>Then 'Modify permissions error thrown'</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>65</v>
       </c>
@@ -7799,7 +7793,7 @@
       <c r="D196" s="21"/>
       <c r="E196" s="21"/>
       <c r="F196" s="22" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G196" s="20"/>
       <c r="H196" s="23"/>
@@ -7820,7 +7814,7 @@
       </c>
       <c r="M196" s="23"/>
     </row>
-    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>65</v>
       </c>
@@ -7831,25 +7825,25 @@
         <v>15</v>
       </c>
       <c r="H197" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I197" s="14">
         <v>46</v>
       </c>
       <c r="J197" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K197" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L197" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
@@ -7878,7 +7872,7 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="199" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
@@ -7889,25 +7883,25 @@
         <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I199" s="14">
         <v>46</v>
       </c>
       <c r="J199" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K199" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L199" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -7918,7 +7912,7 @@
         <v>16</v>
       </c>
       <c r="H200" s="13" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I200" s="14">
         <v>46</v>
@@ -7936,7 +7930,7 @@
         <v>When 'Modify lookup value' } }</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
@@ -7947,7 +7941,7 @@
         <v>18</v>
       </c>
       <c r="H201" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I201" s="14">
         <v>46</v>
@@ -7965,7 +7959,7 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="202" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>65</v>
       </c>
@@ -7978,7 +7972,7 @@
         <v>23</v>
       </c>
       <c r="F202" s="22" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G202" s="20"/>
       <c r="H202" s="23"/>
@@ -7999,7 +7993,7 @@
       </c>
       <c r="M202" s="23"/>
     </row>
-    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
@@ -8013,25 +8007,25 @@
         <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I203" s="14">
         <v>47</v>
       </c>
       <c r="J203" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K203" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L203" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' }</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
@@ -8063,7 +8057,7 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
@@ -8077,25 +8071,25 @@
         <v>15</v>
       </c>
       <c r="H205" s="13" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="I205" s="14">
         <v>47</v>
       </c>
       <c r="J205" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K205" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L205" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>65</v>
       </c>
@@ -8109,7 +8103,7 @@
         <v>16</v>
       </c>
       <c r="H206" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I206" s="14">
         <v>47</v>
@@ -8127,7 +8121,7 @@
         <v>When 'Delete lookup value' }</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>65</v>
       </c>
@@ -8141,7 +8135,7 @@
         <v>18</v>
       </c>
       <c r="H207" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I207" s="14">
         <v>47</v>
@@ -8159,7 +8153,7 @@
         <v>Then 'Delete permissions error thrown'</v>
       </c>
     </row>
-    <row r="208" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>65</v>
       </c>
@@ -8170,7 +8164,7 @@
       <c r="D208" s="21"/>
       <c r="E208" s="21"/>
       <c r="F208" s="22" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G208" s="20"/>
       <c r="H208" s="23"/>
@@ -8191,7 +8185,7 @@
       </c>
       <c r="M208" s="23"/>
     </row>
-    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>65</v>
       </c>
@@ -8202,25 +8196,25 @@
         <v>15</v>
       </c>
       <c r="H209" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I209" s="14">
         <v>48</v>
       </c>
       <c r="J209" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K209" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L209" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>65</v>
       </c>
@@ -8249,7 +8243,7 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="211" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>65</v>
       </c>
@@ -8260,25 +8254,25 @@
         <v>15</v>
       </c>
       <c r="H211" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I211" s="14">
         <v>48</v>
       </c>
       <c r="J211" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K211" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L211" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>65</v>
       </c>
@@ -8289,7 +8283,7 @@
         <v>16</v>
       </c>
       <c r="H212" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I212" s="14">
         <v>48</v>
@@ -8307,7 +8301,7 @@
         <v>When 'Delete lookup value' } }</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>65</v>
       </c>
@@ -8318,7 +8312,7 @@
         <v>18</v>
       </c>
       <c r="H213" s="13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I213" s="14">
         <v>48</v>
@@ -8336,7 +8330,7 @@
         <v>Then 'Lookup value does not exist'</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>65</v>
       </c>
@@ -8372,7 +8366,7 @@
       </c>
       <c r="M214" s="23"/>
     </row>
-    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>65</v>
       </c>
@@ -8389,25 +8383,25 @@
         <v>15</v>
       </c>
       <c r="H215" s="13" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I215" s="14">
         <v>49</v>
       </c>
       <c r="J215" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="K215" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted permissions</v>
       </c>
       <c r="L215" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted permissions' } }</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>65</v>
       </c>
@@ -8436,7 +8430,7 @@
         <v>Given 'Lookup value' } }</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>65</v>
       </c>
@@ -8447,25 +8441,25 @@
         <v>15</v>
       </c>
       <c r="H217" s="13" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="I217" s="14">
         <v>49</v>
       </c>
       <c r="J217" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K217" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L217" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>65</v>
       </c>
@@ -8482,7 +8476,7 @@
         <v>16</v>
       </c>
       <c r="H218" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I218" s="14">
         <v>49</v>
@@ -8500,7 +8494,7 @@
         <v>When 'Open Lookup Values page' }</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>65</v>
       </c>
@@ -8517,7 +8511,7 @@
         <v>18</v>
       </c>
       <c r="H219" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I219" s="14">
         <v>49</v>
@@ -8535,7 +8529,7 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>65</v>
       </c>
@@ -8569,7 +8563,7 @@
       </c>
       <c r="M220" s="23"/>
     </row>
-    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>65</v>
       </c>
@@ -8583,25 +8577,25 @@
         <v>15</v>
       </c>
       <c r="H221" s="13" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="I221" s="14">
         <v>50</v>
       </c>
       <c r="J221" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K221" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L221" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>65</v>
       </c>
@@ -8615,7 +8609,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I222" s="14">
         <v>50</v>
@@ -8633,7 +8627,7 @@
         <v>Given 'Clear last error' } }</v>
       </c>
     </row>
-    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>65</v>
       </c>
@@ -8647,7 +8641,7 @@
         <v>16</v>
       </c>
       <c r="H223" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I223" s="14">
         <v>50</v>
@@ -8665,7 +8659,7 @@
         <v>When 'Open Lookup Values page' } }</v>
       </c>
     </row>
-    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
@@ -8679,7 +8673,7 @@
         <v>18</v>
       </c>
       <c r="H224" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I224" s="14">
         <v>50</v>
@@ -8697,7 +8691,7 @@
         <v>Then 'No error thrown'</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>65</v>
       </c>
@@ -8735,7 +8729,7 @@
       </c>
       <c r="M225" s="23"/>
     </row>
-    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>65</v>
       </c>
@@ -8755,25 +8749,25 @@
         <v>15</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="I226" s="14">
         <v>51</v>
       </c>
       <c r="J226" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K226" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L226" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>65</v>
       </c>
@@ -8793,7 +8787,7 @@
         <v>16</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I227" s="14">
         <v>51</v>
@@ -8811,7 +8805,7 @@
         <v>When 'Open customer card' }</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>65</v>
       </c>
@@ -8831,7 +8825,7 @@
         <v>18</v>
       </c>
       <c r="H228" s="13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I228" s="14">
         <v>51</v>
@@ -8849,7 +8843,7 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>65</v>
       </c>
@@ -8885,7 +8879,7 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
@@ -8902,25 +8896,25 @@
         <v>15</v>
       </c>
       <c r="H230" s="13" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="I230" s="14">
         <v>52</v>
       </c>
       <c r="J230" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K230" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L230" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' } }</v>
-      </c>
-    </row>
-    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>65</v>
       </c>
@@ -8937,7 +8931,7 @@
         <v>16</v>
       </c>
       <c r="H231" s="13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I231" s="14">
         <v>52</v>
@@ -8955,7 +8949,7 @@
         <v>When 'Open customer card' } }</v>
       </c>
     </row>
-    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>65</v>
       </c>
@@ -8972,7 +8966,7 @@
         <v>18</v>
       </c>
       <c r="H232" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I232" s="14">
         <v>52</v>
@@ -8990,7 +8984,7 @@
         <v>Then 'Lookup value field shown'</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>65</v>
       </c>
@@ -9007,7 +9001,7 @@
         <v>23</v>
       </c>
       <c r="F233" s="22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G233" s="20"/>
       <c r="H233" s="23"/>
@@ -9028,7 +9022,7 @@
       </c>
       <c r="M233" s="23"/>
     </row>
-    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>65</v>
       </c>
@@ -9048,25 +9042,25 @@
         <v>15</v>
       </c>
       <c r="H234" s="13" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="I234" s="14">
         <v>53</v>
       </c>
       <c r="J234" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="K234" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions</v>
       </c>
       <c r="L234" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' }</v>
-      </c>
-    </row>
-    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions' }</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>65</v>
       </c>
@@ -9086,7 +9080,7 @@
         <v>16</v>
       </c>
       <c r="H235" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I235" s="14">
         <v>53</v>
@@ -9104,7 +9098,7 @@
         <v>When 'Open customer list' }</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>65</v>
       </c>
@@ -9124,7 +9118,7 @@
         <v>18</v>
       </c>
       <c r="H236" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I236" s="14">
         <v>53</v>
@@ -9142,7 +9136,7 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>65</v>
       </c>
@@ -9157,7 +9151,7 @@
       </c>
       <c r="E237" s="21"/>
       <c r="F237" s="22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G237" s="20"/>
       <c r="H237" s="23"/>
@@ -9178,7 +9172,7 @@
       </c>
       <c r="M237" s="23"/>
     </row>
-    <row r="238" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>65</v>
       </c>
@@ -9195,25 +9189,25 @@
         <v>15</v>
       </c>
       <c r="H238" s="13" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="I238" s="14">
         <v>54</v>
       </c>
       <c r="J238" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Starting restricted base permissions</v>
+        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K238" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Starting restricted base permissions</v>
+        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L238" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Starting restricted base permissions' } }</v>
-      </c>
-    </row>
-    <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>65</v>
       </c>
@@ -9230,7 +9224,7 @@
         <v>16</v>
       </c>
       <c r="H239" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I239" s="14">
         <v>54</v>
@@ -9248,7 +9242,7 @@
         <v>When 'Open customer list' } }</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>65</v>
       </c>
@@ -9265,7 +9259,7 @@
         <v>18</v>
       </c>
       <c r="H240" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I240" s="14">
         <v>54</v>
@@ -9283,7 +9277,6 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
-    <row r="241" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="32">
@@ -9298,116 +9291,116 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="28" priority="29">
+    <cfRule type="containsBlanks" dxfId="38" priority="29">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G184 G189:G190 G196 G213:G1048576">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:G188">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:G195">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:G199">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G200">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:G202 G206:G208">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203:G205">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:G211">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adjusted Customer Template use to BC19
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968C1E39-8E42-4DE9-9A53-1BCE87483A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57347BF-8262-4195-AE87-A632CB2FFFCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-19320" yWindow="780" windowWidth="18510" windowHeight="15600" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="193">
   <si>
     <t>Feature</t>
   </si>
@@ -324,15 +324,6 @@
     <t>Lookup value on sales document is populated with lookup value of customer</t>
   </si>
   <si>
-    <t>Create customer from configuration template with lookup value</t>
-  </si>
-  <si>
-    <t>Create customer from configuration template</t>
-  </si>
-  <si>
-    <t>Lookup value on customer is populated with lookup value of configuration template</t>
-  </si>
-  <si>
     <t>Posting</t>
   </si>
   <si>
@@ -492,9 +483,6 @@
     <t>Blanket sales order document page</t>
   </si>
   <si>
-    <t>Configuration template (customer) with lookup value</t>
-  </si>
-  <si>
     <t>Released sales order with lookup value and with line with require shipment location</t>
   </si>
   <si>
@@ -502,9 +490,6 @@
   </si>
   <si>
     <t>Inheritance - Contact</t>
-  </si>
-  <si>
-    <t>Inheritance - Customer / Configuration Templates</t>
   </si>
   <si>
     <t>Inheritance - Warehouse Shipment</t>
@@ -639,6 +624,18 @@
   </si>
   <si>
     <t>Non-restrictive base permissions extended with Lookup Value permissions</t>
+  </si>
+  <si>
+    <t>Inheritance - Customer Templates</t>
+  </si>
+  <si>
+    <t>Create customer from customer template with lookup value</t>
+  </si>
+  <si>
+    <t>Create customer card</t>
+  </si>
+  <si>
+    <t>Lookup value on customer is populated with lookup value of customer template</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M240"/>
+  <dimension ref="A1:M241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H221" sqref="H221"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1522,7 +1519,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -1541,7 +1538,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="8" t="str">
@@ -1603,7 +1600,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I4" s="14">
         <v>1</v>
@@ -1756,7 +1753,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I9" s="14">
         <v>2</v>
@@ -1788,7 +1785,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I10" s="14">
         <v>2</v>
@@ -1918,7 +1915,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I14" s="14">
         <v>3</v>
@@ -1950,7 +1947,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I15" s="14">
         <v>3</v>
@@ -2045,7 +2042,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
       <c r="H18" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="18" t="str">
@@ -2105,7 +2102,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I20" s="14">
         <v>4</v>
@@ -2134,7 +2131,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I21" s="14">
         <v>4</v>
@@ -2258,7 +2255,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I25" s="14">
         <v>5</v>
@@ -2290,7 +2287,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I26" s="14">
         <v>5</v>
@@ -2425,7 +2422,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I30" s="14">
         <v>6</v>
@@ -2460,7 +2457,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I31" s="14">
         <v>6</v>
@@ -2601,7 +2598,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I35" s="14">
         <v>7</v>
@@ -2636,7 +2633,7 @@
         <v>15</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I36" s="14">
         <v>7</v>
@@ -2777,7 +2774,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I40" s="14">
         <v>8</v>
@@ -2812,7 +2809,7 @@
         <v>15</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I41" s="14">
         <v>8</v>
@@ -2953,7 +2950,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I45" s="14">
         <v>9</v>
@@ -2988,7 +2985,7 @@
         <v>15</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I46" s="14">
         <v>9</v>
@@ -3129,7 +3126,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I50" s="14">
         <v>10</v>
@@ -3164,7 +3161,7 @@
         <v>15</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I51" s="14">
         <v>10</v>
@@ -3305,7 +3302,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I55" s="14">
         <v>11</v>
@@ -3340,7 +3337,7 @@
         <v>15</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I56" s="14">
         <v>11</v>
@@ -3441,7 +3438,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="5"/>
       <c r="H59" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="18" t="str">
@@ -3503,7 +3500,7 @@
         <v>15</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I61" s="14">
         <v>12</v>
@@ -3532,7 +3529,7 @@
         <v>15</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I62" s="14">
         <v>12</v>
@@ -3656,7 +3653,7 @@
         <v>15</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I66" s="14">
         <v>13</v>
@@ -3688,7 +3685,7 @@
         <v>15</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I67" s="14">
         <v>13</v>
@@ -3818,7 +3815,7 @@
         <v>15</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I71" s="14">
         <v>14</v>
@@ -3850,7 +3847,7 @@
         <v>15</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I72" s="14">
         <v>14</v>
@@ -3945,7 +3942,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="5"/>
       <c r="H75" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="18" t="str">
@@ -4005,7 +4002,7 @@
         <v>15</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I77" s="14">
         <v>15</v>
@@ -4034,7 +4031,7 @@
         <v>15</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I78" s="14">
         <v>15</v>
@@ -4063,7 +4060,7 @@
         <v>15</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I79" s="14">
         <v>15</v>
@@ -4092,7 +4089,7 @@
         <v>15</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I80" s="14">
         <v>15</v>
@@ -4216,7 +4213,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I84" s="14">
         <v>16</v>
@@ -4248,7 +4245,7 @@
         <v>15</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I85" s="14">
         <v>16</v>
@@ -4378,7 +4375,7 @@
         <v>15</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I89" s="14">
         <v>17</v>
@@ -4410,7 +4407,7 @@
         <v>15</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I90" s="14">
         <v>17</v>
@@ -4442,7 +4439,7 @@
         <v>15</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I91" s="14">
         <v>17</v>
@@ -4474,7 +4471,7 @@
         <v>15</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I92" s="14">
         <v>17</v>
@@ -4561,7 +4558,7 @@
         <v>65</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C95" s="20"/>
       <c r="D95" s="21"/>
@@ -4593,13 +4590,13 @@
         <v>65</v>
       </c>
       <c r="B96" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I96" s="14">
         <v>30</v>
@@ -4623,13 +4620,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I97" s="14">
         <v>30</v>
@@ -4653,13 +4650,13 @@
         <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G98" t="s">
         <v>15</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I98" s="14">
         <v>30</v>
@@ -4683,7 +4680,7 @@
         <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G99" t="s">
         <v>16</v>
@@ -4713,7 +4710,7 @@
         <v>65</v>
       </c>
       <c r="B100" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G100" t="s">
         <v>18</v>
@@ -4743,7 +4740,7 @@
         <v>65</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="21"/>
@@ -4775,13 +4772,13 @@
         <v>65</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G102" t="s">
         <v>15</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I102" s="14">
         <v>31</v>
@@ -4805,13 +4802,13 @@
         <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G103" t="s">
         <v>15</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I103" s="14">
         <v>31</v>
@@ -4835,13 +4832,13 @@
         <v>65</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G104" t="s">
         <v>15</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I104" s="14">
         <v>31</v>
@@ -4865,13 +4862,13 @@
         <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G105" t="s">
         <v>15</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I105" s="14">
         <v>31</v>
@@ -4895,13 +4892,13 @@
         <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G106" t="s">
         <v>15</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I106" s="14">
         <v>31</v>
@@ -4925,7 +4922,7 @@
         <v>65</v>
       </c>
       <c r="B107" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G107" t="s">
         <v>16</v>
@@ -4955,7 +4952,7 @@
         <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G108" t="s">
         <v>18</v>
@@ -4993,7 +4990,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="5"/>
       <c r="H109" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I109" s="9"/>
       <c r="J109" s="18" t="str">
@@ -5058,7 +5055,7 @@
         <v>15</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I111" s="14">
         <v>18</v>
@@ -5189,7 +5186,7 @@
         <v>15</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I115" s="14">
         <v>19</v>
@@ -5322,7 +5319,7 @@
         <v>15</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I119" s="14">
         <v>20</v>
@@ -5460,7 +5457,7 @@
         <v>15</v>
       </c>
       <c r="H123" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I123" s="14">
         <v>21</v>
@@ -5596,7 +5593,7 @@
       <c r="F127" s="7"/>
       <c r="G127" s="5"/>
       <c r="H127" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I127" s="9"/>
       <c r="J127" s="18" t="str">
@@ -5618,7 +5615,7 @@
         <v>65</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C128" s="20"/>
       <c r="D128" s="20"/>
@@ -5650,7 +5647,7 @@
         <v>65</v>
       </c>
       <c r="B129" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D129"/>
       <c r="E129"/>
@@ -5659,7 +5656,7 @@
         <v>15</v>
       </c>
       <c r="H129" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I129" s="28">
         <v>24</v>
@@ -5683,7 +5680,7 @@
         <v>65</v>
       </c>
       <c r="B130" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D130"/>
       <c r="E130"/>
@@ -5692,7 +5689,7 @@
         <v>15</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I130" s="28">
         <v>24</v>
@@ -5716,7 +5713,7 @@
         <v>65</v>
       </c>
       <c r="B131" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D131"/>
       <c r="E131"/>
@@ -5749,7 +5746,7 @@
         <v>65</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D132"/>
       <c r="E132"/>
@@ -5782,13 +5779,13 @@
         <v>65</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C133" s="20"/>
       <c r="D133" s="21"/>
       <c r="E133" s="21"/>
       <c r="F133" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G133" s="20"/>
       <c r="H133" s="23"/>
@@ -5814,13 +5811,13 @@
         <v>65</v>
       </c>
       <c r="B134" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G134" t="s">
         <v>15</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I134" s="14">
         <v>26</v>
@@ -5844,13 +5841,13 @@
         <v>65</v>
       </c>
       <c r="B135" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G135" t="s">
         <v>15</v>
       </c>
       <c r="H135" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I135" s="14">
         <v>26</v>
@@ -5874,13 +5871,13 @@
         <v>65</v>
       </c>
       <c r="B136" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G136" t="s">
         <v>16</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I136" s="14">
         <v>26</v>
@@ -5904,13 +5901,13 @@
         <v>65</v>
       </c>
       <c r="B137" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G137" t="s">
         <v>18</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I137" s="14">
         <v>26</v>
@@ -5934,13 +5931,13 @@
         <v>65</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
       <c r="E138" s="21"/>
       <c r="F138" s="22" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="G138" s="20"/>
       <c r="H138" s="23"/>
@@ -5949,15 +5946,15 @@
       </c>
       <c r="J138" s="20" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+        <v>[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
       <c r="K138" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+        <v>//[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
       <c r="L138" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0028 'Create customer from configuration template with lookup value' {</v>
+        <v>Scenario 0028 'Create customer from customer template with lookup value' {</v>
       </c>
       <c r="M138" s="20"/>
     </row>
@@ -5966,28 +5963,28 @@
         <v>65</v>
       </c>
       <c r="B139" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="I139" s="14">
         <v>28</v>
       </c>
       <c r="J139" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="K139" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>//[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="L139" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Configuration template (customer) with lookup value' } }</v>
+        <v>Given 'Customer template with lookup value' } }</v>
       </c>
       <c r="M139"/>
     </row>
@@ -5996,28 +5993,28 @@
         <v>65</v>
       </c>
       <c r="B140" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="G140" t="s">
         <v>16</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="I140" s="14">
         <v>28</v>
       </c>
       <c r="J140" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create customer from configuration template</v>
+        <v>[WHEN] Create customer card</v>
       </c>
       <c r="K140" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create customer from configuration template</v>
+        <v>//[WHEN] Create customer card</v>
       </c>
       <c r="L140" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create customer from configuration template' } }</v>
+        <v>When 'Create customer card' } }</v>
       </c>
       <c r="M140"/>
     </row>
@@ -6026,28 +6023,28 @@
         <v>65</v>
       </c>
       <c r="B141" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="G141" t="s">
         <v>18</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="I141" s="14">
         <v>28</v>
       </c>
       <c r="J141" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
+        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
       <c r="K141" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
+        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
       <c r="L141" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of configuration template' } }</v>
+        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
       </c>
       <c r="M141"/>
     </row>
@@ -6056,7 +6053,7 @@
         <v>65</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="6"/>
@@ -6064,7 +6061,7 @@
       <c r="F142" s="7"/>
       <c r="G142" s="5"/>
       <c r="H142" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I142" s="9"/>
       <c r="J142" s="18" t="str">
@@ -6086,7 +6083,7 @@
         <v>65</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C143" s="20" t="s">
         <v>37</v>
@@ -6094,7 +6091,7 @@
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G143" s="20"/>
       <c r="H143" s="23"/>
@@ -6120,7 +6117,7 @@
         <v>65</v>
       </c>
       <c r="B144" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C144" t="s">
         <v>37</v>
@@ -6129,7 +6126,7 @@
         <v>15</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I144" s="14">
         <v>22</v>
@@ -6152,7 +6149,7 @@
         <v>65</v>
       </c>
       <c r="B145" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C145" t="s">
         <v>37</v>
@@ -6161,7 +6158,7 @@
         <v>16</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I145" s="14">
         <v>22</v>
@@ -6184,7 +6181,7 @@
         <v>65</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C146" t="s">
         <v>37</v>
@@ -6193,7 +6190,7 @@
         <v>18</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I146" s="14">
         <v>22</v>
@@ -6216,7 +6213,7 @@
         <v>65</v>
       </c>
       <c r="B147" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C147" t="s">
         <v>37</v>
@@ -6225,7 +6222,7 @@
         <v>18</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I147" s="14">
         <v>22</v>
@@ -6248,7 +6245,7 @@
         <v>65</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C148" s="20" t="s">
         <v>37</v>
@@ -6258,7 +6255,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G148" s="20"/>
       <c r="H148" s="23"/>
@@ -6284,7 +6281,7 @@
         <v>65</v>
       </c>
       <c r="B149" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C149" t="s">
         <v>37</v>
@@ -6296,7 +6293,7 @@
         <v>15</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I149" s="14">
         <v>27</v>
@@ -6319,7 +6316,7 @@
         <v>65</v>
       </c>
       <c r="B150" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C150" t="s">
         <v>37</v>
@@ -6331,7 +6328,7 @@
         <v>16</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I150" s="14">
         <v>27</v>
@@ -6354,7 +6351,7 @@
         <v>65</v>
       </c>
       <c r="B151" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C151" t="s">
         <v>37</v>
@@ -6366,7 +6363,7 @@
         <v>18</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I151" s="14">
         <v>27</v>
@@ -6389,7 +6386,7 @@
         <v>65</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C152" s="20" t="s">
         <v>66</v>
@@ -6397,7 +6394,7 @@
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G152" s="20"/>
       <c r="H152" s="23"/>
@@ -6420,10 +6417,10 @@
     </row>
     <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B153" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C153" t="s">
         <v>66</v>
@@ -6432,7 +6429,7 @@
         <v>15</v>
       </c>
       <c r="H153" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I153" s="14">
         <v>23</v>
@@ -6452,10 +6449,10 @@
     </row>
     <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B154" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C154" t="s">
         <v>66</v>
@@ -6464,7 +6461,7 @@
         <v>15</v>
       </c>
       <c r="H154" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I154" s="14">
         <v>23</v>
@@ -6484,10 +6481,10 @@
     </row>
     <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B155" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C155" t="s">
         <v>66</v>
@@ -6496,7 +6493,7 @@
         <v>15</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I155" s="14">
         <v>23</v>
@@ -6519,7 +6516,7 @@
         <v>65</v>
       </c>
       <c r="B156" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C156" t="s">
         <v>66</v>
@@ -6528,7 +6525,7 @@
         <v>16</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I156" s="14">
         <v>23</v>
@@ -6551,7 +6548,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C157" t="s">
         <v>66</v>
@@ -6560,7 +6557,7 @@
         <v>18</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I157" s="14">
         <v>23</v>
@@ -6583,7 +6580,7 @@
         <v>65</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C158" s="20" t="s">
         <v>66</v>
@@ -6593,7 +6590,7 @@
         <v>23</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G158" s="20"/>
       <c r="H158" s="23"/>
@@ -6616,10 +6613,10 @@
     </row>
     <row r="159" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B159" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C159" t="s">
         <v>66</v>
@@ -6631,7 +6628,7 @@
         <v>15</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I159" s="14">
         <v>25</v>
@@ -6651,10 +6648,10 @@
     </row>
     <row r="160" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B160" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C160" t="s">
         <v>66</v>
@@ -6666,7 +6663,7 @@
         <v>15</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I160" s="14">
         <v>25</v>
@@ -6686,10 +6683,10 @@
     </row>
     <row r="161" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B161" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C161" t="s">
         <v>66</v>
@@ -6701,7 +6698,7 @@
         <v>15</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I161" s="14">
         <v>25</v>
@@ -6724,7 +6721,7 @@
         <v>65</v>
       </c>
       <c r="B162" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C162" t="s">
         <v>66</v>
@@ -6736,7 +6733,7 @@
         <v>16</v>
       </c>
       <c r="H162" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I162" s="14">
         <v>25</v>
@@ -6759,7 +6756,7 @@
         <v>65</v>
       </c>
       <c r="B163" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C163" t="s">
         <v>66</v>
@@ -6771,7 +6768,7 @@
         <v>18</v>
       </c>
       <c r="H163" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I163" s="14">
         <v>25</v>
@@ -6794,7 +6791,7 @@
         <v>65</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
@@ -6802,7 +6799,7 @@
       <c r="F164" s="7"/>
       <c r="G164" s="5"/>
       <c r="H164" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I164" s="9"/>
       <c r="J164" s="18" t="str">
@@ -6824,13 +6821,13 @@
         <v>65</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C165" s="20"/>
       <c r="D165" s="21"/>
       <c r="E165" s="21"/>
       <c r="F165" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G165" s="20"/>
       <c r="H165" s="23"/>
@@ -6856,13 +6853,13 @@
         <v>65</v>
       </c>
       <c r="B166" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G166" t="s">
         <v>15</v>
       </c>
       <c r="H166" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I166" s="14">
         <v>29</v>
@@ -6885,13 +6882,13 @@
         <v>65</v>
       </c>
       <c r="B167" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G167" t="s">
         <v>16</v>
       </c>
       <c r="H167" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I167" s="14">
         <v>29</v>
@@ -6914,13 +6911,13 @@
         <v>65</v>
       </c>
       <c r="B168" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G168" t="s">
         <v>18</v>
       </c>
       <c r="H168" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I168" s="14">
         <v>29</v>
@@ -6943,7 +6940,7 @@
         <v>65</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
@@ -6951,7 +6948,7 @@
       <c r="F169" s="7"/>
       <c r="G169" s="5"/>
       <c r="H169" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I169" s="9"/>
       <c r="J169" s="18" t="str">
@@ -6968,12 +6965,12 @@
       </c>
       <c r="M169" s="8"/>
     </row>
-    <row r="170" spans="1:13" ht="30.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C170" s="20"/>
       <c r="D170" s="21"/>
@@ -6981,7 +6978,7 @@
         <v>23</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G170" s="20"/>
       <c r="H170" s="23"/>
@@ -7002,12 +6999,12 @@
       </c>
       <c r="M170" s="23"/>
     </row>
-    <row r="171" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>23</v>
@@ -7016,7 +7013,7 @@
         <v>15</v>
       </c>
       <c r="H171" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I171" s="14">
         <v>41</v>
@@ -7034,12 +7031,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="172" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>65</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E172" s="11" t="s">
         <v>23</v>
@@ -7048,7 +7045,7 @@
         <v>16</v>
       </c>
       <c r="H172" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I172" s="14">
         <v>41</v>
@@ -7066,12 +7063,12 @@
         <v>When 'Create lookup value' }</v>
       </c>
     </row>
-    <row r="173" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>23</v>
@@ -7080,7 +7077,7 @@
         <v>18</v>
       </c>
       <c r="H173" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I173" s="14">
         <v>41</v>
@@ -7098,18 +7095,18 @@
         <v>Then 'Insert permissions error thrown'</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
       <c r="F174" s="22" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G174" s="20"/>
       <c r="H174" s="23"/>
@@ -7130,18 +7127,18 @@
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G175" t="s">
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I175" s="14">
         <v>42</v>
@@ -7159,18 +7156,18 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="176" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>65</v>
       </c>
       <c r="B176" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G176" t="s">
         <v>16</v>
       </c>
       <c r="H176" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I176" s="14">
         <v>42</v>
@@ -7188,18 +7185,18 @@
         <v>When 'Create lookup value' } }</v>
       </c>
     </row>
-    <row r="177" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>65</v>
       </c>
       <c r="B177" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G177" t="s">
         <v>18</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I177" s="14">
         <v>42</v>
@@ -7217,12 +7214,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C178" s="20"/>
       <c r="D178" s="21"/>
@@ -7230,7 +7227,7 @@
         <v>23</v>
       </c>
       <c r="F178" s="22" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
@@ -7251,12 +7248,12 @@
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
       <c r="B179" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>23</v>
@@ -7265,7 +7262,7 @@
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I179" s="14">
         <v>43</v>
@@ -7283,12 +7280,12 @@
         <v>Given 'Unrestricted permissions' }</v>
       </c>
     </row>
-    <row r="180" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>65</v>
       </c>
       <c r="B180" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>23</v>
@@ -7297,7 +7294,7 @@
         <v>15</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I180" s="14">
         <v>43</v>
@@ -7315,12 +7312,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="181" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>65</v>
       </c>
       <c r="B181" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>23</v>
@@ -7329,7 +7326,7 @@
         <v>15</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I181" s="14">
         <v>43</v>
@@ -7347,12 +7344,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="182" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>65</v>
       </c>
       <c r="B182" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>23</v>
@@ -7361,7 +7358,7 @@
         <v>16</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I182" s="14">
         <v>43</v>
@@ -7379,12 +7376,12 @@
         <v>When 'Read lookup value' }</v>
       </c>
     </row>
-    <row r="183" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>65</v>
       </c>
       <c r="B183" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>23</v>
@@ -7393,7 +7390,7 @@
         <v>18</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I183" s="14">
         <v>43</v>
@@ -7411,18 +7408,18 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B184" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C184" s="20"/>
       <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="22" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="23"/>
@@ -7443,18 +7440,18 @@
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
       <c r="B185" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
@@ -7472,18 +7469,18 @@
         <v>Given 'Unrestricted permissions' } }</v>
       </c>
     </row>
-    <row r="186" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
       <c r="B186" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G186" t="s">
         <v>15</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I186" s="14">
         <v>44</v>
@@ -7501,18 +7498,18 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
       <c r="B187" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G187" t="s">
         <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
@@ -7530,18 +7527,18 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="188" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G188" t="s">
         <v>16</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I188" s="14">
         <v>44</v>
@@ -7559,18 +7556,18 @@
         <v>When 'Read lookup value' } }</v>
       </c>
     </row>
-    <row r="189" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>65</v>
       </c>
       <c r="B189" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G189" t="s">
         <v>18</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I189" s="14">
         <v>44</v>
@@ -7588,12 +7585,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B190" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="21"/>
@@ -7601,7 +7598,7 @@
         <v>23</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="23"/>
@@ -7622,12 +7619,12 @@
       </c>
       <c r="M190" s="23"/>
     </row>
-    <row r="191" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
       <c r="B191" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>23</v>
@@ -7636,7 +7633,7 @@
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
@@ -7654,12 +7651,12 @@
         <v>Given 'Unrestricted permissions' }</v>
       </c>
     </row>
-    <row r="192" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>65</v>
       </c>
       <c r="B192" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E192" s="11" t="s">
         <v>23</v>
@@ -7668,7 +7665,7 @@
         <v>15</v>
       </c>
       <c r="H192" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I192" s="14">
         <v>45</v>
@@ -7686,12 +7683,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="193" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>23</v>
@@ -7700,7 +7697,7 @@
         <v>15</v>
       </c>
       <c r="H193" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I193" s="14">
         <v>45</v>
@@ -7718,12 +7715,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="194" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
       <c r="B194" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>23</v>
@@ -7732,7 +7729,7 @@
         <v>16</v>
       </c>
       <c r="H194" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I194" s="14">
         <v>45</v>
@@ -7750,12 +7747,12 @@
         <v>When 'Modify lookup value' }</v>
       </c>
     </row>
-    <row r="195" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>65</v>
       </c>
       <c r="B195" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>23</v>
@@ -7764,7 +7761,7 @@
         <v>18</v>
       </c>
       <c r="H195" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I195" s="14">
         <v>45</v>
@@ -7782,18 +7779,18 @@
         <v>Then 'Modify permissions error thrown'</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B196" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C196" s="20"/>
       <c r="D196" s="21"/>
       <c r="E196" s="21"/>
       <c r="F196" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G196" s="20"/>
       <c r="H196" s="23"/>
@@ -7814,18 +7811,18 @@
       </c>
       <c r="M196" s="23"/>
     </row>
-    <row r="197" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>65</v>
       </c>
       <c r="B197" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G197" t="s">
         <v>15</v>
       </c>
       <c r="H197" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I197" s="14">
         <v>46</v>
@@ -7843,18 +7840,18 @@
         <v>Given 'Unrestricted permissions' } }</v>
       </c>
     </row>
-    <row r="198" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
       <c r="B198" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G198" t="s">
         <v>15</v>
       </c>
       <c r="H198" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I198" s="14">
         <v>46</v>
@@ -7872,18 +7869,18 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
       <c r="B199" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G199" t="s">
         <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I199" s="14">
         <v>46</v>
@@ -7901,18 +7898,18 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="200" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
       <c r="B200" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G200" t="s">
         <v>16</v>
       </c>
       <c r="H200" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I200" s="14">
         <v>46</v>
@@ -7930,18 +7927,18 @@
         <v>When 'Modify lookup value' } }</v>
       </c>
     </row>
-    <row r="201" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
       <c r="B201" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G201" t="s">
         <v>18</v>
       </c>
       <c r="H201" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I201" s="14">
         <v>46</v>
@@ -7959,12 +7956,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C202" s="20"/>
       <c r="D202" s="21"/>
@@ -7972,7 +7969,7 @@
         <v>23</v>
       </c>
       <c r="F202" s="22" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G202" s="20"/>
       <c r="H202" s="23"/>
@@ -7993,12 +7990,12 @@
       </c>
       <c r="M202" s="23"/>
     </row>
-    <row r="203" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
       <c r="B203" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>23</v>
@@ -8007,7 +8004,7 @@
         <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I203" s="14">
         <v>47</v>
@@ -8025,12 +8022,12 @@
         <v>Given 'Unrestricted permissions' }</v>
       </c>
     </row>
-    <row r="204" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
       <c r="B204" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E204" s="11" t="s">
         <v>23</v>
@@ -8039,7 +8036,7 @@
         <v>15</v>
       </c>
       <c r="H204" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I204" s="14">
         <v>47</v>
@@ -8057,12 +8054,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="205" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
       <c r="B205" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>23</v>
@@ -8071,7 +8068,7 @@
         <v>15</v>
       </c>
       <c r="H205" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I205" s="14">
         <v>47</v>
@@ -8089,12 +8086,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="206" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>65</v>
       </c>
       <c r="B206" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>23</v>
@@ -8103,7 +8100,7 @@
         <v>16</v>
       </c>
       <c r="H206" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I206" s="14">
         <v>47</v>
@@ -8121,12 +8118,12 @@
         <v>When 'Delete lookup value' }</v>
       </c>
     </row>
-    <row r="207" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>65</v>
       </c>
       <c r="B207" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>23</v>
@@ -8135,7 +8132,7 @@
         <v>18</v>
       </c>
       <c r="H207" s="13" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I207" s="14">
         <v>47</v>
@@ -8153,18 +8150,18 @@
         <v>Then 'Delete permissions error thrown'</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B208" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C208" s="20"/>
       <c r="D208" s="21"/>
       <c r="E208" s="21"/>
       <c r="F208" s="22" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G208" s="20"/>
       <c r="H208" s="23"/>
@@ -8185,18 +8182,18 @@
       </c>
       <c r="M208" s="23"/>
     </row>
-    <row r="209" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>65</v>
       </c>
       <c r="B209" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G209" t="s">
         <v>15</v>
       </c>
       <c r="H209" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I209" s="14">
         <v>48</v>
@@ -8214,18 +8211,18 @@
         <v>Given 'Unrestricted permissions' } }</v>
       </c>
     </row>
-    <row r="210" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>65</v>
       </c>
       <c r="B210" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G210" t="s">
         <v>15</v>
       </c>
       <c r="H210" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I210" s="14">
         <v>48</v>
@@ -8243,18 +8240,18 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>65</v>
       </c>
       <c r="B211" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G211" t="s">
         <v>15</v>
       </c>
       <c r="H211" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I211" s="14">
         <v>48</v>
@@ -8272,18 +8269,18 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="212" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>65</v>
       </c>
       <c r="B212" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G212" t="s">
         <v>16</v>
       </c>
       <c r="H212" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I212" s="14">
         <v>48</v>
@@ -8301,18 +8298,18 @@
         <v>When 'Delete lookup value' } }</v>
       </c>
     </row>
-    <row r="213" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>65</v>
       </c>
       <c r="B213" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G213" t="s">
         <v>18</v>
       </c>
       <c r="H213" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I213" s="14">
         <v>48</v>
@@ -8330,12 +8327,12 @@
         <v>Then 'Lookup value does not exist'</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B214" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C214" s="20"/>
       <c r="D214" s="21" t="s">
@@ -8345,7 +8342,7 @@
         <v>23</v>
       </c>
       <c r="F214" s="22" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G214" s="20"/>
       <c r="H214" s="23"/>
@@ -8366,12 +8363,12 @@
       </c>
       <c r="M214" s="23"/>
     </row>
-    <row r="215" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>65</v>
       </c>
       <c r="B215" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D215" s="11" t="s">
         <v>23</v>
@@ -8383,7 +8380,7 @@
         <v>15</v>
       </c>
       <c r="H215" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I215" s="14">
         <v>49</v>
@@ -8401,18 +8398,18 @@
         <v>Given 'Unrestricted permissions' } }</v>
       </c>
     </row>
-    <row r="216" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>65</v>
       </c>
       <c r="B216" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G216" t="s">
         <v>15</v>
       </c>
       <c r="H216" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I216" s="14">
         <v>49</v>
@@ -8430,18 +8427,18 @@
         <v>Given 'Lookup value' } }</v>
       </c>
     </row>
-    <row r="217" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>65</v>
       </c>
       <c r="B217" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G217" t="s">
         <v>15</v>
       </c>
       <c r="H217" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I217" s="14">
         <v>49</v>
@@ -8459,12 +8456,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="218" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>65</v>
       </c>
       <c r="B218" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D218" s="11" t="s">
         <v>23</v>
@@ -8476,7 +8473,7 @@
         <v>16</v>
       </c>
       <c r="H218" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I218" s="14">
         <v>49</v>
@@ -8494,12 +8491,12 @@
         <v>When 'Open Lookup Values page' }</v>
       </c>
     </row>
-    <row r="219" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>65</v>
       </c>
       <c r="B219" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D219" s="11" t="s">
         <v>23</v>
@@ -8511,7 +8508,7 @@
         <v>18</v>
       </c>
       <c r="H219" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I219" s="14">
         <v>49</v>
@@ -8529,12 +8526,12 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B220" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C220" s="20"/>
       <c r="D220" s="21" t="s">
@@ -8542,7 +8539,7 @@
       </c>
       <c r="E220" s="21"/>
       <c r="F220" s="22" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G220" s="20"/>
       <c r="H220" s="23"/>
@@ -8563,12 +8560,12 @@
       </c>
       <c r="M220" s="23"/>
     </row>
-    <row r="221" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>65</v>
       </c>
       <c r="B221" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D221" s="11" t="s">
         <v>23</v>
@@ -8577,7 +8574,7 @@
         <v>15</v>
       </c>
       <c r="H221" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I221" s="14">
         <v>50</v>
@@ -8595,12 +8592,12 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="222" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>65</v>
       </c>
       <c r="B222" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D222" s="11" t="s">
         <v>23</v>
@@ -8609,7 +8606,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I222" s="14">
         <v>50</v>
@@ -8627,12 +8624,12 @@
         <v>Given 'Clear last error' } }</v>
       </c>
     </row>
-    <row r="223" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>65</v>
       </c>
       <c r="B223" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D223" s="11" t="s">
         <v>23</v>
@@ -8641,7 +8638,7 @@
         <v>16</v>
       </c>
       <c r="H223" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I223" s="14">
         <v>50</v>
@@ -8659,12 +8656,12 @@
         <v>When 'Open Lookup Values page' } }</v>
       </c>
     </row>
-    <row r="224" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
       <c r="B224" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D224" s="11" t="s">
         <v>23</v>
@@ -8673,7 +8670,7 @@
         <v>18</v>
       </c>
       <c r="H224" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I224" s="14">
         <v>50</v>
@@ -8691,12 +8688,12 @@
         <v>Then 'No error thrown'</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B225" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C225" s="20" t="s">
         <v>12</v>
@@ -8708,7 +8705,7 @@
         <v>23</v>
       </c>
       <c r="F225" s="22" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G225" s="20"/>
       <c r="H225" s="23"/>
@@ -8729,12 +8726,12 @@
       </c>
       <c r="M225" s="23"/>
     </row>
-    <row r="226" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>65</v>
       </c>
       <c r="B226" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C226" t="s">
         <v>12</v>
@@ -8749,7 +8746,7 @@
         <v>15</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I226" s="14">
         <v>51</v>
@@ -8767,12 +8764,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="227" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>65</v>
       </c>
       <c r="B227" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C227" t="s">
         <v>12</v>
@@ -8787,7 +8784,7 @@
         <v>16</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I227" s="14">
         <v>51</v>
@@ -8805,12 +8802,12 @@
         <v>When 'Open customer card' }</v>
       </c>
     </row>
-    <row r="228" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>65</v>
       </c>
       <c r="B228" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C228" t="s">
         <v>12</v>
@@ -8825,7 +8822,7 @@
         <v>18</v>
       </c>
       <c r="H228" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I228" s="14">
         <v>51</v>
@@ -8843,12 +8840,12 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B229" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C229" s="20" t="s">
         <v>12</v>
@@ -8858,7 +8855,7 @@
       </c>
       <c r="E229" s="21"/>
       <c r="F229" s="22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G229" s="20"/>
       <c r="H229" s="23"/>
@@ -8879,12 +8876,12 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
       <c r="B230" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C230" t="s">
         <v>12</v>
@@ -8896,7 +8893,7 @@
         <v>15</v>
       </c>
       <c r="H230" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I230" s="14">
         <v>52</v>
@@ -8914,12 +8911,12 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="231" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>65</v>
       </c>
       <c r="B231" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C231" t="s">
         <v>12</v>
@@ -8931,7 +8928,7 @@
         <v>16</v>
       </c>
       <c r="H231" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I231" s="14">
         <v>52</v>
@@ -8949,12 +8946,12 @@
         <v>When 'Open customer card' } }</v>
       </c>
     </row>
-    <row r="232" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>65</v>
       </c>
       <c r="B232" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C232" t="s">
         <v>12</v>
@@ -8966,7 +8963,7 @@
         <v>18</v>
       </c>
       <c r="H232" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I232" s="14">
         <v>52</v>
@@ -8984,12 +8981,12 @@
         <v>Then 'Lookup value field shown'</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B233" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C233" s="20" t="s">
         <v>12</v>
@@ -9001,7 +8998,7 @@
         <v>23</v>
       </c>
       <c r="F233" s="22" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G233" s="20"/>
       <c r="H233" s="23"/>
@@ -9022,12 +9019,12 @@
       </c>
       <c r="M233" s="23"/>
     </row>
-    <row r="234" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>65</v>
       </c>
       <c r="B234" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C234" t="s">
         <v>12</v>
@@ -9042,7 +9039,7 @@
         <v>15</v>
       </c>
       <c r="H234" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I234" s="14">
         <v>53</v>
@@ -9060,12 +9057,12 @@
         <v>Given 'Non-restrictive base permissions' }</v>
       </c>
     </row>
-    <row r="235" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>65</v>
       </c>
       <c r="B235" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C235" t="s">
         <v>12</v>
@@ -9080,7 +9077,7 @@
         <v>16</v>
       </c>
       <c r="H235" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I235" s="14">
         <v>53</v>
@@ -9098,12 +9095,12 @@
         <v>When 'Open customer list' }</v>
       </c>
     </row>
-    <row r="236" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>65</v>
       </c>
       <c r="B236" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C236" t="s">
         <v>12</v>
@@ -9118,7 +9115,7 @@
         <v>18</v>
       </c>
       <c r="H236" s="13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I236" s="14">
         <v>53</v>
@@ -9136,12 +9133,12 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B237" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>12</v>
@@ -9151,7 +9148,7 @@
       </c>
       <c r="E237" s="21"/>
       <c r="F237" s="22" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G237" s="20"/>
       <c r="H237" s="23"/>
@@ -9172,12 +9169,12 @@
       </c>
       <c r="M237" s="23"/>
     </row>
-    <row r="238" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>65</v>
       </c>
       <c r="B238" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C238" t="s">
         <v>12</v>
@@ -9189,7 +9186,7 @@
         <v>15</v>
       </c>
       <c r="H238" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I238" s="14">
         <v>54</v>
@@ -9207,12 +9204,12 @@
         <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
-    <row r="239" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>65</v>
       </c>
       <c r="B239" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C239" t="s">
         <v>12</v>
@@ -9224,7 +9221,7 @@
         <v>16</v>
       </c>
       <c r="H239" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I239" s="14">
         <v>54</v>
@@ -9242,12 +9239,12 @@
         <v>When 'Open customer list' } }</v>
       </c>
     </row>
-    <row r="240" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>65</v>
       </c>
       <c r="B240" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C240" t="s">
         <v>12</v>
@@ -9259,7 +9256,7 @@
         <v>18</v>
       </c>
       <c r="H240" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I240" s="14">
         <v>54</v>
@@ -9277,6 +9274,7 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
+    <row r="241" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="32">

</xml_diff>

<commit_message>
Testing permissions, - test example 9
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57347BF-8262-4195-AE87-A632CB2FFFCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A20E790-D538-40C8-B826-0437E2E36441}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="780" windowWidth="18510" windowHeight="15600" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="195">
   <si>
     <t>Feature</t>
   </si>
@@ -617,15 +617,6 @@
     <t>Lookup value does not exist</t>
   </si>
   <si>
-    <t>Unrestricted permissions</t>
-  </si>
-  <si>
-    <t>Non-restrictive base permissions</t>
-  </si>
-  <si>
-    <t>Non-restrictive base permissions extended with Lookup Value permissions</t>
-  </si>
-  <si>
     <t>Inheritance - Customer Templates</t>
   </si>
   <si>
@@ -636,6 +627,21 @@
   </si>
   <si>
     <t>Lookup value on customer is populated with lookup value of customer template</t>
+  </si>
+  <si>
+    <t>Full base permissions</t>
+  </si>
+  <si>
+    <t>Full base starting permissions</t>
+  </si>
+  <si>
+    <t>Full base starting permissions extended with Lookup Value permissions</t>
+  </si>
+  <si>
+    <t>Unrestricted starting permissions</t>
+  </si>
+  <si>
+    <t>Full base permissions extended with Lookup Value</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1471,7 @@
   <dimension ref="A1:M241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5931,13 +5937,13 @@
         <v>65</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
       <c r="E138" s="21"/>
       <c r="F138" s="22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G138" s="20"/>
       <c r="H138" s="23"/>
@@ -5963,7 +5969,7 @@
         <v>65</v>
       </c>
       <c r="B139" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
@@ -5993,13 +5999,13 @@
         <v>65</v>
       </c>
       <c r="B140" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G140" t="s">
         <v>16</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I140" s="14">
         <v>28</v>
@@ -6023,13 +6029,13 @@
         <v>65</v>
       </c>
       <c r="B141" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G141" t="s">
         <v>18</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I141" s="14">
         <v>28</v>
@@ -7013,22 +7019,22 @@
         <v>15</v>
       </c>
       <c r="H171" s="13" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I171" s="14">
         <v>41</v>
       </c>
       <c r="J171" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K171" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L171" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base starting permissions' }</v>
       </c>
     </row>
     <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7138,22 +7144,22 @@
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I175" s="14">
         <v>42</v>
       </c>
       <c r="J175" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K175" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L175" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
     <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7262,22 +7268,22 @@
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I179" s="14">
         <v>43</v>
       </c>
       <c r="J179" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K179" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L179" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
+        <v>Given 'Unrestricted starting permissions' }</v>
       </c>
     </row>
     <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7326,22 +7332,22 @@
         <v>15</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I181" s="14">
         <v>43</v>
       </c>
       <c r="J181" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K181" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L181" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base permissions' }</v>
       </c>
     </row>
     <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7451,22 +7457,22 @@
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
       </c>
       <c r="J185" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K185" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L185" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
+        <v>Given 'Unrestricted starting permissions' } }</v>
       </c>
     </row>
     <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7509,22 +7515,22 @@
         <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
       </c>
       <c r="J187" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K187" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L187" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
       </c>
     </row>
     <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7633,22 +7639,22 @@
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
       </c>
       <c r="J191" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K191" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L191" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
+        <v>Given 'Unrestricted starting permissions' }</v>
       </c>
     </row>
     <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7697,22 +7703,22 @@
         <v>15</v>
       </c>
       <c r="H193" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I193" s="14">
         <v>45</v>
       </c>
       <c r="J193" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K193" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L193" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base permissions' }</v>
       </c>
     </row>
     <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7822,22 +7828,22 @@
         <v>15</v>
       </c>
       <c r="H197" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I197" s="14">
         <v>46</v>
       </c>
       <c r="J197" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K197" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L197" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
+        <v>Given 'Unrestricted starting permissions' } }</v>
       </c>
     </row>
     <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7880,22 +7886,22 @@
         <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="I199" s="14">
         <v>46</v>
       </c>
       <c r="J199" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K199" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L199" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
       </c>
     </row>
     <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8004,22 +8010,22 @@
         <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I203" s="14">
         <v>47</v>
       </c>
       <c r="J203" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K203" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L203" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
+        <v>Given 'Unrestricted starting permissions' }</v>
       </c>
     </row>
     <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8068,22 +8074,22 @@
         <v>15</v>
       </c>
       <c r="H205" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I205" s="14">
         <v>47</v>
       </c>
       <c r="J205" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K205" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L205" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base permissions' }</v>
       </c>
     </row>
     <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8193,22 +8199,22 @@
         <v>15</v>
       </c>
       <c r="H209" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I209" s="14">
         <v>48</v>
       </c>
       <c r="J209" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K209" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L209" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
+        <v>Given 'Unrestricted starting permissions' } }</v>
       </c>
     </row>
     <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8251,22 +8257,22 @@
         <v>15</v>
       </c>
       <c r="H211" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="I211" s="14">
         <v>48</v>
       </c>
       <c r="J211" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K211" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L211" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
       </c>
     </row>
     <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8380,22 +8386,22 @@
         <v>15</v>
       </c>
       <c r="H215" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I215" s="14">
         <v>49</v>
       </c>
       <c r="J215" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K215" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L215" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
+        <v>Given 'Unrestricted starting permissions' } }</v>
       </c>
     </row>
     <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8438,22 +8444,22 @@
         <v>15</v>
       </c>
       <c r="H217" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="I217" s="14">
         <v>49</v>
       </c>
       <c r="J217" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K217" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L217" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base permissions' }</v>
       </c>
     </row>
     <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8574,22 +8580,22 @@
         <v>15</v>
       </c>
       <c r="H221" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="I221" s="14">
         <v>50</v>
       </c>
       <c r="J221" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K221" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L221" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
       </c>
     </row>
     <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8746,22 +8752,22 @@
         <v>15</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I226" s="14">
         <v>51</v>
       </c>
       <c r="J226" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K226" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L226" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base starting permissions' }</v>
       </c>
     </row>
     <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8876,7 +8882,7 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
@@ -8893,22 +8899,22 @@
         <v>15</v>
       </c>
       <c r="H230" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I230" s="14">
         <v>52</v>
       </c>
       <c r="J230" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K230" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L230" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
     <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9039,22 +9045,22 @@
         <v>15</v>
       </c>
       <c r="H234" s="13" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I234" s="14">
         <v>53</v>
       </c>
       <c r="J234" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K234" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L234" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
+        <v>Given 'Full base starting permissions' }</v>
       </c>
     </row>
     <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9169,7 +9175,7 @@
       </c>
       <c r="M237" s="23"/>
     </row>
-    <row r="238" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>65</v>
       </c>
@@ -9186,22 +9192,22 @@
         <v>15</v>
       </c>
       <c r="H238" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I238" s="14">
         <v>54</v>
       </c>
       <c r="J238" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K238" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L238" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
       </c>
     </row>
     <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Synced BC18 branch with main
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968C1E39-8E42-4DE9-9A53-1BCE87483A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28717834-BFC1-4A81-9878-40EF84417242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="196">
   <si>
     <t>Feature</t>
   </si>
@@ -324,15 +324,6 @@
     <t>Lookup value on sales document is populated with lookup value of customer</t>
   </si>
   <si>
-    <t>Create customer from configuration template with lookup value</t>
-  </si>
-  <si>
-    <t>Create customer from configuration template</t>
-  </si>
-  <si>
-    <t>Lookup value on customer is populated with lookup value of configuration template</t>
-  </si>
-  <si>
     <t>Posting</t>
   </si>
   <si>
@@ -492,9 +483,6 @@
     <t>Blanket sales order document page</t>
   </si>
   <si>
-    <t>Configuration template (customer) with lookup value</t>
-  </si>
-  <si>
     <t>Released sales order with lookup value and with line with require shipment location</t>
   </si>
   <si>
@@ -502,9 +490,6 @@
   </si>
   <si>
     <t>Inheritance - Contact</t>
-  </si>
-  <si>
-    <t>Inheritance - Customer / Configuration Templates</t>
   </si>
   <si>
     <t>Inheritance - Warehouse Shipment</t>
@@ -632,13 +617,34 @@
     <t>Lookup value does not exist</t>
   </si>
   <si>
-    <t>Unrestricted permissions</t>
-  </si>
-  <si>
-    <t>Non-restrictive base permissions</t>
-  </si>
-  <si>
-    <t>Non-restrictive base permissions extended with Lookup Value permissions</t>
+    <t>Inheritance - Customer Templates</t>
+  </si>
+  <si>
+    <t>Create customer from customer template with lookup value</t>
+  </si>
+  <si>
+    <t>Create customer card</t>
+  </si>
+  <si>
+    <t>Lookup value on customer is populated with lookup value of customer template</t>
+  </si>
+  <si>
+    <t>Full base permissions</t>
+  </si>
+  <si>
+    <t>Full base starting permissions</t>
+  </si>
+  <si>
+    <t>Full base starting permissions extended with Lookup Value permissions</t>
+  </si>
+  <si>
+    <t>Unrestricted starting permissions</t>
+  </si>
+  <si>
+    <t>Full base permissions extended with Lookup Value</t>
+  </si>
+  <si>
+    <t>NOTE: the test for the other 34 pages have not been implemented yet an issue (#6) has been recorded for that on GitHub</t>
   </si>
 </sst>
 </file>
@@ -848,69 +854,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1127,6 +1070,69 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1141,28 +1147,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M240" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:M240" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="39">
+  <autoFilter ref="A1:M241" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="36"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="33">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="31">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1465,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M240"/>
+  <dimension ref="A1:M242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H221" sqref="H221"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1507,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1522,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -1541,7 +1547,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="8" t="str">
@@ -1603,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I4" s="14">
         <v>1</v>
@@ -1756,7 +1762,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I9" s="14">
         <v>2</v>
@@ -1788,7 +1794,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I10" s="14">
         <v>2</v>
@@ -1918,7 +1924,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I14" s="14">
         <v>3</v>
@@ -1950,7 +1956,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I15" s="14">
         <v>3</v>
@@ -2045,7 +2051,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
       <c r="H18" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="18" t="str">
@@ -2105,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I20" s="14">
         <v>4</v>
@@ -2134,7 +2140,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I21" s="14">
         <v>4</v>
@@ -2258,7 +2264,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I25" s="14">
         <v>5</v>
@@ -2290,7 +2296,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I26" s="14">
         <v>5</v>
@@ -2425,7 +2431,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I30" s="14">
         <v>6</v>
@@ -2460,7 +2466,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I31" s="14">
         <v>6</v>
@@ -2601,7 +2607,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I35" s="14">
         <v>7</v>
@@ -2636,7 +2642,7 @@
         <v>15</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I36" s="14">
         <v>7</v>
@@ -2777,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I40" s="14">
         <v>8</v>
@@ -2812,7 +2818,7 @@
         <v>15</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I41" s="14">
         <v>8</v>
@@ -2953,7 +2959,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I45" s="14">
         <v>9</v>
@@ -2988,7 +2994,7 @@
         <v>15</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I46" s="14">
         <v>9</v>
@@ -3129,7 +3135,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I50" s="14">
         <v>10</v>
@@ -3164,7 +3170,7 @@
         <v>15</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I51" s="14">
         <v>10</v>
@@ -3305,7 +3311,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I55" s="14">
         <v>11</v>
@@ -3340,7 +3346,7 @@
         <v>15</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I56" s="14">
         <v>11</v>
@@ -3441,7 +3447,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="5"/>
       <c r="H59" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="18" t="str">
@@ -3503,7 +3509,7 @@
         <v>15</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I61" s="14">
         <v>12</v>
@@ -3532,7 +3538,7 @@
         <v>15</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I62" s="14">
         <v>12</v>
@@ -3656,7 +3662,7 @@
         <v>15</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I66" s="14">
         <v>13</v>
@@ -3688,7 +3694,7 @@
         <v>15</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I67" s="14">
         <v>13</v>
@@ -3818,7 +3824,7 @@
         <v>15</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I71" s="14">
         <v>14</v>
@@ -3850,7 +3856,7 @@
         <v>15</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I72" s="14">
         <v>14</v>
@@ -3945,7 +3951,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="5"/>
       <c r="H75" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="18" t="str">
@@ -4005,7 +4011,7 @@
         <v>15</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I77" s="14">
         <v>15</v>
@@ -4034,7 +4040,7 @@
         <v>15</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I78" s="14">
         <v>15</v>
@@ -4063,7 +4069,7 @@
         <v>15</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I79" s="14">
         <v>15</v>
@@ -4092,7 +4098,7 @@
         <v>15</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I80" s="14">
         <v>15</v>
@@ -4216,7 +4222,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I84" s="14">
         <v>16</v>
@@ -4248,7 +4254,7 @@
         <v>15</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I85" s="14">
         <v>16</v>
@@ -4378,7 +4384,7 @@
         <v>15</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I89" s="14">
         <v>17</v>
@@ -4410,7 +4416,7 @@
         <v>15</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I90" s="14">
         <v>17</v>
@@ -4442,7 +4448,7 @@
         <v>15</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I91" s="14">
         <v>17</v>
@@ -4474,7 +4480,7 @@
         <v>15</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I92" s="14">
         <v>17</v>
@@ -4561,7 +4567,7 @@
         <v>65</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C95" s="20"/>
       <c r="D95" s="21"/>
@@ -4593,13 +4599,13 @@
         <v>65</v>
       </c>
       <c r="B96" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I96" s="14">
         <v>30</v>
@@ -4623,13 +4629,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I97" s="14">
         <v>30</v>
@@ -4653,13 +4659,13 @@
         <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G98" t="s">
         <v>15</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I98" s="14">
         <v>30</v>
@@ -4683,7 +4689,7 @@
         <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G99" t="s">
         <v>16</v>
@@ -4713,7 +4719,7 @@
         <v>65</v>
       </c>
       <c r="B100" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G100" t="s">
         <v>18</v>
@@ -4743,7 +4749,7 @@
         <v>65</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="21"/>
@@ -4775,13 +4781,13 @@
         <v>65</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G102" t="s">
         <v>15</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I102" s="14">
         <v>31</v>
@@ -4805,13 +4811,13 @@
         <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G103" t="s">
         <v>15</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I103" s="14">
         <v>31</v>
@@ -4835,13 +4841,13 @@
         <v>65</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G104" t="s">
         <v>15</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I104" s="14">
         <v>31</v>
@@ -4865,13 +4871,13 @@
         <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G105" t="s">
         <v>15</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I105" s="14">
         <v>31</v>
@@ -4895,13 +4901,13 @@
         <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G106" t="s">
         <v>15</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I106" s="14">
         <v>31</v>
@@ -4925,7 +4931,7 @@
         <v>65</v>
       </c>
       <c r="B107" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G107" t="s">
         <v>16</v>
@@ -4955,7 +4961,7 @@
         <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G108" t="s">
         <v>18</v>
@@ -4993,7 +4999,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="5"/>
       <c r="H109" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I109" s="9"/>
       <c r="J109" s="18" t="str">
@@ -5058,7 +5064,7 @@
         <v>15</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I111" s="14">
         <v>18</v>
@@ -5189,7 +5195,7 @@
         <v>15</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I115" s="14">
         <v>19</v>
@@ -5322,7 +5328,7 @@
         <v>15</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I119" s="14">
         <v>20</v>
@@ -5460,7 +5466,7 @@
         <v>15</v>
       </c>
       <c r="H123" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I123" s="14">
         <v>21</v>
@@ -5596,7 +5602,7 @@
       <c r="F127" s="7"/>
       <c r="G127" s="5"/>
       <c r="H127" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I127" s="9"/>
       <c r="J127" s="18" t="str">
@@ -5618,7 +5624,7 @@
         <v>65</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C128" s="20"/>
       <c r="D128" s="20"/>
@@ -5650,7 +5656,7 @@
         <v>65</v>
       </c>
       <c r="B129" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D129"/>
       <c r="E129"/>
@@ -5659,7 +5665,7 @@
         <v>15</v>
       </c>
       <c r="H129" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I129" s="28">
         <v>24</v>
@@ -5683,7 +5689,7 @@
         <v>65</v>
       </c>
       <c r="B130" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D130"/>
       <c r="E130"/>
@@ -5692,7 +5698,7 @@
         <v>15</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I130" s="28">
         <v>24</v>
@@ -5716,7 +5722,7 @@
         <v>65</v>
       </c>
       <c r="B131" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D131"/>
       <c r="E131"/>
@@ -5749,7 +5755,7 @@
         <v>65</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D132"/>
       <c r="E132"/>
@@ -5782,13 +5788,13 @@
         <v>65</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C133" s="20"/>
       <c r="D133" s="21"/>
       <c r="E133" s="21"/>
       <c r="F133" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G133" s="20"/>
       <c r="H133" s="23"/>
@@ -5814,13 +5820,13 @@
         <v>65</v>
       </c>
       <c r="B134" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G134" t="s">
         <v>15</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I134" s="14">
         <v>26</v>
@@ -5844,13 +5850,13 @@
         <v>65</v>
       </c>
       <c r="B135" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G135" t="s">
         <v>15</v>
       </c>
       <c r="H135" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I135" s="14">
         <v>26</v>
@@ -5874,13 +5880,13 @@
         <v>65</v>
       </c>
       <c r="B136" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G136" t="s">
         <v>16</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I136" s="14">
         <v>26</v>
@@ -5904,13 +5910,13 @@
         <v>65</v>
       </c>
       <c r="B137" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G137" t="s">
         <v>18</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I137" s="14">
         <v>26</v>
@@ -5934,13 +5940,13 @@
         <v>65</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
       <c r="E138" s="21"/>
       <c r="F138" s="22" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="G138" s="20"/>
       <c r="H138" s="23"/>
@@ -5949,15 +5955,15 @@
       </c>
       <c r="J138" s="20" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+        <v>[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
       <c r="K138" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0028] Create customer from configuration template with lookup value</v>
+        <v>//[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
       <c r="L138" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0028 'Create customer from configuration template with lookup value' {</v>
+        <v>Scenario 0028 'Create customer from customer template with lookup value' {</v>
       </c>
       <c r="M138" s="20"/>
     </row>
@@ -5966,28 +5972,28 @@
         <v>65</v>
       </c>
       <c r="B139" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="I139" s="14">
         <v>28</v>
       </c>
       <c r="J139" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="K139" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Configuration template (customer) with lookup value</v>
+        <v>//[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="L139" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Configuration template (customer) with lookup value' } }</v>
+        <v>Given 'Customer template with lookup value' } }</v>
       </c>
       <c r="M139"/>
     </row>
@@ -5996,28 +6002,28 @@
         <v>65</v>
       </c>
       <c r="B140" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="G140" t="s">
         <v>16</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="I140" s="14">
         <v>28</v>
       </c>
       <c r="J140" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create customer from configuration template</v>
+        <v>[WHEN] Create customer card</v>
       </c>
       <c r="K140" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create customer from configuration template</v>
+        <v>//[WHEN] Create customer card</v>
       </c>
       <c r="L140" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create customer from configuration template' } }</v>
+        <v>When 'Create customer card' } }</v>
       </c>
       <c r="M140"/>
     </row>
@@ -6026,28 +6032,28 @@
         <v>65</v>
       </c>
       <c r="B141" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="G141" t="s">
         <v>18</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="I141" s="14">
         <v>28</v>
       </c>
       <c r="J141" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
+        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
       <c r="K141" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of configuration template</v>
+        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
       <c r="L141" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of configuration template' } }</v>
+        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
       </c>
       <c r="M141"/>
     </row>
@@ -6056,7 +6062,7 @@
         <v>65</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="6"/>
@@ -6064,7 +6070,7 @@
       <c r="F142" s="7"/>
       <c r="G142" s="5"/>
       <c r="H142" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I142" s="9"/>
       <c r="J142" s="18" t="str">
@@ -6086,7 +6092,7 @@
         <v>65</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C143" s="20" t="s">
         <v>37</v>
@@ -6094,7 +6100,7 @@
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G143" s="20"/>
       <c r="H143" s="23"/>
@@ -6120,7 +6126,7 @@
         <v>65</v>
       </c>
       <c r="B144" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C144" t="s">
         <v>37</v>
@@ -6129,7 +6135,7 @@
         <v>15</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I144" s="14">
         <v>22</v>
@@ -6152,7 +6158,7 @@
         <v>65</v>
       </c>
       <c r="B145" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C145" t="s">
         <v>37</v>
@@ -6161,7 +6167,7 @@
         <v>16</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I145" s="14">
         <v>22</v>
@@ -6184,7 +6190,7 @@
         <v>65</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C146" t="s">
         <v>37</v>
@@ -6193,7 +6199,7 @@
         <v>18</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I146" s="14">
         <v>22</v>
@@ -6216,7 +6222,7 @@
         <v>65</v>
       </c>
       <c r="B147" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C147" t="s">
         <v>37</v>
@@ -6225,7 +6231,7 @@
         <v>18</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I147" s="14">
         <v>22</v>
@@ -6248,7 +6254,7 @@
         <v>65</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C148" s="20" t="s">
         <v>37</v>
@@ -6258,7 +6264,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G148" s="20"/>
       <c r="H148" s="23"/>
@@ -6284,7 +6290,7 @@
         <v>65</v>
       </c>
       <c r="B149" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C149" t="s">
         <v>37</v>
@@ -6296,7 +6302,7 @@
         <v>15</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I149" s="14">
         <v>27</v>
@@ -6319,7 +6325,7 @@
         <v>65</v>
       </c>
       <c r="B150" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C150" t="s">
         <v>37</v>
@@ -6331,7 +6337,7 @@
         <v>16</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I150" s="14">
         <v>27</v>
@@ -6354,7 +6360,7 @@
         <v>65</v>
       </c>
       <c r="B151" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C151" t="s">
         <v>37</v>
@@ -6366,7 +6372,7 @@
         <v>18</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I151" s="14">
         <v>27</v>
@@ -6389,7 +6395,7 @@
         <v>65</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C152" s="20" t="s">
         <v>66</v>
@@ -6397,7 +6403,7 @@
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G152" s="20"/>
       <c r="H152" s="23"/>
@@ -6420,10 +6426,10 @@
     </row>
     <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B153" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C153" t="s">
         <v>66</v>
@@ -6432,7 +6438,7 @@
         <v>15</v>
       </c>
       <c r="H153" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I153" s="14">
         <v>23</v>
@@ -6452,10 +6458,10 @@
     </row>
     <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B154" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C154" t="s">
         <v>66</v>
@@ -6464,7 +6470,7 @@
         <v>15</v>
       </c>
       <c r="H154" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I154" s="14">
         <v>23</v>
@@ -6484,10 +6490,10 @@
     </row>
     <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B155" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C155" t="s">
         <v>66</v>
@@ -6496,7 +6502,7 @@
         <v>15</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I155" s="14">
         <v>23</v>
@@ -6519,7 +6525,7 @@
         <v>65</v>
       </c>
       <c r="B156" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C156" t="s">
         <v>66</v>
@@ -6528,7 +6534,7 @@
         <v>16</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I156" s="14">
         <v>23</v>
@@ -6551,7 +6557,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C157" t="s">
         <v>66</v>
@@ -6560,7 +6566,7 @@
         <v>18</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I157" s="14">
         <v>23</v>
@@ -6583,7 +6589,7 @@
         <v>65</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C158" s="20" t="s">
         <v>66</v>
@@ -6593,7 +6599,7 @@
         <v>23</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G158" s="20"/>
       <c r="H158" s="23"/>
@@ -6616,10 +6622,10 @@
     </row>
     <row r="159" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B159" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C159" t="s">
         <v>66</v>
@@ -6631,7 +6637,7 @@
         <v>15</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I159" s="14">
         <v>25</v>
@@ -6651,10 +6657,10 @@
     </row>
     <row r="160" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B160" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C160" t="s">
         <v>66</v>
@@ -6666,7 +6672,7 @@
         <v>15</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I160" s="14">
         <v>25</v>
@@ -6686,10 +6692,10 @@
     </row>
     <row r="161" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B161" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C161" t="s">
         <v>66</v>
@@ -6701,7 +6707,7 @@
         <v>15</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I161" s="14">
         <v>25</v>
@@ -6724,7 +6730,7 @@
         <v>65</v>
       </c>
       <c r="B162" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C162" t="s">
         <v>66</v>
@@ -6736,7 +6742,7 @@
         <v>16</v>
       </c>
       <c r="H162" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I162" s="14">
         <v>25</v>
@@ -6759,7 +6765,7 @@
         <v>65</v>
       </c>
       <c r="B163" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C163" t="s">
         <v>66</v>
@@ -6771,7 +6777,7 @@
         <v>18</v>
       </c>
       <c r="H163" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I163" s="14">
         <v>25</v>
@@ -6794,7 +6800,7 @@
         <v>65</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
@@ -6802,7 +6808,7 @@
       <c r="F164" s="7"/>
       <c r="G164" s="5"/>
       <c r="H164" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I164" s="9"/>
       <c r="J164" s="18" t="str">
@@ -6824,13 +6830,13 @@
         <v>65</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C165" s="20"/>
       <c r="D165" s="21"/>
       <c r="E165" s="21"/>
       <c r="F165" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G165" s="20"/>
       <c r="H165" s="23"/>
@@ -6856,13 +6862,13 @@
         <v>65</v>
       </c>
       <c r="B166" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G166" t="s">
         <v>15</v>
       </c>
       <c r="H166" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I166" s="14">
         <v>29</v>
@@ -6885,13 +6891,13 @@
         <v>65</v>
       </c>
       <c r="B167" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G167" t="s">
         <v>16</v>
       </c>
       <c r="H167" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I167" s="14">
         <v>29</v>
@@ -6914,13 +6920,13 @@
         <v>65</v>
       </c>
       <c r="B168" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G168" t="s">
         <v>18</v>
       </c>
       <c r="H168" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I168" s="14">
         <v>29</v>
@@ -6943,7 +6949,7 @@
         <v>65</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
@@ -6951,7 +6957,7 @@
       <c r="F169" s="7"/>
       <c r="G169" s="5"/>
       <c r="H169" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I169" s="9"/>
       <c r="J169" s="18" t="str">
@@ -6968,12 +6974,12 @@
       </c>
       <c r="M169" s="8"/>
     </row>
-    <row r="170" spans="1:13" ht="30.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C170" s="20"/>
       <c r="D170" s="21"/>
@@ -6981,7 +6987,7 @@
         <v>23</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G170" s="20"/>
       <c r="H170" s="23"/>
@@ -7002,12 +7008,12 @@
       </c>
       <c r="M170" s="23"/>
     </row>
-    <row r="171" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>23</v>
@@ -7016,30 +7022,30 @@
         <v>15</v>
       </c>
       <c r="H171" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I171" s="14">
         <v>41</v>
       </c>
       <c r="J171" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K171" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L171" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions' }</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>65</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E172" s="11" t="s">
         <v>23</v>
@@ -7048,7 +7054,7 @@
         <v>16</v>
       </c>
       <c r="H172" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I172" s="14">
         <v>41</v>
@@ -7066,12 +7072,12 @@
         <v>When 'Create lookup value' }</v>
       </c>
     </row>
-    <row r="173" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>23</v>
@@ -7080,7 +7086,7 @@
         <v>18</v>
       </c>
       <c r="H173" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I173" s="14">
         <v>41</v>
@@ -7098,18 +7104,18 @@
         <v>Then 'Insert permissions error thrown'</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
       <c r="F174" s="22" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G174" s="20"/>
       <c r="H174" s="23"/>
@@ -7130,47 +7136,47 @@
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G175" t="s">
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I175" s="14">
         <v>42</v>
       </c>
       <c r="J175" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K175" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L175" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>65</v>
       </c>
       <c r="B176" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G176" t="s">
         <v>16</v>
       </c>
       <c r="H176" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I176" s="14">
         <v>42</v>
@@ -7188,18 +7194,18 @@
         <v>When 'Create lookup value' } }</v>
       </c>
     </row>
-    <row r="177" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>65</v>
       </c>
       <c r="B177" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G177" t="s">
         <v>18</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I177" s="14">
         <v>42</v>
@@ -7217,12 +7223,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C178" s="20"/>
       <c r="D178" s="21"/>
@@ -7230,7 +7236,7 @@
         <v>23</v>
       </c>
       <c r="F178" s="22" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
@@ -7251,12 +7257,12 @@
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
       <c r="B179" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>23</v>
@@ -7265,30 +7271,30 @@
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I179" s="14">
         <v>43</v>
       </c>
       <c r="J179" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K179" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L179" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' }</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>65</v>
       </c>
       <c r="B180" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>23</v>
@@ -7297,7 +7303,7 @@
         <v>15</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I180" s="14">
         <v>43</v>
@@ -7315,12 +7321,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="181" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>65</v>
       </c>
       <c r="B181" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>23</v>
@@ -7329,30 +7335,30 @@
         <v>15</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I181" s="14">
         <v>43</v>
       </c>
       <c r="J181" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K181" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L181" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions' }</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>65</v>
       </c>
       <c r="B182" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>23</v>
@@ -7361,7 +7367,7 @@
         <v>16</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I182" s="14">
         <v>43</v>
@@ -7379,12 +7385,12 @@
         <v>When 'Read lookup value' }</v>
       </c>
     </row>
-    <row r="183" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>65</v>
       </c>
       <c r="B183" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>23</v>
@@ -7393,7 +7399,7 @@
         <v>18</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I183" s="14">
         <v>43</v>
@@ -7411,18 +7417,18 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B184" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C184" s="20"/>
       <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="22" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="23"/>
@@ -7443,47 +7449,47 @@
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
       <c r="B185" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
       </c>
       <c r="J185" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K185" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L185" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' } }</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
       <c r="B186" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G186" t="s">
         <v>15</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I186" s="14">
         <v>44</v>
@@ -7501,47 +7507,47 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
       <c r="B187" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G187" t="s">
         <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
       </c>
       <c r="J187" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K187" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L187" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G188" t="s">
         <v>16</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I188" s="14">
         <v>44</v>
@@ -7559,18 +7565,18 @@
         <v>When 'Read lookup value' } }</v>
       </c>
     </row>
-    <row r="189" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>65</v>
       </c>
       <c r="B189" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G189" t="s">
         <v>18</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I189" s="14">
         <v>44</v>
@@ -7588,12 +7594,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B190" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="21"/>
@@ -7601,7 +7607,7 @@
         <v>23</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="23"/>
@@ -7622,12 +7628,12 @@
       </c>
       <c r="M190" s="23"/>
     </row>
-    <row r="191" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
       <c r="B191" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>23</v>
@@ -7636,30 +7642,30 @@
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
       </c>
       <c r="J191" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K191" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L191" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' }</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>65</v>
       </c>
       <c r="B192" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E192" s="11" t="s">
         <v>23</v>
@@ -7668,7 +7674,7 @@
         <v>15</v>
       </c>
       <c r="H192" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I192" s="14">
         <v>45</v>
@@ -7686,12 +7692,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="193" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>23</v>
@@ -7700,30 +7706,30 @@
         <v>15</v>
       </c>
       <c r="H193" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I193" s="14">
         <v>45</v>
       </c>
       <c r="J193" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K193" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L193" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="194" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions' }</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
       <c r="B194" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>23</v>
@@ -7732,7 +7738,7 @@
         <v>16</v>
       </c>
       <c r="H194" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I194" s="14">
         <v>45</v>
@@ -7750,12 +7756,12 @@
         <v>When 'Modify lookup value' }</v>
       </c>
     </row>
-    <row r="195" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>65</v>
       </c>
       <c r="B195" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>23</v>
@@ -7764,7 +7770,7 @@
         <v>18</v>
       </c>
       <c r="H195" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I195" s="14">
         <v>45</v>
@@ -7782,18 +7788,18 @@
         <v>Then 'Modify permissions error thrown'</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B196" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C196" s="20"/>
       <c r="D196" s="21"/>
       <c r="E196" s="21"/>
       <c r="F196" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G196" s="20"/>
       <c r="H196" s="23"/>
@@ -7814,47 +7820,47 @@
       </c>
       <c r="M196" s="23"/>
     </row>
-    <row r="197" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>65</v>
       </c>
       <c r="B197" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G197" t="s">
         <v>15</v>
       </c>
       <c r="H197" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I197" s="14">
         <v>46</v>
       </c>
       <c r="J197" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K197" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L197" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' } }</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
       <c r="B198" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G198" t="s">
         <v>15</v>
       </c>
       <c r="H198" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I198" s="14">
         <v>46</v>
@@ -7872,47 +7878,47 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
       <c r="B199" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G199" t="s">
         <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I199" s="14">
         <v>46</v>
       </c>
       <c r="J199" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K199" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L199" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="200" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
       <c r="B200" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G200" t="s">
         <v>16</v>
       </c>
       <c r="H200" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I200" s="14">
         <v>46</v>
@@ -7930,18 +7936,18 @@
         <v>When 'Modify lookup value' } }</v>
       </c>
     </row>
-    <row r="201" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
       <c r="B201" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G201" t="s">
         <v>18</v>
       </c>
       <c r="H201" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I201" s="14">
         <v>46</v>
@@ -7959,12 +7965,12 @@
         <v>Then 'Lookup value exists'</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C202" s="20"/>
       <c r="D202" s="21"/>
@@ -7972,7 +7978,7 @@
         <v>23</v>
       </c>
       <c r="F202" s="22" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G202" s="20"/>
       <c r="H202" s="23"/>
@@ -7993,12 +7999,12 @@
       </c>
       <c r="M202" s="23"/>
     </row>
-    <row r="203" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
       <c r="B203" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>23</v>
@@ -8007,30 +8013,30 @@
         <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I203" s="14">
         <v>47</v>
       </c>
       <c r="J203" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K203" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L203" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' }</v>
-      </c>
-    </row>
-    <row r="204" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' }</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
       <c r="B204" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E204" s="11" t="s">
         <v>23</v>
@@ -8039,7 +8045,7 @@
         <v>15</v>
       </c>
       <c r="H204" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I204" s="14">
         <v>47</v>
@@ -8057,12 +8063,12 @@
         <v>Given 'Lookup Value' }</v>
       </c>
     </row>
-    <row r="205" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
       <c r="B205" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>23</v>
@@ -8071,30 +8077,30 @@
         <v>15</v>
       </c>
       <c r="H205" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I205" s="14">
         <v>47</v>
       </c>
       <c r="J205" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K205" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L205" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="206" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions' }</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>65</v>
       </c>
       <c r="B206" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>23</v>
@@ -8103,7 +8109,7 @@
         <v>16</v>
       </c>
       <c r="H206" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I206" s="14">
         <v>47</v>
@@ -8121,12 +8127,12 @@
         <v>When 'Delete lookup value' }</v>
       </c>
     </row>
-    <row r="207" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>65</v>
       </c>
       <c r="B207" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>23</v>
@@ -8135,7 +8141,7 @@
         <v>18</v>
       </c>
       <c r="H207" s="13" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I207" s="14">
         <v>47</v>
@@ -8153,18 +8159,18 @@
         <v>Then 'Delete permissions error thrown'</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B208" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C208" s="20"/>
       <c r="D208" s="21"/>
       <c r="E208" s="21"/>
       <c r="F208" s="22" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G208" s="20"/>
       <c r="H208" s="23"/>
@@ -8185,47 +8191,47 @@
       </c>
       <c r="M208" s="23"/>
     </row>
-    <row r="209" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>65</v>
       </c>
       <c r="B209" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G209" t="s">
         <v>15</v>
       </c>
       <c r="H209" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I209" s="14">
         <v>48</v>
       </c>
       <c r="J209" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K209" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L209" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="210" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' } }</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>65</v>
       </c>
       <c r="B210" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G210" t="s">
         <v>15</v>
       </c>
       <c r="H210" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I210" s="14">
         <v>48</v>
@@ -8243,47 +8249,47 @@
         <v>Given 'Lookup Value' } }</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>65</v>
       </c>
       <c r="B211" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G211" t="s">
         <v>15</v>
       </c>
       <c r="H211" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I211" s="14">
         <v>48</v>
       </c>
       <c r="J211" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K211" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L211" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="212" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>65</v>
       </c>
       <c r="B212" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G212" t="s">
         <v>16</v>
       </c>
       <c r="H212" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I212" s="14">
         <v>48</v>
@@ -8301,18 +8307,18 @@
         <v>When 'Delete lookup value' } }</v>
       </c>
     </row>
-    <row r="213" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>65</v>
       </c>
       <c r="B213" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G213" t="s">
         <v>18</v>
       </c>
       <c r="H213" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I213" s="14">
         <v>48</v>
@@ -8330,12 +8336,12 @@
         <v>Then 'Lookup value does not exist'</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B214" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C214" s="20"/>
       <c r="D214" s="21" t="s">
@@ -8345,7 +8351,7 @@
         <v>23</v>
       </c>
       <c r="F214" s="22" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G214" s="20"/>
       <c r="H214" s="23"/>
@@ -8366,12 +8372,12 @@
       </c>
       <c r="M214" s="23"/>
     </row>
-    <row r="215" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>65</v>
       </c>
       <c r="B215" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D215" s="11" t="s">
         <v>23</v>
@@ -8383,36 +8389,36 @@
         <v>15</v>
       </c>
       <c r="H215" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I215" s="14">
         <v>49</v>
       </c>
       <c r="J215" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted permissions</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K215" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted permissions</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L215" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted permissions' } }</v>
-      </c>
-    </row>
-    <row r="216" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Unrestricted starting permissions' } }</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>65</v>
       </c>
       <c r="B216" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G216" t="s">
         <v>15</v>
       </c>
       <c r="H216" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I216" s="14">
         <v>49</v>
@@ -8430,41 +8436,41 @@
         <v>Given 'Lookup value' } }</v>
       </c>
     </row>
-    <row r="217" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>65</v>
       </c>
       <c r="B217" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G217" t="s">
         <v>15</v>
       </c>
       <c r="H217" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I217" s="14">
         <v>49</v>
       </c>
       <c r="J217" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K217" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L217" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="218" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions' }</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>65</v>
       </c>
       <c r="B218" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D218" s="11" t="s">
         <v>23</v>
@@ -8476,7 +8482,7 @@
         <v>16</v>
       </c>
       <c r="H218" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I218" s="14">
         <v>49</v>
@@ -8494,12 +8500,12 @@
         <v>When 'Open Lookup Values page' }</v>
       </c>
     </row>
-    <row r="219" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>65</v>
       </c>
       <c r="B219" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D219" s="11" t="s">
         <v>23</v>
@@ -8511,7 +8517,7 @@
         <v>18</v>
       </c>
       <c r="H219" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I219" s="14">
         <v>49</v>
@@ -8529,12 +8535,12 @@
         <v>Then 'Read permissions error thrown'</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B220" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C220" s="20"/>
       <c r="D220" s="21" t="s">
@@ -8542,7 +8548,7 @@
       </c>
       <c r="E220" s="21"/>
       <c r="F220" s="22" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G220" s="20"/>
       <c r="H220" s="23"/>
@@ -8563,12 +8569,12 @@
       </c>
       <c r="M220" s="23"/>
     </row>
-    <row r="221" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>65</v>
       </c>
       <c r="B221" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D221" s="11" t="s">
         <v>23</v>
@@ -8577,30 +8583,30 @@
         <v>15</v>
       </c>
       <c r="H221" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I221" s="14">
         <v>50</v>
       </c>
       <c r="J221" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K221" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L221" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="222" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>65</v>
       </c>
       <c r="B222" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D222" s="11" t="s">
         <v>23</v>
@@ -8609,7 +8615,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I222" s="14">
         <v>50</v>
@@ -8627,12 +8633,12 @@
         <v>Given 'Clear last error' } }</v>
       </c>
     </row>
-    <row r="223" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>65</v>
       </c>
       <c r="B223" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D223" s="11" t="s">
         <v>23</v>
@@ -8641,7 +8647,7 @@
         <v>16</v>
       </c>
       <c r="H223" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I223" s="14">
         <v>50</v>
@@ -8659,12 +8665,12 @@
         <v>When 'Open Lookup Values page' } }</v>
       </c>
     </row>
-    <row r="224" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
       <c r="B224" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D224" s="11" t="s">
         <v>23</v>
@@ -8673,7 +8679,7 @@
         <v>18</v>
       </c>
       <c r="H224" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I224" s="14">
         <v>50</v>
@@ -8691,12 +8697,12 @@
         <v>Then 'No error thrown'</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B225" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C225" s="20" t="s">
         <v>12</v>
@@ -8708,7 +8714,7 @@
         <v>23</v>
       </c>
       <c r="F225" s="22" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G225" s="20"/>
       <c r="H225" s="23"/>
@@ -8729,12 +8735,12 @@
       </c>
       <c r="M225" s="23"/>
     </row>
-    <row r="226" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>65</v>
       </c>
       <c r="B226" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C226" t="s">
         <v>12</v>
@@ -8749,30 +8755,30 @@
         <v>15</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I226" s="14">
         <v>51</v>
       </c>
       <c r="J226" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K226" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L226" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="227" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions' }</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>65</v>
       </c>
       <c r="B227" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C227" t="s">
         <v>12</v>
@@ -8787,7 +8793,7 @@
         <v>16</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I227" s="14">
         <v>51</v>
@@ -8805,12 +8811,12 @@
         <v>When 'Open customer card' }</v>
       </c>
     </row>
-    <row r="228" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>65</v>
       </c>
       <c r="B228" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C228" t="s">
         <v>12</v>
@@ -8825,7 +8831,7 @@
         <v>18</v>
       </c>
       <c r="H228" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I228" s="14">
         <v>51</v>
@@ -8843,12 +8849,12 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B229" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C229" s="20" t="s">
         <v>12</v>
@@ -8858,7 +8864,7 @@
       </c>
       <c r="E229" s="21"/>
       <c r="F229" s="22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G229" s="20"/>
       <c r="H229" s="23"/>
@@ -8879,12 +8885,12 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
       <c r="B230" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C230" t="s">
         <v>12</v>
@@ -8896,30 +8902,30 @@
         <v>15</v>
       </c>
       <c r="H230" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I230" s="14">
         <v>52</v>
       </c>
       <c r="J230" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K230" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L230" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="231" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>65</v>
       </c>
       <c r="B231" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C231" t="s">
         <v>12</v>
@@ -8931,7 +8937,7 @@
         <v>16</v>
       </c>
       <c r="H231" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I231" s="14">
         <v>52</v>
@@ -8949,12 +8955,12 @@
         <v>When 'Open customer card' } }</v>
       </c>
     </row>
-    <row r="232" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>65</v>
       </c>
       <c r="B232" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C232" t="s">
         <v>12</v>
@@ -8966,7 +8972,7 @@
         <v>18</v>
       </c>
       <c r="H232" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I232" s="14">
         <v>52</v>
@@ -8984,12 +8990,12 @@
         <v>Then 'Lookup value field shown'</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B233" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C233" s="20" t="s">
         <v>12</v>
@@ -9001,7 +9007,7 @@
         <v>23</v>
       </c>
       <c r="F233" s="22" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G233" s="20"/>
       <c r="H233" s="23"/>
@@ -9022,12 +9028,12 @@
       </c>
       <c r="M233" s="23"/>
     </row>
-    <row r="234" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>65</v>
       </c>
       <c r="B234" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C234" t="s">
         <v>12</v>
@@ -9042,30 +9048,30 @@
         <v>15</v>
       </c>
       <c r="H234" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I234" s="14">
         <v>53</v>
       </c>
       <c r="J234" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K234" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L234" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions' }</v>
-      </c>
-    </row>
-    <row r="235" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions' }</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>65</v>
       </c>
       <c r="B235" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C235" t="s">
         <v>12</v>
@@ -9080,7 +9086,7 @@
         <v>16</v>
       </c>
       <c r="H235" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I235" s="14">
         <v>53</v>
@@ -9098,12 +9104,12 @@
         <v>When 'Open customer list' }</v>
       </c>
     </row>
-    <row r="236" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>65</v>
       </c>
       <c r="B236" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C236" t="s">
         <v>12</v>
@@ -9118,7 +9124,7 @@
         <v>18</v>
       </c>
       <c r="H236" s="13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I236" s="14">
         <v>53</v>
@@ -9136,12 +9142,12 @@
         <v>Then 'Lookup value field not shown'</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B237" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>12</v>
@@ -9151,7 +9157,7 @@
       </c>
       <c r="E237" s="21"/>
       <c r="F237" s="22" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G237" s="20"/>
       <c r="H237" s="23"/>
@@ -9172,12 +9178,12 @@
       </c>
       <c r="M237" s="23"/>
     </row>
-    <row r="238" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>65</v>
       </c>
       <c r="B238" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C238" t="s">
         <v>12</v>
@@ -9189,30 +9195,30 @@
         <v>15</v>
       </c>
       <c r="H238" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I238" s="14">
         <v>54</v>
       </c>
       <c r="J238" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K238" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-restrictive base permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L238" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-restrictive base permissions extended with Lookup Value permissions' } }</v>
-      </c>
-    </row>
-    <row r="239" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>65</v>
       </c>
       <c r="B239" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C239" t="s">
         <v>12</v>
@@ -9224,7 +9230,7 @@
         <v>16</v>
       </c>
       <c r="H239" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I239" s="14">
         <v>54</v>
@@ -9242,12 +9248,12 @@
         <v>When 'Open customer list' } }</v>
       </c>
     </row>
-    <row r="240" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>65</v>
       </c>
       <c r="B240" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C240" t="s">
         <v>12</v>
@@ -9259,7 +9265,7 @@
         <v>18</v>
       </c>
       <c r="H240" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I240" s="14">
         <v>54</v>
@@ -9277,6 +9283,24 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
+    <row r="241" spans="3:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C241" t="s">
+        <v>195</v>
+      </c>
+      <c r="J241" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[FEATURE]  </v>
+      </c>
+      <c r="K241" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[FEATURE]  </v>
+      </c>
+      <c r="L241" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="242" spans="3:12" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="32">
@@ -9291,116 +9315,116 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="38" priority="29">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G184 G189:G190 G196 G213:G1048576">
-    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:G188">
-    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:G195">
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:G199">
-    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G200">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:G202 G206:G208">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203:G205">
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:G211">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added ATDD.TestScriptor .ps1 files
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28717834-BFC1-4A81-9878-40EF84417242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4732D5B-8C1B-47B5-BA37-6AFF3B91D908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -854,6 +854,69 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1070,69 +1133,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1147,28 +1147,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:M241" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="31">
-      <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1473,9 +1473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:M242"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1559,7 +1557,7 @@
         <v>//[FEATURE] LookupValue UT Customer</v>
       </c>
       <c r="L2" s="30" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue UT Customer' {</v>
       </c>
       <c r="M2" s="8"/>
@@ -1591,7 +1589,7 @@
         <v>//[SCENARIO #0001] Assign lookup value to customer</v>
       </c>
       <c r="L3" s="37" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0001 'Assign lookup value to customer' {</v>
       </c>
       <c r="M3" s="23" t="s">
@@ -1623,8 +1621,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L4" s="29" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="5" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1652,8 +1650,8 @@
         <v>//[GIVEN] Customer</v>
       </c>
       <c r="L5" s="29" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer'</v>
       </c>
     </row>
     <row r="6" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1681,8 +1679,8 @@
         <v>//[WHEN] Set lookup value on customer</v>
       </c>
       <c r="L6" s="29" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on customer' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on customer'</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1710,8 +1708,8 @@
         <v>//[THEN] Customer has lookup value code field populated</v>
       </c>
       <c r="L7" s="29" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1743,7 +1741,7 @@
         <v>//[SCENARIO #0002] Assign non-existing lookup value to customer</v>
       </c>
       <c r="L8" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0002 'Assign non-existing lookup value to customer' {</v>
       </c>
       <c r="M8" s="23"/>
@@ -1776,8 +1774,8 @@
         <v>//[GIVEN] Non-existing lookup value</v>
       </c>
       <c r="L9" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-existing lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
     <row r="10" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1808,8 +1806,8 @@
         <v>//[GIVEN] Customer record variable</v>
       </c>
       <c r="L10" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer record variable' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer record variable'</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1840,8 +1838,8 @@
         <v>//[WHEN] Set non-existing lookup value on customer</v>
       </c>
       <c r="L11" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set non-existing lookup value on customer' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set non-existing lookup value on customer'</v>
       </c>
     </row>
     <row r="12" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1872,8 +1870,8 @@
         <v>//[THEN] Non existing lookup value error thrown</v>
       </c>
       <c r="L12" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Non existing lookup value error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non existing lookup value error thrown' }</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1905,7 +1903,7 @@
         <v>//[SCENARIO #0003] Assign lookup value on customer card</v>
       </c>
       <c r="L13" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0003 'Assign lookup value on customer card' {</v>
       </c>
       <c r="M13" s="23"/>
@@ -1938,8 +1936,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L14" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="15" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1970,8 +1968,8 @@
         <v>//[GIVEN] Customer card</v>
       </c>
       <c r="L15" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer card'</v>
       </c>
     </row>
     <row r="16" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2002,8 +2000,8 @@
         <v>//[WHEN] Set lookup value on customer card</v>
       </c>
       <c r="L16" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on customer card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on customer card'</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2034,7 +2032,7 @@
         <v>//[THEN] Customer has lookup value code field populated</v>
       </c>
       <c r="L17" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Customer has lookup value code field populated' } }</v>
       </c>
     </row>
@@ -2063,7 +2061,7 @@
         <v>//[FEATURE] LookupValue UT Sales Document</v>
       </c>
       <c r="L18" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue UT Sales Document' {</v>
       </c>
       <c r="M18" s="8"/>
@@ -2095,7 +2093,7 @@
         <v>//[SCENARIO #0004] Assign lookup value to sales header</v>
       </c>
       <c r="L19" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0004 'Assign lookup value to sales header' {</v>
       </c>
       <c r="M19" s="23"/>
@@ -2125,8 +2123,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L20" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="21" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2154,8 +2152,8 @@
         <v>//[GIVEN] Sales header</v>
       </c>
       <c r="L21" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header'</v>
       </c>
     </row>
     <row r="22" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2183,8 +2181,8 @@
         <v>//[WHEN] Set lookup value on sales header</v>
       </c>
       <c r="L22" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales header' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales header'</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2212,8 +2210,8 @@
         <v>//[THEN] Sales header has lookup value code field populated</v>
       </c>
       <c r="L23" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales header has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales header has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2245,7 +2243,7 @@
         <v>//[SCENARIO #0005] Assign non-existing lookup value on sales header</v>
       </c>
       <c r="L24" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0005 'Assign non-existing lookup value on sales header' {</v>
       </c>
       <c r="M24" s="23"/>
@@ -2278,8 +2276,8 @@
         <v>//[GIVEN] Non-existing lookup value</v>
       </c>
       <c r="L25" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-existing lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
     <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2310,8 +2308,8 @@
         <v>//[GIVEN] Sales header record variable</v>
       </c>
       <c r="L26" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header record variable' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header record variable'</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2342,8 +2340,8 @@
         <v>//[WHEN] Set non-existing lookup value to sales header</v>
       </c>
       <c r="L27" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set non-existing lookup value to sales header' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set non-existing lookup value to sales header'</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2374,8 +2372,8 @@
         <v>//[THEN] Non existing lookup value error was thrown</v>
       </c>
       <c r="L28" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Non existing lookup value error was thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2409,7 +2407,7 @@
         <v>//[SCENARIO #0006] Assign lookup value on sales quote document page</v>
       </c>
       <c r="L29" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0006 'Assign lookup value on sales quote document page' {</v>
       </c>
       <c r="M29" s="23"/>
@@ -2445,8 +2443,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L30" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="31" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2480,8 +2478,8 @@
         <v>//[GIVEN] Sales quote document page</v>
       </c>
       <c r="L31" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales quote document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales quote document page'</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2515,8 +2513,8 @@
         <v>//[WHEN] Set lookup value on sales quote document</v>
       </c>
       <c r="L32" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales quote document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales quote document'</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2550,8 +2548,8 @@
         <v>//[THEN] Sales quote has lookup value code field populated</v>
       </c>
       <c r="L33" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales quote has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales quote has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2585,7 +2583,7 @@
         <v>//[SCENARIO #0007] Assign lookup value on sales order document page</v>
       </c>
       <c r="L34" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0007 'Assign lookup value on sales order document page' {</v>
       </c>
       <c r="M34" s="23"/>
@@ -2621,8 +2619,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L35" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="36" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2656,8 +2654,8 @@
         <v>//[GIVEN] Sales order document page</v>
       </c>
       <c r="L36" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales order document page'</v>
       </c>
     </row>
     <row r="37" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2691,8 +2689,8 @@
         <v>//[WHEN] Set lookup value on sales order document</v>
       </c>
       <c r="L37" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales order document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales order document'</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2726,8 +2724,8 @@
         <v>//[THEN] Sales order has lookup value code field populated</v>
       </c>
       <c r="L38" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales order has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales order has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2761,7 +2759,7 @@
         <v>//[SCENARIO #0008] Assign lookup value on sales invoice document page</v>
       </c>
       <c r="L39" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0008 'Assign lookup value on sales invoice document page' {</v>
       </c>
       <c r="M39" s="23"/>
@@ -2797,8 +2795,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L40" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="41" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2832,8 +2830,8 @@
         <v>//[GIVEN] Sales invoice document page</v>
       </c>
       <c r="L41" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales invoice document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales invoice document page'</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2867,8 +2865,8 @@
         <v>//[WHEN] Set lookup value on sales invoice document</v>
       </c>
       <c r="L42" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales invoice document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales invoice document'</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2902,8 +2900,8 @@
         <v>//[THEN] Sales invoice has lookup value code field populated</v>
       </c>
       <c r="L43" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales invoice has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales invoice has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2937,7 +2935,7 @@
         <v>//[SCENARIO #0009] Assign lookup value on sales credit memo document page</v>
       </c>
       <c r="L44" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0009 'Assign lookup value on sales credit memo document page' {</v>
       </c>
       <c r="M44" s="23"/>
@@ -2973,8 +2971,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L45" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="46" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3008,8 +3006,8 @@
         <v>//[GIVEN] Sales credit memo document page</v>
       </c>
       <c r="L46" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales credit memo document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales credit memo document page'</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3043,8 +3041,8 @@
         <v>//[WHEN] Set lookup value on sales credit memo document</v>
       </c>
       <c r="L47" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales credit memo document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales credit memo document'</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3078,8 +3076,8 @@
         <v>//[THEN] Sales credit memo has lookup value code field populated</v>
       </c>
       <c r="L48" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales credit memo has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales credit memo has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3113,7 +3111,7 @@
         <v>//[SCENARIO #0010] Assign lookup value on sales return order document page</v>
       </c>
       <c r="L49" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0010 'Assign lookup value on sales return order document page' {</v>
       </c>
       <c r="M49" s="23"/>
@@ -3149,8 +3147,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L50" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="51" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3184,8 +3182,8 @@
         <v>//[GIVEN] Sales return order document page</v>
       </c>
       <c r="L51" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales return order document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales return order document page'</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3219,8 +3217,8 @@
         <v>//[WHEN] Set lookup value on sales return order document</v>
       </c>
       <c r="L52" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on sales return order document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on sales return order document'</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3254,8 +3252,8 @@
         <v>//[THEN] Sales return order has lookup value code field populated</v>
       </c>
       <c r="L53" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales return order has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales return order has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3289,7 +3287,7 @@
         <v>//[SCENARIO #0011] Assign lookup value on blanket sales order document page</v>
       </c>
       <c r="L54" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0011 'Assign lookup value on blanket sales order document page' {</v>
       </c>
       <c r="M54" s="23"/>
@@ -3325,8 +3323,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L55" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="56" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3360,8 +3358,8 @@
         <v>//[GIVEN] Blanket sales order document page</v>
       </c>
       <c r="L56" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Blanket sales order document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Blanket sales order document page'</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3395,8 +3393,8 @@
         <v>//[WHEN] Set lookup value on blanket sales order document</v>
       </c>
       <c r="L57" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on blanket sales order document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on blanket sales order document'</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3430,7 +3428,7 @@
         <v>//[THEN] Blanket sales order has lookup value code field populated</v>
       </c>
       <c r="L58" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Blanket sales order has lookup value code field populated' } }</v>
       </c>
     </row>
@@ -3459,7 +3457,7 @@
         <v>//[FEATURE] LookupValue UT Customer Template</v>
       </c>
       <c r="L59" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue UT Customer Template' {</v>
       </c>
       <c r="M59" s="8"/>
@@ -3491,7 +3489,7 @@
         <v>//[SCENARIO #0012] Assign lookup value to customer template</v>
       </c>
       <c r="L60" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0012 'Assign lookup value to customer template' {</v>
       </c>
       <c r="M60" s="23" t="s">
@@ -3523,8 +3521,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L61" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="62" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3552,8 +3550,8 @@
         <v>//[GIVEN] Customer template</v>
       </c>
       <c r="L62" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template'</v>
       </c>
     </row>
     <row r="63" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3581,8 +3579,8 @@
         <v>//[WHEN] Set lookup value on customer template</v>
       </c>
       <c r="L63" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on customer template' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on customer template'</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3610,8 +3608,8 @@
         <v>//[THEN] Customer template has lookup value code field populated</v>
       </c>
       <c r="L64" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer template has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer template has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3643,7 +3641,7 @@
         <v>//[SCENARIO #0013] Assign non-existing lookup value to customer template</v>
       </c>
       <c r="L65" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0013 'Assign non-existing lookup value to customer template' {</v>
       </c>
       <c r="M65" s="23"/>
@@ -3676,8 +3674,8 @@
         <v>//[GIVEN] Non-existing lookup value</v>
       </c>
       <c r="L66" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-existing lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
     <row r="67" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3708,8 +3706,8 @@
         <v>//[GIVEN] Customer template record variable</v>
       </c>
       <c r="L67" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template record variable' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template record variable'</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3740,8 +3738,8 @@
         <v>//[WHEN] Set non-existing lookup value to customer template</v>
       </c>
       <c r="L68" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set non-existing lookup value to customer template' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set non-existing lookup value to customer template'</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3772,8 +3770,8 @@
         <v>//[THEN] Non existing lookup value error was thrown</v>
       </c>
       <c r="L69" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Non existing lookup value error was thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3805,7 +3803,7 @@
         <v>//[SCENARIO #0014] Assign lookup value on customer template card</v>
       </c>
       <c r="L70" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0014 'Assign lookup value on customer template card' {</v>
       </c>
       <c r="M70" s="23"/>
@@ -3838,8 +3836,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L71" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="72" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3870,8 +3868,8 @@
         <v>//[GIVEN] Customer template card</v>
       </c>
       <c r="L72" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template card'</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3902,8 +3900,8 @@
         <v>//[WHEN] Set lookup value on customer template card</v>
       </c>
       <c r="L73" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on customer template card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on customer template card'</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3934,7 +3932,7 @@
         <v>//[THEN] Customer template has lookup value code field populated</v>
       </c>
       <c r="L74" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Customer template has lookup value code field populated' } }</v>
       </c>
     </row>
@@ -3963,7 +3961,7 @@
         <v>//[FEATURE] LookupValue Warehouse Shipment</v>
       </c>
       <c r="L75" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Warehouse Shipment' {</v>
       </c>
       <c r="M75" s="8"/>
@@ -3995,7 +3993,7 @@
         <v>//[SCENARIO #0015] Assign lookup value to warehouse shipment line</v>
       </c>
       <c r="L76" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0015 'Assign lookup value to warehouse shipment line' {</v>
       </c>
       <c r="M76" s="23"/>
@@ -4025,8 +4023,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L77" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="78" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4054,8 +4052,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L78" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
     </row>
     <row r="79" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4083,8 +4081,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L79" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4112,8 +4110,8 @@
         <v>//[GIVEN] Warehouse shipment from released sales order with line with require shipment location</v>
       </c>
       <c r="L80" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment from released sales order with line with require shipment location' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4141,8 +4139,8 @@
         <v>//[WHEN] Set lookup value on warehouse shipment line</v>
       </c>
       <c r="L81" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on warehouse shipment line' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on warehouse shipment line'</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4170,8 +4168,8 @@
         <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="L82" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4203,7 +4201,7 @@
         <v>//[SCENARIO #0016] Assign non-existing lookup value on warehouse shipment line</v>
       </c>
       <c r="L83" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0016 'Assign non-existing lookup value on warehouse shipment line' {</v>
       </c>
       <c r="M83" s="23"/>
@@ -4236,8 +4234,8 @@
         <v>//[GIVEN] Non-existing lookup value</v>
       </c>
       <c r="L84" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-existing lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
     <row r="85" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4268,8 +4266,8 @@
         <v>//[GIVEN] Warehouse shipment line record variable</v>
       </c>
       <c r="L85" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line record variable' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment line record variable'</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4300,8 +4298,8 @@
         <v>//[WHEN] Set non-existing lookup value to warehouse shipment line</v>
       </c>
       <c r="L86" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set non-existing lookup value to warehouse shipment line' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set non-existing lookup value to warehouse shipment line'</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4332,8 +4330,8 @@
         <v>//[THEN] Non existing lookup value error was thrown</v>
       </c>
       <c r="L87" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Non existing lookup value error was thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4365,7 +4363,7 @@
         <v>//[SCENARIO #0017] Assign lookup value to warehouse shipment line on warehouse shipment document page</v>
       </c>
       <c r="L88" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0017 'Assign lookup value to warehouse shipment line on warehouse shipment document page' {</v>
       </c>
       <c r="M88" s="23"/>
@@ -4398,8 +4396,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L89" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="90" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4430,8 +4428,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L90" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4462,8 +4460,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L91" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4494,8 +4492,8 @@
         <v>//[GIVEN] Warehouse shipment from released sales order with line with require shipment location</v>
       </c>
       <c r="L92" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment from released sales order with line with require shipment location' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4526,8 +4524,8 @@
         <v>//[WHEN] Set lookup value on warehouse shipment line on warehouse shipment document page</v>
       </c>
       <c r="L93" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set lookup value on warehouse shipment line on warehouse shipment document page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set lookup value on warehouse shipment line on warehouse shipment document page'</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4558,8 +4556,8 @@
         <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="L94" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4589,7 +4587,7 @@
         <v>//[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
       </c>
       <c r="L95" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0030 'Create warehouse shipment from sales order with lookup value' {</v>
       </c>
       <c r="M95" s="20"/>
@@ -4619,8 +4617,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L96" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
       <c r="M96"/>
     </row>
@@ -4649,8 +4647,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L97" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
       <c r="M97"/>
     </row>
@@ -4679,8 +4677,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L98" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
       <c r="M98"/>
     </row>
@@ -4709,8 +4707,8 @@
         <v>//[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="L99" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create warehouse shipment from released sales order with lookup value and with line with require shipment location'</v>
       </c>
       <c r="M99"/>
     </row>
@@ -4739,8 +4737,8 @@
         <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="L100" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Warehouse shipment line has lookup value code field populated'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
       <c r="M100"/>
     </row>
@@ -4771,7 +4769,7 @@
         <v>//[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
       </c>
       <c r="L101" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0031 'Get sales order with lookup value on warehouse shipment' {</v>
       </c>
       <c r="M101" s="20"/>
@@ -4801,8 +4799,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L102" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
       <c r="M102"/>
     </row>
@@ -4831,8 +4829,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L103" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
       <c r="M103"/>
     </row>
@@ -4861,8 +4859,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L104" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
       <c r="M104"/>
     </row>
@@ -4891,8 +4889,8 @@
         <v>//[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
       </c>
       <c r="L105" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Released sales order with lookup value and with line with require shipment location' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Released sales order with lookup value and with line with require shipment location'</v>
       </c>
       <c r="M105"/>
     </row>
@@ -4921,8 +4919,8 @@
         <v>//[GIVEN] Warehouse shipment without lines</v>
       </c>
       <c r="L106" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment without lines' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment without lines'</v>
       </c>
       <c r="M106"/>
     </row>
@@ -4951,8 +4949,8 @@
         <v>//[WHEN] Get sales order with lookup value on warehouse shipment</v>
       </c>
       <c r="L107" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Get sales order with lookup value on warehouse shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Get sales order with lookup value on warehouse shipment'</v>
       </c>
       <c r="M107"/>
     </row>
@@ -4981,7 +4979,7 @@
         <v>//[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
       <c r="L108" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Warehouse shipment line has lookup value code field populated' } }</v>
       </c>
       <c r="M108"/>
@@ -5011,7 +5009,7 @@
         <v>//[FEATURE] LookupValue Sales Archive</v>
       </c>
       <c r="L109" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Sales Archive' {</v>
       </c>
       <c r="M109" s="8"/>
@@ -5045,7 +5043,7 @@
         <v>//[SCENARIO #0018] Archive sales order with lookup value</v>
       </c>
       <c r="L110" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0018 'Archive sales order with lookup value' {</v>
       </c>
       <c r="M110" s="23"/>
@@ -5078,8 +5076,8 @@
         <v>//[GIVEN] Sales order with Lookup value</v>
       </c>
       <c r="L111" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
     <row r="112" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5110,8 +5108,8 @@
         <v>//[WHEN] Sales order is archived</v>
       </c>
       <c r="L112" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is archived' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales order is archived'</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5142,8 +5140,8 @@
         <v>//[THEN] Archived sales order has lookup value from sales order</v>
       </c>
       <c r="L113" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales order has lookup value from sales order'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales order has lookup value from sales order' }</v>
       </c>
       <c r="M113"/>
     </row>
@@ -5176,7 +5174,7 @@
         <v>//[SCENARIO #0019] Archive sales quote with lookup value</v>
       </c>
       <c r="L114" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0019 'Archive sales quote with lookup value' {</v>
       </c>
       <c r="M114" s="20"/>
@@ -5209,8 +5207,8 @@
         <v>//[GIVEN] Sales quote with Lookup value</v>
       </c>
       <c r="L115" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales quote with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales quote with Lookup value'</v>
       </c>
       <c r="M115"/>
     </row>
@@ -5242,8 +5240,8 @@
         <v>//[WHEN] Sales quote is archived</v>
       </c>
       <c r="L116" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales quote is archived' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales quote is archived'</v>
       </c>
       <c r="M116"/>
     </row>
@@ -5275,8 +5273,8 @@
         <v>//[THEN] Archived sales quote has lookup value from sales quote</v>
       </c>
       <c r="L117" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales quote has lookup value from sales quote'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales quote has lookup value from sales quote' }</v>
       </c>
       <c r="M117"/>
     </row>
@@ -5309,7 +5307,7 @@
         <v>//[SCENARIO #0020] Archive sales return order with lookup value</v>
       </c>
       <c r="L118" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0020 'Archive sales return order with lookup value' {</v>
       </c>
       <c r="M118" s="20"/>
@@ -5342,8 +5340,8 @@
         <v>//[GIVEN] Sales return order with Lookup value</v>
       </c>
       <c r="L119" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales return order with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales return order with Lookup value'</v>
       </c>
       <c r="M119"/>
     </row>
@@ -5375,8 +5373,8 @@
         <v>//[WHEN] Sales return order is archived</v>
       </c>
       <c r="L120" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales return order is archived' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales return order is archived'</v>
       </c>
       <c r="M120"/>
     </row>
@@ -5408,8 +5406,8 @@
         <v>//[THEN] Archived sales return order has lookup value from sales return order</v>
       </c>
       <c r="L121" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales return order has lookup value from sales return order'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales return order has lookup value from sales return order' }</v>
       </c>
       <c r="M121"/>
     </row>
@@ -5444,7 +5442,7 @@
         <v>//[SCENARIO #0021] Check that lookup value is shown right on Sales List Archive</v>
       </c>
       <c r="L122" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0021 'Check that lookup value is shown right on Sales List Archive' {</v>
       </c>
       <c r="M122" s="23"/>
@@ -5480,8 +5478,8 @@
         <v>//[GIVEN] Sales document with Lookup value</v>
       </c>
       <c r="L123" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales document with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales document with Lookup value'</v>
       </c>
     </row>
     <row r="124" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5515,8 +5513,8 @@
         <v>//[WHEN] Sales document is archived</v>
       </c>
       <c r="L124" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales document is archived' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales document is archived'</v>
       </c>
     </row>
     <row r="125" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5550,8 +5548,8 @@
         <v>//[THEN] Archived sales document has lookup value from sales document</v>
       </c>
       <c r="L125" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Archived sales document has lookup value from sales document' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Archived sales document has lookup value from sales document'</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5585,7 +5583,7 @@
         <v>//[THEN] lookup value is shown right on Sales List Archive</v>
       </c>
       <c r="L126" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'lookup value is shown right on Sales List Archive' } }</v>
       </c>
     </row>
@@ -5614,7 +5612,7 @@
         <v>//[FEATURE] LookupValue Inheritance</v>
       </c>
       <c r="L127" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Inheritance' {</v>
       </c>
       <c r="M127" s="8"/>
@@ -5646,7 +5644,7 @@
         <v>//[SCENARIO #0024] Assign customer lookup value to sales document</v>
       </c>
       <c r="L128" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0024 'Assign customer lookup value to sales document' {</v>
       </c>
       <c r="M128" s="20"/>
@@ -5679,8 +5677,8 @@
         <v>//[GIVEN] Customer with Lookup value</v>
       </c>
       <c r="L129" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with Lookup value'</v>
       </c>
       <c r="M129"/>
     </row>
@@ -5712,8 +5710,8 @@
         <v>//[GIVEN] Sales document (invoice) without Lookup value</v>
       </c>
       <c r="L130" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales document (invoice) without Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales document (invoice) without Lookup value'</v>
       </c>
       <c r="M130"/>
     </row>
@@ -5745,8 +5743,8 @@
         <v>//[WHEN] Set customer on sales header</v>
       </c>
       <c r="L131" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Set customer on sales header' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Set customer on sales header'</v>
       </c>
       <c r="M131"/>
     </row>
@@ -5778,8 +5776,8 @@
         <v>//[THEN] Lookup value on sales document is populated with lookup value of customer</v>
       </c>
       <c r="L132" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on sales document is populated with lookup value of customer'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value on sales document is populated with lookup value of customer' }</v>
       </c>
       <c r="M132"/>
     </row>
@@ -5810,7 +5808,7 @@
         <v>//[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
       </c>
       <c r="L133" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0026 'Check that lookup value is inherited from customer template to customer when creating customer from contact' {</v>
       </c>
       <c r="M133" s="20"/>
@@ -5840,8 +5838,8 @@
         <v>//[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="L134" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template with lookup value'</v>
       </c>
       <c r="M134"/>
     </row>
@@ -5870,8 +5868,8 @@
         <v>//[GIVEN] Contact</v>
       </c>
       <c r="L135" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Contact' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Contact'</v>
       </c>
       <c r="M135"/>
     </row>
@@ -5900,8 +5898,8 @@
         <v>//[WHEN] Customer is created from contact</v>
       </c>
       <c r="L136" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Customer is created from contact' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Customer is created from contact'</v>
       </c>
       <c r="M136"/>
     </row>
@@ -5930,8 +5928,8 @@
         <v>//[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
       </c>
       <c r="L137" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer has lookup value code field populated with lookup value from customer template'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer has lookup value code field populated with lookup value from customer template' }</v>
       </c>
       <c r="M137"/>
     </row>
@@ -5962,7 +5960,7 @@
         <v>//[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
       <c r="L138" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0028 'Create customer from customer template with lookup value' {</v>
       </c>
       <c r="M138" s="20"/>
@@ -5992,8 +5990,8 @@
         <v>//[GIVEN] Customer template with lookup value</v>
       </c>
       <c r="L139" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template with lookup value'</v>
       </c>
       <c r="M139"/>
     </row>
@@ -6022,8 +6020,8 @@
         <v>//[WHEN] Create customer card</v>
       </c>
       <c r="L140" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create customer card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create customer card'</v>
       </c>
       <c r="M140"/>
     </row>
@@ -6052,7 +6050,7 @@
         <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
       <c r="L141" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
       </c>
       <c r="M141"/>
@@ -6082,7 +6080,7 @@
         <v>//[FEATURE] LookupValue Posting</v>
       </c>
       <c r="L142" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Posting' {</v>
       </c>
       <c r="M142" s="8"/>
@@ -6116,7 +6114,7 @@
         <v>//[SCENARIO #0022] Check that posted sales invoice and shipment inherit lookup value from sales order</v>
       </c>
       <c r="L143" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0022 'Check that posted sales invoice and shipment inherit lookup value from sales order' {</v>
       </c>
       <c r="M143" s="23"/>
@@ -6149,8 +6147,8 @@
         <v>//[GIVEN] Sales order with Lookup value</v>
       </c>
       <c r="L144" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order with Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
     <row r="145" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6181,8 +6179,8 @@
         <v>//[WHEN] Sales order is posted (invoice &amp; ship)</v>
       </c>
       <c r="L145" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is posted (invoice &amp; ship)' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
     <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6213,8 +6211,8 @@
         <v>//[THEN] Posted sales invoice has lookup value from sales order</v>
       </c>
       <c r="L146" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posted sales invoice has lookup value from sales order' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posted sales invoice has lookup value from sales order'</v>
       </c>
     </row>
     <row r="147" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6245,8 +6243,8 @@
         <v>//[THEN] Sales shipment has lookup value from sales order</v>
       </c>
       <c r="L147" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Sales shipment has lookup value from sales order'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Sales shipment has lookup value from sales order' }</v>
       </c>
     </row>
     <row r="148" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6280,7 +6278,7 @@
         <v>//[SCENARIO #0027] Check posting throws error on sales order with empty lookup value</v>
       </c>
       <c r="L148" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0027 'Check posting throws error on sales order with empty lookup value' {</v>
       </c>
       <c r="M148" s="23"/>
@@ -6316,8 +6314,8 @@
         <v>//[GIVEN] Sales order without Lookup value</v>
       </c>
       <c r="L149" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order without Lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales order without Lookup value'</v>
       </c>
     </row>
     <row r="150" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6351,8 +6349,8 @@
         <v>//[WHEN] Sales order is posted (invoice &amp; ship)</v>
       </c>
       <c r="L150" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is posted (invoice &amp; ship)' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
     <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6386,8 +6384,8 @@
         <v>//[THEN] Missing lookup value on sales order error thrown</v>
       </c>
       <c r="L151" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Missing lookup value on sales order error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Missing lookup value on sales order error thrown' }</v>
       </c>
     </row>
     <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6419,7 +6417,7 @@
         <v>//[SCENARIO #0023] Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line</v>
       </c>
       <c r="L152" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0023 'Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line' {</v>
       </c>
       <c r="M152" s="23"/>
@@ -6452,8 +6450,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L153" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
     </row>
     <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6484,8 +6482,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L154" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
     <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6516,8 +6514,8 @@
         <v>//[GIVEN] Warehouse shipment line with Lookup value created from Sales order</v>
       </c>
       <c r="L155" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line with Lookup value created from Sales order' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment line with Lookup value created from Sales order'</v>
       </c>
     </row>
     <row r="156" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6548,8 +6546,8 @@
         <v>//[WHEN] Warehouse shipment is posted</v>
       </c>
       <c r="L156" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Warehouse shipment is posted' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Warehouse shipment is posted'</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6580,8 +6578,8 @@
         <v>//[THEN] Posted warehouse shipment line has lookup value from warehouse shipment line</v>
       </c>
       <c r="L157" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posted warehouse shipment line has lookup value from warehouse shipment line'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posted warehouse shipment line has lookup value from warehouse shipment line' }</v>
       </c>
     </row>
     <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6615,7 +6613,7 @@
         <v>//[SCENARIO #0025] Check posting throws error on sales order with empty lookup value</v>
       </c>
       <c r="L158" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0025 'Check posting throws error on sales order with empty lookup value' {</v>
       </c>
       <c r="M158" s="23"/>
@@ -6651,8 +6649,8 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
       <c r="L159" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Location with require shipment' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
       </c>
     </row>
     <row r="160" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6686,8 +6684,8 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="L160" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse employee for current user' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
     <row r="161" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6721,8 +6719,8 @@
         <v>//[GIVEN] Warehouse shipment line created from Sales order without  lookup value</v>
       </c>
       <c r="L161" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line created from Sales order without  lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment line created from Sales order without  lookup value'</v>
       </c>
     </row>
     <row r="162" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6756,8 +6754,8 @@
         <v>//[WHEN] Warehouse shipment is posted</v>
       </c>
       <c r="L162" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Warehouse shipment is posted' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Warehouse shipment is posted'</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6791,7 +6789,7 @@
         <v>//[THEN] Missing lookup value on sales order error thrown</v>
       </c>
       <c r="L163" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Missing lookup value on sales order error thrown' } }</v>
       </c>
     </row>
@@ -6820,7 +6818,7 @@
         <v>//[FEATURE] LookupValue Report</v>
       </c>
       <c r="L164" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Report' {</v>
       </c>
       <c r="M164" s="8"/>
@@ -6852,7 +6850,7 @@
         <v>//[SCENARIO #0029] Test that lookup value shows on CustomerList report</v>
       </c>
       <c r="L165" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0029 'Test that lookup value shows on CustomerList report' {</v>
       </c>
       <c r="M165" s="23"/>
@@ -6882,8 +6880,8 @@
         <v>//[GIVEN] 2 customers with different lookup value</v>
       </c>
       <c r="L166" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given '2 customers with different lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given '2 customers with different lookup value'</v>
       </c>
     </row>
     <row r="167" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6911,8 +6909,8 @@
         <v>//[WHEN] Run report CustomerList</v>
       </c>
       <c r="L167" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Run report CustomerList' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Run report CustomerList'</v>
       </c>
     </row>
     <row r="168" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6940,7 +6938,7 @@
         <v>//[THEN] Report dataset contains both customers with lookup value</v>
       </c>
       <c r="L168" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Report dataset contains both customers with lookup value' } }</v>
       </c>
     </row>
@@ -6969,7 +6967,7 @@
         <v>//[FEATURE] LookupValue Permissions</v>
       </c>
       <c r="L169" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'LookupValue Permissions' {</v>
       </c>
       <c r="M169" s="8"/>
@@ -7003,7 +7001,7 @@
         <v>//[SCENARIO #0041] Create lookup value without permissions</v>
       </c>
       <c r="L170" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0041 'Create lookup value without permissions' {</v>
       </c>
       <c r="M170" s="23"/>
@@ -7036,8 +7034,8 @@
         <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L171" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
     <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7068,8 +7066,8 @@
         <v>//[WHEN] Create lookup value</v>
       </c>
       <c r="L172" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create lookup value'</v>
       </c>
     </row>
     <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7100,8 +7098,8 @@
         <v>//[THEN] Insert permissions error thrown</v>
       </c>
       <c r="L173" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Insert permissions error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Insert permissions error thrown' }</v>
       </c>
     </row>
     <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7131,7 +7129,7 @@
         <v>//[SCENARIO #0042] Create lookup value with permissions</v>
       </c>
       <c r="L174" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0042 'Create lookup value with permissions' {</v>
       </c>
       <c r="M174" s="23"/>
@@ -7161,8 +7159,8 @@
         <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L175" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
     <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7190,8 +7188,8 @@
         <v>//[WHEN] Create lookup value</v>
       </c>
       <c r="L176" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Create lookup value'</v>
       </c>
     </row>
     <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7219,8 +7217,8 @@
         <v>//[THEN] Lookup value exists</v>
       </c>
       <c r="L177" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value exists'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7252,7 +7250,7 @@
         <v>//[SCENARIO #0043] Read lookup value without permissions</v>
       </c>
       <c r="L178" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0043 'Read lookup value without permissions' {</v>
       </c>
       <c r="M178" s="23"/>
@@ -7285,8 +7283,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L179" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7317,8 +7315,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L180" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7349,8 +7347,8 @@
         <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L181" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions'</v>
       </c>
     </row>
     <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7381,8 +7379,8 @@
         <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L182" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Read lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Read lookup value'</v>
       </c>
     </row>
     <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7413,8 +7411,8 @@
         <v>//[THEN] Read permissions error thrown</v>
       </c>
       <c r="L183" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Read permissions error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
     <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7444,7 +7442,7 @@
         <v>//[SCENARIO #0044] Read lookup value with permissions</v>
       </c>
       <c r="L184" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0044 'Read lookup value with permissions' {</v>
       </c>
       <c r="M184" s="23"/>
@@ -7474,8 +7472,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L185" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7503,8 +7501,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L186" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7532,8 +7530,8 @@
         <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L187" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
     <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7561,8 +7559,8 @@
         <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L188" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Read lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Read lookup value'</v>
       </c>
     </row>
     <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7590,8 +7588,8 @@
         <v>//[THEN] Lookup value exists</v>
       </c>
       <c r="L189" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value exists'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
     <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7623,7 +7621,7 @@
         <v>//[SCENARIO #0045] Modify lookup value without permissions</v>
       </c>
       <c r="L190" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0045 'Modify lookup value without permissions' {</v>
       </c>
       <c r="M190" s="23"/>
@@ -7656,8 +7654,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L191" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7688,8 +7686,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L192" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7720,8 +7718,8 @@
         <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L193" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions'</v>
       </c>
     </row>
     <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7752,8 +7750,8 @@
         <v>//[WHEN] Modify lookup value</v>
       </c>
       <c r="L194" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Modify lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Modify lookup value'</v>
       </c>
     </row>
     <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7784,8 +7782,8 @@
         <v>//[THEN] Modify permissions error thrown</v>
       </c>
       <c r="L195" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Modify permissions error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Modify permissions error thrown' }</v>
       </c>
     </row>
     <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7815,7 +7813,7 @@
         <v>//[SCENARIO #0046] Modify lookup value with permissions</v>
       </c>
       <c r="L196" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0046 'Modify lookup value with permissions' {</v>
       </c>
       <c r="M196" s="23"/>
@@ -7845,8 +7843,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L197" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7874,8 +7872,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L198" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7903,8 +7901,8 @@
         <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L199" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
     <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7932,8 +7930,8 @@
         <v>//[WHEN] Modify lookup value</v>
       </c>
       <c r="L200" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Modify lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Modify lookup value'</v>
       </c>
     </row>
     <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7961,8 +7959,8 @@
         <v>//[THEN] Lookup value exists</v>
       </c>
       <c r="L201" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value exists'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7994,7 +7992,7 @@
         <v>//[SCENARIO #0047] Delete lookup value without permissions</v>
       </c>
       <c r="L202" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0047 'Delete lookup value without permissions' {</v>
       </c>
       <c r="M202" s="23"/>
@@ -8027,8 +8025,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L203" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8059,8 +8057,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L204" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8091,8 +8089,8 @@
         <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L205" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions'</v>
       </c>
     </row>
     <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8123,8 +8121,8 @@
         <v>//[WHEN] Delete lookup value</v>
       </c>
       <c r="L206" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Delete lookup value' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete lookup value'</v>
       </c>
     </row>
     <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8155,8 +8153,8 @@
         <v>//[THEN] Delete permissions error thrown</v>
       </c>
       <c r="L207" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Delete permissions error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Delete permissions error thrown' }</v>
       </c>
     </row>
     <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8186,7 +8184,7 @@
         <v>//[SCENARIO #0048] Delete lookup value with permissions</v>
       </c>
       <c r="L208" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0048 'Delete lookup value with permissions' {</v>
       </c>
       <c r="M208" s="23"/>
@@ -8216,8 +8214,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L209" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8245,8 +8243,8 @@
         <v>//[GIVEN] Lookup Value</v>
       </c>
       <c r="L210" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8274,8 +8272,8 @@
         <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L211" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
     <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8303,8 +8301,8 @@
         <v>//[WHEN] Delete lookup value</v>
       </c>
       <c r="L212" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Delete lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete lookup value'</v>
       </c>
     </row>
     <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8332,8 +8330,8 @@
         <v>//[THEN] Lookup value does not exist</v>
       </c>
       <c r="L213" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value does not exist'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value does not exist' }</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8367,7 +8365,7 @@
         <v>//[SCENARIO #0049] Open Lookup Values Page without permissions</v>
       </c>
       <c r="L214" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0049 'Open Lookup Values Page without permissions' {</v>
       </c>
       <c r="M214" s="23"/>
@@ -8403,8 +8401,8 @@
         <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L215" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
     <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8432,8 +8430,8 @@
         <v>//[GIVEN] Lookup value</v>
       </c>
       <c r="L216" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value'</v>
       </c>
     </row>
     <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8461,8 +8459,8 @@
         <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L217" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions'</v>
       </c>
     </row>
     <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8496,8 +8494,8 @@
         <v>//[WHEN] Open Lookup Values page</v>
       </c>
       <c r="L218" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open Lookup Values page' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
     <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8531,8 +8529,8 @@
         <v>//[THEN] Read permissions error thrown</v>
       </c>
       <c r="L219" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Read permissions error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8564,7 +8562,7 @@
         <v>//[SCENARIO #0050] Open Lookup Values Page with permissions</v>
       </c>
       <c r="L220" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0050 'Open Lookup Values Page with permissions' {</v>
       </c>
       <c r="M220" s="23"/>
@@ -8597,8 +8595,8 @@
         <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L221" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions extended with Lookup Value' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
     <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8629,8 +8627,8 @@
         <v>//[GIVEN] Clear last error</v>
       </c>
       <c r="L222" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Clear last error' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Clear last error'</v>
       </c>
     </row>
     <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8661,8 +8659,8 @@
         <v>//[WHEN] Open Lookup Values page</v>
       </c>
       <c r="L223" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open Lookup Values page' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
     <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8693,8 +8691,8 @@
         <v>//[THEN] No error thrown</v>
       </c>
       <c r="L224" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'No error thrown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No error thrown' }</v>
       </c>
     </row>
     <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8730,7 +8728,7 @@
         <v>//[SCENARIO #0051] Check lookup value on customer card without permissions</v>
       </c>
       <c r="L225" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0051 'Check lookup value on customer card without permissions' {</v>
       </c>
       <c r="M225" s="23"/>
@@ -8769,8 +8767,8 @@
         <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L226" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
     <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8807,8 +8805,8 @@
         <v>//[WHEN] Open customer card</v>
       </c>
       <c r="L227" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer card' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card'</v>
       </c>
     </row>
     <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8845,8 +8843,8 @@
         <v>//[THEN] Lookup value field not shown</v>
       </c>
       <c r="L228" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field not shown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
     <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8880,7 +8878,7 @@
         <v>//[SCENARIO #0052] Check lookup value on customer card with permissions</v>
       </c>
       <c r="L229" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0052 'Check lookup value on customer card with permissions' {</v>
       </c>
       <c r="M229" s="23"/>
@@ -8916,8 +8914,8 @@
         <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L230" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
     <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8951,8 +8949,8 @@
         <v>//[WHEN] Open customer card</v>
       </c>
       <c r="L231" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer card' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer card'</v>
       </c>
     </row>
     <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8986,8 +8984,8 @@
         <v>//[THEN] Lookup value field shown</v>
       </c>
       <c r="L232" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field shown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field shown' }</v>
       </c>
     </row>
     <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9023,7 +9021,7 @@
         <v>//[SCENARIO #0053] Check lookup value on customer list without permissions</v>
       </c>
       <c r="L233" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0053 'Check lookup value on customer list without permissions' {</v>
       </c>
       <c r="M233" s="23"/>
@@ -9062,8 +9060,8 @@
         <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L234" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
     <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9100,8 +9098,8 @@
         <v>//[WHEN] Open customer list</v>
       </c>
       <c r="L235" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer list' }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list'</v>
       </c>
     </row>
     <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9138,8 +9136,8 @@
         <v>//[THEN] Lookup value field not shown</v>
       </c>
       <c r="L236" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value field not shown'</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
     <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9173,7 +9171,7 @@
         <v>//[SCENARIO #0054] Check lookup value on customer list with permissions</v>
       </c>
       <c r="L237" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0054 'Check lookup value on customer list with permissions' {</v>
       </c>
       <c r="M237" s="23"/>
@@ -9209,8 +9207,8 @@
         <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L238" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions extended with Lookup Value permissions' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
     <row r="239" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9244,8 +9242,8 @@
         <v>//[WHEN] Open customer list</v>
       </c>
       <c r="L239" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Open customer list' } }</v>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Open customer list'</v>
       </c>
     </row>
     <row r="240" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9279,7 +9277,7 @@
         <v>//[THEN] Lookup value field shown</v>
       </c>
       <c r="L240" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
@@ -9296,7 +9294,7 @@
         <v xml:space="preserve">//[FEATURE]  </v>
       </c>
       <c r="L241" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v/>
       </c>
     </row>
@@ -9315,116 +9313,116 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="28" priority="29">
+    <cfRule type="containsBlanks" dxfId="38" priority="29">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G184 G189:G190 G196 G213:G1048576">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:G188">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:G195">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:G199">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G200">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:G202 G206:G208">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203:G205">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:G211">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added extra groupings to enable detailed folding
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4732D5B-8C1B-47B5-BA37-6AFF3B91D908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B16254-D519-4344-9BCF-98AC3733100A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -855,6 +855,9 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -873,9 +876,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1165,10 +1165,10 @@
     <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1473,9 +1473,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:M242"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
@@ -1596,7 +1598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v>Given 'Customer'</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>When 'Set lookup value on customer'</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>Then 'Customer has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
@@ -1746,7 +1748,7 @@
       </c>
       <c r="M8" s="23"/>
     </row>
-    <row r="9" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>Given 'Customer record variable'</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1842,7 +1844,7 @@
         <v>When 'Set non-existing lookup value on customer'</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>Then 'Non existing lookup value error thrown' }</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -2098,7 +2100,7 @@
       </c>
       <c r="M19" s="23"/>
     </row>
-    <row r="20" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2127,7 +2129,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2156,7 +2158,7 @@
         <v>Given 'Sales header'</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>When 'Set lookup value on sales header'</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>Then 'Sales header has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
@@ -2248,7 +2250,7 @@
       </c>
       <c r="M24" s="23"/>
     </row>
-    <row r="25" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2280,7 +2282,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2314,7 @@
         <v>Given 'Sales header record variable'</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2344,7 +2346,7 @@
         <v>When 'Set non-existing lookup value to sales header'</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2376,7 +2378,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>11</v>
       </c>
@@ -2412,7 +2414,7 @@
       </c>
       <c r="M29" s="23"/>
     </row>
-    <row r="30" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2447,7 +2449,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>Given 'Sales quote document page'</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2517,7 +2519,7 @@
         <v>When 'Set lookup value on sales quote document'</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2552,7 +2554,7 @@
         <v>Then 'Sales quote has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
@@ -2588,7 +2590,7 @@
       </c>
       <c r="M34" s="23"/>
     </row>
-    <row r="35" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2623,7 +2625,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2658,7 +2660,7 @@
         <v>Given 'Sales order document page'</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2693,7 +2695,7 @@
         <v>When 'Set lookup value on sales order document'</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2728,7 +2730,7 @@
         <v>Then 'Sales order has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>11</v>
       </c>
@@ -2764,7 +2766,7 @@
       </c>
       <c r="M39" s="23"/>
     </row>
-    <row r="40" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2799,7 +2801,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>Given 'Sales invoice document page'</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2869,7 +2871,7 @@
         <v>When 'Set lookup value on sales invoice document'</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2904,7 +2906,7 @@
         <v>Then 'Sales invoice has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>11</v>
       </c>
@@ -2940,7 +2942,7 @@
       </c>
       <c r="M44" s="23"/>
     </row>
-    <row r="45" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2975,7 +2977,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3010,7 +3012,7 @@
         <v>Given 'Sales credit memo document page'</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>When 'Set lookup value on sales credit memo document'</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3080,7 +3082,7 @@
         <v>Then 'Sales credit memo has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>11</v>
       </c>
@@ -3116,7 +3118,7 @@
       </c>
       <c r="M49" s="23"/>
     </row>
-    <row r="50" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>Given 'Sales return order document page'</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>When 'Set lookup value on sales return order document'</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -3256,7 +3258,7 @@
         <v>Then 'Sales return order has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>11</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3525,7 +3527,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3554,7 +3556,7 @@
         <v>Given 'Customer template'</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>When 'Set lookup value on customer template'</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -3612,7 +3614,7 @@
         <v>Then 'Customer template has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>11</v>
       </c>
@@ -3646,7 +3648,7 @@
       </c>
       <c r="M65" s="23"/>
     </row>
-    <row r="66" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3678,7 +3680,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>Given 'Customer template record variable'</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>When 'Set non-existing lookup value to customer template'</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3774,7 +3776,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>11</v>
       </c>
@@ -3998,7 +4000,7 @@
       </c>
       <c r="M76" s="23"/>
     </row>
-    <row r="77" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -4027,7 +4029,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -4056,7 +4058,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -4085,7 +4087,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -4114,7 +4116,7 @@
         <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -4143,7 +4145,7 @@
         <v>When 'Set lookup value on warehouse shipment line'</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>65</v>
       </c>
@@ -4172,7 +4174,7 @@
         <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>65</v>
       </c>
@@ -4206,7 +4208,7 @@
       </c>
       <c r="M83" s="23"/>
     </row>
-    <row r="84" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>65</v>
       </c>
@@ -4238,7 +4240,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -4270,7 +4272,7 @@
         <v>Given 'Warehouse shipment line record variable'</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>65</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>When 'Set non-existing lookup value to warehouse shipment line'</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>65</v>
       </c>
@@ -4334,7 +4336,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
         <v>65</v>
       </c>
@@ -4368,7 +4370,7 @@
       </c>
       <c r="M88" s="23"/>
     </row>
-    <row r="89" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>65</v>
       </c>
@@ -4400,7 +4402,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>65</v>
       </c>
@@ -4432,7 +4434,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="16.5" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>65</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>65</v>
       </c>
@@ -4496,7 +4498,7 @@
         <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>65</v>
       </c>
@@ -4528,7 +4530,7 @@
         <v>When 'Set lookup value on warehouse shipment line on warehouse shipment document page'</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>65</v>
       </c>
@@ -4560,7 +4562,7 @@
         <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
         <v>65</v>
       </c>
@@ -4592,7 +4594,7 @@
       </c>
       <c r="M95" s="20"/>
     </row>
-    <row r="96" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>65</v>
       </c>
@@ -4622,7 +4624,7 @@
       </c>
       <c r="M96"/>
     </row>
-    <row r="97" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>65</v>
       </c>
@@ -4652,7 +4654,7 @@
       </c>
       <c r="M97"/>
     </row>
-    <row r="98" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -4682,7 +4684,7 @@
       </c>
       <c r="M98"/>
     </row>
-    <row r="99" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>65</v>
       </c>
@@ -4712,7 +4714,7 @@
       </c>
       <c r="M99"/>
     </row>
-    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>65</v>
       </c>
@@ -5048,7 +5050,7 @@
       </c>
       <c r="M110" s="23"/>
     </row>
-    <row r="111" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>65</v>
       </c>
@@ -5080,7 +5082,7 @@
         <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>65</v>
       </c>
@@ -5112,7 +5114,7 @@
         <v>When 'Sales order is archived'</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>65</v>
       </c>
@@ -5145,7 +5147,7 @@
       </c>
       <c r="M113"/>
     </row>
-    <row r="114" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="s">
         <v>65</v>
       </c>
@@ -5179,7 +5181,7 @@
       </c>
       <c r="M114" s="20"/>
     </row>
-    <row r="115" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>65</v>
       </c>
@@ -5212,7 +5214,7 @@
       </c>
       <c r="M115"/>
     </row>
-    <row r="116" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>65</v>
       </c>
@@ -5245,7 +5247,7 @@
       </c>
       <c r="M116"/>
     </row>
-    <row r="117" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>65</v>
       </c>
@@ -5278,7 +5280,7 @@
       </c>
       <c r="M117"/>
     </row>
-    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="s">
         <v>65</v>
       </c>
@@ -5312,7 +5314,7 @@
       </c>
       <c r="M118" s="20"/>
     </row>
-    <row r="119" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>65</v>
       </c>
@@ -5345,7 +5347,7 @@
       </c>
       <c r="M119"/>
     </row>
-    <row r="120" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>65</v>
       </c>
@@ -5378,7 +5380,7 @@
       </c>
       <c r="M120"/>
     </row>
-    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>65</v>
       </c>
@@ -5411,7 +5413,7 @@
       </c>
       <c r="M121"/>
     </row>
-    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
         <v>65</v>
       </c>
@@ -5649,7 +5651,7 @@
       </c>
       <c r="M128" s="20"/>
     </row>
-    <row r="129" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>65</v>
       </c>
@@ -5682,7 +5684,7 @@
       </c>
       <c r="M129"/>
     </row>
-    <row r="130" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>65</v>
       </c>
@@ -5715,7 +5717,7 @@
       </c>
       <c r="M130"/>
     </row>
-    <row r="131" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>65</v>
       </c>
@@ -5748,7 +5750,7 @@
       </c>
       <c r="M131"/>
     </row>
-    <row r="132" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>65</v>
       </c>
@@ -5781,7 +5783,7 @@
       </c>
       <c r="M132"/>
     </row>
-    <row r="133" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
         <v>65</v>
       </c>
@@ -5813,7 +5815,7 @@
       </c>
       <c r="M133" s="20"/>
     </row>
-    <row r="134" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>65</v>
       </c>
@@ -5843,7 +5845,7 @@
       </c>
       <c r="M134"/>
     </row>
-    <row r="135" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>65</v>
       </c>
@@ -5873,7 +5875,7 @@
       </c>
       <c r="M135"/>
     </row>
-    <row r="136" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>65</v>
       </c>
@@ -5903,7 +5905,7 @@
       </c>
       <c r="M136"/>
     </row>
-    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>65</v>
       </c>
@@ -5933,7 +5935,7 @@
       </c>
       <c r="M137"/>
     </row>
-    <row r="138" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="s">
         <v>65</v>
       </c>
@@ -5965,7 +5967,7 @@
       </c>
       <c r="M138" s="20"/>
     </row>
-    <row r="139" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>65</v>
       </c>
@@ -5995,7 +5997,7 @@
       </c>
       <c r="M139"/>
     </row>
-    <row r="140" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>65</v>
       </c>
@@ -6119,7 +6121,7 @@
       </c>
       <c r="M143" s="23"/>
     </row>
-    <row r="144" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>65</v>
       </c>
@@ -6151,7 +6153,7 @@
         <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>65</v>
       </c>
@@ -6183,7 +6185,7 @@
         <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>65</v>
       </c>
@@ -6215,7 +6217,7 @@
         <v>Then 'Posted sales invoice has lookup value from sales order'</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>65</v>
       </c>
@@ -6247,7 +6249,7 @@
         <v>Then 'Sales shipment has lookup value from sales order' }</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
         <v>65</v>
       </c>
@@ -6283,7 +6285,7 @@
       </c>
       <c r="M148" s="23"/>
     </row>
-    <row r="149" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>65</v>
       </c>
@@ -6318,7 +6320,7 @@
         <v>Given 'Sales order without Lookup value'</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>65</v>
       </c>
@@ -6353,7 +6355,7 @@
         <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>65</v>
       </c>
@@ -6388,7 +6390,7 @@
         <v>Then 'Missing lookup value on sales order error thrown' }</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
         <v>65</v>
       </c>
@@ -6422,7 +6424,7 @@
       </c>
       <c r="M152" s="23"/>
     </row>
-    <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>104</v>
       </c>
@@ -6454,7 +6456,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>104</v>
       </c>
@@ -6486,7 +6488,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>104</v>
       </c>
@@ -6518,7 +6520,7 @@
         <v>Given 'Warehouse shipment line with Lookup value created from Sales order'</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>65</v>
       </c>
@@ -6550,7 +6552,7 @@
         <v>When 'Warehouse shipment is posted'</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>65</v>
       </c>
@@ -6582,7 +6584,7 @@
         <v>Then 'Posted warehouse shipment line has lookup value from warehouse shipment line' }</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="s">
         <v>65</v>
       </c>
@@ -7006,7 +7008,7 @@
       </c>
       <c r="M170" s="23"/>
     </row>
-    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
@@ -7038,7 +7040,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>65</v>
       </c>
@@ -7070,7 +7072,7 @@
         <v>When 'Create lookup value'</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
@@ -7102,7 +7104,7 @@
         <v>Then 'Insert permissions error thrown' }</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
@@ -7134,7 +7136,7 @@
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
@@ -7163,7 +7165,7 @@
         <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>65</v>
       </c>
@@ -7192,7 +7194,7 @@
         <v>When 'Create lookup value'</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>65</v>
       </c>
@@ -7221,7 +7223,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
@@ -7255,7 +7257,7 @@
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
@@ -7287,7 +7289,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>65</v>
       </c>
@@ -7319,7 +7321,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>65</v>
       </c>
@@ -7351,7 +7353,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>65</v>
       </c>
@@ -7383,7 +7385,7 @@
         <v>When 'Read lookup value'</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>65</v>
       </c>
@@ -7415,7 +7417,7 @@
         <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
@@ -7447,7 +7449,7 @@
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
@@ -7476,7 +7478,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
@@ -7505,7 +7507,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
@@ -7534,7 +7536,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>65</v>
       </c>
@@ -7563,7 +7565,7 @@
         <v>When 'Read lookup value'</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>65</v>
       </c>
@@ -7592,7 +7594,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
         <v>65</v>
       </c>
@@ -7626,7 +7628,7 @@
       </c>
       <c r="M190" s="23"/>
     </row>
-    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
@@ -7658,7 +7660,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>65</v>
       </c>
@@ -7690,7 +7692,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>65</v>
       </c>
@@ -7722,7 +7724,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
@@ -7754,7 +7756,7 @@
         <v>When 'Modify lookup value'</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>65</v>
       </c>
@@ -7786,7 +7788,7 @@
         <v>Then 'Modify permissions error thrown' }</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>65</v>
       </c>
@@ -7818,7 +7820,7 @@
       </c>
       <c r="M196" s="23"/>
     </row>
-    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>65</v>
       </c>
@@ -7847,7 +7849,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
@@ -7876,7 +7878,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
@@ -7905,7 +7907,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -7934,7 +7936,7 @@
         <v>When 'Modify lookup value'</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
@@ -7963,7 +7965,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>65</v>
       </c>
@@ -7997,7 +7999,7 @@
       </c>
       <c r="M202" s="23"/>
     </row>
-    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
@@ -8029,7 +8031,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
@@ -8061,7 +8063,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
@@ -8093,7 +8095,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>65</v>
       </c>
@@ -8125,7 +8127,7 @@
         <v>When 'Delete lookup value'</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>65</v>
       </c>
@@ -8157,7 +8159,7 @@
         <v>Then 'Delete permissions error thrown' }</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>65</v>
       </c>
@@ -8189,7 +8191,7 @@
       </c>
       <c r="M208" s="23"/>
     </row>
-    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>65</v>
       </c>
@@ -8218,7 +8220,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>65</v>
       </c>
@@ -8247,7 +8249,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>65</v>
       </c>
@@ -8276,7 +8278,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>65</v>
       </c>
@@ -8305,7 +8307,7 @@
         <v>When 'Delete lookup value'</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>65</v>
       </c>
@@ -8334,7 +8336,7 @@
         <v>Then 'Lookup value does not exist' }</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>65</v>
       </c>
@@ -8370,7 +8372,7 @@
       </c>
       <c r="M214" s="23"/>
     </row>
-    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>65</v>
       </c>
@@ -8405,7 +8407,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>65</v>
       </c>
@@ -8434,7 +8436,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>65</v>
       </c>
@@ -8463,7 +8465,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>65</v>
       </c>
@@ -8498,7 +8500,7 @@
         <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>65</v>
       </c>
@@ -8533,7 +8535,7 @@
         <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>65</v>
       </c>
@@ -8567,7 +8569,7 @@
       </c>
       <c r="M220" s="23"/>
     </row>
-    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>65</v>
       </c>
@@ -8599,7 +8601,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>65</v>
       </c>
@@ -8631,7 +8633,7 @@
         <v>Given 'Clear last error'</v>
       </c>
     </row>
-    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>65</v>
       </c>
@@ -8663,7 +8665,7 @@
         <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
-    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
@@ -8695,7 +8697,7 @@
         <v>Then 'No error thrown' }</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>65</v>
       </c>
@@ -8733,7 +8735,7 @@
       </c>
       <c r="M225" s="23"/>
     </row>
-    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>65</v>
       </c>
@@ -8771,7 +8773,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>65</v>
       </c>
@@ -8809,7 +8811,7 @@
         <v>When 'Open customer card'</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>65</v>
       </c>
@@ -8847,7 +8849,7 @@
         <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>65</v>
       </c>
@@ -8883,7 +8885,7 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
@@ -8918,7 +8920,7 @@
         <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
-    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>65</v>
       </c>
@@ -8953,7 +8955,7 @@
         <v>When 'Open customer card'</v>
       </c>
     </row>
-    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>65</v>
       </c>
@@ -8988,7 +8990,7 @@
         <v>Then 'Lookup value field shown' }</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>65</v>
       </c>
@@ -9026,7 +9028,7 @@
       </c>
       <c r="M233" s="23"/>
     </row>
-    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>65</v>
       </c>
@@ -9064,7 +9066,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>65</v>
       </c>
@@ -9102,7 +9104,7 @@
         <v>When 'Open customer list'</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>65</v>
       </c>
@@ -9140,7 +9142,7 @@
         <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Added unit tests for subscribers that extend business logic of standard application
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B16254-D519-4344-9BCF-98AC3733100A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808C87E3-771F-438F-9226-264787BE575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="217">
   <si>
     <t>Feature</t>
   </si>
@@ -644,7 +644,70 @@
     <t>Full base permissions extended with Lookup Value</t>
   </si>
   <si>
-    <t>NOTE: the test for the other 34 pages have not been implemented yet an issue (#6) has been recorded for that on GitHub</t>
+    <t>NOTE: the test for the other 34 pages have not been implemented yet; an issue (#6) has been recorded for that on GitHub</t>
+  </si>
+  <si>
+    <t>Sales header without lookup value</t>
+  </si>
+  <si>
+    <t>Missing lookup value on sales header error thrown</t>
+  </si>
+  <si>
+    <t>Check failure OnBeforePostSalesDocEvent subscriber</t>
+  </si>
+  <si>
+    <t>Sales header with lookup value</t>
+  </si>
+  <si>
+    <t>Check failure OnBeforePostSourceDocumentEvent subscriber</t>
+  </si>
+  <si>
+    <t>Sales header with number and lookup value</t>
+  </si>
+  <si>
+    <t>Sales header with number and without lookup value</t>
+  </si>
+  <si>
+    <t>Check success OnBeforePostSourceDocumentEvent subscriber</t>
+  </si>
+  <si>
+    <t>Check success OnBeforePostSalesDocEvent subscriber</t>
+  </si>
+  <si>
+    <t>Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</t>
+  </si>
+  <si>
+    <t>Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</t>
+  </si>
+  <si>
+    <t>Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</t>
+  </si>
+  <si>
+    <t>Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</t>
+  </si>
+  <si>
+    <t>Warehouse shipment line</t>
+  </si>
+  <si>
+    <t>Lookup value on warehouse shipment line is populated with lookup value of sales header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnBeforeCreateShptLineFromSalesLineEvent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnBeforePostSalesDocEvent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnBeforePostSourceDocumentEvent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnApplyTemplateOnBeforeCustomerModifyEvent </t>
   </si>
 </sst>
 </file>
@@ -692,7 +755,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,6 +777,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -745,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -848,12 +917,128 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -917,222 +1102,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1147,28 +1116,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:M241" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M280" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:M280" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="15">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1471,13 +1440,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M242"/>
+  <dimension ref="A1:M281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+      <selection activeCell="E287" sqref="E287"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
@@ -1598,7 +1567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1627,7 +1596,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1656,7 +1625,7 @@
         <v>Given 'Customer'</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1685,7 +1654,7 @@
         <v>When 'Set lookup value on customer'</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1714,7 +1683,7 @@
         <v>Then 'Customer has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
@@ -1748,7 +1717,7 @@
       </c>
       <c r="M8" s="23"/>
     </row>
-    <row r="9" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1780,7 +1749,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1812,7 +1781,7 @@
         <v>Given 'Customer record variable'</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1844,7 +1813,7 @@
         <v>When 'Set non-existing lookup value on customer'</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1876,7 +1845,7 @@
         <v>Then 'Non existing lookup value error thrown' }</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -2100,7 +2069,7 @@
       </c>
       <c r="M19" s="23"/>
     </row>
-    <row r="20" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2129,7 +2098,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2158,7 +2127,7 @@
         <v>Given 'Sales header'</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -2187,7 +2156,7 @@
         <v>When 'Set lookup value on sales header'</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2216,7 +2185,7 @@
         <v>Then 'Sales header has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
@@ -2250,7 +2219,7 @@
       </c>
       <c r="M24" s="23"/>
     </row>
-    <row r="25" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2282,7 +2251,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +2283,7 @@
         <v>Given 'Sales header record variable'</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2346,7 +2315,7 @@
         <v>When 'Set non-existing lookup value to sales header'</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2378,7 +2347,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +2383,7 @@
       </c>
       <c r="M29" s="23"/>
     </row>
-    <row r="30" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2449,7 +2418,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2484,7 +2453,7 @@
         <v>Given 'Sales quote document page'</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2519,7 +2488,7 @@
         <v>When 'Set lookup value on sales quote document'</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2554,7 +2523,7 @@
         <v>Then 'Sales quote has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
@@ -2590,7 +2559,7 @@
       </c>
       <c r="M34" s="23"/>
     </row>
-    <row r="35" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2625,7 +2594,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2660,7 +2629,7 @@
         <v>Given 'Sales order document page'</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2695,7 +2664,7 @@
         <v>When 'Set lookup value on sales order document'</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2730,7 +2699,7 @@
         <v>Then 'Sales order has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>11</v>
       </c>
@@ -2766,7 +2735,7 @@
       </c>
       <c r="M39" s="23"/>
     </row>
-    <row r="40" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2801,7 +2770,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2836,7 +2805,7 @@
         <v>Given 'Sales invoice document page'</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2871,7 +2840,7 @@
         <v>When 'Set lookup value on sales invoice document'</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2906,7 +2875,7 @@
         <v>Then 'Sales invoice has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>11</v>
       </c>
@@ -2942,7 +2911,7 @@
       </c>
       <c r="M44" s="23"/>
     </row>
-    <row r="45" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2977,7 +2946,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3012,7 +2981,7 @@
         <v>Given 'Sales credit memo document page'</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3047,7 +3016,7 @@
         <v>When 'Set lookup value on sales credit memo document'</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3082,7 +3051,7 @@
         <v>Then 'Sales credit memo has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>11</v>
       </c>
@@ -3118,7 +3087,7 @@
       </c>
       <c r="M49" s="23"/>
     </row>
-    <row r="50" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -3153,7 +3122,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3188,7 +3157,7 @@
         <v>Given 'Sales return order document page'</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3223,7 +3192,7 @@
         <v>When 'Set lookup value on sales return order document'</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -3258,7 +3227,7 @@
         <v>Then 'Sales return order has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>11</v>
       </c>
@@ -3498,7 +3467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3527,7 +3496,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3556,7 +3525,7 @@
         <v>Given 'Customer template'</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3585,7 +3554,7 @@
         <v>When 'Set lookup value on customer template'</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -3614,7 +3583,7 @@
         <v>Then 'Customer template has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>11</v>
       </c>
@@ -3648,7 +3617,7 @@
       </c>
       <c r="M65" s="23"/>
     </row>
-    <row r="66" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3680,7 +3649,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -3712,7 +3681,7 @@
         <v>Given 'Customer template record variable'</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -3744,7 +3713,7 @@
         <v>When 'Set non-existing lookup value to customer template'</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3776,7 +3745,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>11</v>
       </c>
@@ -4000,7 +3969,7 @@
       </c>
       <c r="M76" s="23"/>
     </row>
-    <row r="77" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -4029,7 +3998,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -4058,7 +4027,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -4087,7 +4056,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -4116,7 +4085,7 @@
         <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -4145,7 +4114,7 @@
         <v>When 'Set lookup value on warehouse shipment line'</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>65</v>
       </c>
@@ -4174,7 +4143,7 @@
         <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>65</v>
       </c>
@@ -4208,7 +4177,7 @@
       </c>
       <c r="M83" s="23"/>
     </row>
-    <row r="84" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>65</v>
       </c>
@@ -4240,7 +4209,7 @@
         <v>Given 'Non-existing lookup value'</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -4272,7 +4241,7 @@
         <v>Given 'Warehouse shipment line record variable'</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>65</v>
       </c>
@@ -4304,7 +4273,7 @@
         <v>When 'Set non-existing lookup value to warehouse shipment line'</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>65</v>
       </c>
@@ -4336,7 +4305,7 @@
         <v>Then 'Non existing lookup value error was thrown' }</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
         <v>65</v>
       </c>
@@ -4370,7 +4339,7 @@
       </c>
       <c r="M88" s="23"/>
     </row>
-    <row r="89" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>65</v>
       </c>
@@ -4402,7 +4371,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>65</v>
       </c>
@@ -4434,7 +4403,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.5" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>65</v>
       </c>
@@ -4466,7 +4435,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>65</v>
       </c>
@@ -4498,7 +4467,7 @@
         <v>Given 'Warehouse shipment from released sales order with line with require shipment location'</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>65</v>
       </c>
@@ -4530,7 +4499,7 @@
         <v>When 'Set lookup value on warehouse shipment line on warehouse shipment document page'</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>65</v>
       </c>
@@ -4562,7 +4531,7 @@
         <v>Then 'Warehouse shipment line has lookup value code field populated' }</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
         <v>65</v>
       </c>
@@ -4580,7 +4549,7 @@
       <c r="I95" s="24">
         <v>30</v>
       </c>
-      <c r="J95" s="20" t="str">
+      <c r="J95" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0030] Create warehouse shipment from sales order with lookup value</v>
       </c>
@@ -4594,7 +4563,7 @@
       </c>
       <c r="M95" s="20"/>
     </row>
-    <row r="96" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>65</v>
       </c>
@@ -4610,7 +4579,7 @@
       <c r="I96" s="14">
         <v>30</v>
       </c>
-      <c r="J96" t="str">
+      <c r="J96" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Lookup value</v>
       </c>
@@ -4624,7 +4593,7 @@
       </c>
       <c r="M96"/>
     </row>
-    <row r="97" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>65</v>
       </c>
@@ -4640,7 +4609,7 @@
       <c r="I97" s="14">
         <v>30</v>
       </c>
-      <c r="J97" t="str">
+      <c r="J97" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Location with require shipment</v>
       </c>
@@ -4654,7 +4623,7 @@
       </c>
       <c r="M97"/>
     </row>
-    <row r="98" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -4670,7 +4639,7 @@
       <c r="I98" s="14">
         <v>30</v>
       </c>
-      <c r="J98" t="str">
+      <c r="J98" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Warehouse employee for current user</v>
       </c>
@@ -4684,7 +4653,7 @@
       </c>
       <c r="M98"/>
     </row>
-    <row r="99" spans="1:13" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>65</v>
       </c>
@@ -4700,7 +4669,7 @@
       <c r="I99" s="14">
         <v>30</v>
       </c>
-      <c r="J99" t="str">
+      <c r="J99" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Create warehouse shipment from released sales order with lookup value and with line with require shipment location</v>
       </c>
@@ -4714,7 +4683,7 @@
       </c>
       <c r="M99"/>
     </row>
-    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>65</v>
       </c>
@@ -4730,7 +4699,7 @@
       <c r="I100" s="14">
         <v>30</v>
       </c>
-      <c r="J100" t="str">
+      <c r="J100" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
@@ -4762,7 +4731,7 @@
       <c r="I101" s="24">
         <v>31</v>
       </c>
-      <c r="J101" s="20" t="str">
+      <c r="J101" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0031] Get sales order with lookup value on warehouse shipment</v>
       </c>
@@ -4792,7 +4761,7 @@
       <c r="I102" s="14">
         <v>31</v>
       </c>
-      <c r="J102" t="str">
+      <c r="J102" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Lookup value</v>
       </c>
@@ -4822,7 +4791,7 @@
       <c r="I103" s="14">
         <v>31</v>
       </c>
-      <c r="J103" t="str">
+      <c r="J103" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Location with require shipment</v>
       </c>
@@ -4852,7 +4821,7 @@
       <c r="I104" s="14">
         <v>31</v>
       </c>
-      <c r="J104" t="str">
+      <c r="J104" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Warehouse employee for current user</v>
       </c>
@@ -4882,7 +4851,7 @@
       <c r="I105" s="14">
         <v>31</v>
       </c>
-      <c r="J105" t="str">
+      <c r="J105" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Released sales order with lookup value and with line with require shipment location</v>
       </c>
@@ -4912,7 +4881,7 @@
       <c r="I106" s="14">
         <v>31</v>
       </c>
-      <c r="J106" t="str">
+      <c r="J106" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Warehouse shipment without lines</v>
       </c>
@@ -4942,7 +4911,7 @@
       <c r="I107" s="14">
         <v>31</v>
       </c>
-      <c r="J107" t="str">
+      <c r="J107" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Get sales order with lookup value on warehouse shipment</v>
       </c>
@@ -4972,7 +4941,7 @@
       <c r="I108" s="14">
         <v>31</v>
       </c>
-      <c r="J108" t="str">
+      <c r="J108" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Warehouse shipment line has lookup value code field populated</v>
       </c>
@@ -5050,7 +5019,7 @@
       </c>
       <c r="M110" s="23"/>
     </row>
-    <row r="111" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>65</v>
       </c>
@@ -5082,7 +5051,7 @@
         <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>65</v>
       </c>
@@ -5114,7 +5083,7 @@
         <v>When 'Sales order is archived'</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>65</v>
       </c>
@@ -5147,7 +5116,7 @@
       </c>
       <c r="M113"/>
     </row>
-    <row r="114" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="s">
         <v>65</v>
       </c>
@@ -5181,7 +5150,7 @@
       </c>
       <c r="M114" s="20"/>
     </row>
-    <row r="115" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>65</v>
       </c>
@@ -5214,7 +5183,7 @@
       </c>
       <c r="M115"/>
     </row>
-    <row r="116" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>65</v>
       </c>
@@ -5247,7 +5216,7 @@
       </c>
       <c r="M116"/>
     </row>
-    <row r="117" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>65</v>
       </c>
@@ -5280,7 +5249,7 @@
       </c>
       <c r="M117"/>
     </row>
-    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="s">
         <v>65</v>
       </c>
@@ -5314,7 +5283,7 @@
       </c>
       <c r="M118" s="20"/>
     </row>
-    <row r="119" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>65</v>
       </c>
@@ -5347,7 +5316,7 @@
       </c>
       <c r="M119"/>
     </row>
-    <row r="120" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>65</v>
       </c>
@@ -5380,7 +5349,7 @@
       </c>
       <c r="M120"/>
     </row>
-    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>65</v>
       </c>
@@ -5413,7 +5382,7 @@
       </c>
       <c r="M121"/>
     </row>
-    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
         <v>65</v>
       </c>
@@ -5554,7 +5523,7 @@
         <v>Then 'Archived sales document has lookup value from sales document'</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>65</v>
       </c>
@@ -5589,7 +5558,7 @@
         <v>Then 'lookup value is shown right on Sales List Archive' } }</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="15" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>65</v>
       </c>
@@ -5637,7 +5606,7 @@
       <c r="I128" s="24">
         <v>24</v>
       </c>
-      <c r="J128" s="20" t="str">
+      <c r="J128" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0024] Assign customer lookup value to sales document</v>
       </c>
@@ -5651,7 +5620,7 @@
       </c>
       <c r="M128" s="20"/>
     </row>
-    <row r="129" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>65</v>
       </c>
@@ -5670,7 +5639,7 @@
       <c r="I129" s="28">
         <v>24</v>
       </c>
-      <c r="J129" t="str">
+      <c r="J129" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Customer with Lookup value</v>
       </c>
@@ -5684,7 +5653,7 @@
       </c>
       <c r="M129"/>
     </row>
-    <row r="130" spans="1:13" ht="15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>65</v>
       </c>
@@ -5703,7 +5672,7 @@
       <c r="I130" s="28">
         <v>24</v>
       </c>
-      <c r="J130" t="str">
+      <c r="J130" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Sales document (invoice) without Lookup value</v>
       </c>
@@ -5717,7 +5686,7 @@
       </c>
       <c r="M130"/>
     </row>
-    <row r="131" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>65</v>
       </c>
@@ -5736,7 +5705,7 @@
       <c r="I131" s="28">
         <v>24</v>
       </c>
-      <c r="J131" t="str">
+      <c r="J131" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Set customer on sales header</v>
       </c>
@@ -5750,7 +5719,7 @@
       </c>
       <c r="M131"/>
     </row>
-    <row r="132" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>65</v>
       </c>
@@ -5769,7 +5738,7 @@
       <c r="I132" s="28">
         <v>24</v>
       </c>
-      <c r="J132" t="str">
+      <c r="J132" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Lookup value on sales document is populated with lookup value of customer</v>
       </c>
@@ -5783,7 +5752,7 @@
       </c>
       <c r="M132"/>
     </row>
-    <row r="133" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
         <v>65</v>
       </c>
@@ -5801,7 +5770,7 @@
       <c r="I133" s="24">
         <v>26</v>
       </c>
-      <c r="J133" s="20" t="str">
+      <c r="J133" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0026] Check that lookup value is inherited from customer template to customer when creating customer from contact</v>
       </c>
@@ -5815,7 +5784,7 @@
       </c>
       <c r="M133" s="20"/>
     </row>
-    <row r="134" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>65</v>
       </c>
@@ -5831,7 +5800,7 @@
       <c r="I134" s="14">
         <v>26</v>
       </c>
-      <c r="J134" t="str">
+      <c r="J134" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Customer template with lookup value</v>
       </c>
@@ -5845,7 +5814,7 @@
       </c>
       <c r="M134"/>
     </row>
-    <row r="135" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>65</v>
       </c>
@@ -5861,7 +5830,7 @@
       <c r="I135" s="14">
         <v>26</v>
       </c>
-      <c r="J135" t="str">
+      <c r="J135" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Contact</v>
       </c>
@@ -5875,7 +5844,7 @@
       </c>
       <c r="M135"/>
     </row>
-    <row r="136" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>65</v>
       </c>
@@ -5891,7 +5860,7 @@
       <c r="I136" s="14">
         <v>26</v>
       </c>
-      <c r="J136" t="str">
+      <c r="J136" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Customer is created from contact</v>
       </c>
@@ -5905,7 +5874,7 @@
       </c>
       <c r="M136"/>
     </row>
-    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>65</v>
       </c>
@@ -5921,7 +5890,7 @@
       <c r="I137" s="14">
         <v>26</v>
       </c>
-      <c r="J137" t="str">
+      <c r="J137" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Customer has lookup value code field populated with lookup value from customer template</v>
       </c>
@@ -5935,7 +5904,7 @@
       </c>
       <c r="M137"/>
     </row>
-    <row r="138" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="s">
         <v>65</v>
       </c>
@@ -5953,7 +5922,7 @@
       <c r="I138" s="24">
         <v>28</v>
       </c>
-      <c r="J138" s="20" t="str">
+      <c r="J138" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0028] Create customer from customer template with lookup value</v>
       </c>
@@ -5983,7 +5952,7 @@
       <c r="I139" s="14">
         <v>28</v>
       </c>
-      <c r="J139" t="str">
+      <c r="J139" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Customer template with lookup value</v>
       </c>
@@ -6013,7 +5982,7 @@
       <c r="I140" s="14">
         <v>28</v>
       </c>
-      <c r="J140" t="str">
+      <c r="J140" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Create customer card</v>
       </c>
@@ -6043,7 +6012,7 @@
       <c r="I141" s="14">
         <v>28</v>
       </c>
-      <c r="J141" t="str">
+      <c r="J141" s="13" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
       </c>
@@ -6121,7 +6090,7 @@
       </c>
       <c r="M143" s="23"/>
     </row>
-    <row r="144" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>65</v>
       </c>
@@ -6153,7 +6122,7 @@
         <v>Given 'Sales order with Lookup value'</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>65</v>
       </c>
@@ -6185,7 +6154,7 @@
         <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>65</v>
       </c>
@@ -6217,7 +6186,7 @@
         <v>Then 'Posted sales invoice has lookup value from sales order'</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>65</v>
       </c>
@@ -6249,7 +6218,7 @@
         <v>Then 'Sales shipment has lookup value from sales order' }</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
         <v>65</v>
       </c>
@@ -6285,7 +6254,7 @@
       </c>
       <c r="M148" s="23"/>
     </row>
-    <row r="149" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>65</v>
       </c>
@@ -6320,7 +6289,7 @@
         <v>Given 'Sales order without Lookup value'</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>65</v>
       </c>
@@ -6355,7 +6324,7 @@
         <v>When 'Sales order is posted (invoice &amp; ship)'</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>65</v>
       </c>
@@ -6390,7 +6359,7 @@
         <v>Then 'Missing lookup value on sales order error thrown' }</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
         <v>65</v>
       </c>
@@ -6424,7 +6393,7 @@
       </c>
       <c r="M152" s="23"/>
     </row>
-    <row r="153" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>104</v>
       </c>
@@ -6456,7 +6425,7 @@
         <v>Given 'Location with require shipment'</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>104</v>
       </c>
@@ -6488,7 +6457,7 @@
         <v>Given 'Warehouse employee for current user'</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>104</v>
       </c>
@@ -6520,7 +6489,7 @@
         <v>Given 'Warehouse shipment line with Lookup value created from Sales order'</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>65</v>
       </c>
@@ -6552,7 +6521,7 @@
         <v>When 'Warehouse shipment is posted'</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>65</v>
       </c>
@@ -6584,7 +6553,7 @@
         <v>Then 'Posted warehouse shipment line has lookup value from warehouse shipment line' }</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="s">
         <v>65</v>
       </c>
@@ -7008,7 +6977,7 @@
       </c>
       <c r="M170" s="23"/>
     </row>
-    <row r="171" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
@@ -7040,7 +7009,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>65</v>
       </c>
@@ -7072,7 +7041,7 @@
         <v>When 'Create lookup value'</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>65</v>
       </c>
@@ -7104,7 +7073,7 @@
         <v>Then 'Insert permissions error thrown' }</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
@@ -7136,7 +7105,7 @@
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
@@ -7165,7 +7134,7 @@
         <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>65</v>
       </c>
@@ -7194,7 +7163,7 @@
         <v>When 'Create lookup value'</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>65</v>
       </c>
@@ -7223,7 +7192,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
         <v>65</v>
       </c>
@@ -7257,7 +7226,7 @@
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
@@ -7289,7 +7258,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>65</v>
       </c>
@@ -7321,7 +7290,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>65</v>
       </c>
@@ -7353,7 +7322,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>65</v>
       </c>
@@ -7385,7 +7354,7 @@
         <v>When 'Read lookup value'</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>65</v>
       </c>
@@ -7417,7 +7386,7 @@
         <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
         <v>65</v>
       </c>
@@ -7449,7 +7418,7 @@
       </c>
       <c r="M184" s="23"/>
     </row>
-    <row r="185" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>65</v>
       </c>
@@ -7478,7 +7447,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
@@ -7507,7 +7476,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
@@ -7536,7 +7505,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>65</v>
       </c>
@@ -7565,7 +7534,7 @@
         <v>When 'Read lookup value'</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>65</v>
       </c>
@@ -7594,7 +7563,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
         <v>65</v>
       </c>
@@ -7628,7 +7597,7 @@
       </c>
       <c r="M190" s="23"/>
     </row>
-    <row r="191" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
@@ -7660,7 +7629,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>65</v>
       </c>
@@ -7692,7 +7661,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>65</v>
       </c>
@@ -7724,7 +7693,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>65</v>
       </c>
@@ -7756,7 +7725,7 @@
         <v>When 'Modify lookup value'</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>65</v>
       </c>
@@ -7788,7 +7757,7 @@
         <v>Then 'Modify permissions error thrown' }</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>65</v>
       </c>
@@ -7820,7 +7789,7 @@
       </c>
       <c r="M196" s="23"/>
     </row>
-    <row r="197" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>65</v>
       </c>
@@ -7849,7 +7818,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
@@ -7878,7 +7847,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
@@ -7907,7 +7876,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -7936,7 +7905,7 @@
         <v>When 'Modify lookup value'</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
@@ -7965,7 +7934,7 @@
         <v>Then 'Lookup value exists' }</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>65</v>
       </c>
@@ -7999,7 +7968,7 @@
       </c>
       <c r="M202" s="23"/>
     </row>
-    <row r="203" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
@@ -8031,7 +8000,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
@@ -8063,7 +8032,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
@@ -8095,7 +8064,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="206" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>65</v>
       </c>
@@ -8127,7 +8096,7 @@
         <v>When 'Delete lookup value'</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>65</v>
       </c>
@@ -8159,7 +8128,7 @@
         <v>Then 'Delete permissions error thrown' }</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>65</v>
       </c>
@@ -8191,7 +8160,7 @@
       </c>
       <c r="M208" s="23"/>
     </row>
-    <row r="209" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>65</v>
       </c>
@@ -8220,7 +8189,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="210" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>65</v>
       </c>
@@ -8249,7 +8218,7 @@
         <v>Given 'Lookup Value'</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>65</v>
       </c>
@@ -8278,7 +8247,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="212" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>65</v>
       </c>
@@ -8307,7 +8276,7 @@
         <v>When 'Delete lookup value'</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>65</v>
       </c>
@@ -8336,7 +8305,7 @@
         <v>Then 'Lookup value does not exist' }</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>65</v>
       </c>
@@ -8372,7 +8341,7 @@
       </c>
       <c r="M214" s="23"/>
     </row>
-    <row r="215" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>65</v>
       </c>
@@ -8407,7 +8376,7 @@
         <v>Given 'Unrestricted starting permissions'</v>
       </c>
     </row>
-    <row r="216" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>65</v>
       </c>
@@ -8436,7 +8405,7 @@
         <v>Given 'Lookup value'</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>65</v>
       </c>
@@ -8465,7 +8434,7 @@
         <v>Given 'Full base permissions'</v>
       </c>
     </row>
-    <row r="218" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>65</v>
       </c>
@@ -8500,7 +8469,7 @@
         <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>65</v>
       </c>
@@ -8535,7 +8504,7 @@
         <v>Then 'Read permissions error thrown' }</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>65</v>
       </c>
@@ -8569,7 +8538,7 @@
       </c>
       <c r="M220" s="23"/>
     </row>
-    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>65</v>
       </c>
@@ -8601,7 +8570,7 @@
         <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
-    <row r="222" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>65</v>
       </c>
@@ -8633,7 +8602,7 @@
         <v>Given 'Clear last error'</v>
       </c>
     </row>
-    <row r="223" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>65</v>
       </c>
@@ -8665,7 +8634,7 @@
         <v>When 'Open Lookup Values page'</v>
       </c>
     </row>
-    <row r="224" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>65</v>
       </c>
@@ -8697,7 +8666,7 @@
         <v>Then 'No error thrown' }</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>65</v>
       </c>
@@ -8735,7 +8704,7 @@
       </c>
       <c r="M225" s="23"/>
     </row>
-    <row r="226" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>65</v>
       </c>
@@ -8773,7 +8742,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="227" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>65</v>
       </c>
@@ -8811,7 +8780,7 @@
         <v>When 'Open customer card'</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>65</v>
       </c>
@@ -8849,7 +8818,7 @@
         <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>65</v>
       </c>
@@ -8885,7 +8854,7 @@
       </c>
       <c r="M229" s="23"/>
     </row>
-    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>65</v>
       </c>
@@ -8920,7 +8889,7 @@
         <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
-    <row r="231" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>65</v>
       </c>
@@ -8955,7 +8924,7 @@
         <v>When 'Open customer card'</v>
       </c>
     </row>
-    <row r="232" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>65</v>
       </c>
@@ -8990,7 +8959,7 @@
         <v>Then 'Lookup value field shown' }</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>65</v>
       </c>
@@ -9028,7 +8997,7 @@
       </c>
       <c r="M233" s="23"/>
     </row>
-    <row r="234" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>65</v>
       </c>
@@ -9066,7 +9035,7 @@
         <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
-    <row r="235" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>65</v>
       </c>
@@ -9104,7 +9073,7 @@
         <v>When 'Open customer list'</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>65</v>
       </c>
@@ -9142,7 +9111,7 @@
         <v>Then 'Lookup value field not shown' }</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>65</v>
       </c>
@@ -9283,7 +9252,7 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
-    <row r="241" spans="3:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C241" t="s">
         <v>195</v>
       </c>
@@ -9300,10 +9269,1234 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="3:12" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C242" s="5"/>
+      <c r="D242" s="6"/>
+      <c r="E242" s="6"/>
+      <c r="F242" s="7"/>
+      <c r="G242" s="5"/>
+      <c r="H242" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I242" s="9"/>
+      <c r="J242" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue UT Posting</v>
+      </c>
+      <c r="K242" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue UT Posting</v>
+      </c>
+      <c r="L242" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue UT Posting' {</v>
+      </c>
+      <c r="M242" s="8"/>
+    </row>
+    <row r="243" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B243" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C243" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D243" s="21"/>
+      <c r="E243" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F243" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G243" s="20"/>
+      <c r="H243" s="23"/>
+      <c r="I243" s="24">
+        <v>100</v>
+      </c>
+      <c r="J243" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
+      </c>
+      <c r="K243" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
+      </c>
+      <c r="L243" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0100 'Check failure OnBeforePostSalesDocEvent subscriber' {</v>
+      </c>
+      <c r="M243" s="23"/>
+    </row>
+    <row r="244" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>11</v>
+      </c>
+      <c r="B244" t="s">
+        <v>96</v>
+      </c>
+      <c r="C244" t="s">
+        <v>26</v>
+      </c>
+      <c r="E244" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G244" t="s">
+        <v>15</v>
+      </c>
+      <c r="H244" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I244" s="14">
+        <v>100</v>
+      </c>
+      <c r="J244" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header without lookup value</v>
+      </c>
+      <c r="K244" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header without lookup value</v>
+      </c>
+      <c r="L244" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header without lookup value'</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>11</v>
+      </c>
+      <c r="B245" t="s">
+        <v>96</v>
+      </c>
+      <c r="C245" t="s">
+        <v>26</v>
+      </c>
+      <c r="E245" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G245" t="s">
+        <v>16</v>
+      </c>
+      <c r="H245" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="I245" s="14">
+        <v>100</v>
+      </c>
+      <c r="J245" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
+      </c>
+      <c r="K245" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
+      </c>
+      <c r="L245" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnBeforePostSalesDocEvent '</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>11</v>
+      </c>
+      <c r="B246" t="s">
+        <v>96</v>
+      </c>
+      <c r="C246" t="s">
+        <v>26</v>
+      </c>
+      <c r="E246" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G246" t="s">
+        <v>18</v>
+      </c>
+      <c r="H246" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="I246" s="14">
+        <v>100</v>
+      </c>
+      <c r="J246" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Missing lookup value on sales header error thrown</v>
+      </c>
+      <c r="K246" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Missing lookup value on sales header error thrown</v>
+      </c>
+      <c r="L246" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Missing lookup value on sales header error thrown' }</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B247" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C247" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D247" s="21"/>
+      <c r="E247" s="21"/>
+      <c r="F247" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G247" s="20"/>
+      <c r="H247" s="23"/>
+      <c r="I247" s="24">
+        <v>101</v>
+      </c>
+      <c r="J247" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
+      </c>
+      <c r="K247" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
+      </c>
+      <c r="L247" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0101 'Check success OnBeforePostSalesDocEvent subscriber' {</v>
+      </c>
+      <c r="M247" s="23"/>
+    </row>
+    <row r="248" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>11</v>
+      </c>
+      <c r="B248" t="s">
+        <v>96</v>
+      </c>
+      <c r="C248" t="s">
+        <v>26</v>
+      </c>
+      <c r="G248" t="s">
+        <v>15</v>
+      </c>
+      <c r="H248" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="I248" s="14">
+        <v>101</v>
+      </c>
+      <c r="J248" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="K248" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="L248" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header with lookup value'</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>11</v>
+      </c>
+      <c r="B249" t="s">
+        <v>96</v>
+      </c>
+      <c r="C249" t="s">
+        <v>26</v>
+      </c>
+      <c r="G249" t="s">
+        <v>16</v>
+      </c>
+      <c r="H249" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="I249" s="14">
+        <v>101</v>
+      </c>
+      <c r="J249" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
+      </c>
+      <c r="K249" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
+      </c>
+      <c r="L249" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnBeforePostSalesDocEvent '</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>11</v>
+      </c>
+      <c r="B250" t="s">
+        <v>96</v>
+      </c>
+      <c r="C250" t="s">
+        <v>26</v>
+      </c>
+      <c r="G250" t="s">
+        <v>18</v>
+      </c>
+      <c r="H250" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I250" s="14">
+        <v>101</v>
+      </c>
+      <c r="J250" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] No error thrown</v>
+      </c>
+      <c r="K250" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] No error thrown</v>
+      </c>
+      <c r="L250" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No error thrown' }</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B251" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C251" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D251" s="21"/>
+      <c r="E251" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F251" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="G251" s="20"/>
+      <c r="H251" s="23"/>
+      <c r="I251" s="24">
+        <v>102</v>
+      </c>
+      <c r="J251" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
+      </c>
+      <c r="K251" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
+      </c>
+      <c r="L251" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0102 'Check failure OnBeforePostSourceDocumentEvent subscriber' {</v>
+      </c>
+      <c r="M251" s="23"/>
+    </row>
+    <row r="252" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>104</v>
+      </c>
+      <c r="B252" t="s">
+        <v>96</v>
+      </c>
+      <c r="C252" t="s">
+        <v>66</v>
+      </c>
+      <c r="E252" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G252" t="s">
+        <v>15</v>
+      </c>
+      <c r="H252" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I252" s="14">
+        <v>102</v>
+      </c>
+      <c r="J252" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header with number and without lookup value</v>
+      </c>
+      <c r="K252" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header with number and without lookup value</v>
+      </c>
+      <c r="L252" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header with number and without lookup value'</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>65</v>
+      </c>
+      <c r="B253" t="s">
+        <v>96</v>
+      </c>
+      <c r="C253" t="s">
+        <v>66</v>
+      </c>
+      <c r="E253" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G253" t="s">
+        <v>16</v>
+      </c>
+      <c r="H253" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="I253" s="14">
+        <v>102</v>
+      </c>
+      <c r="J253" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
+      </c>
+      <c r="K253" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
+      </c>
+      <c r="L253" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnBeforePostSourceDocumentEvent '</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>65</v>
+      </c>
+      <c r="B254" t="s">
+        <v>96</v>
+      </c>
+      <c r="C254" t="s">
+        <v>66</v>
+      </c>
+      <c r="E254" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G254" t="s">
+        <v>18</v>
+      </c>
+      <c r="H254" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="I254" s="14">
+        <v>102</v>
+      </c>
+      <c r="J254" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Missing lookup value on sales header error thrown</v>
+      </c>
+      <c r="K254" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Missing lookup value on sales header error thrown</v>
+      </c>
+      <c r="L254" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Missing lookup value on sales header error thrown' }</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B255" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C255" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D255" s="21"/>
+      <c r="E255" s="21"/>
+      <c r="F255" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="G255" s="20"/>
+      <c r="H255" s="23"/>
+      <c r="I255" s="24">
+        <v>103</v>
+      </c>
+      <c r="J255" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
+      </c>
+      <c r="K255" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
+      </c>
+      <c r="L255" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0103 'Check success OnBeforePostSourceDocumentEvent subscriber' {</v>
+      </c>
+      <c r="M255" s="23"/>
+    </row>
+    <row r="256" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>104</v>
+      </c>
+      <c r="B256" t="s">
+        <v>96</v>
+      </c>
+      <c r="C256" t="s">
+        <v>66</v>
+      </c>
+      <c r="G256" t="s">
+        <v>15</v>
+      </c>
+      <c r="H256" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="I256" s="14">
+        <v>103</v>
+      </c>
+      <c r="J256" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header with number and lookup value</v>
+      </c>
+      <c r="K256" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header with number and lookup value</v>
+      </c>
+      <c r="L256" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header with number and lookup value'</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>65</v>
+      </c>
+      <c r="B257" t="s">
+        <v>96</v>
+      </c>
+      <c r="C257" t="s">
+        <v>66</v>
+      </c>
+      <c r="G257" t="s">
+        <v>16</v>
+      </c>
+      <c r="H257" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="I257" s="14">
+        <v>103</v>
+      </c>
+      <c r="J257" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
+      </c>
+      <c r="K257" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
+      </c>
+      <c r="L257" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnBeforePostSourceDocumentEvent '</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>65</v>
+      </c>
+      <c r="B258" t="s">
+        <v>96</v>
+      </c>
+      <c r="C258" t="s">
+        <v>66</v>
+      </c>
+      <c r="G258" t="s">
+        <v>18</v>
+      </c>
+      <c r="H258" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="I258" s="14">
+        <v>103</v>
+      </c>
+      <c r="J258" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] No error thrown</v>
+      </c>
+      <c r="K258" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] No error thrown</v>
+      </c>
+      <c r="L258" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No error thrown' } }</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C259" s="5"/>
+      <c r="D259" s="6"/>
+      <c r="E259" s="6"/>
+      <c r="F259" s="7"/>
+      <c r="G259" s="5"/>
+      <c r="H259" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I259" s="9"/>
+      <c r="J259" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue UT Inheritance</v>
+      </c>
+      <c r="K259" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue UT Inheritance</v>
+      </c>
+      <c r="L259" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue UT Inheritance' {</v>
+      </c>
+      <c r="M259" s="8"/>
+    </row>
+    <row r="260" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B260" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C260" s="20"/>
+      <c r="D260" s="21"/>
+      <c r="E260" s="21"/>
+      <c r="F260" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="G260" s="20"/>
+      <c r="H260" s="23"/>
+      <c r="I260" s="24">
+        <v>104</v>
+      </c>
+      <c r="J260" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
+      </c>
+      <c r="K260" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
+      </c>
+      <c r="L260" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0104 'Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber' {</v>
+      </c>
+      <c r="M260" s="23"/>
+    </row>
+    <row r="261" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>11</v>
+      </c>
+      <c r="B261" t="s">
+        <v>150</v>
+      </c>
+      <c r="G261" t="s">
+        <v>15</v>
+      </c>
+      <c r="H261" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I261" s="28">
+        <v>104</v>
+      </c>
+      <c r="J261" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with Lookup value</v>
+      </c>
+      <c r="K261" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with Lookup value</v>
+      </c>
+      <c r="L261" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with Lookup value'</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>11</v>
+      </c>
+      <c r="B262" t="s">
+        <v>150</v>
+      </c>
+      <c r="G262" t="s">
+        <v>15</v>
+      </c>
+      <c r="H262" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I262" s="28">
+        <v>104</v>
+      </c>
+      <c r="J262" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header without lookup value</v>
+      </c>
+      <c r="K262" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header without lookup value</v>
+      </c>
+      <c r="L262" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header without lookup value'</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>11</v>
+      </c>
+      <c r="B263" t="s">
+        <v>150</v>
+      </c>
+      <c r="G263" t="s">
+        <v>16</v>
+      </c>
+      <c r="H263" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I263" s="28">
+        <v>104</v>
+      </c>
+      <c r="J263" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
+      </c>
+      <c r="K263" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
+      </c>
+      <c r="L263" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent '</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>11</v>
+      </c>
+      <c r="B264" t="s">
+        <v>150</v>
+      </c>
+      <c r="G264" t="s">
+        <v>18</v>
+      </c>
+      <c r="H264" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I264" s="28">
+        <v>104</v>
+      </c>
+      <c r="J264" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value on sales document is populated with lookup value of customer</v>
+      </c>
+      <c r="K264" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value on sales document is populated with lookup value of customer</v>
+      </c>
+      <c r="L264" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value on sales document is populated with lookup value of customer' }</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B265" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C265" s="20"/>
+      <c r="D265" s="21"/>
+      <c r="E265" s="21"/>
+      <c r="F265" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="G265" s="20"/>
+      <c r="H265" s="23"/>
+      <c r="I265" s="24">
+        <v>105</v>
+      </c>
+      <c r="J265" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
+      </c>
+      <c r="K265" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
+      </c>
+      <c r="L265" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0105 'Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber' {</v>
+      </c>
+      <c r="M265" s="23"/>
+    </row>
+    <row r="266" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>11</v>
+      </c>
+      <c r="B266" t="s">
+        <v>151</v>
+      </c>
+      <c r="G266" t="s">
+        <v>15</v>
+      </c>
+      <c r="H266" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I266" s="14">
+        <v>105</v>
+      </c>
+      <c r="J266" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="K266" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="L266" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template with lookup value'</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>11</v>
+      </c>
+      <c r="B267" t="s">
+        <v>151</v>
+      </c>
+      <c r="G267" t="s">
+        <v>15</v>
+      </c>
+      <c r="H267" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I267" s="14">
+        <v>105</v>
+      </c>
+      <c r="J267" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer</v>
+      </c>
+      <c r="K267" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer</v>
+      </c>
+      <c r="L267" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer'</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>11</v>
+      </c>
+      <c r="B268" t="s">
+        <v>151</v>
+      </c>
+      <c r="G268" t="s">
+        <v>16</v>
+      </c>
+      <c r="H268" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="I268" s="14">
+        <v>105</v>
+      </c>
+      <c r="J268" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
+      </c>
+      <c r="K268" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
+      </c>
+      <c r="L268" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent '</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>11</v>
+      </c>
+      <c r="B269" t="s">
+        <v>151</v>
+      </c>
+      <c r="G269" t="s">
+        <v>18</v>
+      </c>
+      <c r="H269" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="I269" s="14">
+        <v>105</v>
+      </c>
+      <c r="J269" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
+      </c>
+      <c r="K269" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
+      </c>
+      <c r="L269" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value on customer is populated with lookup value of customer template' }</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B270" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C270" s="20"/>
+      <c r="D270" s="21"/>
+      <c r="E270" s="21"/>
+      <c r="F270" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="G270" s="20"/>
+      <c r="H270" s="23"/>
+      <c r="I270" s="24">
+        <v>106</v>
+      </c>
+      <c r="J270" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
+      </c>
+      <c r="K270" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
+      </c>
+      <c r="L270" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0106 'Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber' {</v>
+      </c>
+      <c r="M270" s="23"/>
+    </row>
+    <row r="271" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>11</v>
+      </c>
+      <c r="B271" t="s">
+        <v>186</v>
+      </c>
+      <c r="G271" t="s">
+        <v>15</v>
+      </c>
+      <c r="H271" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I271" s="14">
+        <v>106</v>
+      </c>
+      <c r="J271" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="K271" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer template with lookup value</v>
+      </c>
+      <c r="L271" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer template with lookup value'</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>11</v>
+      </c>
+      <c r="B272" t="s">
+        <v>186</v>
+      </c>
+      <c r="G272" t="s">
+        <v>15</v>
+      </c>
+      <c r="H272" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I272" s="14">
+        <v>106</v>
+      </c>
+      <c r="J272" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer</v>
+      </c>
+      <c r="K272" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer</v>
+      </c>
+      <c r="L272" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer'</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>11</v>
+      </c>
+      <c r="B273" t="s">
+        <v>186</v>
+      </c>
+      <c r="G273" t="s">
+        <v>16</v>
+      </c>
+      <c r="H273" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="I273" s="14">
+        <v>106</v>
+      </c>
+      <c r="J273" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
+      </c>
+      <c r="K273" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
+      </c>
+      <c r="L273" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnApplyTemplateOnBeforeCustomerModifyEvent '</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>11</v>
+      </c>
+      <c r="B274" t="s">
+        <v>186</v>
+      </c>
+      <c r="G274" t="s">
+        <v>18</v>
+      </c>
+      <c r="H274" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="I274" s="14">
+        <v>106</v>
+      </c>
+      <c r="J274" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
+      </c>
+      <c r="K274" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
+      </c>
+      <c r="L274" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C275" s="5"/>
+      <c r="D275" s="6"/>
+      <c r="E275" s="6"/>
+      <c r="F275" s="7"/>
+      <c r="G275" s="5"/>
+      <c r="H275" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I275" s="9"/>
+      <c r="J275" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue UT Warehouse Shipment</v>
+      </c>
+      <c r="K275" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue UT Warehouse Shipment</v>
+      </c>
+      <c r="L275" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue UT Warehouse Shipment' {</v>
+      </c>
+      <c r="M275" s="8"/>
+    </row>
+    <row r="276" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B276" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C276" s="38"/>
+      <c r="D276" s="39"/>
+      <c r="E276" s="39"/>
+      <c r="F276" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="G276" s="38"/>
+      <c r="H276" s="41"/>
+      <c r="I276" s="42">
+        <v>107</v>
+      </c>
+      <c r="J276" s="43" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+      </c>
+      <c r="K276" s="44" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+      </c>
+      <c r="L276" s="45" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0107 'Check OnBeforeCreateShptLineFromSalesLineEvent subscriber' {</v>
+      </c>
+      <c r="M276" s="41"/>
+    </row>
+    <row r="277" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>11</v>
+      </c>
+      <c r="B277" t="s">
+        <v>152</v>
+      </c>
+      <c r="G277" t="s">
+        <v>15</v>
+      </c>
+      <c r="H277" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="I277" s="14">
+        <v>107</v>
+      </c>
+      <c r="J277" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="K277" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="L277" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header with lookup value'</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>11</v>
+      </c>
+      <c r="B278" t="s">
+        <v>152</v>
+      </c>
+      <c r="G278" t="s">
+        <v>15</v>
+      </c>
+      <c r="H278" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="I278" s="14">
+        <v>107</v>
+      </c>
+      <c r="J278" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse shipment line</v>
+      </c>
+      <c r="K278" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse shipment line</v>
+      </c>
+      <c r="L278" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>11</v>
+      </c>
+      <c r="B279" t="s">
+        <v>152</v>
+      </c>
+      <c r="G279" t="s">
+        <v>16</v>
+      </c>
+      <c r="H279" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I279" s="14">
+        <v>107</v>
+      </c>
+      <c r="J279" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v xml:space="preserve">[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
+      </c>
+      <c r="K279" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v xml:space="preserve">//[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
+      </c>
+      <c r="L279" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'OnBeforeCreateShptLineFromSalesLineEvent '</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>11</v>
+      </c>
+      <c r="B280" t="s">
+        <v>152</v>
+      </c>
+      <c r="G280" t="s">
+        <v>18</v>
+      </c>
+      <c r="H280" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="I280" s="14">
+        <v>107</v>
+      </c>
+      <c r="J280" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
+      </c>
+      <c r="K280" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
+      </c>
+      <c r="L280" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value on warehouse shipment line is populated with lookup value of sales header' } }</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="I1:I274 I276:I1048576">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9314,117 +10507,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
+  <conditionalFormatting sqref="D1:D274 D276:D1048576">
+    <cfRule type="cellIs" dxfId="11" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="38" priority="29">
+  <conditionalFormatting sqref="A1:B274 A276:B1048576">
+    <cfRule type="containsBlanks" dxfId="10" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G184 G189:G190 G196 G213:G1048576">
-    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
+  <conditionalFormatting sqref="E1:E274 E276:E1048576">
+    <cfRule type="cellIs" dxfId="9" priority="46" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G274 G276:G1048576">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
+  <conditionalFormatting sqref="I275">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D275">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G185:G188">
-    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
+  <conditionalFormatting sqref="A275:B275">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A275))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E275">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G275">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G191:G195">
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G197:G199">
-    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G200">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G201:G202 G206:G208">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G203:G205">
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G209:G211">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G212">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added ATDD scenarios for chapter 12 separately
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808C87E3-771F-438F-9226-264787BE575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3F01A-F974-4532-B9C1-F071A4D5240A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="201">
   <si>
     <t>Feature</t>
   </si>
@@ -647,42 +647,9 @@
     <t>NOTE: the test for the other 34 pages have not been implemented yet; an issue (#6) has been recorded for that on GitHub</t>
   </si>
   <si>
-    <t>Sales header without lookup value</t>
-  </si>
-  <si>
-    <t>Missing lookup value on sales header error thrown</t>
-  </si>
-  <si>
-    <t>Check failure OnBeforePostSalesDocEvent subscriber</t>
-  </si>
-  <si>
     <t>Sales header with lookup value</t>
   </si>
   <si>
-    <t>Check failure OnBeforePostSourceDocumentEvent subscriber</t>
-  </si>
-  <si>
-    <t>Sales header with number and lookup value</t>
-  </si>
-  <si>
-    <t>Sales header with number and without lookup value</t>
-  </si>
-  <si>
-    <t>Check success OnBeforePostSourceDocumentEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check success OnBeforePostSalesDocEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</t>
-  </si>
-  <si>
     <t>Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</t>
   </si>
   <si>
@@ -693,21 +660,6 @@
   </si>
   <si>
     <t xml:space="preserve">OnBeforeCreateShptLineFromSalesLineEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnBeforePostSalesDocEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnBeforePostSourceDocumentEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnApplyTemplateOnBeforeCustomerModifyEvent </t>
   </si>
 </sst>
 </file>
@@ -942,55 +894,7 @@
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -1116,28 +1020,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M280" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:M280" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M246" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:M246" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="13">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1440,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M281"/>
+  <dimension ref="A1:M247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E287" sqref="E287"/>
+      <selection activeCell="A242" sqref="A242:XFD275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -9252,7 +9156,7 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
-    <row r="241" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
         <v>195</v>
       </c>
@@ -9269,140 +9173,123 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="5" t="s">
+    <row r="242" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B242" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C242" s="5"/>
-      <c r="D242" s="6"/>
-      <c r="E242" s="6"/>
-      <c r="F242" s="7"/>
-      <c r="G242" s="5"/>
-      <c r="H242" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I242" s="9"/>
-      <c r="J242" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue UT Posting</v>
-      </c>
-      <c r="K242" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue UT Posting</v>
-      </c>
-      <c r="L242" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue UT Posting' {</v>
-      </c>
-      <c r="M242" s="8"/>
-    </row>
-    <row r="243" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="20" t="s">
+      <c r="B242" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C242" s="38"/>
+      <c r="D242" s="39"/>
+      <c r="E242" s="39"/>
+      <c r="F242" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="G242" s="38"/>
+      <c r="H242" s="41"/>
+      <c r="I242" s="42">
+        <v>107</v>
+      </c>
+      <c r="J242" s="43" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+      </c>
+      <c r="K242" s="44" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+      </c>
+      <c r="L242" s="45" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0107 'Check OnBeforeCreateShptLineFromSalesLineEvent subscriber' {</v>
+      </c>
+      <c r="M242" s="41"/>
+    </row>
+    <row r="243" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>11</v>
       </c>
-      <c r="B243" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C243" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D243" s="21"/>
-      <c r="E243" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F243" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="G243" s="20"/>
-      <c r="H243" s="23"/>
-      <c r="I243" s="24">
-        <v>100</v>
-      </c>
-      <c r="J243" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
-      </c>
-      <c r="K243" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
-      </c>
-      <c r="L243" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0100 'Check failure OnBeforePostSalesDocEvent subscriber' {</v>
-      </c>
-      <c r="M243" s="23"/>
+      <c r="B243" t="s">
+        <v>152</v>
+      </c>
+      <c r="G243" t="s">
+        <v>15</v>
+      </c>
+      <c r="H243" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I243" s="14">
+        <v>107</v>
+      </c>
+      <c r="J243" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="K243" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Sales header with lookup value</v>
+      </c>
+      <c r="L243" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Sales header with lookup value'</v>
+      </c>
     </row>
     <row r="244" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>11</v>
       </c>
       <c r="B244" t="s">
-        <v>96</v>
-      </c>
-      <c r="C244" t="s">
-        <v>26</v>
-      </c>
-      <c r="E244" s="11" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="G244" t="s">
         <v>15</v>
       </c>
       <c r="H244" s="13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I244" s="14">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="J244" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header without lookup value</v>
+        <v>[GIVEN] Warehouse shipment line</v>
       </c>
       <c r="K244" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header without lookup value</v>
+        <v>//[GIVEN] Warehouse shipment line</v>
       </c>
       <c r="L244" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header without lookup value'</v>
-      </c>
-    </row>
-    <row r="245" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>11</v>
       </c>
       <c r="B245" t="s">
-        <v>96</v>
-      </c>
-      <c r="C245" t="s">
-        <v>26</v>
-      </c>
-      <c r="E245" s="11" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="G245" t="s">
         <v>16</v>
       </c>
       <c r="H245" s="13" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I245" s="14">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="J245" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
+        <v xml:space="preserve">[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
       </c>
       <c r="K245" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
+        <v xml:space="preserve">//[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
       </c>
       <c r="L245" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSalesDocEvent '</v>
+        <v>When 'OnBeforeCreateShptLineFromSalesLineEvent '</v>
       </c>
     </row>
     <row r="246" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -9410,1092 +9297,33 @@
         <v>11</v>
       </c>
       <c r="B246" t="s">
-        <v>96</v>
-      </c>
-      <c r="C246" t="s">
-        <v>26</v>
-      </c>
-      <c r="E246" s="11" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="G246" t="s">
         <v>18</v>
       </c>
       <c r="H246" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I246" s="14">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="J246" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Missing lookup value on sales header error thrown</v>
+        <v>[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
       </c>
       <c r="K246" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Missing lookup value on sales header error thrown</v>
+        <v>//[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
       </c>
       <c r="L246" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Missing lookup value on sales header error thrown' }</v>
-      </c>
-    </row>
-    <row r="247" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B247" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C247" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D247" s="21"/>
-      <c r="E247" s="21"/>
-      <c r="F247" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="G247" s="20"/>
-      <c r="H247" s="23"/>
-      <c r="I247" s="24">
-        <v>101</v>
-      </c>
-      <c r="J247" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
-      </c>
-      <c r="K247" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
-      </c>
-      <c r="L247" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0101 'Check success OnBeforePostSalesDocEvent subscriber' {</v>
-      </c>
-      <c r="M247" s="23"/>
-    </row>
-    <row r="248" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>11</v>
-      </c>
-      <c r="B248" t="s">
-        <v>96</v>
-      </c>
-      <c r="C248" t="s">
-        <v>26</v>
-      </c>
-      <c r="G248" t="s">
-        <v>15</v>
-      </c>
-      <c r="H248" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="I248" s="14">
-        <v>101</v>
-      </c>
-      <c r="J248" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="K248" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="L248" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with lookup value'</v>
-      </c>
-    </row>
-    <row r="249" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>11</v>
-      </c>
-      <c r="B249" t="s">
-        <v>96</v>
-      </c>
-      <c r="C249" t="s">
-        <v>26</v>
-      </c>
-      <c r="G249" t="s">
-        <v>16</v>
-      </c>
-      <c r="H249" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="I249" s="14">
-        <v>101</v>
-      </c>
-      <c r="J249" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
-      </c>
-      <c r="K249" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
-      </c>
-      <c r="L249" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSalesDocEvent '</v>
-      </c>
-    </row>
-    <row r="250" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>11</v>
-      </c>
-      <c r="B250" t="s">
-        <v>96</v>
-      </c>
-      <c r="C250" t="s">
-        <v>26</v>
-      </c>
-      <c r="G250" t="s">
-        <v>18</v>
-      </c>
-      <c r="H250" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="I250" s="14">
-        <v>101</v>
-      </c>
-      <c r="J250" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] No error thrown</v>
-      </c>
-      <c r="K250" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] No error thrown</v>
-      </c>
-      <c r="L250" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'No error thrown' }</v>
-      </c>
-    </row>
-    <row r="251" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B251" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C251" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D251" s="21"/>
-      <c r="E251" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F251" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="G251" s="20"/>
-      <c r="H251" s="23"/>
-      <c r="I251" s="24">
-        <v>102</v>
-      </c>
-      <c r="J251" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
-      </c>
-      <c r="K251" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
-      </c>
-      <c r="L251" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0102 'Check failure OnBeforePostSourceDocumentEvent subscriber' {</v>
-      </c>
-      <c r="M251" s="23"/>
-    </row>
-    <row r="252" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>104</v>
-      </c>
-      <c r="B252" t="s">
-        <v>96</v>
-      </c>
-      <c r="C252" t="s">
-        <v>66</v>
-      </c>
-      <c r="E252" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G252" t="s">
-        <v>15</v>
-      </c>
-      <c r="H252" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="I252" s="14">
-        <v>102</v>
-      </c>
-      <c r="J252" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with number and without lookup value</v>
-      </c>
-      <c r="K252" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with number and without lookup value</v>
-      </c>
-      <c r="L252" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with number and without lookup value'</v>
-      </c>
-    </row>
-    <row r="253" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>65</v>
-      </c>
-      <c r="B253" t="s">
-        <v>96</v>
-      </c>
-      <c r="C253" t="s">
-        <v>66</v>
-      </c>
-      <c r="E253" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G253" t="s">
-        <v>16</v>
-      </c>
-      <c r="H253" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="I253" s="14">
-        <v>102</v>
-      </c>
-      <c r="J253" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
-      </c>
-      <c r="K253" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
-      </c>
-      <c r="L253" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSourceDocumentEvent '</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>65</v>
-      </c>
-      <c r="B254" t="s">
-        <v>96</v>
-      </c>
-      <c r="C254" t="s">
-        <v>66</v>
-      </c>
-      <c r="E254" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G254" t="s">
-        <v>18</v>
-      </c>
-      <c r="H254" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="I254" s="14">
-        <v>102</v>
-      </c>
-      <c r="J254" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Missing lookup value on sales header error thrown</v>
-      </c>
-      <c r="K254" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Missing lookup value on sales header error thrown</v>
-      </c>
-      <c r="L254" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Missing lookup value on sales header error thrown' }</v>
-      </c>
-    </row>
-    <row r="255" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B255" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C255" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D255" s="21"/>
-      <c r="E255" s="21"/>
-      <c r="F255" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G255" s="20"/>
-      <c r="H255" s="23"/>
-      <c r="I255" s="24">
-        <v>103</v>
-      </c>
-      <c r="J255" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
-      </c>
-      <c r="K255" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
-      </c>
-      <c r="L255" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0103 'Check success OnBeforePostSourceDocumentEvent subscriber' {</v>
-      </c>
-      <c r="M255" s="23"/>
-    </row>
-    <row r="256" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>104</v>
-      </c>
-      <c r="B256" t="s">
-        <v>96</v>
-      </c>
-      <c r="C256" t="s">
-        <v>66</v>
-      </c>
-      <c r="G256" t="s">
-        <v>15</v>
-      </c>
-      <c r="H256" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="I256" s="14">
-        <v>103</v>
-      </c>
-      <c r="J256" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with number and lookup value</v>
-      </c>
-      <c r="K256" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with number and lookup value</v>
-      </c>
-      <c r="L256" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with number and lookup value'</v>
-      </c>
-    </row>
-    <row r="257" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>65</v>
-      </c>
-      <c r="B257" t="s">
-        <v>96</v>
-      </c>
-      <c r="C257" t="s">
-        <v>66</v>
-      </c>
-      <c r="G257" t="s">
-        <v>16</v>
-      </c>
-      <c r="H257" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="I257" s="14">
-        <v>103</v>
-      </c>
-      <c r="J257" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
-      </c>
-      <c r="K257" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
-      </c>
-      <c r="L257" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSourceDocumentEvent '</v>
-      </c>
-    </row>
-    <row r="258" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
-        <v>65</v>
-      </c>
-      <c r="B258" t="s">
-        <v>96</v>
-      </c>
-      <c r="C258" t="s">
-        <v>66</v>
-      </c>
-      <c r="G258" t="s">
-        <v>18</v>
-      </c>
-      <c r="H258" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="I258" s="14">
-        <v>103</v>
-      </c>
-      <c r="J258" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] No error thrown</v>
-      </c>
-      <c r="K258" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] No error thrown</v>
-      </c>
-      <c r="L258" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'No error thrown' } }</v>
-      </c>
-    </row>
-    <row r="259" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B259" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C259" s="5"/>
-      <c r="D259" s="6"/>
-      <c r="E259" s="6"/>
-      <c r="F259" s="7"/>
-      <c r="G259" s="5"/>
-      <c r="H259" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I259" s="9"/>
-      <c r="J259" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue UT Inheritance</v>
-      </c>
-      <c r="K259" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue UT Inheritance</v>
-      </c>
-      <c r="L259" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue UT Inheritance' {</v>
-      </c>
-      <c r="M259" s="8"/>
-    </row>
-    <row r="260" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B260" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="C260" s="20"/>
-      <c r="D260" s="21"/>
-      <c r="E260" s="21"/>
-      <c r="F260" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="G260" s="20"/>
-      <c r="H260" s="23"/>
-      <c r="I260" s="24">
-        <v>104</v>
-      </c>
-      <c r="J260" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
-      </c>
-      <c r="K260" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
-      </c>
-      <c r="L260" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0104 'Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber' {</v>
-      </c>
-      <c r="M260" s="23"/>
-    </row>
-    <row r="261" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>11</v>
-      </c>
-      <c r="B261" t="s">
-        <v>150</v>
-      </c>
-      <c r="G261" t="s">
-        <v>15</v>
-      </c>
-      <c r="H261" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="I261" s="28">
-        <v>104</v>
-      </c>
-      <c r="J261" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with Lookup value</v>
-      </c>
-      <c r="K261" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with Lookup value</v>
-      </c>
-      <c r="L261" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with Lookup value'</v>
-      </c>
-    </row>
-    <row r="262" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>11</v>
-      </c>
-      <c r="B262" t="s">
-        <v>150</v>
-      </c>
-      <c r="G262" t="s">
-        <v>15</v>
-      </c>
-      <c r="H262" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="I262" s="28">
-        <v>104</v>
-      </c>
-      <c r="J262" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header without lookup value</v>
-      </c>
-      <c r="K262" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header without lookup value</v>
-      </c>
-      <c r="L262" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header without lookup value'</v>
-      </c>
-    </row>
-    <row r="263" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>11</v>
-      </c>
-      <c r="B263" t="s">
-        <v>150</v>
-      </c>
-      <c r="G263" t="s">
-        <v>16</v>
-      </c>
-      <c r="H263" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="I263" s="28">
-        <v>104</v>
-      </c>
-      <c r="J263" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
-      </c>
-      <c r="K263" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
-      </c>
-      <c r="L263" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent '</v>
-      </c>
-    </row>
-    <row r="264" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>11</v>
-      </c>
-      <c r="B264" t="s">
-        <v>150</v>
-      </c>
-      <c r="G264" t="s">
-        <v>18</v>
-      </c>
-      <c r="H264" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I264" s="28">
-        <v>104</v>
-      </c>
-      <c r="J264" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on sales document is populated with lookup value of customer</v>
-      </c>
-      <c r="K264" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on sales document is populated with lookup value of customer</v>
-      </c>
-      <c r="L264" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on sales document is populated with lookup value of customer' }</v>
-      </c>
-    </row>
-    <row r="265" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B265" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C265" s="20"/>
-      <c r="D265" s="21"/>
-      <c r="E265" s="21"/>
-      <c r="F265" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="G265" s="20"/>
-      <c r="H265" s="23"/>
-      <c r="I265" s="24">
-        <v>105</v>
-      </c>
-      <c r="J265" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
-      </c>
-      <c r="K265" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
-      </c>
-      <c r="L265" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0105 'Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber' {</v>
-      </c>
-      <c r="M265" s="23"/>
-    </row>
-    <row r="266" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>11</v>
-      </c>
-      <c r="B266" t="s">
-        <v>151</v>
-      </c>
-      <c r="G266" t="s">
-        <v>15</v>
-      </c>
-      <c r="H266" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I266" s="14">
-        <v>105</v>
-      </c>
-      <c r="J266" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="K266" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="L266" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value'</v>
-      </c>
-    </row>
-    <row r="267" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>11</v>
-      </c>
-      <c r="B267" t="s">
-        <v>151</v>
-      </c>
-      <c r="G267" t="s">
-        <v>15</v>
-      </c>
-      <c r="H267" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I267" s="14">
-        <v>105</v>
-      </c>
-      <c r="J267" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer</v>
-      </c>
-      <c r="K267" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer</v>
-      </c>
-      <c r="L267" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer'</v>
-      </c>
-    </row>
-    <row r="268" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>11</v>
-      </c>
-      <c r="B268" t="s">
-        <v>151</v>
-      </c>
-      <c r="G268" t="s">
-        <v>16</v>
-      </c>
-      <c r="H268" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="I268" s="14">
-        <v>105</v>
-      </c>
-      <c r="J268" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
-      </c>
-      <c r="K268" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
-      </c>
-      <c r="L268" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent '</v>
-      </c>
-    </row>
-    <row r="269" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>11</v>
-      </c>
-      <c r="B269" t="s">
-        <v>151</v>
-      </c>
-      <c r="G269" t="s">
-        <v>18</v>
-      </c>
-      <c r="H269" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="I269" s="14">
-        <v>105</v>
-      </c>
-      <c r="J269" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="K269" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="L269" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of customer template' }</v>
-      </c>
-    </row>
-    <row r="270" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B270" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C270" s="20"/>
-      <c r="D270" s="21"/>
-      <c r="E270" s="21"/>
-      <c r="F270" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="G270" s="20"/>
-      <c r="H270" s="23"/>
-      <c r="I270" s="24">
-        <v>106</v>
-      </c>
-      <c r="J270" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
-      </c>
-      <c r="K270" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
-      </c>
-      <c r="L270" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0106 'Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber' {</v>
-      </c>
-      <c r="M270" s="23"/>
-    </row>
-    <row r="271" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>11</v>
-      </c>
-      <c r="B271" t="s">
-        <v>186</v>
-      </c>
-      <c r="G271" t="s">
-        <v>15</v>
-      </c>
-      <c r="H271" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I271" s="14">
-        <v>106</v>
-      </c>
-      <c r="J271" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="K271" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="L271" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value'</v>
-      </c>
-    </row>
-    <row r="272" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>11</v>
-      </c>
-      <c r="B272" t="s">
-        <v>186</v>
-      </c>
-      <c r="G272" t="s">
-        <v>15</v>
-      </c>
-      <c r="H272" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I272" s="14">
-        <v>106</v>
-      </c>
-      <c r="J272" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer</v>
-      </c>
-      <c r="K272" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer</v>
-      </c>
-      <c r="L272" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer'</v>
-      </c>
-    </row>
-    <row r="273" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>11</v>
-      </c>
-      <c r="B273" t="s">
-        <v>186</v>
-      </c>
-      <c r="G273" t="s">
-        <v>16</v>
-      </c>
-      <c r="H273" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="I273" s="14">
-        <v>106</v>
-      </c>
-      <c r="J273" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
-      </c>
-      <c r="K273" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
-      </c>
-      <c r="L273" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnApplyTemplateOnBeforeCustomerModifyEvent '</v>
-      </c>
-    </row>
-    <row r="274" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
-        <v>11</v>
-      </c>
-      <c r="B274" t="s">
-        <v>186</v>
-      </c>
-      <c r="G274" t="s">
-        <v>18</v>
-      </c>
-      <c r="H274" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="I274" s="14">
-        <v>106</v>
-      </c>
-      <c r="J274" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="K274" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="L274" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
-      </c>
-    </row>
-    <row r="275" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B275" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C275" s="5"/>
-      <c r="D275" s="6"/>
-      <c r="E275" s="6"/>
-      <c r="F275" s="7"/>
-      <c r="G275" s="5"/>
-      <c r="H275" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I275" s="9"/>
-      <c r="J275" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue UT Warehouse Shipment</v>
-      </c>
-      <c r="K275" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue UT Warehouse Shipment</v>
-      </c>
-      <c r="L275" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue UT Warehouse Shipment' {</v>
-      </c>
-      <c r="M275" s="8"/>
-    </row>
-    <row r="276" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B276" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="C276" s="38"/>
-      <c r="D276" s="39"/>
-      <c r="E276" s="39"/>
-      <c r="F276" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="G276" s="38"/>
-      <c r="H276" s="41"/>
-      <c r="I276" s="42">
-        <v>107</v>
-      </c>
-      <c r="J276" s="43" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
-      </c>
-      <c r="K276" s="44" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
-      </c>
-      <c r="L276" s="45" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0107 'Check OnBeforeCreateShptLineFromSalesLineEvent subscriber' {</v>
-      </c>
-      <c r="M276" s="41"/>
-    </row>
-    <row r="277" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>11</v>
-      </c>
-      <c r="B277" t="s">
-        <v>152</v>
-      </c>
-      <c r="G277" t="s">
-        <v>15</v>
-      </c>
-      <c r="H277" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="I277" s="14">
-        <v>107</v>
-      </c>
-      <c r="J277" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="K277" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="L277" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with lookup value'</v>
-      </c>
-    </row>
-    <row r="278" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>11</v>
-      </c>
-      <c r="B278" t="s">
-        <v>152</v>
-      </c>
-      <c r="G278" t="s">
-        <v>15</v>
-      </c>
-      <c r="H278" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="I278" s="14">
-        <v>107</v>
-      </c>
-      <c r="J278" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="K278" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="L278" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line'</v>
-      </c>
-    </row>
-    <row r="279" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>11</v>
-      </c>
-      <c r="B279" t="s">
-        <v>152</v>
-      </c>
-      <c r="G279" t="s">
-        <v>16</v>
-      </c>
-      <c r="H279" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="I279" s="14">
-        <v>107</v>
-      </c>
-      <c r="J279" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
-      </c>
-      <c r="K279" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
-      </c>
-      <c r="L279" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforeCreateShptLineFromSalesLineEvent '</v>
-      </c>
-    </row>
-    <row r="280" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>11</v>
-      </c>
-      <c r="B280" t="s">
-        <v>152</v>
-      </c>
-      <c r="G280" t="s">
-        <v>18</v>
-      </c>
-      <c r="H280" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="I280" s="14">
-        <v>107</v>
-      </c>
-      <c r="J280" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
-      </c>
-      <c r="K280" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
-      </c>
-      <c r="L280" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value on warehouse shipment line is populated with lookup value of sales header' } }</v>
       </c>
     </row>
-    <row r="281" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="I1:I274 I276:I1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -10507,67 +9335,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D274 D276:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="51" operator="equal">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B274 A276:B1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="50">
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="containsBlanks" dxfId="4" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E274 E276:E1048576">
-    <cfRule type="cellIs" dxfId="9" priority="46" operator="equal">
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G274 G276:G1048576">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I275">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D275">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A275:B275">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A275))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E275">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G275">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adjusted LooukupValue Posting due to ATTD.TestScriptor example
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3F01A-F974-4532-B9C1-F071A4D5240A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB791F94-196B-4E71-B724-C3A4C5D0DD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-25320" yWindow="285" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="203">
   <si>
     <t>Feature</t>
   </si>
@@ -327,36 +327,18 @@
     <t>Posting</t>
   </si>
   <si>
-    <t>Check that posted sales invoice and shipment inherit lookup value from sales order</t>
-  </si>
-  <si>
-    <t>Sales order is posted (invoice &amp; ship)</t>
-  </si>
-  <si>
     <t>Posted sales invoice has lookup value from sales order</t>
   </si>
   <si>
     <t>Sales shipment has lookup value from sales order</t>
   </si>
   <si>
-    <t>Check posting throws error on sales order with empty lookup value</t>
-  </si>
-  <si>
     <t>Missing lookup value on sales order error thrown</t>
   </si>
   <si>
-    <t>Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line</t>
-  </si>
-  <si>
     <t>Lookup Value</t>
   </si>
   <si>
-    <t>Warehouse shipment is posted</t>
-  </si>
-  <si>
-    <t>Posted warehouse shipment line has lookup value from warehouse shipment line</t>
-  </si>
-  <si>
     <t>Check that lookup value is inherited from customer template to customer when creating customer from contact</t>
   </si>
   <si>
@@ -453,9 +435,6 @@
     <t>Sales document (invoice) without Lookup value</t>
   </si>
   <si>
-    <t>Sales order without Lookup value</t>
-  </si>
-  <si>
     <t>Warehouse employee for current user</t>
   </si>
   <si>
@@ -466,12 +445,6 @@
   </si>
   <si>
     <t>Warehouse shipment without lines</t>
-  </si>
-  <si>
-    <t>Warehouse shipment line with Lookup value created from Sales order</t>
-  </si>
-  <si>
-    <t>Warehouse shipment line created from Sales order without  lookup value</t>
   </si>
   <si>
     <t>Location with require shipment</t>
@@ -660,6 +633,39 @@
   </si>
   <si>
     <t xml:space="preserve">OnBeforeCreateShptLineFromSalesLineEvent </t>
+  </si>
+  <si>
+    <t>Sales order with lookup value</t>
+  </si>
+  <si>
+    <t>Sales order without lookup value</t>
+  </si>
+  <si>
+    <t>Warehouse shipment line from sales order without lookup value</t>
+  </si>
+  <si>
+    <t>Warehouse shipment line from sales order with lookup value</t>
+  </si>
+  <si>
+    <t>Post sales order (invoice &amp; ship)</t>
+  </si>
+  <si>
+    <t>Post Warehouse shipment</t>
+  </si>
+  <si>
+    <t>Posted warehouse shipment line has lookup value from sales order</t>
+  </si>
+  <si>
+    <t>Posted sales invoice and shipment inherit lookup value from sales order</t>
+  </si>
+  <si>
+    <t>Posting throws error on sales order with empty lookup value</t>
+  </si>
+  <si>
+    <t>Posted warehouse shipment line inherits lookup value from sales order</t>
+  </si>
+  <si>
+    <t>Posting throws error on warehouse shipment line with empty lookup value</t>
   </si>
 </sst>
 </file>
@@ -896,54 +902,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1006,6 +964,54 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1020,28 +1026,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M246" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M246" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:M246" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1346,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:M247"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242:XFD275"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1401,7 +1407,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -1420,7 +1426,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="8" t="str">
@@ -1482,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I4" s="14">
         <v>1</v>
@@ -1635,7 +1641,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I9" s="14">
         <v>2</v>
@@ -1667,7 +1673,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I10" s="14">
         <v>2</v>
@@ -1797,7 +1803,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I14" s="14">
         <v>3</v>
@@ -1829,7 +1835,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I15" s="14">
         <v>3</v>
@@ -1924,7 +1930,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
       <c r="H18" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="18" t="str">
@@ -1984,7 +1990,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I20" s="14">
         <v>4</v>
@@ -2013,7 +2019,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I21" s="14">
         <v>4</v>
@@ -2137,7 +2143,7 @@
         <v>15</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I25" s="14">
         <v>5</v>
@@ -2169,7 +2175,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I26" s="14">
         <v>5</v>
@@ -2304,7 +2310,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I30" s="14">
         <v>6</v>
@@ -2339,7 +2345,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I31" s="14">
         <v>6</v>
@@ -2480,7 +2486,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I35" s="14">
         <v>7</v>
@@ -2515,7 +2521,7 @@
         <v>15</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I36" s="14">
         <v>7</v>
@@ -2656,7 +2662,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I40" s="14">
         <v>8</v>
@@ -2691,7 +2697,7 @@
         <v>15</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I41" s="14">
         <v>8</v>
@@ -2832,7 +2838,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I45" s="14">
         <v>9</v>
@@ -2867,7 +2873,7 @@
         <v>15</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I46" s="14">
         <v>9</v>
@@ -3008,7 +3014,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I50" s="14">
         <v>10</v>
@@ -3043,7 +3049,7 @@
         <v>15</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I51" s="14">
         <v>10</v>
@@ -3184,7 +3190,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I55" s="14">
         <v>11</v>
@@ -3219,7 +3225,7 @@
         <v>15</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="I56" s="14">
         <v>11</v>
@@ -3320,7 +3326,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="5"/>
       <c r="H59" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="18" t="str">
@@ -3382,7 +3388,7 @@
         <v>15</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I61" s="14">
         <v>12</v>
@@ -3411,7 +3417,7 @@
         <v>15</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I62" s="14">
         <v>12</v>
@@ -3535,7 +3541,7 @@
         <v>15</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I66" s="14">
         <v>13</v>
@@ -3567,7 +3573,7 @@
         <v>15</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I67" s="14">
         <v>13</v>
@@ -3697,7 +3703,7 @@
         <v>15</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I71" s="14">
         <v>14</v>
@@ -3729,7 +3735,7 @@
         <v>15</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I72" s="14">
         <v>14</v>
@@ -3824,7 +3830,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="5"/>
       <c r="H75" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="18" t="str">
@@ -3884,7 +3890,7 @@
         <v>15</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I77" s="14">
         <v>15</v>
@@ -3913,7 +3919,7 @@
         <v>15</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I78" s="14">
         <v>15</v>
@@ -3942,7 +3948,7 @@
         <v>15</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I79" s="14">
         <v>15</v>
@@ -3971,7 +3977,7 @@
         <v>15</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I80" s="14">
         <v>15</v>
@@ -4095,7 +4101,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I84" s="14">
         <v>16</v>
@@ -4127,7 +4133,7 @@
         <v>15</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I85" s="14">
         <v>16</v>
@@ -4257,7 +4263,7 @@
         <v>15</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I89" s="14">
         <v>17</v>
@@ -4289,7 +4295,7 @@
         <v>15</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I90" s="14">
         <v>17</v>
@@ -4321,7 +4327,7 @@
         <v>15</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I91" s="14">
         <v>17</v>
@@ -4353,7 +4359,7 @@
         <v>15</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I92" s="14">
         <v>17</v>
@@ -4440,7 +4446,7 @@
         <v>65</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C95" s="20"/>
       <c r="D95" s="21"/>
@@ -4472,13 +4478,13 @@
         <v>65</v>
       </c>
       <c r="B96" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G96" t="s">
         <v>15</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I96" s="14">
         <v>30</v>
@@ -4502,13 +4508,13 @@
         <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G97" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I97" s="14">
         <v>30</v>
@@ -4532,13 +4538,13 @@
         <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G98" t="s">
         <v>15</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I98" s="14">
         <v>30</v>
@@ -4562,7 +4568,7 @@
         <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G99" t="s">
         <v>16</v>
@@ -4592,7 +4598,7 @@
         <v>65</v>
       </c>
       <c r="B100" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G100" t="s">
         <v>18</v>
@@ -4622,7 +4628,7 @@
         <v>65</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="21"/>
@@ -4654,13 +4660,13 @@
         <v>65</v>
       </c>
       <c r="B102" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G102" t="s">
         <v>15</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I102" s="14">
         <v>31</v>
@@ -4684,13 +4690,13 @@
         <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G103" t="s">
         <v>15</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I103" s="14">
         <v>31</v>
@@ -4714,13 +4720,13 @@
         <v>65</v>
       </c>
       <c r="B104" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G104" t="s">
         <v>15</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I104" s="14">
         <v>31</v>
@@ -4744,13 +4750,13 @@
         <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G105" t="s">
         <v>15</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="I105" s="14">
         <v>31</v>
@@ -4774,13 +4780,13 @@
         <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G106" t="s">
         <v>15</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I106" s="14">
         <v>31</v>
@@ -4804,7 +4810,7 @@
         <v>65</v>
       </c>
       <c r="B107" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G107" t="s">
         <v>16</v>
@@ -4834,7 +4840,7 @@
         <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G108" t="s">
         <v>18</v>
@@ -4872,7 +4878,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="5"/>
       <c r="H109" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I109" s="9"/>
       <c r="J109" s="18" t="str">
@@ -4937,7 +4943,7 @@
         <v>15</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I111" s="14">
         <v>18</v>
@@ -5068,7 +5074,7 @@
         <v>15</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I115" s="14">
         <v>19</v>
@@ -5201,7 +5207,7 @@
         <v>15</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I119" s="14">
         <v>20</v>
@@ -5339,7 +5345,7 @@
         <v>15</v>
       </c>
       <c r="H123" s="13" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I123" s="14">
         <v>21</v>
@@ -5475,7 +5481,7 @@
       <c r="F127" s="7"/>
       <c r="G127" s="5"/>
       <c r="H127" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I127" s="9"/>
       <c r="J127" s="18" t="str">
@@ -5497,7 +5503,7 @@
         <v>65</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C128" s="20"/>
       <c r="D128" s="20"/>
@@ -5529,7 +5535,7 @@
         <v>65</v>
       </c>
       <c r="B129" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D129"/>
       <c r="E129"/>
@@ -5538,7 +5544,7 @@
         <v>15</v>
       </c>
       <c r="H129" s="13" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I129" s="28">
         <v>24</v>
@@ -5562,7 +5568,7 @@
         <v>65</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D130"/>
       <c r="E130"/>
@@ -5571,7 +5577,7 @@
         <v>15</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I130" s="28">
         <v>24</v>
@@ -5595,7 +5601,7 @@
         <v>65</v>
       </c>
       <c r="B131" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D131"/>
       <c r="E131"/>
@@ -5628,7 +5634,7 @@
         <v>65</v>
       </c>
       <c r="B132" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D132"/>
       <c r="E132"/>
@@ -5661,13 +5667,13 @@
         <v>65</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C133" s="20"/>
       <c r="D133" s="21"/>
       <c r="E133" s="21"/>
       <c r="F133" s="22" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G133" s="20"/>
       <c r="H133" s="23"/>
@@ -5693,13 +5699,13 @@
         <v>65</v>
       </c>
       <c r="B134" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G134" t="s">
         <v>15</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I134" s="14">
         <v>26</v>
@@ -5723,13 +5729,13 @@
         <v>65</v>
       </c>
       <c r="B135" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G135" t="s">
         <v>15</v>
       </c>
       <c r="H135" s="13" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="I135" s="14">
         <v>26</v>
@@ -5753,13 +5759,13 @@
         <v>65</v>
       </c>
       <c r="B136" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G136" t="s">
         <v>16</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I136" s="14">
         <v>26</v>
@@ -5783,13 +5789,13 @@
         <v>65</v>
       </c>
       <c r="B137" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G137" t="s">
         <v>18</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I137" s="14">
         <v>26</v>
@@ -5813,13 +5819,13 @@
         <v>65</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
       <c r="E138" s="21"/>
       <c r="F138" s="22" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="G138" s="20"/>
       <c r="H138" s="23"/>
@@ -5845,13 +5851,13 @@
         <v>65</v>
       </c>
       <c r="B139" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G139" t="s">
         <v>15</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I139" s="14">
         <v>28</v>
@@ -5875,13 +5881,13 @@
         <v>65</v>
       </c>
       <c r="B140" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G140" t="s">
         <v>16</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I140" s="14">
         <v>28</v>
@@ -5905,13 +5911,13 @@
         <v>65</v>
       </c>
       <c r="B141" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G141" t="s">
         <v>18</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="I141" s="14">
         <v>28</v>
@@ -5943,7 +5949,7 @@
       <c r="F142" s="7"/>
       <c r="G142" s="5"/>
       <c r="H142" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I142" s="9"/>
       <c r="J142" s="18" t="str">
@@ -5973,7 +5979,7 @@
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="22" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="G143" s="20"/>
       <c r="H143" s="23"/>
@@ -5982,15 +5988,15 @@
       </c>
       <c r="J143" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0022] Check that posted sales invoice and shipment inherit lookup value from sales order</v>
+        <v>[SCENARIO #0022] Posted sales invoice and shipment inherit lookup value from sales order</v>
       </c>
       <c r="K143" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0022] Check that posted sales invoice and shipment inherit lookup value from sales order</v>
+        <v>//[SCENARIO #0022] Posted sales invoice and shipment inherit lookup value from sales order</v>
       </c>
       <c r="L143" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0022 'Check that posted sales invoice and shipment inherit lookup value from sales order' {</v>
+        <v>Scenario 0022 'Posted sales invoice and shipment inherit lookup value from sales order' {</v>
       </c>
       <c r="M143" s="23"/>
     </row>
@@ -6008,22 +6014,22 @@
         <v>15</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="I144" s="14">
         <v>22</v>
       </c>
       <c r="J144" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales order with Lookup value</v>
+        <v>[GIVEN] Sales order with lookup value</v>
       </c>
       <c r="K144" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales order with Lookup value</v>
+        <v>//[GIVEN] Sales order with lookup value</v>
       </c>
       <c r="L144" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order with Lookup value'</v>
+        <v>Given 'Sales order with lookup value'</v>
       </c>
     </row>
     <row r="145" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6040,22 +6046,22 @@
         <v>16</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="I145" s="14">
         <v>22</v>
       </c>
       <c r="J145" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales order is posted (invoice &amp; ship)</v>
+        <v>[WHEN] Post sales order (invoice &amp; ship)</v>
       </c>
       <c r="K145" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales order is posted (invoice &amp; ship)</v>
+        <v>//[WHEN] Post sales order (invoice &amp; ship)</v>
       </c>
       <c r="L145" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is posted (invoice &amp; ship)'</v>
+        <v>When 'Post sales order (invoice &amp; ship)'</v>
       </c>
     </row>
     <row r="146" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6072,7 +6078,7 @@
         <v>18</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I146" s="14">
         <v>22</v>
@@ -6104,7 +6110,7 @@
         <v>18</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I147" s="14">
         <v>22</v>
@@ -6137,7 +6143,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="22" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="G148" s="20"/>
       <c r="H148" s="23"/>
@@ -6146,15 +6152,15 @@
       </c>
       <c r="J148" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0027] Check posting throws error on sales order with empty lookup value</v>
+        <v>[SCENARIO #0027] Posting throws error on sales order with empty lookup value</v>
       </c>
       <c r="K148" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0027] Check posting throws error on sales order with empty lookup value</v>
+        <v>//[SCENARIO #0027] Posting throws error on sales order with empty lookup value</v>
       </c>
       <c r="L148" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0027 'Check posting throws error on sales order with empty lookup value' {</v>
+        <v>Scenario 0027 'Posting throws error on sales order with empty lookup value' {</v>
       </c>
       <c r="M148" s="23"/>
     </row>
@@ -6175,22 +6181,22 @@
         <v>15</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>139</v>
+        <v>193</v>
       </c>
       <c r="I149" s="14">
         <v>27</v>
       </c>
       <c r="J149" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales order without Lookup value</v>
+        <v>[GIVEN] Sales order without lookup value</v>
       </c>
       <c r="K149" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales order without Lookup value</v>
+        <v>//[GIVEN] Sales order without lookup value</v>
       </c>
       <c r="L149" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales order without Lookup value'</v>
+        <v>Given 'Sales order without lookup value'</v>
       </c>
     </row>
     <row r="150" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6210,22 +6216,22 @@
         <v>16</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="I150" s="14">
         <v>27</v>
       </c>
       <c r="J150" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Sales order is posted (invoice &amp; ship)</v>
+        <v>[WHEN] Post sales order (invoice &amp; ship)</v>
       </c>
       <c r="K150" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Sales order is posted (invoice &amp; ship)</v>
+        <v>//[WHEN] Post sales order (invoice &amp; ship)</v>
       </c>
       <c r="L150" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Sales order is posted (invoice &amp; ship)'</v>
+        <v>When 'Post sales order (invoice &amp; ship)'</v>
       </c>
     </row>
     <row r="151" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6245,7 +6251,7 @@
         <v>18</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I151" s="14">
         <v>27</v>
@@ -6263,7 +6269,7 @@
         <v>Then 'Missing lookup value on sales order error thrown' }</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
         <v>65</v>
       </c>
@@ -6276,7 +6282,7 @@
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="22" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="G152" s="20"/>
       <c r="H152" s="23"/>
@@ -6285,21 +6291,21 @@
       </c>
       <c r="J152" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0023] Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line</v>
+        <v>[SCENARIO #0023] Posted warehouse shipment line inherits lookup value from sales order</v>
       </c>
       <c r="K152" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0023] Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line</v>
+        <v>//[SCENARIO #0023] Posted warehouse shipment line inherits lookup value from sales order</v>
       </c>
       <c r="L152" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0023 'Check that posted warehouse shipment line inherits lookup value from sales order through warehouse shipment line' {</v>
+        <v>Scenario 0023 'Posted warehouse shipment line inherits lookup value from sales order' {</v>
       </c>
       <c r="M152" s="23"/>
     </row>
     <row r="153" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B153" t="s">
         <v>96</v>
@@ -6311,7 +6317,7 @@
         <v>15</v>
       </c>
       <c r="H153" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I153" s="14">
         <v>23</v>
@@ -6331,7 +6337,7 @@
     </row>
     <row r="154" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B154" t="s">
         <v>96</v>
@@ -6343,7 +6349,7 @@
         <v>15</v>
       </c>
       <c r="H154" s="27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I154" s="14">
         <v>23</v>
@@ -6363,7 +6369,7 @@
     </row>
     <row r="155" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B155" t="s">
         <v>96</v>
@@ -6375,22 +6381,22 @@
         <v>15</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="I155" s="14">
         <v>23</v>
       </c>
       <c r="J155" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment line with Lookup value created from Sales order</v>
+        <v>[GIVEN] Warehouse shipment line from sales order with lookup value</v>
       </c>
       <c r="K155" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment line with Lookup value created from Sales order</v>
+        <v>//[GIVEN] Warehouse shipment line from sales order with lookup value</v>
       </c>
       <c r="L155" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line with Lookup value created from Sales order'</v>
+        <v>Given 'Warehouse shipment line from sales order with lookup value'</v>
       </c>
     </row>
     <row r="156" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6407,22 +6413,22 @@
         <v>16</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="I156" s="14">
         <v>23</v>
       </c>
       <c r="J156" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Warehouse shipment is posted</v>
+        <v>[WHEN] Post Warehouse shipment</v>
       </c>
       <c r="K156" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Warehouse shipment is posted</v>
+        <v>//[WHEN] Post Warehouse shipment</v>
       </c>
       <c r="L156" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Warehouse shipment is posted'</v>
+        <v>When 'Post Warehouse shipment'</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6439,22 +6445,22 @@
         <v>18</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="I157" s="14">
         <v>23</v>
       </c>
       <c r="J157" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Posted warehouse shipment line has lookup value from warehouse shipment line</v>
+        <v>[THEN] Posted warehouse shipment line has lookup value from sales order</v>
       </c>
       <c r="K157" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Posted warehouse shipment line has lookup value from warehouse shipment line</v>
+        <v>//[THEN] Posted warehouse shipment line has lookup value from sales order</v>
       </c>
       <c r="L157" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posted warehouse shipment line has lookup value from warehouse shipment line' }</v>
+        <v>Then 'Posted warehouse shipment line has lookup value from sales order' }</v>
       </c>
     </row>
     <row r="158" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6472,7 +6478,7 @@
         <v>23</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="G158" s="20"/>
       <c r="H158" s="23"/>
@@ -6481,21 +6487,21 @@
       </c>
       <c r="J158" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0025] Check posting throws error on sales order with empty lookup value</v>
+        <v>[SCENARIO #0025] Posting throws error on warehouse shipment line with empty lookup value</v>
       </c>
       <c r="K158" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0025] Check posting throws error on sales order with empty lookup value</v>
+        <v>//[SCENARIO #0025] Posting throws error on warehouse shipment line with empty lookup value</v>
       </c>
       <c r="L158" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0025 'Check posting throws error on sales order with empty lookup value' {</v>
+        <v>Scenario 0025 'Posting throws error on warehouse shipment line with empty lookup value' {</v>
       </c>
       <c r="M158" s="23"/>
     </row>
     <row r="159" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B159" t="s">
         <v>96</v>
@@ -6510,7 +6516,7 @@
         <v>15</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I159" s="14">
         <v>25</v>
@@ -6530,7 +6536,7 @@
     </row>
     <row r="160" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B160" t="s">
         <v>96</v>
@@ -6545,7 +6551,7 @@
         <v>15</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I160" s="14">
         <v>25</v>
@@ -6565,7 +6571,7 @@
     </row>
     <row r="161" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B161" t="s">
         <v>96</v>
@@ -6580,22 +6586,22 @@
         <v>15</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="I161" s="14">
         <v>25</v>
       </c>
       <c r="J161" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment line created from Sales order without  lookup value</v>
+        <v>[GIVEN] Warehouse shipment line from sales order without lookup value</v>
       </c>
       <c r="K161" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment line created from Sales order without  lookup value</v>
+        <v>//[GIVEN] Warehouse shipment line from sales order without lookup value</v>
       </c>
       <c r="L161" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line created from Sales order without  lookup value'</v>
+        <v>Given 'Warehouse shipment line from sales order without lookup value'</v>
       </c>
     </row>
     <row r="162" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -6615,22 +6621,22 @@
         <v>16</v>
       </c>
       <c r="H162" s="13" t="s">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="I162" s="14">
         <v>25</v>
       </c>
       <c r="J162" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Warehouse shipment is posted</v>
+        <v>[WHEN] Post Warehouse shipment</v>
       </c>
       <c r="K162" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Warehouse shipment is posted</v>
+        <v>//[WHEN] Post Warehouse shipment</v>
       </c>
       <c r="L162" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Warehouse shipment is posted'</v>
+        <v>When 'Post Warehouse shipment'</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6650,7 +6656,7 @@
         <v>18</v>
       </c>
       <c r="H163" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I163" s="14">
         <v>25</v>
@@ -6673,7 +6679,7 @@
         <v>65</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
@@ -6681,7 +6687,7 @@
       <c r="F164" s="7"/>
       <c r="G164" s="5"/>
       <c r="H164" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I164" s="9"/>
       <c r="J164" s="18" t="str">
@@ -6703,13 +6709,13 @@
         <v>65</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C165" s="20"/>
       <c r="D165" s="21"/>
       <c r="E165" s="21"/>
       <c r="F165" s="22" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G165" s="20"/>
       <c r="H165" s="23"/>
@@ -6735,13 +6741,13 @@
         <v>65</v>
       </c>
       <c r="B166" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G166" t="s">
         <v>15</v>
       </c>
       <c r="H166" s="13" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I166" s="14">
         <v>29</v>
@@ -6764,13 +6770,13 @@
         <v>65</v>
       </c>
       <c r="B167" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G167" t="s">
         <v>16</v>
       </c>
       <c r="H167" s="13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I167" s="14">
         <v>29</v>
@@ -6793,13 +6799,13 @@
         <v>65</v>
       </c>
       <c r="B168" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G168" t="s">
         <v>18</v>
       </c>
       <c r="H168" s="13" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I168" s="14">
         <v>29</v>
@@ -6822,7 +6828,7 @@
         <v>65</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
@@ -6830,7 +6836,7 @@
       <c r="F169" s="7"/>
       <c r="G169" s="5"/>
       <c r="H169" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I169" s="9"/>
       <c r="J169" s="18" t="str">
@@ -6852,7 +6858,7 @@
         <v>65</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C170" s="20"/>
       <c r="D170" s="21"/>
@@ -6860,7 +6866,7 @@
         <v>23</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G170" s="20"/>
       <c r="H170" s="23"/>
@@ -6886,7 +6892,7 @@
         <v>65</v>
       </c>
       <c r="B171" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E171" s="11" t="s">
         <v>23</v>
@@ -6895,7 +6901,7 @@
         <v>15</v>
       </c>
       <c r="H171" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="I171" s="14">
         <v>41</v>
@@ -6918,7 +6924,7 @@
         <v>65</v>
       </c>
       <c r="B172" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E172" s="11" t="s">
         <v>23</v>
@@ -6927,7 +6933,7 @@
         <v>16</v>
       </c>
       <c r="H172" s="13" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="I172" s="14">
         <v>41</v>
@@ -6950,7 +6956,7 @@
         <v>65</v>
       </c>
       <c r="B173" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E173" s="11" t="s">
         <v>23</v>
@@ -6959,7 +6965,7 @@
         <v>18</v>
       </c>
       <c r="H173" s="13" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="I173" s="14">
         <v>41</v>
@@ -6982,13 +6988,13 @@
         <v>65</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
       <c r="F174" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G174" s="20"/>
       <c r="H174" s="23"/>
@@ -7014,13 +7020,13 @@
         <v>65</v>
       </c>
       <c r="B175" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G175" t="s">
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I175" s="14">
         <v>42</v>
@@ -7043,13 +7049,13 @@
         <v>65</v>
       </c>
       <c r="B176" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G176" t="s">
         <v>16</v>
       </c>
       <c r="H176" s="13" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="I176" s="14">
         <v>42</v>
@@ -7072,13 +7078,13 @@
         <v>65</v>
       </c>
       <c r="B177" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G177" t="s">
         <v>18</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I177" s="14">
         <v>42</v>
@@ -7101,7 +7107,7 @@
         <v>65</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C178" s="20"/>
       <c r="D178" s="21"/>
@@ -7109,7 +7115,7 @@
         <v>23</v>
       </c>
       <c r="F178" s="22" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
@@ -7135,7 +7141,7 @@
         <v>65</v>
       </c>
       <c r="B179" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E179" s="11" t="s">
         <v>23</v>
@@ -7144,7 +7150,7 @@
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I179" s="14">
         <v>43</v>
@@ -7167,7 +7173,7 @@
         <v>65</v>
       </c>
       <c r="B180" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E180" s="11" t="s">
         <v>23</v>
@@ -7176,7 +7182,7 @@
         <v>15</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I180" s="14">
         <v>43</v>
@@ -7199,7 +7205,7 @@
         <v>65</v>
       </c>
       <c r="B181" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E181" s="11" t="s">
         <v>23</v>
@@ -7208,7 +7214,7 @@
         <v>15</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I181" s="14">
         <v>43</v>
@@ -7231,7 +7237,7 @@
         <v>65</v>
       </c>
       <c r="B182" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E182" s="11" t="s">
         <v>23</v>
@@ -7240,7 +7246,7 @@
         <v>16</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I182" s="14">
         <v>43</v>
@@ -7263,7 +7269,7 @@
         <v>65</v>
       </c>
       <c r="B183" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E183" s="11" t="s">
         <v>23</v>
@@ -7272,7 +7278,7 @@
         <v>18</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="I183" s="14">
         <v>43</v>
@@ -7295,13 +7301,13 @@
         <v>65</v>
       </c>
       <c r="B184" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C184" s="20"/>
       <c r="D184" s="21"/>
       <c r="E184" s="21"/>
       <c r="F184" s="22" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G184" s="20"/>
       <c r="H184" s="23"/>
@@ -7327,13 +7333,13 @@
         <v>65</v>
       </c>
       <c r="B185" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I185" s="14">
         <v>44</v>
@@ -7356,13 +7362,13 @@
         <v>65</v>
       </c>
       <c r="B186" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G186" t="s">
         <v>15</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I186" s="14">
         <v>44</v>
@@ -7385,13 +7391,13 @@
         <v>65</v>
       </c>
       <c r="B187" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G187" t="s">
         <v>15</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="I187" s="14">
         <v>44</v>
@@ -7414,13 +7420,13 @@
         <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G188" t="s">
         <v>16</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I188" s="14">
         <v>44</v>
@@ -7443,13 +7449,13 @@
         <v>65</v>
       </c>
       <c r="B189" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G189" t="s">
         <v>18</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I189" s="14">
         <v>44</v>
@@ -7472,7 +7478,7 @@
         <v>65</v>
       </c>
       <c r="B190" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="21"/>
@@ -7480,7 +7486,7 @@
         <v>23</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="23"/>
@@ -7506,7 +7512,7 @@
         <v>65</v>
       </c>
       <c r="B191" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E191" s="11" t="s">
         <v>23</v>
@@ -7515,7 +7521,7 @@
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I191" s="14">
         <v>45</v>
@@ -7538,7 +7544,7 @@
         <v>65</v>
       </c>
       <c r="B192" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E192" s="11" t="s">
         <v>23</v>
@@ -7547,7 +7553,7 @@
         <v>15</v>
       </c>
       <c r="H192" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I192" s="14">
         <v>45</v>
@@ -7570,7 +7576,7 @@
         <v>65</v>
       </c>
       <c r="B193" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E193" s="11" t="s">
         <v>23</v>
@@ -7579,7 +7585,7 @@
         <v>15</v>
       </c>
       <c r="H193" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I193" s="14">
         <v>45</v>
@@ -7602,7 +7608,7 @@
         <v>65</v>
       </c>
       <c r="B194" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E194" s="11" t="s">
         <v>23</v>
@@ -7611,7 +7617,7 @@
         <v>16</v>
       </c>
       <c r="H194" s="13" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="I194" s="14">
         <v>45</v>
@@ -7634,7 +7640,7 @@
         <v>65</v>
       </c>
       <c r="B195" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E195" s="11" t="s">
         <v>23</v>
@@ -7643,7 +7649,7 @@
         <v>18</v>
       </c>
       <c r="H195" s="13" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I195" s="14">
         <v>45</v>
@@ -7666,13 +7672,13 @@
         <v>65</v>
       </c>
       <c r="B196" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C196" s="20"/>
       <c r="D196" s="21"/>
       <c r="E196" s="21"/>
       <c r="F196" s="22" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G196" s="20"/>
       <c r="H196" s="23"/>
@@ -7698,13 +7704,13 @@
         <v>65</v>
       </c>
       <c r="B197" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G197" t="s">
         <v>15</v>
       </c>
       <c r="H197" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I197" s="14">
         <v>46</v>
@@ -7727,13 +7733,13 @@
         <v>65</v>
       </c>
       <c r="B198" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G198" t="s">
         <v>15</v>
       </c>
       <c r="H198" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I198" s="14">
         <v>46</v>
@@ -7756,13 +7762,13 @@
         <v>65</v>
       </c>
       <c r="B199" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G199" t="s">
         <v>15</v>
       </c>
       <c r="H199" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="I199" s="14">
         <v>46</v>
@@ -7785,13 +7791,13 @@
         <v>65</v>
       </c>
       <c r="B200" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G200" t="s">
         <v>16</v>
       </c>
       <c r="H200" s="13" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="I200" s="14">
         <v>46</v>
@@ -7814,13 +7820,13 @@
         <v>65</v>
       </c>
       <c r="B201" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G201" t="s">
         <v>18</v>
       </c>
       <c r="H201" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I201" s="14">
         <v>46</v>
@@ -7843,7 +7849,7 @@
         <v>65</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C202" s="20"/>
       <c r="D202" s="21"/>
@@ -7851,7 +7857,7 @@
         <v>23</v>
       </c>
       <c r="F202" s="22" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G202" s="20"/>
       <c r="H202" s="23"/>
@@ -7877,7 +7883,7 @@
         <v>65</v>
       </c>
       <c r="B203" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E203" s="11" t="s">
         <v>23</v>
@@ -7886,7 +7892,7 @@
         <v>15</v>
       </c>
       <c r="H203" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I203" s="14">
         <v>47</v>
@@ -7909,7 +7915,7 @@
         <v>65</v>
       </c>
       <c r="B204" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E204" s="11" t="s">
         <v>23</v>
@@ -7918,7 +7924,7 @@
         <v>15</v>
       </c>
       <c r="H204" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I204" s="14">
         <v>47</v>
@@ -7941,7 +7947,7 @@
         <v>65</v>
       </c>
       <c r="B205" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E205" s="11" t="s">
         <v>23</v>
@@ -7950,7 +7956,7 @@
         <v>15</v>
       </c>
       <c r="H205" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I205" s="14">
         <v>47</v>
@@ -7973,7 +7979,7 @@
         <v>65</v>
       </c>
       <c r="B206" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E206" s="11" t="s">
         <v>23</v>
@@ -7982,7 +7988,7 @@
         <v>16</v>
       </c>
       <c r="H206" s="13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I206" s="14">
         <v>47</v>
@@ -8005,7 +8011,7 @@
         <v>65</v>
       </c>
       <c r="B207" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E207" s="11" t="s">
         <v>23</v>
@@ -8014,7 +8020,7 @@
         <v>18</v>
       </c>
       <c r="H207" s="13" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="I207" s="14">
         <v>47</v>
@@ -8037,13 +8043,13 @@
         <v>65</v>
       </c>
       <c r="B208" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C208" s="20"/>
       <c r="D208" s="21"/>
       <c r="E208" s="21"/>
       <c r="F208" s="22" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G208" s="20"/>
       <c r="H208" s="23"/>
@@ -8069,13 +8075,13 @@
         <v>65</v>
       </c>
       <c r="B209" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G209" t="s">
         <v>15</v>
       </c>
       <c r="H209" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I209" s="14">
         <v>48</v>
@@ -8098,13 +8104,13 @@
         <v>65</v>
       </c>
       <c r="B210" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G210" t="s">
         <v>15</v>
       </c>
       <c r="H210" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I210" s="14">
         <v>48</v>
@@ -8127,13 +8133,13 @@
         <v>65</v>
       </c>
       <c r="B211" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G211" t="s">
         <v>15</v>
       </c>
       <c r="H211" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="I211" s="14">
         <v>48</v>
@@ -8156,13 +8162,13 @@
         <v>65</v>
       </c>
       <c r="B212" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G212" t="s">
         <v>16</v>
       </c>
       <c r="H212" s="13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I212" s="14">
         <v>48</v>
@@ -8185,13 +8191,13 @@
         <v>65</v>
       </c>
       <c r="B213" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G213" t="s">
         <v>18</v>
       </c>
       <c r="H213" s="13" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I213" s="14">
         <v>48</v>
@@ -8214,7 +8220,7 @@
         <v>65</v>
       </c>
       <c r="B214" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C214" s="20"/>
       <c r="D214" s="21" t="s">
@@ -8224,7 +8230,7 @@
         <v>23</v>
       </c>
       <c r="F214" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="G214" s="20"/>
       <c r="H214" s="23"/>
@@ -8250,7 +8256,7 @@
         <v>65</v>
       </c>
       <c r="B215" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D215" s="11" t="s">
         <v>23</v>
@@ -8262,7 +8268,7 @@
         <v>15</v>
       </c>
       <c r="H215" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="I215" s="14">
         <v>49</v>
@@ -8285,13 +8291,13 @@
         <v>65</v>
       </c>
       <c r="B216" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G216" t="s">
         <v>15</v>
       </c>
       <c r="H216" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I216" s="14">
         <v>49</v>
@@ -8314,13 +8320,13 @@
         <v>65</v>
       </c>
       <c r="B217" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G217" t="s">
         <v>15</v>
       </c>
       <c r="H217" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I217" s="14">
         <v>49</v>
@@ -8343,7 +8349,7 @@
         <v>65</v>
       </c>
       <c r="B218" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D218" s="11" t="s">
         <v>23</v>
@@ -8355,7 +8361,7 @@
         <v>16</v>
       </c>
       <c r="H218" s="13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I218" s="14">
         <v>49</v>
@@ -8378,7 +8384,7 @@
         <v>65</v>
       </c>
       <c r="B219" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D219" s="11" t="s">
         <v>23</v>
@@ -8390,7 +8396,7 @@
         <v>18</v>
       </c>
       <c r="H219" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="I219" s="14">
         <v>49</v>
@@ -8413,7 +8419,7 @@
         <v>65</v>
       </c>
       <c r="B220" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C220" s="20"/>
       <c r="D220" s="21" t="s">
@@ -8421,7 +8427,7 @@
       </c>
       <c r="E220" s="21"/>
       <c r="F220" s="22" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G220" s="20"/>
       <c r="H220" s="23"/>
@@ -8447,7 +8453,7 @@
         <v>65</v>
       </c>
       <c r="B221" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D221" s="11" t="s">
         <v>23</v>
@@ -8456,7 +8462,7 @@
         <v>15</v>
       </c>
       <c r="H221" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="I221" s="14">
         <v>50</v>
@@ -8479,7 +8485,7 @@
         <v>65</v>
       </c>
       <c r="B222" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D222" s="11" t="s">
         <v>23</v>
@@ -8488,7 +8494,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="13" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="I222" s="14">
         <v>50</v>
@@ -8511,7 +8517,7 @@
         <v>65</v>
       </c>
       <c r="B223" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D223" s="11" t="s">
         <v>23</v>
@@ -8520,7 +8526,7 @@
         <v>16</v>
       </c>
       <c r="H223" s="13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I223" s="14">
         <v>50</v>
@@ -8543,7 +8549,7 @@
         <v>65</v>
       </c>
       <c r="B224" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D224" s="11" t="s">
         <v>23</v>
@@ -8552,7 +8558,7 @@
         <v>18</v>
       </c>
       <c r="H224" s="13" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I224" s="14">
         <v>50</v>
@@ -8575,7 +8581,7 @@
         <v>65</v>
       </c>
       <c r="B225" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C225" s="20" t="s">
         <v>12</v>
@@ -8587,7 +8593,7 @@
         <v>23</v>
       </c>
       <c r="F225" s="22" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G225" s="20"/>
       <c r="H225" s="23"/>
@@ -8613,7 +8619,7 @@
         <v>65</v>
       </c>
       <c r="B226" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C226" t="s">
         <v>12</v>
@@ -8628,7 +8634,7 @@
         <v>15</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="I226" s="14">
         <v>51</v>
@@ -8651,7 +8657,7 @@
         <v>65</v>
       </c>
       <c r="B227" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C227" t="s">
         <v>12</v>
@@ -8666,7 +8672,7 @@
         <v>16</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I227" s="14">
         <v>51</v>
@@ -8689,7 +8695,7 @@
         <v>65</v>
       </c>
       <c r="B228" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C228" t="s">
         <v>12</v>
@@ -8704,7 +8710,7 @@
         <v>18</v>
       </c>
       <c r="H228" s="13" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I228" s="14">
         <v>51</v>
@@ -8727,7 +8733,7 @@
         <v>65</v>
       </c>
       <c r="B229" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C229" s="20" t="s">
         <v>12</v>
@@ -8737,7 +8743,7 @@
       </c>
       <c r="E229" s="21"/>
       <c r="F229" s="22" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G229" s="20"/>
       <c r="H229" s="23"/>
@@ -8763,7 +8769,7 @@
         <v>65</v>
       </c>
       <c r="B230" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C230" t="s">
         <v>12</v>
@@ -8775,7 +8781,7 @@
         <v>15</v>
       </c>
       <c r="H230" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I230" s="14">
         <v>52</v>
@@ -8798,7 +8804,7 @@
         <v>65</v>
       </c>
       <c r="B231" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C231" t="s">
         <v>12</v>
@@ -8810,7 +8816,7 @@
         <v>16</v>
       </c>
       <c r="H231" s="13" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I231" s="14">
         <v>52</v>
@@ -8833,7 +8839,7 @@
         <v>65</v>
       </c>
       <c r="B232" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C232" t="s">
         <v>12</v>
@@ -8845,7 +8851,7 @@
         <v>18</v>
       </c>
       <c r="H232" s="13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I232" s="14">
         <v>52</v>
@@ -8868,7 +8874,7 @@
         <v>65</v>
       </c>
       <c r="B233" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C233" s="20" t="s">
         <v>12</v>
@@ -8880,7 +8886,7 @@
         <v>23</v>
       </c>
       <c r="F233" s="22" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="G233" s="20"/>
       <c r="H233" s="23"/>
@@ -8906,7 +8912,7 @@
         <v>65</v>
       </c>
       <c r="B234" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C234" t="s">
         <v>12</v>
@@ -8921,7 +8927,7 @@
         <v>15</v>
       </c>
       <c r="H234" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="I234" s="14">
         <v>53</v>
@@ -8944,7 +8950,7 @@
         <v>65</v>
       </c>
       <c r="B235" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C235" t="s">
         <v>12</v>
@@ -8959,7 +8965,7 @@
         <v>16</v>
       </c>
       <c r="H235" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I235" s="14">
         <v>53</v>
@@ -8982,7 +8988,7 @@
         <v>65</v>
       </c>
       <c r="B236" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C236" t="s">
         <v>12</v>
@@ -8997,7 +9003,7 @@
         <v>18</v>
       </c>
       <c r="H236" s="13" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="I236" s="14">
         <v>53</v>
@@ -9020,7 +9026,7 @@
         <v>65</v>
       </c>
       <c r="B237" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>12</v>
@@ -9030,7 +9036,7 @@
       </c>
       <c r="E237" s="21"/>
       <c r="F237" s="22" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G237" s="20"/>
       <c r="H237" s="23"/>
@@ -9056,7 +9062,7 @@
         <v>65</v>
       </c>
       <c r="B238" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C238" t="s">
         <v>12</v>
@@ -9068,7 +9074,7 @@
         <v>15</v>
       </c>
       <c r="H238" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I238" s="14">
         <v>54</v>
@@ -9091,7 +9097,7 @@
         <v>65</v>
       </c>
       <c r="B239" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C239" t="s">
         <v>12</v>
@@ -9103,7 +9109,7 @@
         <v>16</v>
       </c>
       <c r="H239" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I239" s="14">
         <v>54</v>
@@ -9126,7 +9132,7 @@
         <v>65</v>
       </c>
       <c r="B240" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C240" t="s">
         <v>12</v>
@@ -9138,7 +9144,7 @@
         <v>18</v>
       </c>
       <c r="H240" s="13" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I240" s="14">
         <v>54</v>
@@ -9158,7 +9164,7 @@
     </row>
     <row r="241" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="J241" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -9178,13 +9184,13 @@
         <v>11</v>
       </c>
       <c r="B242" s="38" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C242" s="38"/>
       <c r="D242" s="39"/>
       <c r="E242" s="39"/>
       <c r="F242" s="40" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="G242" s="38"/>
       <c r="H242" s="41"/>
@@ -9210,13 +9216,13 @@
         <v>11</v>
       </c>
       <c r="B243" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G243" t="s">
         <v>15</v>
       </c>
       <c r="H243" s="13" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="I243" s="14">
         <v>107</v>
@@ -9239,13 +9245,13 @@
         <v>11</v>
       </c>
       <c r="B244" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G244" t="s">
         <v>15</v>
       </c>
       <c r="H244" s="13" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="I244" s="14">
         <v>107</v>
@@ -9268,13 +9274,13 @@
         <v>11</v>
       </c>
       <c r="B245" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G245" t="s">
         <v>16</v>
       </c>
       <c r="H245" s="13" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I245" s="14">
         <v>107</v>
@@ -9297,13 +9303,13 @@
         <v>11</v>
       </c>
       <c r="B246" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G246" t="s">
         <v>18</v>
       </c>
       <c r="H246" s="13" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="I246" s="14">
         <v>107</v>
@@ -9336,28 +9342,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="50">
+    <cfRule type="containsBlanks" dxfId="14" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed duplicate scenario 107
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB791F94-196B-4E71-B724-C3A4C5D0DD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44CE558-5FFE-4F1A-AC42-61D1FEA1EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="285" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-25320" yWindow="240" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="198">
   <si>
     <t>Feature</t>
   </si>
@@ -618,21 +618,6 @@
   </si>
   <si>
     <t>NOTE: the test for the other 34 pages have not been implemented yet; an issue (#6) has been recorded for that on GitHub</t>
-  </si>
-  <si>
-    <t>Sales header with lookup value</t>
-  </si>
-  <si>
-    <t>Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</t>
-  </si>
-  <si>
-    <t>Warehouse shipment line</t>
-  </si>
-  <si>
-    <t>Lookup value on warehouse shipment line is populated with lookup value of sales header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnBeforeCreateShptLineFromSalesLineEvent </t>
   </si>
   <si>
     <t>Sales order with lookup value</t>
@@ -713,7 +698,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,12 +720,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -772,7 +751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -875,32 +854,60 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -964,54 +971,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1026,28 +985,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M246" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:M246" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:M241" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1350,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M247"/>
+  <dimension ref="A1:M242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242:XFD246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -5979,7 +5938,7 @@
       <c r="D143" s="21"/>
       <c r="E143" s="21"/>
       <c r="F143" s="22" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G143" s="20"/>
       <c r="H143" s="23"/>
@@ -6014,7 +5973,7 @@
         <v>15</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I144" s="14">
         <v>22</v>
@@ -6046,7 +6005,7 @@
         <v>16</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I145" s="14">
         <v>22</v>
@@ -6143,7 +6102,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="22" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G148" s="20"/>
       <c r="H148" s="23"/>
@@ -6181,7 +6140,7 @@
         <v>15</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I149" s="14">
         <v>27</v>
@@ -6216,7 +6175,7 @@
         <v>16</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I150" s="14">
         <v>27</v>
@@ -6282,7 +6241,7 @@
       <c r="D152" s="21"/>
       <c r="E152" s="21"/>
       <c r="F152" s="22" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G152" s="20"/>
       <c r="H152" s="23"/>
@@ -6381,7 +6340,7 @@
         <v>15</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I155" s="14">
         <v>23</v>
@@ -6413,7 +6372,7 @@
         <v>16</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I156" s="14">
         <v>23</v>
@@ -6445,7 +6404,7 @@
         <v>18</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I157" s="14">
         <v>23</v>
@@ -6478,7 +6437,7 @@
         <v>23</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G158" s="20"/>
       <c r="H158" s="23"/>
@@ -6586,7 +6545,7 @@
         <v>15</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I161" s="14">
         <v>25</v>
@@ -6621,7 +6580,7 @@
         <v>16</v>
       </c>
       <c r="H162" s="13" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I162" s="14">
         <v>25</v>
@@ -9162,7 +9121,7 @@
         <v>Then 'Lookup value field shown' } }</v>
       </c>
     </row>
-    <row r="241" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
         <v>186</v>
       </c>
@@ -9179,155 +9138,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B242" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="C242" s="38"/>
-      <c r="D242" s="39"/>
-      <c r="E242" s="39"/>
-      <c r="F242" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="G242" s="38"/>
-      <c r="H242" s="41"/>
-      <c r="I242" s="42">
-        <v>107</v>
-      </c>
-      <c r="J242" s="43" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
-      </c>
-      <c r="K242" s="44" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
-      </c>
-      <c r="L242" s="45" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0107 'Check OnBeforeCreateShptLineFromSalesLineEvent subscriber' {</v>
-      </c>
-      <c r="M242" s="41"/>
-    </row>
-    <row r="243" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>11</v>
-      </c>
-      <c r="B243" t="s">
-        <v>143</v>
-      </c>
-      <c r="G243" t="s">
-        <v>15</v>
-      </c>
-      <c r="H243" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="I243" s="14">
-        <v>107</v>
-      </c>
-      <c r="J243" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="K243" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="L243" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with lookup value'</v>
-      </c>
-    </row>
-    <row r="244" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>11</v>
-      </c>
-      <c r="B244" t="s">
-        <v>143</v>
-      </c>
-      <c r="G244" t="s">
-        <v>15</v>
-      </c>
-      <c r="H244" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="I244" s="14">
-        <v>107</v>
-      </c>
-      <c r="J244" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="K244" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="L244" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line'</v>
-      </c>
-    </row>
-    <row r="245" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>11</v>
-      </c>
-      <c r="B245" t="s">
-        <v>143</v>
-      </c>
-      <c r="G245" t="s">
-        <v>16</v>
-      </c>
-      <c r="H245" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="I245" s="14">
-        <v>107</v>
-      </c>
-      <c r="J245" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
-      </c>
-      <c r="K245" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
-      </c>
-      <c r="L245" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforeCreateShptLineFromSalesLineEvent '</v>
-      </c>
-    </row>
-    <row r="246" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>11</v>
-      </c>
-      <c r="B246" t="s">
-        <v>143</v>
-      </c>
-      <c r="G246" t="s">
-        <v>18</v>
-      </c>
-      <c r="H246" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="I246" s="14">
-        <v>107</v>
-      </c>
-      <c r="J246" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
-      </c>
-      <c r="K246" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
-      </c>
-      <c r="L246" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on warehouse shipment line is populated with lookup value of sales header' } }</v>
-      </c>
-    </row>
-    <row r="247" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="3:12" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="53">
@@ -9342,28 +9153,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="50">
+    <cfRule type="containsBlanks" dxfId="4" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="13" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implemented report extension with test #4
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44CE558-5FFE-4F1A-AC42-61D1FEA1EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B7A9CC-2217-491B-A7A7-DAE13CE83C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="240" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="200">
   <si>
     <t>Feature</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>Posting throws error on warehouse shipment line with empty lookup value</t>
+  </si>
+  <si>
+    <t>Test that lookup value shows on standard Customer - List report</t>
+  </si>
+  <si>
+    <t>Run standard report Customer - List</t>
   </si>
 </sst>
 </file>
@@ -985,8 +991,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M241" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:M241" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M245" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:M245" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
@@ -1309,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M242"/>
+  <dimension ref="A1:M246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242:XFD246"/>
+      <selection activeCell="G250" sqref="G250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6753,7 +6759,7 @@
         <v>When 'Run report CustomerList'</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>65</v>
       </c>
@@ -6779,170 +6785,159 @@
       </c>
       <c r="L168" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Report dataset contains both customers with lookup value' } }</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B169" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C169" s="5"/>
-      <c r="D169" s="6"/>
-      <c r="E169" s="6"/>
-      <c r="F169" s="7"/>
-      <c r="G169" s="5"/>
-      <c r="H169" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I169" s="9"/>
-      <c r="J169" s="18" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue Permissions</v>
-      </c>
-      <c r="K169" s="19" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue Permissions</v>
-      </c>
-      <c r="L169" s="32" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue Permissions' {</v>
-      </c>
-      <c r="M169" s="8"/>
-    </row>
-    <row r="170" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B170" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C170" s="20"/>
-      <c r="D170" s="21"/>
-      <c r="E170" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F170" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="G170" s="20"/>
-      <c r="H170" s="23"/>
-      <c r="I170" s="24">
-        <v>41</v>
-      </c>
-      <c r="J170" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0041] Create lookup value without permissions</v>
-      </c>
-      <c r="K170" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0041] Create lookup value without permissions</v>
-      </c>
-      <c r="L170" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0041 'Create lookup value without permissions' {</v>
-      </c>
-      <c r="M170" s="23"/>
+        <v>Then 'Report dataset contains both customers with lookup value' }</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B169" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C169" s="20"/>
+      <c r="D169" s="21"/>
+      <c r="E169" s="21"/>
+      <c r="F169" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G169" s="20"/>
+      <c r="H169" s="23"/>
+      <c r="I169" s="24">
+        <v>32</v>
+      </c>
+      <c r="J169" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0032] Test that lookup value shows on standard Customer - List report</v>
+      </c>
+      <c r="K169" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0032] Test that lookup value shows on standard Customer - List report</v>
+      </c>
+      <c r="L169" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0032 'Test that lookup value shows on standard Customer - List report' {</v>
+      </c>
+      <c r="M169" s="23"/>
+    </row>
+    <row r="170" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>65</v>
+      </c>
+      <c r="B170" t="s">
+        <v>104</v>
+      </c>
+      <c r="G170" t="s">
+        <v>15</v>
+      </c>
+      <c r="H170" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I170" s="14">
+        <v>32</v>
+      </c>
+      <c r="J170" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] 2 customers with different lookup value</v>
+      </c>
+      <c r="K170" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] 2 customers with different lookup value</v>
+      </c>
+      <c r="L170" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given '2 customers with different lookup value'</v>
+      </c>
     </row>
     <row r="171" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>65</v>
       </c>
       <c r="B171" t="s">
+        <v>104</v>
+      </c>
+      <c r="G171" t="s">
+        <v>16</v>
+      </c>
+      <c r="H171" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="I171" s="14">
+        <v>32</v>
+      </c>
+      <c r="J171" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Run standard report Customer - List</v>
+      </c>
+      <c r="K171" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Run standard report Customer - List</v>
+      </c>
+      <c r="L171" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Run standard report Customer - List'</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>65</v>
+      </c>
+      <c r="B172" t="s">
+        <v>104</v>
+      </c>
+      <c r="G172" t="s">
+        <v>18</v>
+      </c>
+      <c r="H172" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I172" s="14">
+        <v>32</v>
+      </c>
+      <c r="J172" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Report dataset contains both customers with lookup value</v>
+      </c>
+      <c r="K172" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Report dataset contains both customers with lookup value</v>
+      </c>
+      <c r="L172" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Report dataset contains both customers with lookup value' } }</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B173" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E171" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G171" t="s">
-        <v>15</v>
-      </c>
-      <c r="H171" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="I171" s="14">
-        <v>41</v>
-      </c>
-      <c r="J171" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Full base starting permissions</v>
-      </c>
-      <c r="K171" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Full base starting permissions</v>
-      </c>
-      <c r="L171" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions'</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>65</v>
-      </c>
-      <c r="B172" t="s">
-        <v>144</v>
-      </c>
-      <c r="E172" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G172" t="s">
-        <v>16</v>
-      </c>
-      <c r="H172" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="I172" s="14">
-        <v>41</v>
-      </c>
-      <c r="J172" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Create lookup value</v>
-      </c>
-      <c r="K172" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Create lookup value</v>
-      </c>
-      <c r="L172" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Create lookup value'</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>65</v>
-      </c>
-      <c r="B173" t="s">
-        <v>144</v>
-      </c>
-      <c r="E173" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G173" t="s">
-        <v>18</v>
-      </c>
-      <c r="H173" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="I173" s="14">
-        <v>41</v>
-      </c>
-      <c r="J173" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Insert permissions error thrown</v>
-      </c>
-      <c r="K173" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Insert permissions error thrown</v>
-      </c>
-      <c r="L173" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Insert permissions error thrown' }</v>
-      </c>
-    </row>
-    <row r="174" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C173" s="5"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="7"/>
+      <c r="G173" s="5"/>
+      <c r="H173" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="I173" s="9"/>
+      <c r="J173" s="18" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue Permissions</v>
+      </c>
+      <c r="K173" s="19" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue Permissions</v>
+      </c>
+      <c r="L173" s="32" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue Permissions' {</v>
+      </c>
+      <c r="M173" s="8"/>
+    </row>
+    <row r="174" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
         <v>65</v>
       </c>
@@ -6951,56 +6946,61 @@
       </c>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
-      <c r="E174" s="21"/>
+      <c r="E174" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="F174" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G174" s="20"/>
       <c r="H174" s="23"/>
       <c r="I174" s="24">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J174" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0042] Create lookup value with permissions</v>
+        <v>[SCENARIO #0041] Create lookup value without permissions</v>
       </c>
       <c r="K174" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0042] Create lookup value with permissions</v>
+        <v>//[SCENARIO #0041] Create lookup value without permissions</v>
       </c>
       <c r="L174" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0042 'Create lookup value with permissions' {</v>
+        <v>Scenario 0041 'Create lookup value without permissions' {</v>
       </c>
       <c r="M174" s="23"/>
     </row>
-    <row r="175" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>65</v>
       </c>
       <c r="B175" t="s">
         <v>144</v>
       </c>
+      <c r="E175" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G175" t="s">
         <v>15</v>
       </c>
       <c r="H175" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I175" s="14">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J175" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
+        <v>[GIVEN] Full base starting permissions</v>
       </c>
       <c r="K175" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
+        <v>//[GIVEN] Full base starting permissions</v>
       </c>
       <c r="L175" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
+        <v>Given 'Full base starting permissions'</v>
       </c>
     </row>
     <row r="176" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7010,6 +7010,9 @@
       <c r="B176" t="s">
         <v>144</v>
       </c>
+      <c r="E176" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G176" t="s">
         <v>16</v>
       </c>
@@ -7017,7 +7020,7 @@
         <v>151</v>
       </c>
       <c r="I176" s="14">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J176" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -7039,26 +7042,29 @@
       <c r="B177" t="s">
         <v>144</v>
       </c>
+      <c r="E177" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G177" t="s">
         <v>18</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I177" s="14">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J177" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value exists</v>
+        <v>[THEN] Insert permissions error thrown</v>
       </c>
       <c r="K177" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value exists</v>
+        <v>//[THEN] Insert permissions error thrown</v>
       </c>
       <c r="L177" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value exists' }</v>
+        <v>Then 'Insert permissions error thrown' }</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7070,61 +7076,56 @@
       </c>
       <c r="C178" s="20"/>
       <c r="D178" s="21"/>
-      <c r="E178" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="E178" s="21"/>
       <c r="F178" s="22" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="G178" s="20"/>
       <c r="H178" s="23"/>
       <c r="I178" s="24">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J178" s="25" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0043] Read lookup value without permissions</v>
+        <v>[SCENARIO #0042] Create lookup value with permissions</v>
       </c>
       <c r="K178" s="26" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0043] Read lookup value without permissions</v>
+        <v>//[SCENARIO #0042] Create lookup value with permissions</v>
       </c>
       <c r="L178" s="33" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0043 'Read lookup value without permissions' {</v>
+        <v>Scenario 0042 'Create lookup value with permissions' {</v>
       </c>
       <c r="M178" s="23"/>
     </row>
-    <row r="179" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
       <c r="B179" t="s">
         <v>144</v>
       </c>
-      <c r="E179" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G179" t="s">
         <v>15</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I179" s="14">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J179" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted starting permissions</v>
+        <v>[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="K179" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted starting permissions</v>
+        <v>//[GIVEN] Full base starting permissions extended with Lookup Value permissions</v>
       </c>
       <c r="L179" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions'</v>
+        <v>Given 'Full base starting permissions extended with Lookup Value permissions'</v>
       </c>
     </row>
     <row r="180" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7134,29 +7135,26 @@
       <c r="B180" t="s">
         <v>144</v>
       </c>
-      <c r="E180" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G180" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="I180" s="14">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J180" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup Value</v>
+        <v>[WHEN] Create lookup value</v>
       </c>
       <c r="K180" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup Value</v>
+        <v>//[WHEN] Create lookup value</v>
       </c>
       <c r="L180" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value'</v>
+        <v>When 'Create lookup value'</v>
       </c>
     </row>
     <row r="181" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7166,62 +7164,61 @@
       <c r="B181" t="s">
         <v>144</v>
       </c>
-      <c r="E181" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G181" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="I181" s="14">
+        <v>42</v>
+      </c>
+      <c r="J181" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Lookup value exists</v>
+      </c>
+      <c r="K181" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Lookup value exists</v>
+      </c>
+      <c r="L181" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Lookup value exists' }</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B182" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C182" s="20"/>
+      <c r="D182" s="21"/>
+      <c r="E182" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F182" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="G182" s="20"/>
+      <c r="H182" s="23"/>
+      <c r="I182" s="24">
         <v>43</v>
       </c>
-      <c r="J181" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Full base permissions</v>
-      </c>
-      <c r="K181" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Full base permissions</v>
-      </c>
-      <c r="L181" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions'</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>65</v>
-      </c>
-      <c r="B182" t="s">
-        <v>144</v>
-      </c>
-      <c r="E182" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G182" t="s">
-        <v>16</v>
-      </c>
-      <c r="H182" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="I182" s="14">
-        <v>43</v>
-      </c>
-      <c r="J182" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Read lookup value</v>
-      </c>
-      <c r="K182" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Read lookup value</v>
-      </c>
-      <c r="L182" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Read lookup value'</v>
-      </c>
+      <c r="J182" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0043] Read lookup value without permissions</v>
+      </c>
+      <c r="K182" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0043] Read lookup value without permissions</v>
+      </c>
+      <c r="L182" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0043 'Read lookup value without permissions' {</v>
+      </c>
+      <c r="M182" s="23"/>
     </row>
     <row r="183" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
@@ -7234,58 +7231,58 @@
         <v>23</v>
       </c>
       <c r="G183" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="I183" s="14">
         <v>43</v>
       </c>
       <c r="J183" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Read permissions error thrown</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K183" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Read permissions error thrown</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L183" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Read permissions error thrown' }</v>
-      </c>
-    </row>
-    <row r="184" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B184" s="20" t="s">
+        <v>Given 'Unrestricted starting permissions'</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>65</v>
+      </c>
+      <c r="B184" t="s">
         <v>144</v>
       </c>
-      <c r="C184" s="20"/>
-      <c r="D184" s="21"/>
-      <c r="E184" s="21"/>
-      <c r="F184" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="G184" s="20"/>
-      <c r="H184" s="23"/>
-      <c r="I184" s="24">
-        <v>44</v>
-      </c>
-      <c r="J184" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0044] Read lookup value with permissions</v>
-      </c>
-      <c r="K184" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0044] Read lookup value with permissions</v>
-      </c>
-      <c r="L184" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0044 'Read lookup value with permissions' {</v>
-      </c>
-      <c r="M184" s="23"/>
+      <c r="E184" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G184" t="s">
+        <v>15</v>
+      </c>
+      <c r="H184" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I184" s="14">
+        <v>43</v>
+      </c>
+      <c r="J184" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup Value</v>
+      </c>
+      <c r="K184" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup Value</v>
+      </c>
+      <c r="L184" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
+      </c>
     </row>
     <row r="185" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
@@ -7294,26 +7291,29 @@
       <c r="B185" t="s">
         <v>144</v>
       </c>
+      <c r="E185" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I185" s="14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J185" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted starting permissions</v>
+        <v>[GIVEN] Full base permissions</v>
       </c>
       <c r="K185" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted starting permissions</v>
+        <v>//[GIVEN] Full base permissions</v>
       </c>
       <c r="L185" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions'</v>
+        <v>Given 'Full base permissions'</v>
       </c>
     </row>
     <row r="186" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7323,85 +7323,94 @@
       <c r="B186" t="s">
         <v>144</v>
       </c>
+      <c r="E186" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G186" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>100</v>
+        <v>166</v>
       </c>
       <c r="I186" s="14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J186" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup Value</v>
+        <v>[WHEN] Read lookup value</v>
       </c>
       <c r="K186" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup Value</v>
+        <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L186" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup Value'</v>
-      </c>
-    </row>
-    <row r="187" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>When 'Read lookup value'</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>65</v>
       </c>
       <c r="B187" t="s">
         <v>144</v>
       </c>
+      <c r="E187" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G187" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="I187" s="14">
+        <v>43</v>
+      </c>
+      <c r="J187" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="K187" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Read permissions error thrown</v>
+      </c>
+      <c r="L187" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Read permissions error thrown' }</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B188" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C188" s="20"/>
+      <c r="D188" s="21"/>
+      <c r="E188" s="21"/>
+      <c r="F188" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="G188" s="20"/>
+      <c r="H188" s="23"/>
+      <c r="I188" s="24">
         <v>44</v>
       </c>
-      <c r="J187" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
-      </c>
-      <c r="K187" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
-      </c>
-      <c r="L187" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Full base permissions extended with Lookup Value'</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>65</v>
-      </c>
-      <c r="B188" t="s">
-        <v>144</v>
-      </c>
-      <c r="G188" t="s">
-        <v>16</v>
-      </c>
-      <c r="H188" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="I188" s="14">
-        <v>44</v>
-      </c>
-      <c r="J188" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Read lookup value</v>
-      </c>
-      <c r="K188" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Read lookup value</v>
-      </c>
-      <c r="L188" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Read lookup value'</v>
-      </c>
+      <c r="J188" s="25" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0044] Read lookup value with permissions</v>
+      </c>
+      <c r="K188" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0044] Read lookup value with permissions</v>
+      </c>
+      <c r="L188" s="33" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0044 'Read lookup value with permissions' {</v>
+      </c>
+      <c r="M188" s="23"/>
     </row>
     <row r="189" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
@@ -7411,91 +7420,83 @@
         <v>144</v>
       </c>
       <c r="G189" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="I189" s="14">
         <v>44</v>
       </c>
       <c r="J189" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value exists</v>
+        <v>[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="K189" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value exists</v>
+        <v>//[GIVEN] Unrestricted starting permissions</v>
       </c>
       <c r="L189" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value exists' }</v>
-      </c>
-    </row>
-    <row r="190" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B190" s="20" t="s">
+        <v>Given 'Unrestricted starting permissions'</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>65</v>
+      </c>
+      <c r="B190" t="s">
         <v>144</v>
       </c>
-      <c r="C190" s="20"/>
-      <c r="D190" s="21"/>
-      <c r="E190" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F190" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="G190" s="20"/>
-      <c r="H190" s="23"/>
-      <c r="I190" s="24">
-        <v>45</v>
-      </c>
-      <c r="J190" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0045] Modify lookup value without permissions</v>
-      </c>
-      <c r="K190" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0045] Modify lookup value without permissions</v>
-      </c>
-      <c r="L190" s="33" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0045 'Modify lookup value without permissions' {</v>
-      </c>
-      <c r="M190" s="23"/>
-    </row>
-    <row r="191" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="G190" t="s">
+        <v>15</v>
+      </c>
+      <c r="H190" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I190" s="14">
+        <v>44</v>
+      </c>
+      <c r="J190" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup Value</v>
+      </c>
+      <c r="K190" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup Value</v>
+      </c>
+      <c r="L190" s="31" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup Value'</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
       <c r="B191" t="s">
         <v>144</v>
       </c>
-      <c r="E191" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G191" t="s">
         <v>15</v>
       </c>
       <c r="H191" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I191" s="14">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J191" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Unrestricted starting permissions</v>
+        <v>[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="K191" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Unrestricted starting permissions</v>
+        <v>//[GIVEN] Full base permissions extended with Lookup Value</v>
       </c>
       <c r="L191" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Unrestricted starting permissions'</v>
+        <v>Given 'Full base permissions extended with Lookup Value'</v>
       </c>
     </row>
     <row r="192" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7505,29 +7506,26 @@
       <c r="B192" t="s">
         <v>144</v>
       </c>
-      <c r="E192" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G192" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H192" s="13" t="s">
-        <v>100</v>
+        <v>166</v>
       </c>
       <c r="I192" s="14">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J192" s="16" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup Value</v>
+        <v>[WHEN] Read lookup value</v>
       </c>
       <c r="K192" s="17" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup Value</v>
+        <v>//[WHEN] Read lookup value</v>
       </c>
       <c r="L192" s="31" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Ro